<commit_message>
feat: convert xlsx to json AB#11832
</commit_message>
<xml_diff>
--- a/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
+++ b/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\IBF-system\interfaces\IBF-dashboard\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2B5335-B331-45C2-89C1-E5F3915897F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACED27E5-F012-463C-BB7F-D1B1569D9E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15195" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
@@ -468,7 +468,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,6 +490,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -515,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -530,6 +536,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,7 +853,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D31E7F-BFF5-4ADE-901A-4F6BC662C23D}">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -860,9 +869,14 @@
     <col min="5" max="5" width="11.26171875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="88.89453125" style="3" customWidth="1"/>
     <col min="7" max="7" width="11.26171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.26171875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="13.47265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.89453125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="8.83984375" style="10"/>
+    <col min="107" max="107" width="93.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -884,8 +898,9 @@
       <c r="G1" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:16" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -901,8 +916,44 @@
       <c r="G2" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="H2" s="12" t="str">
+        <f>IF(A1="section","{","")</f>
+        <v>{</v>
+      </c>
+      <c r="I2" s="10" t="str">
+        <f>IF(A2=A1,"",""""&amp;A2&amp;""": {")</f>
+        <v>"aggregates": {</v>
+      </c>
+      <c r="J2" s="10" t="str">
+        <f>IF(B2=B1,"",""""&amp;B2&amp;""": {")</f>
+        <v>"population_affected": {</v>
+      </c>
+      <c r="K2" s="10" t="str">
+        <f>""""&amp;C2&amp;""": """&amp;F2&amp;""""</f>
+        <v>"UGA": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."</v>
+      </c>
+      <c r="L2" s="10" t="str">
+        <f>IF(B3=B2,",","}")</f>
+        <v>,</v>
+      </c>
+      <c r="M2" s="10" t="str">
+        <f>IF(B2=B3,"",IF(A2=A3,",",""))</f>
+        <v/>
+      </c>
+      <c r="N2" s="10" t="str">
+        <f>IF(A3=A2,"",IF(A3="","}","},"))</f>
+        <v/>
+      </c>
+      <c r="O2" s="10" t="str">
+        <f>IF(A3="","}","")</f>
+        <v/>
+      </c>
+      <c r="P2" s="10" t="str">
+        <f>H2&amp;I2&amp;J2&amp;K2&amp;L2&amp;M2&amp;N2&amp;O2</f>
+        <v>{"aggregates": {"population_affected": {"UGA": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].",</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -918,8 +969,44 @@
       <c r="G3" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="201.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="H3" s="12" t="str">
+        <f t="shared" ref="H3:H66" si="0">IF(A2="section","{","")</f>
+        <v/>
+      </c>
+      <c r="I3" s="10" t="str">
+        <f t="shared" ref="I3:I66" si="1">IF(A3=A2,"",""""&amp;A3&amp;""": {")</f>
+        <v/>
+      </c>
+      <c r="J3" s="10" t="str">
+        <f t="shared" ref="J3:J66" si="2">IF(B3=B2,"",""""&amp;B3&amp;""": {")</f>
+        <v/>
+      </c>
+      <c r="K3" s="10" t="str">
+        <f t="shared" ref="K3:K66" si="3">""""&amp;C3&amp;""": """&amp;F3&amp;""""</f>
+        <v>"EGY": "Number of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br/&gt;Explanation Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."</v>
+      </c>
+      <c r="L3" s="10" t="str">
+        <f t="shared" ref="L3:L66" si="4">IF(B4=B3,",","}")</f>
+        <v>,</v>
+      </c>
+      <c r="M3" s="10" t="str">
+        <f t="shared" ref="M3:M66" si="5">IF(B3=B4,"",IF(A3=A4,",",""))</f>
+        <v/>
+      </c>
+      <c r="N3" s="10" t="str">
+        <f t="shared" ref="N3:N66" si="6">IF(A4=A3,"",IF(A4="","}","},"))</f>
+        <v/>
+      </c>
+      <c r="O3" s="10" t="str">
+        <f t="shared" ref="O3:O66" si="7">IF(A4="","}","")</f>
+        <v/>
+      </c>
+      <c r="P3" s="10" t="str">
+        <f t="shared" ref="P3:P66" si="8">H3&amp;I3&amp;J3&amp;K3&amp;L3&amp;M3&amp;N3&amp;O3</f>
+        <v>"EGY": "Number of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br/&gt;Explanation Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds.",</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="201.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -935,8 +1022,44 @@
       <c r="G4" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="H4" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J4" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K4" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ZWE": "Number of people exposed is calculated by the population living in the droughts alert threshold reached area within the district currently triggered. The number of people and the drought extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): Worldpop &lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source drought alert thresold reached: ENSO: Seasonal ERSSTv5 (1991-2020 base period) 3-month running average in Niño 3.4 (5oNorth-5oSouth) (170-120oWest)).&lt;br /&gt;&lt;a href='https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt'&gt;https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt &lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Crop Yield data: izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA, &lt;a href = 'https://doi.org/10.1594/PANGAEA'&gt;https://doi.org/10.1594/PANGAEA.909132,Supplement&lt;/a&gt;.909132,Supplement to: Iizumi, Toshichika; Sakai, T (2020): The global dataset of historical yields for major crops 1981–2016. Scientific Data, 7(1), &lt;a href = 'https://doi.org/10.1038/s41597-020-0433-7'&gt;https://doi.org/10.1038/s41597-020-0433-7&lt;/a&gt;."</v>
+      </c>
+      <c r="L4" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M4" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N4" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O4" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P4" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"ZWE": "Number of people exposed is calculated by the population living in the droughts alert threshold reached area within the district currently triggered. The number of people and the drought extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): Worldpop &lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source drought alert thresold reached: ENSO: Seasonal ERSSTv5 (1991-2020 base period) 3-month running average in Niño 3.4 (5oNorth-5oSouth) (170-120oWest)).&lt;br /&gt;&lt;a href='https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt'&gt;https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt &lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Crop Yield data: izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA, &lt;a href = 'https://doi.org/10.1594/PANGAEA'&gt;https://doi.org/10.1594/PANGAEA.909132,Supplement&lt;/a&gt;.909132,Supplement to: Iizumi, Toshichika; Sakai, T (2020): The global dataset of historical yields for major crops 1981–2016. Scientific Data, 7(1), &lt;a href = 'https://doi.org/10.1038/s41597-020-0433-7'&gt;https://doi.org/10.1038/s41597-020-0433-7&lt;/a&gt;."},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -952,8 +1075,44 @@
       <c r="G5" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="H5" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I5" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J5" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"population_affected_percentage": {</v>
+      </c>
+      <c r="K5" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "Percentage of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source (Population Data):&lt;/b&gt; High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."</v>
+      </c>
+      <c r="L5" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M5" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N5" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O5" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P5" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"population_affected_percentage": {"UGA": "Percentage of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source (Population Data):&lt;/b&gt; High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].",</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -969,8 +1128,44 @@
       <c r="G6" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H6" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I6" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J6" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K6" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"EGY": "Percentage of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br/&gt;Explanation Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."</v>
+      </c>
+      <c r="L6" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M6" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N6" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O6" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P6" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"EGY": "Percentage of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br/&gt;Explanation Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -986,8 +1181,44 @@
       <c r="G7" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="H7" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I7" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J7" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"populationTotal": {</v>
+      </c>
+      <c r="K7" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"</v>
+      </c>
+      <c r="L7" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M7" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N7" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O7" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P7" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"populationTotal": {"UGA": "Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1003,8 +1234,44 @@
       <c r="G8" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H8" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I8" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J8" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K8" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ZWE": "Source link Zimbabwe. Worldpop data:&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;Estimates of total number of people per grid square broken down by gender and age groupings.&lt;/li&gt;&lt;li&gt;Accessed 07-2020 The mapping approach is Pezzulo, C. et al. Sub-national mapping of population pyramids and dependency ratios in Africa and Asia. Sci. Data 4:170089 doi:10.1038/sdata.2017.89 (2017)&lt;/li&gt;&lt;/ul&gt;"</v>
+      </c>
+      <c r="L8" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M8" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N8" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O8" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P8" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"ZWE": "Source link Zimbabwe. Worldpop data:&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;Estimates of total number of people per grid square broken down by gender and age groupings.&lt;/li&gt;&lt;li&gt;Accessed 07-2020 The mapping approach is Pezzulo, C. et al. Sub-national mapping of population pyramids and dependency ratios in Africa and Asia. Sci. Data 4:170089 doi:10.1038/sdata.2017.89 (2017)&lt;/li&gt;&lt;/ul&gt;"},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1020,8 +1287,44 @@
       <c r="G9" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H9" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I9" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J9" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"female_head_hh": {</v>
+      </c>
+      <c r="K9" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "Estimated exposed number of people living in female-headed households living in the flood extent area within the areas currently triggered. This number is calculated by multiplying the overall percentage of households with adult females as decision-maker and main income producer in an area, by the total exposed population in that area.&lt;br /&gt;&lt;br /&gt;Note that the estimate number is not the number of households, but the number of people living in a housholds. In this calculation a household size of 4.7 is used as average estimate.&lt;br /&gt;&lt;br /&gt;. The number of people in female headed households in the flood extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source data:&lt;ul&gt;&lt;li&gt;Female Headed Households: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014.&lt;/li&gt;&lt;li&gt;Total Population: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Flood extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt;&lt;/ul&gt;:"</v>
+      </c>
+      <c r="L9" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M9" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N9" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O9" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P9" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"female_head_hh": {"UGA": "Estimated exposed number of people living in female-headed households living in the flood extent area within the areas currently triggered. This number is calculated by multiplying the overall percentage of households with adult females as decision-maker and main income producer in an area, by the total exposed population in that area.&lt;br /&gt;&lt;br /&gt;Note that the estimate number is not the number of households, but the number of people living in a housholds. In this calculation a household size of 4.7 is used as average estimate.&lt;br /&gt;&lt;br /&gt;. The number of people in female headed households in the flood extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source data:&lt;ul&gt;&lt;li&gt;Female Headed Households: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014.&lt;/li&gt;&lt;li&gt;Total Population: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Flood extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt;&lt;/ul&gt;:"},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1037,8 +1340,44 @@
       <c r="G10" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H10" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I10" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J10" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"population_u8": {</v>
+      </c>
+      <c r="K10" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "Estimate exposed number of people under 8 years of age living in the flood extent area within the areas currently triggered. This number is calculated by multiplying the overall percentage of households with people under 8 years of age, by the total exposed population in that area. The number of people under 8 years of age in the flood extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source data:&lt;ul&gt;&lt;li&gt;Population under 8: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014.&lt;/li&gt;&lt;li&gt;Total Population: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Flood extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt;&lt;/ul&gt;:"</v>
+      </c>
+      <c r="L10" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M10" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N10" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O10" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P10" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"population_u8": {"UGA": "Estimate exposed number of people under 8 years of age living in the flood extent area within the areas currently triggered. This number is calculated by multiplying the overall percentage of households with people under 8 years of age, by the total exposed population in that area. The number of people under 8 years of age in the flood extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source data:&lt;ul&gt;&lt;li&gt;Population under 8: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014.&lt;/li&gt;&lt;li&gt;Total Population: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Flood extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt;&lt;/ul&gt;:"},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1054,8 +1393,44 @@
       <c r="G11" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H11" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I11" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J11" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"population_over65": {</v>
+      </c>
+      <c r="K11" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "Estimate exposed number of people over 65 years of age living in the flood extent area within the areas currently triggered. This number is calculated by multiplying the overall percentage of households with people over 65 years of age, by the total exposed population in that area. The number of people over 65 years of age in the flood extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source data:&lt;ul&gt;&lt;li&gt;Population over 65: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014.&lt;/li&gt;&lt;li&gt;Total Population: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Flood extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt;&lt;/ul&gt;:"</v>
+      </c>
+      <c r="L11" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M11" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N11" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O11" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P11" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"population_over65": {"UGA": "Estimate exposed number of people over 65 years of age living in the flood extent area within the areas currently triggered. This number is calculated by multiplying the overall percentage of households with people over 65 years of age, by the total exposed population in that area. The number of people over 65 years of age in the flood extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source data:&lt;ul&gt;&lt;li&gt;Population over 65: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014.&lt;/li&gt;&lt;li&gt;Total Population: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Flood extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt;&lt;/ul&gt;:"},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1071,8 +1446,44 @@
       <c r="G12" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H12" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I12" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J12" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"potential_cases": {</v>
+      </c>
+      <c r="K12" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"PHL": "Number of potential dengue cases, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"</v>
+      </c>
+      <c r="L12" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M12" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N12" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O12" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P12" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"potential_cases": {"PHL": "Number of potential dengue cases, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;",</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1088,8 +1499,44 @@
       <c r="G13" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H13" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I13" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J13" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K13" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ETH": "Potential number of cases are calculated with the assumtion of a rough proportionality between malaria mosquito enviromental suitability and malaria risk. Then estimating a time lag between optimal malaria mosquito environmental conditions and the peak in number of malaria cases."</v>
+      </c>
+      <c r="L13" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M13" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N13" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O13" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P13" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"ETH": "Potential number of cases are calculated with the assumtion of a rough proportionality between malaria mosquito enviromental suitability and malaria risk. Then estimating a time lag between optimal malaria mosquito environmental conditions and the peak in number of malaria cases."},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1105,8 +1552,44 @@
       <c r="G14" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H14" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I14" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J14" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"potential_cases_U5": {</v>
+      </c>
+      <c r="K14" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ETH": "Potential cases under 5. Vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"</v>
+      </c>
+      <c r="L14" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M14" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N14" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O14" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P14" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"potential_cases_U5": {"ETH": "Potential cases under 5. Vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1122,8 +1605,44 @@
       <c r="G15" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H15" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I15" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J15" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"potential_cases_U9": {</v>
+      </c>
+      <c r="K15" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"PHL": "Number of potential dengue cases among children under 9 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"</v>
+      </c>
+      <c r="L15" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M15" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N15" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O15" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P15" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"potential_cases_U9": {"PHL": "Number of potential dengue cases among children under 9 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -1139,8 +1658,44 @@
       <c r="G16" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H16" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I16" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J16" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"potential_cases_65": {</v>
+      </c>
+      <c r="K16" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"PHL": "Number of potential dengue cases among people above 65 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"</v>
+      </c>
+      <c r="L16" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M16" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N16" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O16" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P16" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"potential_cases_65": {"PHL": "Number of potential dengue cases among people above 65 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;",</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1156,8 +1711,44 @@
       <c r="G17" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H17" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I17" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J17" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K17" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ETH": "Elderly: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates &lt;a href=\"https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates\"&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"</v>
+      </c>
+      <c r="L17" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M17" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N17" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O17" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P17" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"ETH": "Elderly: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates &lt;a href=\"https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates\"&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -1173,8 +1764,44 @@
       <c r="G18" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H18" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I18" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J18" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"small_ruminants_exposed": {</v>
+      </c>
+      <c r="K18" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ZWE": "Number of exposed small ruminants (sheep and goats) is calculated by the small ruminants per province within the droughts alert threshold reached area currently triggered. Livestock numbers small ruminants exists of the number of small ruminants multiplied with the Livestock unit (LSU): 0.1 as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source Links:&lt;ul&gt;&lt;li&gt;Number of small ruminants (sheep and goats) mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021&lt;/li&gt;&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href=\"https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0 \"&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0. &lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"</v>
+      </c>
+      <c r="L18" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M18" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N18" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O18" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P18" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"small_ruminants_exposed": {"ZWE": "Number of exposed small ruminants (sheep and goats) is calculated by the small ruminants per province within the droughts alert threshold reached area currently triggered. Livestock numbers small ruminants exists of the number of small ruminants multiplied with the Livestock unit (LSU): 0.1 as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source Links:&lt;ul&gt;&lt;li&gt;Number of small ruminants (sheep and goats) mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021&lt;/li&gt;&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href=\"https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0 \"&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0. &lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -1190,8 +1817,44 @@
       <c r="G19" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="H19" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I19" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J19" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"cattle_exposed": {</v>
+      </c>
+      <c r="K19" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ZWE": "Number of exposed cattle is calculated by the cattle per province within the droughts alert threshold reached area currently triggered. Livestock numbers cattle exists of the number of cattle multiplied with the Livestock unit (LSU): 1.0 as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source Links:&lt;ul&gt;&lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season.Published: 21st of April 2021.&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;.&lt;/li&gt;&lt;/ul&gt;"</v>
+      </c>
+      <c r="L19" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M19" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N19" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v>},</v>
+      </c>
+      <c r="O19" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P19" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"cattle_exposed": {"ZWE": "Number of exposed cattle is calculated by the cattle per province within the droughts alert threshold reached area currently triggered. Livestock numbers cattle exists of the number of cattle multiplied with the Livestock unit (LSU): 1.0 as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source Links:&lt;ul&gt;&lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season.Published: 21st of April 2021.&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;.&lt;/li&gt;&lt;/ul&gt;"}},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
@@ -1207,8 +1870,44 @@
       <c r="G20" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="H20" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I20" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>"matrix": {</v>
+      </c>
+      <c r="J20" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"population_affected": {</v>
+      </c>
+      <c r="K20" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."</v>
+      </c>
+      <c r="L20" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M20" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N20" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O20" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P20" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"matrix": {"population_affected": {"UGA": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].",</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -1224,8 +1923,44 @@
       <c r="G21" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H21" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I21" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J21" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K21" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"EGY": "Number of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."</v>
+      </c>
+      <c r="L21" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M21" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N21" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O21" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P21" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"EGY": "Number of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds.",</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -1241,8 +1976,44 @@
       <c r="G22" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="H22" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I22" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J22" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K22" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ZWE": "Number of people exposed is calculated by the population living in the droughts alert threshold reached area within the district currently triggered. The number of people and the drought extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): Worldpop &lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source drought alert thresold reached: ENSO: Seasonal ERSSTv5 (1991-2020 base period) 3-month running average in Niño 3.4 (5oNorth-5oSouth) (170-120oWest)).&lt;br /&gt;&lt;a href='https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt'&gt;https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt &lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Crop Yield data: izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA, &lt;a href = 'https://doi.org/10.1594/PANGAEA'&gt;https://doi.org/10.1594/PANGAEA.909132,Supplement&lt;/a&gt;.909132,Supplement to: Iizumi, Toshichika; Sakai, T (2020): The global dataset of historical yields for major crops 1981–2016. Scientific Data, 7(1), &lt;a href = 'https://doi.org/10.1038/s41597-020-0433-7'&gt;https://doi.org/10.1038/s41597-020-0433-7&lt;/a&gt;."</v>
+      </c>
+      <c r="L22" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M22" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N22" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O22" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P22" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"ZWE": "Number of people exposed is calculated by the population living in the droughts alert threshold reached area within the district currently triggered. The number of people and the drought extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): Worldpop &lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source drought alert thresold reached: ENSO: Seasonal ERSSTv5 (1991-2020 base period) 3-month running average in Niño 3.4 (5oNorth-5oSouth) (170-120oWest)).&lt;br /&gt;&lt;a href='https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt'&gt;https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt &lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Crop Yield data: izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA, &lt;a href = 'https://doi.org/10.1594/PANGAEA'&gt;https://doi.org/10.1594/PANGAEA.909132,Supplement&lt;/a&gt;.909132,Supplement to: Iizumi, Toshichika; Sakai, T (2020): The global dataset of historical yields for major crops 1981–2016. Scientific Data, 7(1), &lt;a href = 'https://doi.org/10.1038/s41597-020-0433-7'&gt;https://doi.org/10.1038/s41597-020-0433-7&lt;/a&gt;."},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -1258,8 +2029,44 @@
       <c r="G23" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="H23" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I23" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J23" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"population_affected_percentage": {</v>
+      </c>
+      <c r="K23" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "Percentage of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."</v>
+      </c>
+      <c r="L23" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M23" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N23" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O23" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P23" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"population_affected_percentage": {"UGA": "Percentage of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].",</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -1275,8 +2082,44 @@
       <c r="G24" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H24" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I24" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J24" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K24" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"EGY": "Percentage of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."</v>
+      </c>
+      <c r="L24" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M24" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N24" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O24" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P24" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"EGY": "Percentage of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
@@ -1292,8 +2135,44 @@
       <c r="G25" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="H25" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I25" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J25" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"populationTotal": {</v>
+      </c>
+      <c r="K25" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"</v>
+      </c>
+      <c r="L25" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M25" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N25" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O25" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P25" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"populationTotal": {"UGA": "Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
         <v>42</v>
       </c>
@@ -1309,8 +2188,44 @@
       <c r="G26" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H26" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I26" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J26" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K26" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ZWE": "Source link Zimbabwe. Worldpop data:&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;Estimates of total number of people per grid square broken down by gender and age groupings.&lt;/li&gt;&lt;li&gt;Accessed 07-2020 The mapping approach is Pezzulo, C. et al. Sub-national mapping of population pyramids and dependency ratios in Africa and Asia. Sci. Data 4:170089 doi:10.1038/sdata.2017.89 (2017)&lt;/li&gt;&lt;/ul&gt;"</v>
+      </c>
+      <c r="L26" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M26" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N26" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O26" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P26" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"ZWE": "Source link Zimbabwe. Worldpop data:&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;Estimates of total number of people per grid square broken down by gender and age groupings.&lt;/li&gt;&lt;li&gt;Accessed 07-2020 The mapping approach is Pezzulo, C. et al. Sub-national mapping of population pyramids and dependency ratios in Africa and Asia. Sci. Data 4:170089 doi:10.1038/sdata.2017.89 (2017)&lt;/li&gt;&lt;/ul&gt;"},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
         <v>42</v>
       </c>
@@ -1326,8 +2241,44 @@
       <c r="G27" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H27" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I27" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J27" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"female_head_hh": {</v>
+      </c>
+      <c r="K27" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "Percentage of people living in female headed households.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."</v>
+      </c>
+      <c r="L27" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M27" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N27" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O27" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P27" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"female_head_hh": {"UGA": "Percentage of people living in female headed households.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014.",</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
         <v>42</v>
       </c>
@@ -1343,8 +2294,44 @@
       <c r="G28" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H28" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I28" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J28" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K28" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"PHL": "Percentage of people living in female-headed households. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"</v>
+      </c>
+      <c r="L28" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M28" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N28" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O28" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P28" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"PHL": "Percentage of people living in female-headed households. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
@@ -1360,8 +2347,44 @@
       <c r="G29" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H29" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I29" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J29" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"population_u5": {</v>
+      </c>
+      <c r="K29" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ETH": "Under age: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"</v>
+      </c>
+      <c r="L29" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M29" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N29" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O29" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P29" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"population_u5": {"ETH": "Under age: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
         <v>42</v>
       </c>
@@ -1377,8 +2400,44 @@
       <c r="G30" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H30" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I30" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J30" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"population_u8": {</v>
+      </c>
+      <c r="K30" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "Percentage of people under 8 years old.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."</v>
+      </c>
+      <c r="L30" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M30" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N30" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O30" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P30" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"population_u8": {"UGA": "Percentage of people under 8 years old.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."},</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
         <v>42</v>
       </c>
@@ -1394,8 +2453,44 @@
       <c r="G31" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H31" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I31" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J31" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"population_u9": {</v>
+      </c>
+      <c r="K31" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"PHL": "Percentage of people under 9 years of age. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"</v>
+      </c>
+      <c r="L31" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M31" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N31" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O31" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P31" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"population_u9": {"PHL": "Percentage of people under 9 years of age. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
@@ -1411,8 +2506,44 @@
       <c r="G32" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H32" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I32" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J32" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"population_over65": {</v>
+      </c>
+      <c r="K32" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "Percentage of people over 65 years old.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."</v>
+      </c>
+      <c r="L32" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M32" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N32" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O32" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P32" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"population_over65": {"UGA": "Percentage of people over 65 years old.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014.",</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
@@ -1428,8 +2559,44 @@
       <c r="G33" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H33" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I33" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J33" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K33" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"PHL": "Percentage of people over 65 years of age. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"</v>
+      </c>
+      <c r="L33" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M33" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N33" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O33" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P33" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"PHL": "Percentage of people over 65 years of age. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
@@ -1445,8 +2612,44 @@
       <c r="G34" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H34" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I34" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J34" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"glofas_stations": {</v>
+      </c>
+      <c r="K34" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 5 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60/70/80% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"</v>
+      </c>
+      <c r="L34" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M34" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N34" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O34" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P34" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"glofas_stations": {"UGA": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 5 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60/70/80% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
@@ -1462,8 +2665,44 @@
       <c r="G35" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H35" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I35" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J35" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"typhoon_tracks": {</v>
+      </c>
+      <c r="K35" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"PHL": "This layer provides the location where the Global Flood Awareness System (Typhoon) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 5 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60/70/80% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"</v>
+      </c>
+      <c r="L35" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M35" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N35" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O35" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P35" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"typhoon_tracks": {"PHL": "This layer provides the location where the Global Flood Awareness System (Typhoon) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 5 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60/70/80% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -1479,8 +2718,44 @@
       <c r="G36" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H36" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I36" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J36" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"red_cross_branches": {</v>
+      </c>
+      <c r="K36" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Uganda Red Cross Society (URCS). Year: 2020."</v>
+      </c>
+      <c r="L36" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M36" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N36" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O36" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P36" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"red_cross_branches": {"UGA": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Uganda Red Cross Society (URCS). Year: 2020.",</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
@@ -1496,8 +2771,44 @@
       <c r="G37" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H37" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I37" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J37" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K37" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ZWE": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link Zimbabwe: ZRCS last updated July 2021 at provincial level."</v>
+      </c>
+      <c r="L37" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M37" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N37" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O37" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P37" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"ZWE": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link Zimbabwe: ZRCS last updated July 2021 at provincial level.",</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -1513,8 +2824,44 @@
       <c r="G38" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H38" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I38" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J38" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K38" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ZMB": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Zambia Red Cross Society (ZRCS). Year: 2020."</v>
+      </c>
+      <c r="L38" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M38" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N38" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O38" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P38" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"ZMB": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Zambia Red Cross Society (ZRCS). Year: 2020.",</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
@@ -1530,8 +2877,44 @@
       <c r="G39" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H39" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I39" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J39" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K39" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ETH": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Ethiopia Red Cross Society (ERCS). Year: 2020."</v>
+      </c>
+      <c r="L39" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M39" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N39" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O39" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P39" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"ETH": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Ethiopia Red Cross Society (ERCS). Year: 2020.",</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
@@ -1547,8 +2930,44 @@
       <c r="G40" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H40" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I40" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J40" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K40" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"KEN": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Kenya Red Cross Society (KRCS). Year: 2020."</v>
+      </c>
+      <c r="L40" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M40" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N40" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O40" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P40" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"KEN": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Kenya Red Cross Society (KRCS). Year: 2020.",</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
@@ -1564,8 +2983,44 @@
       <c r="G41" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="H41" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I41" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J41" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K41" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"EGY": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Egyptian Red Crescent Society (ERCS). Year: 2020."</v>
+      </c>
+      <c r="L41" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M41" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N41" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O41" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P41" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"EGY": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Egyptian Red Crescent Society (ERCS). Year: 2020."},</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
@@ -1581,8 +3036,44 @@
       <c r="G42" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="H42" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I42" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J42" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"waterpoints": {</v>
+      </c>
+      <c r="K42" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"</v>
+      </c>
+      <c r="L42" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M42" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N42" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O42" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P42" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"waterpoints": {"UGA": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -1598,8 +3089,44 @@
       <c r="G43" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H43" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I43" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J43" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"flood_extent": {</v>
+      </c>
+      <c r="K43" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."</v>
+      </c>
+      <c r="L43" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M43" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N43" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O43" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P43" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"flood_extent": {"UGA": "The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -1615,8 +3142,44 @@
       <c r="G44" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H44" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I44" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J44" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"rainfall_extent": {</v>
+      </c>
+      <c r="K44" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"EGY": "Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."</v>
+      </c>
+      <c r="L44" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M44" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N44" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O44" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P44" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"rainfall_extent": {"EGY": "Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
@@ -1632,8 +3195,44 @@
       <c r="G45" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H45" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I45" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J45" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"cropland": {</v>
+      </c>
+      <c r="K45" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"</v>
+      </c>
+      <c r="L45" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M45" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N45" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O45" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P45" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"cropland": {"UGA": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010",</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
         <v>42</v>
       </c>
@@ -1649,8 +3248,44 @@
       <c r="G46" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="H46" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I46" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J46" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K46" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ZWE": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link Zimbabwe: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"</v>
+      </c>
+      <c r="L46" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M46" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N46" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O46" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P46" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"ZWE": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link Zimbabwe: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
         <v>42</v>
       </c>
@@ -1666,8 +3301,44 @@
       <c r="G47" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="H47" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I47" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J47" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"grassland": {</v>
+      </c>
+      <c r="K47" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"</v>
+      </c>
+      <c r="L47" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M47" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N47" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O47" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P47" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"grassland": {"UGA": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
         <v>42</v>
       </c>
@@ -1683,8 +3354,44 @@
       <c r="G48" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="H48" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I48" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J48" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"wall_type": {</v>
+      </c>
+      <c r="K48" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "Percentage of households with permanent wall materials; percentage of buildings with (partly) concrete or brick walls.&lt;br /&gt;&lt;br /&gt;Source link: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."</v>
+      </c>
+      <c r="L48" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M48" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N48" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O48" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P48" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"wall_type": {"UGA": "Percentage of households with permanent wall materials; percentage of buildings with (partly) concrete or brick walls.&lt;br /&gt;&lt;br /&gt;Source link: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."},</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
         <v>42</v>
       </c>
@@ -1700,8 +3407,44 @@
       <c r="G49" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H49" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I49" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J49" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"roof_type": {</v>
+      </c>
+      <c r="K49" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "Percentage of households with permanent roof materials; percentage of buildings with (partly) concrete or iron or aluminium roofs.&lt;br /&gt;&lt;br /&gt;Source link: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."</v>
+      </c>
+      <c r="L49" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M49" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N49" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O49" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P49" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"roof_type": {"UGA": "Percentage of households with permanent roof materials; percentage of buildings with (partly) concrete or iron or aluminium roofs.&lt;br /&gt;&lt;br /&gt;Source link: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."},</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
         <v>42</v>
       </c>
@@ -1717,8 +3460,44 @@
       <c r="G50" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H50" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I50" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J50" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"poverty_incidence": {</v>
+      </c>
+      <c r="K50" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "Poverty Incidence is defined by the Multidiemensional Poverty Index and a $2 a day threshold. The layer gives an estimate of people living in poverty.&lt;br /&gt;&lt;br /&gt;Source: Tatem AJ, Gething PW, Bhatt S, Weiss D and Pezzulo C (2013) Pilot high resolution poverty maps, University of Southampton/Oxford. DOI: 10.5258/SOTON/WP00285. Year: 2010"</v>
+      </c>
+      <c r="L50" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M50" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N50" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O50" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P50" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"poverty_incidence": {"UGA": "Poverty Incidence is defined by the Multidiemensional Poverty Index and a $2 a day threshold. The layer gives an estimate of people living in poverty.&lt;br /&gt;&lt;br /&gt;Source: Tatem AJ, Gething PW, Bhatt S, Weiss D and Pezzulo C (2013) Pilot high resolution poverty maps, University of Southampton/Oxford. DOI: 10.5258/SOTON/WP00285. Year: 2010"},</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
         <v>42</v>
       </c>
@@ -1734,8 +3513,44 @@
       <c r="G51" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H51" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I51" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J51" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"flood_vulnerability_index": {</v>
+      </c>
+      <c r="K51" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "The disaster vulnerability index is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts of floods. The National Society and Technical Working group selected the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Poverty: Poverty incidence&lt;/li&gt;&lt;li&gt;20% Gender: Female headed household&lt;/li&gt;&lt;li&gt;10% Age: Population below 8-years&lt;/li&gt;&lt;li&gt;10% Age: population 65+,&lt;/li&gt;&lt;li&gt;10 % type of construction: permanent wall type&lt;/li&gt;&lt;li&gt;10 %type of construction: permanent roof type&lt;/li&gt;&lt;li&gt;20% Refugees legal status #of displaced person&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;For furhter information please refere to the Eap. For source links, see each individual layer."</v>
+      </c>
+      <c r="L51" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M51" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N51" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O51" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P51" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"flood_vulnerability_index": {"UGA": "The disaster vulnerability index is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts of floods. The National Society and Technical Working group selected the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Poverty: Poverty incidence&lt;/li&gt;&lt;li&gt;20% Gender: Female headed household&lt;/li&gt;&lt;li&gt;10% Age: Population below 8-years&lt;/li&gt;&lt;li&gt;10% Age: population 65+,&lt;/li&gt;&lt;li&gt;10 % type of construction: permanent wall type&lt;/li&gt;&lt;li&gt;10 %type of construction: permanent roof type&lt;/li&gt;&lt;li&gt;20% Refugees legal status #of displaced person&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;For furhter information please refere to the Eap. For source links, see each individual layer."},</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
         <v>42</v>
       </c>
@@ -1751,8 +3566,44 @@
       <c r="G52" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H52" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I52" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J52" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"dam": {</v>
+      </c>
+      <c r="K52" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ZWE": "This layer represents a selection of dams, and their associated reservoirs in Zimbabwe. The selection is made, based on the  Zimbabwe National Water Authority.&lt;br /&gt;&lt;br /&gt;Source Link Zimbabwe:&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.zinwa.co.zw/dam-levels/'&gt;https://www.zinwa.co.zw/dam-levels/&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"</v>
+      </c>
+      <c r="L52" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M52" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N52" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O52" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P52" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"dam": {"ZWE": "This layer represents a selection of dams, and their associated reservoirs in Zimbabwe. The selection is made, based on the  Zimbabwe National Water Authority.&lt;br /&gt;&lt;br /&gt;Source Link Zimbabwe:&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.zinwa.co.zw/dam-levels/'&gt;https://www.zinwa.co.zw/dam-levels/&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"},</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
         <v>42</v>
       </c>
@@ -1768,8 +3619,44 @@
       <c r="G53" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="H53" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I53" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J53" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"drought_vulnerability_index": {</v>
+      </c>
+      <c r="K53" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ZWE": "The drought vulnerability index is a composite index for the context of exposure to drought and the capacity to anticipate, cope with and recover from the impacts of droughts. The ZRCS selected nine main criteria:&lt;ul&gt;&lt;li&gt;14% Labor constrained households: 7 %unemployment rate 15+  and 7% economically non-active&lt;/li&gt;&lt;li&gt;15% Child, women and elderly headed households: 5% Female headed HH , 5% Head of Household (19-), 5% Head of Household (65+)&lt;/li&gt;&lt;li&gt;14% People with disabilities&lt;/li&gt;&lt;li&gt;15 % Pregnant and breast-feeding women, and children under five years: 5% pregnant women, 5% breast-feeding women, 5% children under five years&lt;/li&gt;&lt;li&gt;14 % Severe acute malnutrition&lt;/li&gt;&lt;li&gt;7% employment agriculture&lt;/li&gt;&lt;li&gt;7% cattle per km2&lt;/li&gt;&lt;li&gt;7% HIV prevalence&lt;/li&gt;&lt;li&gt;7% HIV ART Coverage&lt;/li&gt;&lt;/ul&gt;"</v>
+      </c>
+      <c r="L53" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M53" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N53" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O53" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P53" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"drought_vulnerability_index": {"ZWE": "The drought vulnerability index is a composite index for the context of exposure to drought and the capacity to anticipate, cope with and recover from the impacts of droughts. The ZRCS selected nine main criteria:&lt;ul&gt;&lt;li&gt;14% Labor constrained households: 7 %unemployment rate 15+  and 7% economically non-active&lt;/li&gt;&lt;li&gt;15% Child, women and elderly headed households: 5% Female headed HH , 5% Head of Household (19-), 5% Head of Household (65+)&lt;/li&gt;&lt;li&gt;14% People with disabilities&lt;/li&gt;&lt;li&gt;15 % Pregnant and breast-feeding women, and children under five years: 5% pregnant women, 5% breast-feeding women, 5% children under five years&lt;/li&gt;&lt;li&gt;14 % Severe acute malnutrition&lt;/li&gt;&lt;li&gt;7% employment agriculture&lt;/li&gt;&lt;li&gt;7% cattle per km2&lt;/li&gt;&lt;li&gt;7% HIV prevalence&lt;/li&gt;&lt;li&gt;7% HIV ART Coverage&lt;/li&gt;&lt;/ul&gt;"},</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
         <v>42</v>
       </c>
@@ -1785,8 +3672,44 @@
       <c r="G54" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H54" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I54" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J54" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"covidrisk": {</v>
+      </c>
+      <c r="K54" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "The COVID-19 Risk Index is a composite index for the context of exposure, vulnerability to COVID and the capacity to anticipate, cope with and recover from the impacts of COVID-19 (a higher percentage indicates a higher risk to COVID-19). The National Society  selected the following criteria below:&lt;br /&gt;&lt;br /&gt;Exposure&lt;ul&gt;&lt;li&gt;population / km2&lt;/li&gt;&lt;/ul&gt;Vulnerability&lt;ul&gt;&lt;li&gt;% population 65+&lt;/li&gt;&lt;li&gt;% poverty incidence&lt;/li&gt;&lt;/ul&gt;Lack of Coping Capacity&lt;ul&gt;&lt;li&gt;% with no toilet facility&lt;/li&gt;&lt;li&gt;% access to safe drinking water&lt;/li&gt;&lt;li&gt;% illiterate&lt;/li&gt;&lt;li&gt;% with mobile access&lt;/li&gt;&lt;li&gt;% with internet access&lt;/li&gt;&lt;li&gt;% received remittances&lt;/li&gt;&lt;li&gt;HIV: incidence per 100&lt;/li&gt;&lt;li&gt;MALARIA: Plasmodium Falciparum incidence per 1000&lt;/li&gt;&lt;li&gt;% households which consume less than two meals per day&lt;/li&gt;&lt;li&gt;# healh facilities per person&lt;/li&gt;&lt;li&gt;% with a health facility within 5 km&lt;/li&gt;&lt;/ul&gt;&lt;br/&gt;Source link: &lt;a href='https://nlrc.maps.arcgis.com/apps/opsdashboard/index.html#/9ca9f0f452b04046b8594a74c31f0c3b'&gt;https://nlrc.maps.arcgis.com/apps/opsdashboard/index.html#/9ca9f0f452b04046b8594a74c31f0c3b&lt;/a&gt;."</v>
+      </c>
+      <c r="L54" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M54" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N54" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O54" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P54" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"covidrisk": {"UGA": "The COVID-19 Risk Index is a composite index for the context of exposure, vulnerability to COVID and the capacity to anticipate, cope with and recover from the impacts of COVID-19 (a higher percentage indicates a higher risk to COVID-19). The National Society  selected the following criteria below:&lt;br /&gt;&lt;br /&gt;Exposure&lt;ul&gt;&lt;li&gt;population / km2&lt;/li&gt;&lt;/ul&gt;Vulnerability&lt;ul&gt;&lt;li&gt;% population 65+&lt;/li&gt;&lt;li&gt;% poverty incidence&lt;/li&gt;&lt;/ul&gt;Lack of Coping Capacity&lt;ul&gt;&lt;li&gt;% with no toilet facility&lt;/li&gt;&lt;li&gt;% access to safe drinking water&lt;/li&gt;&lt;li&gt;% illiterate&lt;/li&gt;&lt;li&gt;% with mobile access&lt;/li&gt;&lt;li&gt;% with internet access&lt;/li&gt;&lt;li&gt;% received remittances&lt;/li&gt;&lt;li&gt;HIV: incidence per 100&lt;/li&gt;&lt;li&gt;MALARIA: Plasmodium Falciparum incidence per 1000&lt;/li&gt;&lt;li&gt;% households which consume less than two meals per day&lt;/li&gt;&lt;li&gt;# healh facilities per person&lt;/li&gt;&lt;li&gt;% with a health facility within 5 km&lt;/li&gt;&lt;/ul&gt;&lt;br/&gt;Source link: &lt;a href='https://nlrc.maps.arcgis.com/apps/opsdashboard/index.html#/9ca9f0f452b04046b8594a74c31f0c3b'&gt;https://nlrc.maps.arcgis.com/apps/opsdashboard/index.html#/9ca9f0f452b04046b8594a74c31f0c3b&lt;/a&gt;."},</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
         <v>42</v>
       </c>
@@ -1802,8 +3725,44 @@
       <c r="G55" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H55" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I55" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J55" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"health_sites": {</v>
+      </c>
+      <c r="K55" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"PHL": "Health facilities by type and location. Health facility types &lt;strong&gt;hospital&lt;/strong&gt; and &lt;strong&gt;clinic&lt;/strong&gt; are shown with different markers. Other types are omitted and rare in the data.&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;a/&gt;"</v>
+      </c>
+      <c r="L55" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M55" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N55" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O55" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P55" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"health_sites": {"PHL": "Health facilities by type and location. Health facility types &lt;strong&gt;hospital&lt;/strong&gt; and &lt;strong&gt;clinic&lt;/strong&gt; are shown with different markers. Other types are omitted and rare in the data.&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;a/&gt;"},</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
         <v>42</v>
       </c>
@@ -1819,8 +3778,44 @@
       <c r="G56" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="H56" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I56" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J56" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"population": {</v>
+      </c>
+      <c r="K56" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"UGA": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"</v>
+      </c>
+      <c r="L56" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M56" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N56" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O56" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P56" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"population": {"UGA": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
         <v>42</v>
       </c>
@@ -1836,8 +3831,44 @@
       <c r="G57" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H57" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I57" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J57" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"flood_susceptibility": {</v>
+      </c>
+      <c r="K57" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"EGY": "Flood susceptibility identifies the most vulnerable areas based on physical characteristics that determine the propensity for flooding” (Vojtek and Vojtekova, 2019). The mapping of flood susceptible areas involves the analysis of multiple criteria for different characteristics of the region that collectively contribute to the likelihood of floods.&lt;br/&gt;&lt;br/&gt;Nine influencing parameters based on a variety of satellite imagery and spatial datasets are the input factors of the model, such as topographical (Elevation model, Slope), physical (Land cover, Hydrological soil group) and hydrological properties (Height Above Nearest Drainage, Distance from Nearest Drainage, Topographic Wetness Index Slope, Rain intensity, Rain duration). Set of weights based on expert knowledge (The Analytical Hierarchical Process) from REACH (2019) was adapted in this analysis.&lt;br/&gt;&lt;br/&gt;&lt;strong&gt;LEGEND:&lt;/strong&gt; There are 4 classes of flood susceptibility. The higher the flood susceptibility, the darker blue the color.&lt;br/&gt;&lt;br/&gt;SOURCES:&lt;ul&gt;&lt;li&gt;REACH. Yemen Flood Susceptibility. 2019. &lt;a href='https://reliefweb.int/sites/reliefweb.int/files/resources/REACH_YEM_MethodologyNote_HVA_FloodSusceptibility_01APR2020_EN_V2.pdf'&gt;https://reliefweb.int/sites/reliefweb.int/files/resources/REACH_YEM_MethodologyNote_HVA_FloodSusceptibility_01APR2020_EN_V2.pdf&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Vojtek, M.; Vojteková, J. Flood Susceptibility Mapping on a National Scale in Slovakia Using the Analytical Hierarchy Process. Water 2019, 11, 364. &lt;a href='https://doi.org/10.3390/w11020364'&gt;https://doi.org/10.3390/w11020364&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"</v>
+      </c>
+      <c r="L57" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M57" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N57" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O57" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P57" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"flood_susceptibility": {"EGY": "Flood susceptibility identifies the most vulnerable areas based on physical characteristics that determine the propensity for flooding” (Vojtek and Vojtekova, 2019). The mapping of flood susceptible areas involves the analysis of multiple criteria for different characteristics of the region that collectively contribute to the likelihood of floods.&lt;br/&gt;&lt;br/&gt;Nine influencing parameters based on a variety of satellite imagery and spatial datasets are the input factors of the model, such as topographical (Elevation model, Slope), physical (Land cover, Hydrological soil group) and hydrological properties (Height Above Nearest Drainage, Distance from Nearest Drainage, Topographic Wetness Index Slope, Rain intensity, Rain duration). Set of weights based on expert knowledge (The Analytical Hierarchical Process) from REACH (2019) was adapted in this analysis.&lt;br/&gt;&lt;br/&gt;&lt;strong&gt;LEGEND:&lt;/strong&gt; There are 4 classes of flood susceptibility. The higher the flood susceptibility, the darker blue the color.&lt;br/&gt;&lt;br/&gt;SOURCES:&lt;ul&gt;&lt;li&gt;REACH. Yemen Flood Susceptibility. 2019. &lt;a href='https://reliefweb.int/sites/reliefweb.int/files/resources/REACH_YEM_MethodologyNote_HVA_FloodSusceptibility_01APR2020_EN_V2.pdf'&gt;https://reliefweb.int/sites/reliefweb.int/files/resources/REACH_YEM_MethodologyNote_HVA_FloodSusceptibility_01APR2020_EN_V2.pdf&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Vojtek, M.; Vojteková, J. Flood Susceptibility Mapping on a National Scale in Slovakia Using the Analytical Hierarchy Process. Water 2019, 11, 364. &lt;a href='https://doi.org/10.3390/w11020364'&gt;https://doi.org/10.3390/w11020364&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"},</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="s">
         <v>42</v>
       </c>
@@ -1853,8 +3884,44 @@
       <c r="G58" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H58" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I58" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J58" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"dengue_cases_average": {</v>
+      </c>
+      <c r="K58" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"PHL": "Number of dengue cases per administrative division per year. &lt;br /&gt;&lt;br /&gt;Source: &lt;a href=\"https://doh.gov.ph/statistics\"&gt;https://doh.gov.ph/statistics/&lt;/a&gt;"</v>
+      </c>
+      <c r="L58" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M58" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N58" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O58" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P58" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"dengue_cases_average": {"PHL": "Number of dengue cases per administrative division per year. &lt;br /&gt;&lt;br /&gt;Source: &lt;a href=\"https://doh.gov.ph/statistics\"&gt;https://doh.gov.ph/statistics/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="s">
         <v>42</v>
       </c>
@@ -1870,8 +3937,44 @@
       <c r="G59" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H59" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I59" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J59" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"dengue_incidence_average": {</v>
+      </c>
+      <c r="K59" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"PHL": "Number of dengue cases per 10.000.000 people per administrative division per year. &lt;br /&gt;&lt;br /&gt;Source: &lt;a href=\"https://doh.gov.ph/statistics\"&gt;https://doh.gov.ph/statistics/&lt;/a&gt;"</v>
+      </c>
+      <c r="L59" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M59" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N59" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O59" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P59" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"dengue_incidence_average": {"PHL": "Number of dengue cases per 10.000.000 people per administrative division per year. &lt;br /&gt;&lt;br /&gt;Source: &lt;a href=\"https://doh.gov.ph/statistics\"&gt;https://doh.gov.ph/statistics/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
         <v>42</v>
       </c>
@@ -1887,8 +3990,44 @@
       <c r="G60" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H60" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I60" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J60" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"potential_cases": {</v>
+      </c>
+      <c r="K60" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"PHL": "Number of potential dengue cases, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"</v>
+      </c>
+      <c r="L60" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M60" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N60" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O60" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P60" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"potential_cases": {"PHL": "Number of potential dengue cases, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;",</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
         <v>42</v>
       </c>
@@ -1904,8 +4043,44 @@
       <c r="G61" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H61" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I61" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J61" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K61" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ETH": "Potential number of cases are calculated with the assumtion of a rough proportionality between malaria mosquito enviromental suitability and malaria risk. Then estimating a time lag between optimal malaria mosquito environmental conditions and the peak in number of malaria cases."</v>
+      </c>
+      <c r="L61" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M61" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N61" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O61" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P61" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"ETH": "Potential number of cases are calculated with the assumtion of a rough proportionality between malaria mosquito enviromental suitability and malaria risk. Then estimating a time lag between optimal malaria mosquito environmental conditions and the peak in number of malaria cases."},</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
         <v>42</v>
       </c>
@@ -1921,8 +4096,44 @@
       <c r="G62" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H62" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I62" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J62" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"potential_cases_U5": {</v>
+      </c>
+      <c r="K62" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ETH": "Potential cases under 5. Vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"</v>
+      </c>
+      <c r="L62" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M62" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N62" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O62" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P62" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"potential_cases_U5": {"ETH": "Potential cases under 5. Vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
         <v>42</v>
       </c>
@@ -1938,8 +4149,44 @@
       <c r="G63" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H63" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I63" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J63" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"potential_cases_U9": {</v>
+      </c>
+      <c r="K63" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"PHL": "Number of potential dengue cases among children under 9 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"</v>
+      </c>
+      <c r="L63" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M63" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N63" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O63" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P63" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"potential_cases_U9": {"PHL": "Number of potential dengue cases among children under 9 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
         <v>42</v>
       </c>
@@ -1955,8 +4202,44 @@
       <c r="G64" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H64" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I64" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J64" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"potential_cases_65": {</v>
+      </c>
+      <c r="K64" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"PHL": "Number of potential dengue cases among people above 65 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"</v>
+      </c>
+      <c r="L64" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>,</v>
+      </c>
+      <c r="M64" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N64" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O64" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P64" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"potential_cases_65": {"PHL": "Number of potential dengue cases among people above 65 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href=\"https://data.humdata.org/dataset/philippines-pre-disaster-indicators\"&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;",</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
         <v>42</v>
       </c>
@@ -1972,8 +4255,44 @@
       <c r="G65" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="H65" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I65" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J65" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K65" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ETH": "Elderly: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates &lt;a href=\"https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates\"&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"</v>
+      </c>
+      <c r="L65" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M65" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N65" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O65" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P65" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"ETH": "Elderly: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates &lt;a href=\"https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates\"&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
         <v>42</v>
       </c>
@@ -1989,8 +4308,44 @@
       <c r="G66" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="H66" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I66" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J66" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>"small_ruminants": {</v>
+      </c>
+      <c r="K66" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>"ZWE": "Small ruminants exists of the summarised number sheep &amp; goats livestock numbers multiplied with the Livestock unit (LSU): 0.1 as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source link Zimbabwe:&lt;ul&gt;&lt;li&gt;Number of small ruminants (sheep and goats) mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021.&lt;/li&gt;&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href=\"https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0\"&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"</v>
+      </c>
+      <c r="L66" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>}</v>
+      </c>
+      <c r="M66" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>,</v>
+      </c>
+      <c r="N66" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O66" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P66" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>"small_ruminants": {"ZWE": "Small ruminants exists of the summarised number sheep &amp; goats livestock numbers multiplied with the Livestock unit (LSU): 0.1 as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source link Zimbabwe:&lt;ul&gt;&lt;li&gt;Number of small ruminants (sheep and goats) mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021.&lt;/li&gt;&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href=\"https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0\"&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"},</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
         <v>42</v>
       </c>
@@ -2006,8 +4361,44 @@
       <c r="G67" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H67" s="12" t="str">
+        <f t="shared" ref="H67:H86" si="9">IF(A66="section","{","")</f>
+        <v/>
+      </c>
+      <c r="I67" s="10" t="str">
+        <f t="shared" ref="I67:I85" si="10">IF(A67=A66,"",""""&amp;A67&amp;""": {")</f>
+        <v/>
+      </c>
+      <c r="J67" s="10" t="str">
+        <f t="shared" ref="J67:J85" si="11">IF(B67=B66,"",""""&amp;B67&amp;""": {")</f>
+        <v>"cattle": {</v>
+      </c>
+      <c r="K67" s="10" t="str">
+        <f t="shared" ref="K67:K85" si="12">""""&amp;C67&amp;""": """&amp;F67&amp;""""</f>
+        <v>"ZWE": "Livestock numbers cattle exists of the number of cattle multiplied with the Livestock unit (LSU): 1.0  as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source Links Zimbabwe:&lt;ul&gt;&lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021.&lt;/li&gt;&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href=\"https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0\"&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;.&lt;/li&gt;&lt;/ul&gt;"</v>
+      </c>
+      <c r="L67" s="10" t="str">
+        <f t="shared" ref="L67:L85" si="13">IF(B68=B67,",","}")</f>
+        <v>}</v>
+      </c>
+      <c r="M67" s="10" t="str">
+        <f t="shared" ref="M67:M85" si="14">IF(B67=B68,"",IF(A67=A68,",",""))</f>
+        <v>,</v>
+      </c>
+      <c r="N67" s="10" t="str">
+        <f t="shared" ref="N67:N85" si="15">IF(A68=A67,"",IF(A68="","}","},"))</f>
+        <v/>
+      </c>
+      <c r="O67" s="10" t="str">
+        <f t="shared" ref="O67:O86" si="16">IF(A68="","}","")</f>
+        <v/>
+      </c>
+      <c r="P67" s="10" t="str">
+        <f t="shared" ref="P67:P85" si="17">H67&amp;I67&amp;J67&amp;K67&amp;L67&amp;M67&amp;N67&amp;O67</f>
+        <v>"cattle": {"ZWE": "Livestock numbers cattle exists of the number of cattle multiplied with the Livestock unit (LSU): 1.0  as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source Links Zimbabwe:&lt;ul&gt;&lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021.&lt;/li&gt;&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href=\"https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0\"&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;.&lt;/li&gt;&lt;/ul&gt;"},</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
         <v>42</v>
       </c>
@@ -2023,8 +4414,44 @@
       <c r="G68" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H68" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I68" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J68" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"small_ruminants_exposed": {</v>
+      </c>
+      <c r="K68" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"ZWE": "Number of exposed small ruminants (sheep and goats) is calculated by the small ruminants per province within the droughts alert threshold reached area currently triggered. Livestock numbers small ruminants exists of the number of small ruminants multiplied with the Livestock unit (LSU): 0.1 as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source Links:&lt;ul&gt;&lt;li&gt;Number of small ruminants (sheep and goats) mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021&lt;/li&gt;&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href=\"https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0 \"&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0. &lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"</v>
+      </c>
+      <c r="L68" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M68" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v>,</v>
+      </c>
+      <c r="N68" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O68" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P68" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"small_ruminants_exposed": {"ZWE": "Number of exposed small ruminants (sheep and goats) is calculated by the small ruminants per province within the droughts alert threshold reached area currently triggered. Livestock numbers small ruminants exists of the number of small ruminants multiplied with the Livestock unit (LSU): 0.1 as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source Links:&lt;ul&gt;&lt;li&gt;Number of small ruminants (sheep and goats) mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021&lt;/li&gt;&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href=\"https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0 \"&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0. &lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"},</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
         <v>42</v>
       </c>
@@ -2040,8 +4467,44 @@
       <c r="G69" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H69" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I69" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J69" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"cattle_exposed": {</v>
+      </c>
+      <c r="K69" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"ZWE": "Number of exposed cattle is calculated by the cattle per province within the droughts alert threshold reached area currently triggered. Livestock numbers cattle exists of the number of cattle multiplied with the Livestock unit (LSU): 1.0 as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source Links:&lt;ul&gt;&lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season.Published: 21st of April 2021.&lt;/li&gt;&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;.&lt;/li&gt;&lt;/ul&gt;"</v>
+      </c>
+      <c r="L69" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M69" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v>,</v>
+      </c>
+      <c r="N69" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O69" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P69" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"cattle_exposed": {"ZWE": "Number of exposed cattle is calculated by the cattle per province within the droughts alert threshold reached area currently triggered. Livestock numbers cattle exists of the number of cattle multiplied with the Livestock unit (LSU): 1.0 as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source Links:&lt;ul&gt;&lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season.Published: 21st of April 2021.&lt;/li&gt;&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;.&lt;/li&gt;&lt;/ul&gt;"},</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
         <v>42</v>
       </c>
@@ -2057,8 +4520,44 @@
       <c r="G70" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H70" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I70" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J70" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"Hotspot_General": {</v>
+      </c>
+      <c r="K70" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"ETH": "Woreda need priority class: Hotspot Woredas Classification Final &lt;a href=\"http://www.ndrmc.gov.et/\"&gt;http://www.ndrmc.gov.et/&lt;/a&gt;"</v>
+      </c>
+      <c r="L70" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M70" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v>,</v>
+      </c>
+      <c r="N70" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O70" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P70" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"Hotspot_General": {"ETH": "Woreda need priority class: Hotspot Woredas Classification Final &lt;a href=\"http://www.ndrmc.gov.et/\"&gt;http://www.ndrmc.gov.et/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
         <v>42</v>
       </c>
@@ -2074,8 +4573,44 @@
       <c r="G71" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H71" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I71" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J71" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"Hotspot_Water": {</v>
+      </c>
+      <c r="K71" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"ETH": "WASH  need priority class: Hotspot Woredas Classification WASH &lt;a href=\"http://www.ndrmc.gov.et/\"&gt;http://www.ndrmc.gov.et/&lt;/a&gt;"</v>
+      </c>
+      <c r="L71" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M71" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v>,</v>
+      </c>
+      <c r="N71" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O71" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P71" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"Hotspot_Water": {"ETH": "WASH  need priority class: Hotspot Woredas Classification WASH &lt;a href=\"http://www.ndrmc.gov.et/\"&gt;http://www.ndrmc.gov.et/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
         <v>42</v>
       </c>
@@ -2091,8 +4626,44 @@
       <c r="G72" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H72" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I72" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J72" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"Hotspot_Health": {</v>
+      </c>
+      <c r="K72" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"ETH": "Health  need priority class: Hotspot Woredas Classification Health &lt;a href=\"http://www.ndrmc.gov.et/\"&gt;http://www.ndrmc.gov.et/&lt;/a&gt;"</v>
+      </c>
+      <c r="L72" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M72" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v>,</v>
+      </c>
+      <c r="N72" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O72" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P72" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"Hotspot_Health": {"ETH": "Health  need priority class: Hotspot Woredas Classification Health &lt;a href=\"http://www.ndrmc.gov.et/\"&gt;http://www.ndrmc.gov.et/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
         <v>42</v>
       </c>
@@ -2108,8 +4679,44 @@
       <c r="G73" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H73" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I73" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J73" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"IPC_forecast_short": {</v>
+      </c>
+      <c r="K73" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"ETH": "IPC short forecast: Most likely food security outcomes - the near-term projection  &lt;a href=\"https://fews.net/IPC\"&gt;https://fews.net/IPC&lt;/a&gt;"</v>
+      </c>
+      <c r="L73" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M73" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v>,</v>
+      </c>
+      <c r="N73" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O73" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P73" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"IPC_forecast_short": {"ETH": "IPC short forecast: Most likely food security outcomes - the near-term projection  &lt;a href=\"https://fews.net/IPC\"&gt;https://fews.net/IPC&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
         <v>42</v>
       </c>
@@ -2125,8 +4732,44 @@
       <c r="G74" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H74" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I74" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J74" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"IPC_forecast_long": {</v>
+      </c>
+      <c r="K74" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"ETH": "IPC long forecast: Most likely food security outcomes -  the medium-term projection &lt;a href=\"https://fews.net/IPC\"&gt;https://fews.net/IPC&lt;/a&gt;"</v>
+      </c>
+      <c r="L74" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M74" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v>,</v>
+      </c>
+      <c r="N74" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O74" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P74" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"IPC_forecast_long": {"ETH": "IPC long forecast: Most likely food security outcomes -  the medium-term projection &lt;a href=\"https://fews.net/IPC\"&gt;https://fews.net/IPC&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
         <v>42</v>
       </c>
@@ -2142,8 +4785,44 @@
       <c r="G75" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H75" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I75" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J75" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"walking_travel_time_to_health": {</v>
+      </c>
+      <c r="K75" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"ETH": "Access to Health walking: Estimated travel time (minutes) to the nearest healthcare facility, walking &lt;a href=\"https://malariaatlas.org/research-project/accessibility-to-healthcare/\"&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"</v>
+      </c>
+      <c r="L75" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M75" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v>,</v>
+      </c>
+      <c r="N75" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O75" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P75" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"walking_travel_time_to_health": {"ETH": "Access to Health walking: Estimated travel time (minutes) to the nearest healthcare facility, walking &lt;a href=\"https://malariaatlas.org/research-project/accessibility-to-healthcare/\"&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
         <v>42</v>
       </c>
@@ -2159,8 +4838,44 @@
       <c r="G76" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H76" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I76" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J76" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"motorized_travel_time_to_health": {</v>
+      </c>
+      <c r="K76" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"ETH": "Access to Health with vehicle: Estimated travel time (minutes) to the nearest healthcare facility, with motorized vehicle &lt;a href=\"https://malariaatlas.org/research-project/accessibility-to-healthcare/\"&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"</v>
+      </c>
+      <c r="L76" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M76" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v>,</v>
+      </c>
+      <c r="N76" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O76" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P76" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"motorized_travel_time_to_health": {"ETH": "Access to Health with vehicle: Estimated travel time (minutes) to the nearest healthcare facility, with motorized vehicle &lt;a href=\"https://malariaatlas.org/research-project/accessibility-to-healthcare/\"&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
         <v>42</v>
       </c>
@@ -2176,8 +4891,44 @@
       <c r="G77" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H77" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I77" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J77" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"travel_time_cities": {</v>
+      </c>
+      <c r="K77" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"ETH": "Predicted travel time (minutes) to nearest city &lt;a href=\"https://malariaatlas.org/research-project/accessibility-to-healthcare/\"&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"</v>
+      </c>
+      <c r="L77" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M77" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v>,</v>
+      </c>
+      <c r="N77" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O77" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P77" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"travel_time_cities": {"ETH": "Predicted travel time (minutes) to nearest city &lt;a href=\"https://malariaatlas.org/research-project/accessibility-to-healthcare/\"&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
         <v>42</v>
       </c>
@@ -2193,8 +4944,44 @@
       <c r="G78" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H78" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I78" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J78" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"malaria_suitable_temperature": {</v>
+      </c>
+      <c r="K78" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"ETH": "Malaria suitability:Temperature suitability index for Plasmodium vivax transmission, 2010 &lt;a href=\"https://malariaatlas.org/research-project/accessibility-to-healthcare/\"&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"</v>
+      </c>
+      <c r="L78" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M78" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v>,</v>
+      </c>
+      <c r="N78" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O78" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P78" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"malaria_suitable_temperature": {"ETH": "Malaria suitability:Temperature suitability index for Plasmodium vivax transmission, 2010 &lt;a href=\"https://malariaatlas.org/research-project/accessibility-to-healthcare/\"&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
         <v>42</v>
       </c>
@@ -2210,8 +4997,44 @@
       <c r="G79" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H79" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I79" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J79" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"malaria_risk": {</v>
+      </c>
+      <c r="K79" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"ETH": "Malaria risk:Spatial limits of Plasmodium vivax malaria transmission (0-none 2- high)  &lt;a href=\"https://malariaatlas.org/\"&gt;https://malariaatlas.org/&lt;/a&gt;"</v>
+      </c>
+      <c r="L79" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M79" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v>,</v>
+      </c>
+      <c r="N79" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O79" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P79" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"malaria_risk": {"ETH": "Malaria risk:Spatial limits of Plasmodium vivax malaria transmission (0-none 2- high)  &lt;a href=\"https://malariaatlas.org/\"&gt;https://malariaatlas.org/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
         <v>42</v>
       </c>
@@ -2227,8 +5050,44 @@
       <c r="G80" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H80" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I80" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J80" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"vulnerable_group": {</v>
+      </c>
+      <c r="K80" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"PHL": "TBD"</v>
+      </c>
+      <c r="L80" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M80" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v>,</v>
+      </c>
+      <c r="N80" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O80" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P80" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"vulnerable_group": {"PHL": "TBD"},</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
         <v>42</v>
       </c>
@@ -2244,8 +5103,44 @@
       <c r="G81" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H81" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I81" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J81" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"vulnerable_housing": {</v>
+      </c>
+      <c r="K81" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"PHL": "TBD"</v>
+      </c>
+      <c r="L81" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M81" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v>,</v>
+      </c>
+      <c r="N81" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O81" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P81" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"vulnerable_housing": {"PHL": "TBD"},</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1" t="s">
         <v>42</v>
       </c>
@@ -2261,8 +5156,44 @@
       <c r="G82" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="H82" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I82" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J82" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"total_idps": {</v>
+      </c>
+      <c r="K82" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"ETH": "Total Internally Displaced People (IDPs) DTM Ethiopia National Displacement Report 7_2022"</v>
+      </c>
+      <c r="L82" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M82" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v>,</v>
+      </c>
+      <c r="N82" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O82" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P82" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"total_idps": {"ETH": "Total Internally Displaced People (IDPs) DTM Ethiopia National Displacement Report 7_2022"},</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
         <v>42</v>
       </c>
@@ -2278,8 +5209,44 @@
       <c r="G83" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" ht="259.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H83" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I83" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J83" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v>"alert_threshold": {</v>
+      </c>
+      <c r="K83" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"PHL": "Administrative divisions that reached alert threshold, in terms of number of potential cases. &lt;br /&gt;&lt;br /&gt; See definition at: &lt;a href=\"https://rodekruis.sharepoint.com/sites/510-CRAVK-510/Gedeelde%20%20documenten/Forms/AllItems.aspx?id=%2Fsites%2F510%2DCRAVK%2D510%2FGedeelde%20%20documenten%2F%5BRD%5D%20Epidemics%20Priority%20Index%2FIBF%2Ddengue%2Fdocuments%2FIBF%5Fdengue%5Ftechnical%5Fnote%2Epdf&amp;parent=%2Fsites%2F510%2DCRAVK%2D510%2FGedeelde%20%20documenten%2F%5BRD%5D%20Epidemics%20Priority%20Index%2FIBF%2Ddengue%2Fdocuments&amp;p=true&amp;originalPath=aHR0cHM6Ly9yb2Rla3J1aXMuc2hhcmVwb2ludC5jb20vc2l0ZXMvNTEwLUNSQVZLLTUxMC9fbGF5b3V0cy8xNS9ndWVzdGFjY2Vzcy5hc3B4P2RvY2lkPTBmOTI0OWIzNWRhNGQ0YzBhOTg1YjMzMzkzZmMzODhkZiZhdXRoa2V5PUFRU0xubmFmR0YtTTJ0MUNHSWcwaGRBJmV4cGlyYXRpb249MjAyMi0wNi0xNFQyMiUzYTAwJTNhMDAuMDAwWiZydGltZT1TS016R0dzeDJVZw\"&gt; link to technical documentation&lt;/a&gt;"</v>
+      </c>
+      <c r="L83" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>,</v>
+      </c>
+      <c r="M83" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="N83" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O83" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P83" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"alert_threshold": {"PHL": "Administrative divisions that reached alert threshold, in terms of number of potential cases. &lt;br /&gt;&lt;br /&gt; See definition at: &lt;a href=\"https://rodekruis.sharepoint.com/sites/510-CRAVK-510/Gedeelde%20%20documenten/Forms/AllItems.aspx?id=%2Fsites%2F510%2DCRAVK%2D510%2FGedeelde%20%20documenten%2F%5BRD%5D%20Epidemics%20Priority%20Index%2FIBF%2Ddengue%2Fdocuments%2FIBF%5Fdengue%5Ftechnical%5Fnote%2Epdf&amp;parent=%2Fsites%2F510%2DCRAVK%2D510%2FGedeelde%20%20documenten%2F%5BRD%5D%20Epidemics%20Priority%20Index%2FIBF%2Ddengue%2Fdocuments&amp;p=true&amp;originalPath=aHR0cHM6Ly9yb2Rla3J1aXMuc2hhcmVwb2ludC5jb20vc2l0ZXMvNTEwLUNSQVZLLTUxMC9fbGF5b3V0cy8xNS9ndWVzdGFjY2Vzcy5hc3B4P2RvY2lkPTBmOTI0OWIzNWRhNGQ0YzBhOTg1YjMzMzkzZmMzODhkZiZhdXRoa2V5PUFRU0xubmFmR0YtTTJ0MUNHSWcwaGRBJmV4cGlyYXRpb249MjAyMi0wNi0xNFQyMiUzYTAwJTNhMDAuMDAwWiZydGltZT1TS016R0dzeDJVZw\"&gt; link to technical documentation&lt;/a&gt;",</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" ht="259.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1" t="s">
         <v>42</v>
       </c>
@@ -2295,8 +5262,44 @@
       <c r="G84" s="4">
         <v>44575</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="H84" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I84" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J84" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="K84" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"ZWE": "The layer shows each province in the country with a drought risk at the end of the growing season (April), and as such determine which districts are triggered when the province is expected to face a negative crop yield anomaly in April.&lt;br /&gt;The drought model is to assess a drought prediction skill of the 3-month running average Niño 3.4 values, and initiates a drought risk when there is a potential negative crop yield anomaly predicted. The model is developed based on XGBoost algorithm learning trained with historical Niño 3.4 to historical crop yield anomalies which is used as drought impact proxy. Loss of crops, livestock loss and child malnutrition and stunting are indicated by the ZRCS DRM working group and representatives from IFRC, PNS and Red Cross Climate Centre (RCCC)  as targeted drought impacts.&lt;br/&gt;&lt;br/&gt;Sources: &lt;ul&gt;&lt;li&gt;ENSO: Seasonal ERSSTv5 (1991-2020 base period) 3-month running average in Niño 3.4 (5oNorth-5oSouth) (170-120oWest))&lt;a href=\"https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt\"&gt;https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Crop Yield data: izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA,&lt;a href=\"https://doi.org/10.1594/PANGAEA.909132\"&gt;https://doi.org/10.1594/PANGAEA.909132&lt;/a&gt;,Supplement to:  izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA, https://doi.org/10.1594/PANGAEA.909132,Supplement to: Iizumi, Toshichika; Sakai, T (2020): The global dataset of historical yields for major crops 1981–2016. Scientific Data, 7(1), &lt;a href=\"https://doi.org/10.1038/s41597-020-0433-7\"&gt;https://doi.org/10.1038/s41597-020-0433-7&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"</v>
+      </c>
+      <c r="L84" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>,</v>
+      </c>
+      <c r="M84" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="N84" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="O84" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P84" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"ZWE": "The layer shows each province in the country with a drought risk at the end of the growing season (April), and as such determine which districts are triggered when the province is expected to face a negative crop yield anomaly in April.&lt;br /&gt;The drought model is to assess a drought prediction skill of the 3-month running average Niño 3.4 values, and initiates a drought risk when there is a potential negative crop yield anomaly predicted. The model is developed based on XGBoost algorithm learning trained with historical Niño 3.4 to historical crop yield anomalies which is used as drought impact proxy. Loss of crops, livestock loss and child malnutrition and stunting are indicated by the ZRCS DRM working group and representatives from IFRC, PNS and Red Cross Climate Centre (RCCC)  as targeted drought impacts.&lt;br/&gt;&lt;br/&gt;Sources: &lt;ul&gt;&lt;li&gt;ENSO: Seasonal ERSSTv5 (1991-2020 base period) 3-month running average in Niño 3.4 (5oNorth-5oSouth) (170-120oWest))&lt;a href=\"https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt\"&gt;https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Crop Yield data: izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA,&lt;a href=\"https://doi.org/10.1594/PANGAEA.909132\"&gt;https://doi.org/10.1594/PANGAEA.909132&lt;/a&gt;,Supplement to:  izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA, https://doi.org/10.1594/PANGAEA.909132,Supplement to: Iizumi, Toshichika; Sakai, T (2020): The global dataset of historical yields for major crops 1981–2016. Scientific Data, 7(1), &lt;a href=\"https://doi.org/10.1038/s41597-020-0433-7\"&gt;https://doi.org/10.1038/s41597-020-0433-7&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;",</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1" t="s">
         <v>42</v>
       </c>
@@ -2311,6 +5314,52 @@
       </c>
       <c r="G85" s="4">
         <v>44575</v>
+      </c>
+      <c r="H85" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I85" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J85" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="K85" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>"ETH": "An alert is released when two conditions are simultaneously the relative number of malaria cases is anomalous accordance to WHO guidelines, by comparing it to its monthly averages, the second condition is that the absolute number of malaria cases is high and thus likely to require humanitarian intervention."</v>
+      </c>
+      <c r="L85" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>}</v>
+      </c>
+      <c r="M85" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="N85" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>}</v>
+      </c>
+      <c r="O85" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>}</v>
+      </c>
+      <c r="P85" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>"ETH": "An alert is released when two conditions are simultaneously the relative number of malaria cases is anomalous accordance to WHO guidelines, by comparing it to its monthly averages, the second condition is that the absolute number of malaria cases is high and thus likely to require humanitarian intervention."}}}</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="H86" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O86" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: paste converted json into en.json AB#11833
</commit_message>
<xml_diff>
--- a/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
+++ b/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\IBF-system\interfaces\IBF-dashboard\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACED27E5-F012-463C-BB7F-D1B1569D9E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBFD798-2B28-42C0-A612-82411E7B8C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15195" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
@@ -857,7 +857,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -872,7 +872,8 @@
     <col min="8" max="8" width="11.26171875" style="10" customWidth="1"/>
     <col min="9" max="9" width="13.47265625" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.89453125" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="8.83984375" style="10"/>
+    <col min="11" max="11" width="8.83984375" style="10" customWidth="1"/>
+    <col min="12" max="16" width="8.83984375" style="10"/>
     <col min="107" max="107" width="93.3125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5363,6 +5364,11 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="yu56GkSp0KrBPqXR8+3BquDaUA3gBZDhKX5/57+XBI6LaO08EDBarillV6tCJ8JtAtgcdaW47LizBjlvYjMpew==" saltValue="/eU7IniqbAjyzt0Afhbs7A==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0"/>
+  <protectedRanges>
+    <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="H1:P1048576" name="Range1"/>
+    <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>
+  </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: process feedback AB#12042
</commit_message>
<xml_diff>
--- a/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
+++ b/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\IBF-system\interfaces\IBF-dashboard\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800B72E7-2499-4106-BAC2-63E00CBC26BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E643ABC-E031-42FA-A24F-76CA00BE8C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15195" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="README" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="173">
   <si>
     <t>section</t>
   </si>
@@ -75,9 +76,6 @@
     <t>Number of people exposed is calculated by the population living in the droughts alert threshold reached area within the district currently triggered. The number of people and the drought extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): Worldpop &lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source drought alert thresold reached: ENSO: Seasonal ERSSTv5 (1991-2020 base period) 3-month running average in Niño 3.4 (5oNorth-5oSouth) (170-120oWest)).&lt;br /&gt;&lt;a href='https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt'&gt;https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt &lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Crop Yield data: izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA, &lt;a href = 'https://doi.org/10.1594/PANGAEA'&gt;https://doi.org/10.1594/PANGAEA.909132,Supplement&lt;/a&gt;.909132,Supplement to: Iizumi, Toshichika; Sakai, T (2020): The global dataset of historical yields for major crops 1981–2016. Scientific Data, 7(1), &lt;a href = 'https://doi.org/10.1038/s41597-020-0433-7'&gt;https://doi.org/10.1038/s41597-020-0433-7&lt;/a&gt;.</t>
   </si>
   <si>
-    <t>aggregates</t>
-  </si>
-  <si>
     <t>population_affected_percentage</t>
   </si>
   <si>
@@ -162,9 +160,6 @@
     <t>cattle_exposed</t>
   </si>
   <si>
-    <t>matrix</t>
-  </si>
-  <si>
     <t>Number of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds.</t>
   </si>
   <si>
@@ -445,6 +440,120 @@
   </si>
   <si>
     <t>An alert is released when two conditions are simultaneously the relative number of malaria cases is anomalous accordance to WHO guidelines, by comparing it to its monthly averages, the second condition is that the absolute number of malaria cases is high and thus likely to require humanitarian intervention.</t>
+  </si>
+  <si>
+    <t>aggregates-section</t>
+  </si>
+  <si>
+    <t>- The file `layer-popup-info.xlsx` should at any time contain rows for all layers in IBF-dashboard that require popup-texts.</t>
+  </si>
+  <si>
+    <t>- SW-DEV is responsible for keeping this up to date</t>
+  </si>
+  <si>
+    <t>- This involves all entries from `indicator-metadata.json` and all 'point' and 'wms' layers from `layer-metadata.json`</t>
+  </si>
+  <si>
+    <t>- Extend the formula-columns downward</t>
+  </si>
+  <si>
+    <t>- this is done in column D</t>
+  </si>
+  <si>
+    <t>- make as much as possible use of existing entries for other countries or layers</t>
+  </si>
+  <si>
+    <t>- DATA-DEV is responsible for this</t>
+  </si>
+  <si>
+    <t>- if it is an existing entry, but column D is still empty, start with copying the existing full text from the dashboard</t>
+  </si>
+  <si>
+    <t>- whenever a change is made, fill in the date of change in column E</t>
+  </si>
+  <si>
+    <t>- if necessary, check UX copy with HCD</t>
+  </si>
+  <si>
+    <t>- make the changes in column D</t>
+  </si>
+  <si>
+    <t>- update the date of change in column E again</t>
+  </si>
+  <si>
+    <t>- DATA-DEV is responsible for making the changes</t>
+  </si>
+  <si>
+    <t>- Copy the text from column D into column F</t>
+  </si>
+  <si>
+    <t>- and make HTML-compatible changes where necessary</t>
+  </si>
+  <si>
+    <t>  - &lt;br&gt; instead of a new line</t>
+  </si>
+  <si>
+    <t>  - &lt;ul&gt;&lt;li&gt;bullet 1&lt;/li&gt;&lt;li&gt;bullet 2&lt;/li&gt;&lt;/ul&gt; for bullet lists</t>
+  </si>
+  <si>
+    <t>  - &lt;a href="http://example.com"&gt;http://example.com&lt;/a&gt; for links</t>
+  </si>
+  <si>
+    <t>  - etc.</t>
+  </si>
+  <si>
+    <t>- use e.g. [https://wordtohtml.net/](https://wordtohtml.net/) for this as help</t>
+  </si>
+  <si>
+    <t>- IMPORTANT: Do not use any double quotes (") in the text, as they may create problems in the conversion later</t>
+  </si>
+  <si>
+    <t>- update the date of change in column G</t>
+  </si>
+  <si>
+    <t>- DATA-DEV create a PR with the changed XLSX-file.</t>
+  </si>
+  <si>
+    <t>- SW-DEV checks out PR locally</t>
+  </si>
+  <si>
+    <t>- check if dashboard runs without errors</t>
+  </si>
+  <si>
+    <t>- open popups for added/edited layers to see if text comes out right (use the 'date of change' column G for this)</t>
+  </si>
+  <si>
+    <t>layers-section</t>
+  </si>
+  <si>
+    <t>1. [SW-DEV] Keeping rows of file up to date</t>
+  </si>
+  <si>
+    <t>2. [DATA-DEV] Adding/editing info popup</t>
+  </si>
+  <si>
+    <t>3. [DATA-DEV] Check UX copy with HCD</t>
+  </si>
+  <si>
+    <t>4. [DATA-DEV] Transform text to HTML-compatible text</t>
+  </si>
+  <si>
+    <t>5. [DATA-DEV] Upload to Github</t>
+  </si>
+  <si>
+    <t>6. [SW-DEV] Process into dashboard and review</t>
+  </si>
+  <si>
+    <t>- runs script to convert XLSX into JSON</t>
+  </si>
+  <si>
+    <t>  - go to right (this) folder: `cd ./src/assets/i18n`</t>
+  </si>
+  <si>
+    <t>  - if first time, install 'xlsx'-package: `npm i xlsx`</t>
+  </si>
+  <si>
+    <t>  - `node _convert-layer-info-popup-xlsx-to-json.js`</t>
   </si>
 </sst>
 </file>
@@ -549,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -590,6 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -907,23 +1017,23 @@
   <dimension ref="A1:Q86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J84" sqref="J84"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.5234375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.47265625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.3671875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26171875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.26171875" style="2" customWidth="1"/>
     <col min="6" max="6" width="88.89453125" style="3" customWidth="1"/>
     <col min="7" max="7" width="11.26171875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26171875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="13.47265625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="21.89453125" style="5" customWidth="1"/>
-    <col min="11" max="17" width="8.83984375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="11.26171875" style="5" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="13.47265625" style="5" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="21.89453125" style="5" hidden="1" customWidth="1"/>
+    <col min="11" max="17" width="8.83984375" style="5" hidden="1" customWidth="1"/>
     <col min="108" max="108" width="93.3125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -962,7 +1072,7 @@
     </row>
     <row r="2" spans="1:17" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>6</v>
@@ -984,7 +1094,7 @@
       </c>
       <c r="I2" s="11" t="str">
         <f>IF(A2=A1,"",""""&amp;A2&amp;""": {")</f>
-        <v>"aggregates": {</v>
+        <v>"aggregates-section": {</v>
       </c>
       <c r="J2" s="11" t="str">
         <f>IF(B2=B1,"",""""&amp;B2&amp;""": {")</f>
@@ -1016,12 +1126,12 @@
       </c>
       <c r="Q2" s="11" t="str">
         <f>H2&amp;I2&amp;J2&amp;K2&amp;L2&amp;M2&amp;N2&amp;O2</f>
-        <v>{"aggregates": {"population_affected": {"UGA": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].",</v>
+        <v>{"aggregates-section": {"population_affected": {"UGA": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].",</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="12" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>6</v>
@@ -1080,7 +1190,7 @@
     </row>
     <row r="4" spans="1:17" ht="201.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="12" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>6</v>
@@ -1139,10 +1249,10 @@
     </row>
     <row r="5" spans="1:17" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>14</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>7</v>
@@ -1150,7 +1260,7 @@
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="15">
         <v>44575</v>
@@ -1198,10 +1308,10 @@
     </row>
     <row r="6" spans="1:17" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>14</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>8</v>
@@ -1209,7 +1319,7 @@
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="15">
         <v>44575</v>
@@ -1257,10 +1367,10 @@
     </row>
     <row r="7" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="12" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>7</v>
@@ -1268,7 +1378,7 @@
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="15">
         <v>44575</v>
@@ -1316,10 +1426,10 @@
     </row>
     <row r="8" spans="1:17" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="12" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>9</v>
@@ -1327,7 +1437,7 @@
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" s="15">
         <v>44575</v>
@@ -1375,10 +1485,10 @@
     </row>
     <row r="9" spans="1:17" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="12" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>7</v>
@@ -1386,7 +1496,7 @@
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="15">
         <v>44575</v>
@@ -1434,10 +1544,10 @@
     </row>
     <row r="10" spans="1:17" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="12" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>7</v>
@@ -1445,7 +1555,7 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="15">
         <v>44575</v>
@@ -1493,10 +1603,10 @@
     </row>
     <row r="11" spans="1:17" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="12" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>7</v>
@@ -1504,7 +1614,7 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G11" s="15">
         <v>44575</v>
@@ -1552,18 +1662,18 @@
     </row>
     <row r="12" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="12" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G12" s="15">
         <v>44575</v>
@@ -1611,18 +1721,18 @@
     </row>
     <row r="13" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="12" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G13" s="15">
         <v>44575</v>
@@ -1670,18 +1780,18 @@
     </row>
     <row r="14" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="12" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14" s="15">
         <v>44575</v>
@@ -1729,18 +1839,18 @@
     </row>
     <row r="15" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="12" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G15" s="15">
         <v>44575</v>
@@ -1788,18 +1898,18 @@
     </row>
     <row r="16" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="12" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
       <c r="F16" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="15">
         <v>44575</v>
@@ -1847,18 +1957,18 @@
     </row>
     <row r="17" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="12" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G17" s="15">
         <v>44575</v>
@@ -1906,10 +2016,10 @@
     </row>
     <row r="18" spans="1:17" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="12" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>9</v>
@@ -1917,7 +2027,7 @@
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" s="15">
         <v>44575</v>
@@ -1944,11 +2054,11 @@
       </c>
       <c r="M18" s="11" t="str">
         <f t="shared" si="6"/>
-        <v>,</v>
+        <v/>
       </c>
       <c r="N18" s="11" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>},</v>
       </c>
       <c r="O18" s="11" t="str">
         <f t="shared" si="8"/>
@@ -1960,15 +2070,15 @@
       </c>
       <c r="Q18" s="11" t="str">
         <f t="shared" si="9"/>
-        <v>"small_ruminants_exposed": {"ZWE": "Number of exposed small ruminants (sheep and goats) is calculated by the small ruminants per province within the droughts alert threshold reached area currently triggered. Livestock numbers small ruminants exists of the number of small ruminants multiplied with the Livestock unit (LSU): 0.1 as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source Links:&lt;ul&gt;&lt;li&gt;Number of small ruminants (sheep and goats) mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021&lt;/li&gt;&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href=\"https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0 \"&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0. &lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"},</v>
+        <v>"small_ruminants_exposed": {"ZWE": "Number of exposed small ruminants (sheep and goats) is calculated by the small ruminants per province within the droughts alert threshold reached area currently triggered. Livestock numbers small ruminants exists of the number of small ruminants multiplied with the Livestock unit (LSU): 0.1 as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source Links:&lt;ul&gt;&lt;li&gt;Number of small ruminants (sheep and goats) mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021&lt;/li&gt;&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href=\"https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0 \"&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0. &lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="12" t="s">
-        <v>13</v>
+        <v>162</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>9</v>
@@ -1976,7 +2086,7 @@
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G19" s="15">
         <v>44575</v>
@@ -1987,7 +2097,7 @@
       </c>
       <c r="I19" s="11" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>"layers-section": {</v>
       </c>
       <c r="J19" s="11" t="str">
         <f t="shared" si="3"/>
@@ -2003,11 +2113,11 @@
       </c>
       <c r="M19" s="11" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>,</v>
       </c>
       <c r="N19" s="11" t="str">
         <f t="shared" si="7"/>
-        <v>},</v>
+        <v/>
       </c>
       <c r="O19" s="11" t="str">
         <f t="shared" si="8"/>
@@ -2019,12 +2129,12 @@
       </c>
       <c r="Q19" s="11" t="str">
         <f t="shared" si="9"/>
-        <v>"cattle_exposed": {"ZWE": "Number of exposed cattle is calculated by the cattle per province within the droughts alert threshold reached area currently triggered. Livestock numbers cattle exists of the number of cattle multiplied with the Livestock unit (LSU): 1.0 as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source Links:&lt;ul&gt;&lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season.Published: 21st of April 2021.&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;.&lt;/li&gt;&lt;/ul&gt;"}},</v>
+        <v>"layers-section": {"cattle_exposed": {"ZWE": "Number of exposed cattle is calculated by the cattle per province within the droughts alert threshold reached area currently triggered. Livestock numbers cattle exists of the number of cattle multiplied with the Livestock unit (LSU): 1.0 as reference unit to aggregate livestock from various species.&lt;br /&gt;&lt;br /&gt;Source Links:&lt;ul&gt;&lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season.Published: 21st of April 2021.&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;.&lt;/li&gt;&lt;/ul&gt;"},</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>6</v>
@@ -2046,7 +2156,7 @@
       </c>
       <c r="I20" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"matrix": {</v>
+        <v/>
       </c>
       <c r="J20" s="11" t="str">
         <f t="shared" si="3"/>
@@ -2078,12 +2188,12 @@
       </c>
       <c r="Q20" s="11" t="str">
         <f t="shared" si="9"/>
-        <v>"matrix": {"population_affected": {"UGA": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].",</v>
+        <v>"population_affected": {"UGA": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href=\"https://www.ciesin.columbia.edu/data/hrsl/\"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].",</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>6</v>
@@ -2094,7 +2204,7 @@
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G21" s="15">
         <v>44575</v>
@@ -2142,7 +2252,7 @@
     </row>
     <row r="22" spans="1:17" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>6</v>
@@ -2201,10 +2311,10 @@
     </row>
     <row r="23" spans="1:17" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>7</v>
@@ -2212,7 +2322,7 @@
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
       <c r="F23" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G23" s="15">
         <v>44575</v>
@@ -2260,10 +2370,10 @@
     </row>
     <row r="24" spans="1:17" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>8</v>
@@ -2271,7 +2381,7 @@
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G24" s="15">
         <v>44575</v>
@@ -2319,10 +2429,10 @@
     </row>
     <row r="25" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>7</v>
@@ -2330,7 +2440,7 @@
       <c r="D25" s="13"/>
       <c r="E25" s="13"/>
       <c r="F25" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G25" s="15">
         <v>44575</v>
@@ -2378,10 +2488,10 @@
     </row>
     <row r="26" spans="1:17" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>9</v>
@@ -2389,7 +2499,7 @@
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G26" s="15">
         <v>44575</v>
@@ -2437,10 +2547,10 @@
     </row>
     <row r="27" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>7</v>
@@ -2448,7 +2558,7 @@
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
       <c r="F27" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G27" s="15">
         <v>44575</v>
@@ -2496,18 +2606,18 @@
     </row>
     <row r="28" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
       <c r="F28" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G28" s="15">
         <v>44575</v>
@@ -2555,18 +2665,18 @@
     </row>
     <row r="29" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
       <c r="F29" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G29" s="15">
         <v>44575</v>
@@ -2614,10 +2724,10 @@
     </row>
     <row r="30" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>7</v>
@@ -2625,7 +2735,7 @@
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
       <c r="F30" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G30" s="15">
         <v>44575</v>
@@ -2673,18 +2783,18 @@
     </row>
     <row r="31" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G31" s="15">
         <v>44575</v>
@@ -2732,10 +2842,10 @@
     </row>
     <row r="32" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>7</v>
@@ -2743,7 +2853,7 @@
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
       <c r="F32" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G32" s="15">
         <v>44575</v>
@@ -2791,18 +2901,18 @@
     </row>
     <row r="33" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
       <c r="F33" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G33" s="15">
         <v>44575</v>
@@ -2850,10 +2960,10 @@
     </row>
     <row r="34" spans="1:17" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>7</v>
@@ -2861,7 +2971,7 @@
       <c r="D34" s="13"/>
       <c r="E34" s="13"/>
       <c r="F34" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G34" s="15">
         <v>44575</v>
@@ -2909,18 +3019,18 @@
     </row>
     <row r="35" spans="1:17" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" s="13"/>
       <c r="E35" s="13"/>
       <c r="F35" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G35" s="15">
         <v>44575</v>
@@ -2968,10 +3078,10 @@
     </row>
     <row r="36" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>7</v>
@@ -2979,7 +3089,7 @@
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
       <c r="F36" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G36" s="15">
         <v>44575</v>
@@ -3027,10 +3137,10 @@
     </row>
     <row r="37" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>9</v>
@@ -3038,7 +3148,7 @@
       <c r="D37" s="13"/>
       <c r="E37" s="13"/>
       <c r="F37" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G37" s="15">
         <v>44575</v>
@@ -3086,18 +3196,18 @@
     </row>
     <row r="38" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
       <c r="F38" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G38" s="15">
         <v>44575</v>
@@ -3145,18 +3255,18 @@
     </row>
     <row r="39" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
       <c r="F39" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G39" s="15">
         <v>44575</v>
@@ -3204,18 +3314,18 @@
     </row>
     <row r="40" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
       <c r="F40" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G40" s="15">
         <v>44575</v>
@@ -3263,10 +3373,10 @@
     </row>
     <row r="41" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>8</v>
@@ -3274,7 +3384,7 @@
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
       <c r="F41" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G41" s="15">
         <v>44575</v>
@@ -3322,10 +3432,10 @@
     </row>
     <row r="42" spans="1:17" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>7</v>
@@ -3333,7 +3443,7 @@
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
       <c r="F42" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G42" s="15">
         <v>44575</v>
@@ -3381,10 +3491,10 @@
     </row>
     <row r="43" spans="1:17" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>7</v>
@@ -3392,7 +3502,7 @@
       <c r="D43" s="13"/>
       <c r="E43" s="13"/>
       <c r="F43" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G43" s="15">
         <v>44575</v>
@@ -3440,10 +3550,10 @@
     </row>
     <row r="44" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>8</v>
@@ -3451,7 +3561,7 @@
       <c r="D44" s="13"/>
       <c r="E44" s="13"/>
       <c r="F44" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G44" s="15">
         <v>44575</v>
@@ -3499,10 +3609,10 @@
     </row>
     <row r="45" spans="1:17" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>7</v>
@@ -3510,7 +3620,7 @@
       <c r="D45" s="13"/>
       <c r="E45" s="13"/>
       <c r="F45" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G45" s="15">
         <v>44575</v>
@@ -3558,10 +3668,10 @@
     </row>
     <row r="46" spans="1:17" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>9</v>
@@ -3569,7 +3679,7 @@
       <c r="D46" s="13"/>
       <c r="E46" s="13"/>
       <c r="F46" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G46" s="15">
         <v>44575</v>
@@ -3617,10 +3727,10 @@
     </row>
     <row r="47" spans="1:17" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>7</v>
@@ -3628,7 +3738,7 @@
       <c r="D47" s="13"/>
       <c r="E47" s="13"/>
       <c r="F47" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G47" s="15">
         <v>44575</v>
@@ -3676,10 +3786,10 @@
     </row>
     <row r="48" spans="1:17" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>7</v>
@@ -3687,7 +3797,7 @@
       <c r="D48" s="13"/>
       <c r="E48" s="13"/>
       <c r="F48" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G48" s="15">
         <v>44575</v>
@@ -3735,10 +3845,10 @@
     </row>
     <row r="49" spans="1:17" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>7</v>
@@ -3746,7 +3856,7 @@
       <c r="D49" s="13"/>
       <c r="E49" s="13"/>
       <c r="F49" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G49" s="15">
         <v>44575</v>
@@ -3794,10 +3904,10 @@
     </row>
     <row r="50" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C50" s="12" t="s">
         <v>7</v>
@@ -3805,7 +3915,7 @@
       <c r="D50" s="13"/>
       <c r="E50" s="13"/>
       <c r="F50" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G50" s="15">
         <v>44575</v>
@@ -3853,10 +3963,10 @@
     </row>
     <row r="51" spans="1:17" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C51" s="12" t="s">
         <v>7</v>
@@ -3864,7 +3974,7 @@
       <c r="D51" s="13"/>
       <c r="E51" s="13"/>
       <c r="F51" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G51" s="15">
         <v>44575</v>
@@ -3912,10 +4022,10 @@
     </row>
     <row r="52" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C52" s="12" t="s">
         <v>9</v>
@@ -3923,7 +4033,7 @@
       <c r="D52" s="13"/>
       <c r="E52" s="13"/>
       <c r="F52" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G52" s="15">
         <v>44575</v>
@@ -3971,10 +4081,10 @@
     </row>
     <row r="53" spans="1:17" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C53" s="12" t="s">
         <v>9</v>
@@ -3982,7 +4092,7 @@
       <c r="D53" s="13"/>
       <c r="E53" s="13"/>
       <c r="F53" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G53" s="15">
         <v>44575</v>
@@ -4030,10 +4140,10 @@
     </row>
     <row r="54" spans="1:17" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>7</v>
@@ -4041,7 +4151,7 @@
       <c r="D54" s="13"/>
       <c r="E54" s="13"/>
       <c r="F54" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G54" s="15">
         <v>44575</v>
@@ -4089,18 +4199,18 @@
     </row>
     <row r="55" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D55" s="13"/>
       <c r="E55" s="13"/>
       <c r="F55" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G55" s="15">
         <v>44575</v>
@@ -4148,10 +4258,10 @@
     </row>
     <row r="56" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C56" s="12" t="s">
         <v>7</v>
@@ -4159,7 +4269,7 @@
       <c r="D56" s="13"/>
       <c r="E56" s="13"/>
       <c r="F56" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G56" s="15">
         <v>44575</v>
@@ -4207,10 +4317,10 @@
     </row>
     <row r="57" spans="1:17" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C57" s="12" t="s">
         <v>8</v>
@@ -4218,7 +4328,7 @@
       <c r="D57" s="13"/>
       <c r="E57" s="13"/>
       <c r="F57" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G57" s="15">
         <v>44575</v>
@@ -4266,18 +4376,18 @@
     </row>
     <row r="58" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D58" s="13"/>
       <c r="E58" s="13"/>
       <c r="F58" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G58" s="15">
         <v>44575</v>
@@ -4325,18 +4435,18 @@
     </row>
     <row r="59" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D59" s="13"/>
       <c r="E59" s="13"/>
       <c r="F59" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G59" s="15">
         <v>44575</v>
@@ -4384,18 +4494,18 @@
     </row>
     <row r="60" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D60" s="13"/>
       <c r="E60" s="13"/>
       <c r="F60" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G60" s="15">
         <v>44575</v>
@@ -4443,18 +4553,18 @@
     </row>
     <row r="61" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
       <c r="F61" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G61" s="15">
         <v>44575</v>
@@ -4502,18 +4612,18 @@
     </row>
     <row r="62" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
       <c r="F62" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G62" s="15">
         <v>44575</v>
@@ -4561,18 +4671,18 @@
     </row>
     <row r="63" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
       <c r="F63" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G63" s="15">
         <v>44575</v>
@@ -4620,18 +4730,18 @@
     </row>
     <row r="64" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
       <c r="F64" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G64" s="15">
         <v>44575</v>
@@ -4679,18 +4789,18 @@
     </row>
     <row r="65" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
       <c r="F65" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G65" s="15">
         <v>44575</v>
@@ -4738,10 +4848,10 @@
     </row>
     <row r="66" spans="1:17" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C66" s="12" t="s">
         <v>9</v>
@@ -4749,7 +4859,7 @@
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
       <c r="F66" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G66" s="15">
         <v>44575</v>
@@ -4797,10 +4907,10 @@
     </row>
     <row r="67" spans="1:17" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C67" s="12" t="s">
         <v>9</v>
@@ -4808,7 +4918,7 @@
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
       <c r="F67" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G67" s="15">
         <v>44575</v>
@@ -4856,10 +4966,10 @@
     </row>
     <row r="68" spans="1:17" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C68" s="12" t="s">
         <v>9</v>
@@ -4867,7 +4977,7 @@
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
       <c r="F68" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G68" s="15">
         <v>44575</v>
@@ -4915,10 +5025,10 @@
     </row>
     <row r="69" spans="1:17" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C69" s="12" t="s">
         <v>9</v>
@@ -4926,7 +5036,7 @@
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
       <c r="F69" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G69" s="15">
         <v>44575</v>
@@ -4974,18 +5084,18 @@
     </row>
     <row r="70" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
       <c r="F70" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G70" s="15">
         <v>44575</v>
@@ -5033,18 +5143,18 @@
     </row>
     <row r="71" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
       <c r="F71" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G71" s="15">
         <v>44575</v>
@@ -5092,18 +5202,18 @@
     </row>
     <row r="72" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
       <c r="F72" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G72" s="15">
         <v>44575</v>
@@ -5151,18 +5261,18 @@
     </row>
     <row r="73" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
       <c r="F73" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G73" s="15">
         <v>44575</v>
@@ -5210,18 +5320,18 @@
     </row>
     <row r="74" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
       <c r="F74" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G74" s="15">
         <v>44575</v>
@@ -5269,18 +5379,18 @@
     </row>
     <row r="75" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
       <c r="F75" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G75" s="15">
         <v>44575</v>
@@ -5328,18 +5438,18 @@
     </row>
     <row r="76" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
       <c r="F76" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G76" s="15">
         <v>44575</v>
@@ -5387,18 +5497,18 @@
     </row>
     <row r="77" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
       <c r="F77" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G77" s="15">
         <v>44575</v>
@@ -5446,18 +5556,18 @@
     </row>
     <row r="78" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
       <c r="F78" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G78" s="15">
         <v>44575</v>
@@ -5505,18 +5615,18 @@
     </row>
     <row r="79" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
       <c r="F79" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G79" s="15">
         <v>44575</v>
@@ -5564,18 +5674,18 @@
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
       <c r="F80" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G80" s="15">
         <v>44575</v>
@@ -5623,18 +5733,18 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
       <c r="F81" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G81" s="15">
         <v>44575</v>
@@ -5682,18 +5792,18 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
       <c r="F82" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G82" s="15">
         <v>44575</v>
@@ -5741,18 +5851,18 @@
     </row>
     <row r="83" spans="1:17" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
       <c r="F83" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G83" s="15">
         <v>44575</v>
@@ -5800,10 +5910,10 @@
     </row>
     <row r="84" spans="1:17" ht="259.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="12" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C84" s="12" t="s">
         <v>9</v>
@@ -5811,7 +5921,7 @@
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
       <c r="F84" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G84" s="15">
         <v>44575</v>
@@ -5858,19 +5968,19 @@
       </c>
     </row>
     <row r="85" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" s="17" t="s">
-        <v>42</v>
+      <c r="A85" s="12" t="s">
+        <v>162</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D85" s="18"/>
       <c r="E85" s="18"/>
       <c r="F85" s="19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G85" s="20">
         <v>44575</v>
@@ -5947,4 +6057,208 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622978F5-E71A-43A0-BACC-EE5631803CBA}">
+  <dimension ref="A1:A48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="102.05078125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="30" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="30" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="30" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="30" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: corrections to layer descriptions AB#15514
</commit_message>
<xml_diff>
--- a/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
+++ b/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\IBF-system\interfaces\IBF-dashboard\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE7241E-6CEB-48EB-8A3D-76155776757A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00A7122-FB0F-45A6-B7F7-FC01B7115DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13770" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
@@ -1034,9 +1034,6 @@
 &lt;a href='https://prism.philrice.gov.ph/dataproducts/'&gt;https://prism.philrice.gov.ph/dataproducts/&lt;/a&gt; This data is based on the Philippine Rice Information System (PRISM) project which primarily aims to establish a nationwide information system on rice that provide information on rice areas and yield at a particular location and time, and information on factors that are affecting the yield. </t>
   </si>
   <si>
-    <t>&lt;a href='https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard'&gt;https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard&lt;/a&gt; This dataset has been generated by combining PSGC and 4Ps data from DSWD</t>
-  </si>
-  <si>
     <t>Ongoing (updated regularly)</t>
   </si>
   <si>
@@ -1056,12 +1053,6 @@
   <si>
     <t>calculated based on the Pantawid Pamilya Beneficiary Households by Municipality.The source for this data is 
 DSWD, NATIONAL HOUSEHOLD TARGETING OFFICE</t>
-  </si>
-  <si>
-    <t>Forecasted maximum windspeed exposure for each municipalities during the duration of the typhoon event. The source for this forecast data is ECMWF</t>
-  </si>
-  <si>
-    <t>Forecasted track of the Typhoon event. The source for this forecast data is ECMWF</t>
   </si>
   <si>
     <t xml:space="preserve">Probability for a Municipality being with in 50km of the forecasted typhoon track. Source for Typhoon forecast is ECMWF </t>
@@ -1129,14 +1120,8 @@
     <t>&lt;p&gt;Total Number of Housing units in each Municipality&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Forecasted track of the Typhoon event. The source for this forecast data is ECMWF&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;calculated based on the Pantawid Pamilya Beneficiary Households by Municipality.The source for this data is 
 DSWD, NATIONAL HOUSEHOLD TARGETING OFFICE&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Forecasted maximum windspeed exposure for each municipalities during the duration of the typhoon event. The source for this forecast data is ECMWF&lt;/p&gt;</t>
   </si>
   <si>
     <t>MWI</t>
@@ -1215,10 +1200,25 @@
   </si>
   <si>
     <t>The predicted impact (72 hours before landfall) is more than 10% of houses being totally damaged at municipal level, in at least 3 municipalities. The source for predicted impact is 510 typhoon impact prediction model.
-Only municipalities that are included in the EAP can be triggered. For other municipalities all data - such as predicted impact - is visible in the map, but they will never be triggered.</t>
+Only municipalities that are included in the EAP can reach a triggered state. For other municipalities all data - such as predicted impact - is visible in the map, but they will never turn in to a triggered state.</t>
   </si>
   <si>
-    <t>&lt;p&gt;The predicted impact (72 hours before landfall) is more than 10% of houses being totally damaged at municipal level, in at least 3 municipalities. The source for predicted impact is 510 typhoon impact prediction model&lt;br&gt;&lt;br&gt;Only municipalities that are included in the EAP can be triggered. For other municipalities all data - such as predicted impact - is visible in the map, but they will never be triggered.&lt;/p&gt;</t>
+    <t>&lt;p&gt;The predicted impact (72 hours before landfall) is more than 10% of houses being totally damaged at municipal level, in at least 3 municipalities. The source for predicted impact is 510 typhoon impact prediction model.&lt;br&gt;&lt;br&gt;Only municipalities that are included in the EAP can reach a triggered state. For other municipalities all data - such as predicted impact - is visible in the map, but they will never turn in to a triggered state.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Forecasted track of the Typhoon event. The source for this forecast data is ECMWF.</t>
+  </si>
+  <si>
+    <t>Forecasted maximum windspeed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Forecasted maximum windspeed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Forecasted track of the Typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard'&gt;https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard&lt;/a&gt; This dataset has been generated by combining PSGC and 4Ps data from DSWD.</t>
   </si>
 </sst>
 </file>
@@ -1742,7 +1742,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
+      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1803,7 +1803,7 @@
         <v>91</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>18</v>
@@ -1937,10 +1937,10 @@
         <v>91</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>203</v>
@@ -1948,7 +1948,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="6" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="H4" s="7">
         <v>44785</v>
@@ -2003,10 +2003,10 @@
         <v>91</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>203</v>
@@ -2014,7 +2014,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="6" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="H5" s="7">
         <v>44785</v>
@@ -2144,11 +2144,11 @@
         <v>207</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="14" t="str">
@@ -2278,7 +2278,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="6" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H9" s="7">
         <v>44737</v>
@@ -2550,7 +2550,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>203</v>
@@ -2558,7 +2558,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="6" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="H13" s="7">
         <v>44785</v>
@@ -2630,7 +2630,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="6" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H14" s="7">
         <v>44663</v>
@@ -3484,7 +3484,7 @@
         <v>11</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>203</v>
@@ -3492,7 +3492,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="6" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="H27" s="7">
         <v>44798</v>
@@ -4349,7 +4349,7 @@
         <v>118</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>18</v>
@@ -4822,17 +4822,17 @@
         <v>89</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>203</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="6" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H47" s="7">
         <v>44798</v>
@@ -4972,7 +4972,7 @@
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="6" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H49" s="7">
         <v>44663</v>
@@ -5036,11 +5036,11 @@
         <v>207</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F50" s="5"/>
       <c r="G50" s="6" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="H50" s="19"/>
       <c r="I50" s="14" t="str">
@@ -5061,7 +5061,7 @@
       </c>
       <c r="M50" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>"typhoon": "&lt;p&gt;The predicted impact (72 hours before landfall) is more than 10% of houses being totally damaged at municipal level, in at least 3 municipalities. The source for predicted impact is 510 typhoon impact prediction model&lt;br&gt;&lt;br&gt;Only municipalities that are included in the EAP can be triggered. For other municipalities all data - such as predicted impact - is visible in the map, but they will never be triggered.&lt;/p&gt;"</v>
+        <v>"typhoon": "&lt;p&gt;The predicted impact (72 hours before landfall) is more than 10% of houses being totally damaged at municipal level, in at least 3 municipalities. The source for predicted impact is 510 typhoon impact prediction model.&lt;br&gt;&lt;br&gt;Only municipalities that are included in the EAP can reach a triggered state. For other municipalities all data - such as predicted impact - is visible in the map, but they will never turn in to a triggered state.&lt;/p&gt;"</v>
       </c>
       <c r="N50" s="26" t="str">
         <f t="shared" si="5"/>
@@ -5085,7 +5085,7 @@
       </c>
       <c r="S50" s="13" t="str">
         <f t="shared" si="10"/>
-        <v>"typhoon": "&lt;p&gt;The predicted impact (72 hours before landfall) is more than 10% of houses being totally damaged at municipal level, in at least 3 municipalities. The source for predicted impact is 510 typhoon impact prediction model&lt;br&gt;&lt;br&gt;Only municipalities that are included in the EAP can be triggered. For other municipalities all data - such as predicted impact - is visible in the map, but they will never be triggered.&lt;/p&gt;"},</v>
+        <v>"typhoon": "&lt;p&gt;The predicted impact (72 hours before landfall) is more than 10% of houses being totally damaged at municipal level, in at least 3 municipalities. The source for predicted impact is 510 typhoon impact prediction model.&lt;br&gt;&lt;br&gt;Only municipalities that are included in the EAP can reach a triggered state. For other municipalities all data - such as predicted impact - is visible in the map, but they will never turn in to a triggered state.&lt;/p&gt;"},</v>
       </c>
     </row>
     <row r="51" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
@@ -6761,10 +6761,10 @@
         <v>118</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>203</v>
@@ -6772,7 +6772,7 @@
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
       <c r="G75" s="6" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="H75" s="7">
         <v>44785</v>
@@ -6827,10 +6827,10 @@
         <v>118</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D76" s="9" t="s">
         <v>203</v>
@@ -6838,7 +6838,7 @@
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
       <c r="G76" s="6" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="H76" s="7">
         <v>44785</v>
@@ -7096,17 +7096,17 @@
         <v>44</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>203</v>
       </c>
       <c r="E80" s="21" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="F80" s="5"/>
       <c r="G80" s="6" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="H80" s="7">
         <v>44785</v>
@@ -7506,7 +7506,7 @@
         <v>59</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D86" s="9" t="s">
         <v>203</v>
@@ -7514,7 +7514,7 @@
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
       <c r="G86" s="6" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="H86" s="7">
         <v>44798</v>
@@ -7772,7 +7772,7 @@
         <v>32</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>203</v>
@@ -7780,7 +7780,7 @@
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
       <c r="G90" s="6" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="H90" s="7">
         <v>44798</v>
@@ -9062,7 +9062,7 @@
         <v>204</v>
       </c>
       <c r="E109" s="21" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F109" s="5"/>
       <c r="G109" s="6"/>
@@ -9128,7 +9128,7 @@
         <v>203</v>
       </c>
       <c r="E110" s="21" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F110" s="5"/>
       <c r="G110" s="6"/>
@@ -9192,7 +9192,7 @@
         <v>206</v>
       </c>
       <c r="E111" s="21" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F111" s="5"/>
       <c r="G111" s="6"/>
@@ -9258,7 +9258,7 @@
         <v>206</v>
       </c>
       <c r="E112" s="21" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F112" s="5"/>
       <c r="G112" s="6" t="s">
@@ -9317,7 +9317,7 @@
         <v>118</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C113" s="9" t="s">
         <v>19</v>
@@ -9326,11 +9326,11 @@
         <v>204</v>
       </c>
       <c r="E113" s="21" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F113" s="5"/>
       <c r="G113" s="6" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H113" s="7">
         <v>44737</v>
@@ -9385,7 +9385,7 @@
         <v>118</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C114" s="9" t="s">
         <v>19</v>
@@ -9456,11 +9456,11 @@
         <v>204</v>
       </c>
       <c r="E115" s="21" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F115" s="5"/>
       <c r="G115" s="6" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H115" s="7">
         <v>44737</v>
@@ -9524,7 +9524,7 @@
         <v>203</v>
       </c>
       <c r="E116" s="21" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F116" s="5"/>
       <c r="G116" s="6" t="s">
@@ -9590,7 +9590,7 @@
         <v>206</v>
       </c>
       <c r="E117" s="21" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F117" s="5"/>
       <c r="G117" s="6" t="s">
@@ -9658,11 +9658,11 @@
         <v>207</v>
       </c>
       <c r="E118" s="21" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F118" s="5"/>
       <c r="G118" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H118" s="19"/>
       <c r="I118" s="14" t="str">
@@ -10586,7 +10586,7 @@
         <v>67</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D132" s="9" t="s">
         <v>203</v>
@@ -10594,7 +10594,7 @@
       <c r="E132" s="5"/>
       <c r="F132" s="5"/>
       <c r="G132" s="6" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="H132" s="7">
         <v>44798</v>
@@ -11064,7 +11064,7 @@
       <c r="E139" s="5"/>
       <c r="F139" s="5"/>
       <c r="G139" s="6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="H139" s="7">
         <v>44737</v>
@@ -11348,7 +11348,7 @@
         <v>6</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D143" s="9" t="s">
         <v>203</v>
@@ -11356,7 +11356,7 @@
       <c r="E143" s="5"/>
       <c r="F143" s="5"/>
       <c r="G143" s="6" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="H143" s="7">
         <v>44798</v>
@@ -11434,7 +11434,7 @@
       <c r="E144" s="5"/>
       <c r="F144" s="5"/>
       <c r="G144" s="6" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H144" s="7">
         <v>44663</v>
@@ -11828,7 +11828,7 @@
       <c r="E150" s="5"/>
       <c r="F150" s="5"/>
       <c r="G150" s="6" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H150" s="7">
         <v>44737</v>
@@ -12030,7 +12030,7 @@
         <v>10</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D153" s="9" t="s">
         <v>203</v>
@@ -12038,7 +12038,7 @@
       <c r="E153" s="5"/>
       <c r="F153" s="5"/>
       <c r="G153" s="6" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="H153" s="7">
         <v>44798</v>
@@ -12114,7 +12114,7 @@
       <c r="E154" s="5"/>
       <c r="F154" s="5"/>
       <c r="G154" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H154" s="7">
         <v>44663</v>
@@ -13166,7 +13166,7 @@
         <v>11</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D170" s="9" t="s">
         <v>203</v>
@@ -13174,7 +13174,7 @@
       <c r="E170" s="5"/>
       <c r="F170" s="5"/>
       <c r="G170" s="6" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="H170" s="7">
         <v>44798</v>
@@ -14038,11 +14038,11 @@
         <v>207</v>
       </c>
       <c r="E183" s="21" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F183" s="5"/>
       <c r="G183" s="6" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H183" s="19"/>
       <c r="I183" s="14" t="str">
@@ -14104,11 +14104,11 @@
         <v>207</v>
       </c>
       <c r="E184" s="21" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F184" s="5"/>
       <c r="G184" s="6" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="H184" s="19"/>
       <c r="I184" s="14" t="str">
@@ -14227,7 +14227,7 @@
         <v>118</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C186" s="9" t="s">
         <v>19</v>
@@ -14238,7 +14238,7 @@
       <c r="E186" s="5"/>
       <c r="F186" s="5"/>
       <c r="G186" s="6" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="H186" s="7">
         <v>44737</v>
@@ -14770,7 +14770,7 @@
         <v>34</v>
       </c>
       <c r="C194" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D194" s="9" t="s">
         <v>203</v>
@@ -15642,11 +15642,11 @@
         <v>207</v>
       </c>
       <c r="E207" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F207" s="5"/>
       <c r="G207" s="6" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="H207" s="19"/>
       <c r="I207" s="14" t="str">
@@ -16034,11 +16034,11 @@
         <v>207</v>
       </c>
       <c r="E213" s="27" t="s">
-        <v>263</v>
+        <v>303</v>
       </c>
       <c r="F213" s="5"/>
       <c r="G213" s="6" t="s">
-        <v>285</v>
+        <v>306</v>
       </c>
       <c r="H213" s="7">
         <v>44575</v>
@@ -16061,7 +16061,7 @@
       </c>
       <c r="M213" s="13" t="str">
         <f t="shared" si="37"/>
-        <v>"typhoon": "&lt;p&gt;Forecasted track of the Typhoon event. The source for this forecast data is ECMWF&lt;/p&gt;"</v>
+        <v>"typhoon": "&lt;p&gt;Forecasted track of the Typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;"</v>
       </c>
       <c r="N213" s="26" t="str">
         <f t="shared" si="38"/>
@@ -16085,7 +16085,7 @@
       </c>
       <c r="S213" s="13" t="str">
         <f t="shared" si="43"/>
-        <v>"typhoon_track": {"PHL": {"typhoon": "&lt;p&gt;Forecasted track of the Typhoon event. The source for this forecast data is ECMWF&lt;/p&gt;"}},</v>
+        <v>"typhoon_track": {"PHL": {"typhoon": "&lt;p&gt;Forecasted track of the Typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;"}},</v>
       </c>
     </row>
     <row r="214" spans="1:19" ht="316.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
@@ -16256,7 +16256,7 @@
       <c r="E216" s="5"/>
       <c r="F216" s="5"/>
       <c r="G216" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H216" s="7">
         <v>44663</v>
@@ -16328,11 +16328,11 @@
         <v>207</v>
       </c>
       <c r="E217" s="21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F217" s="5"/>
       <c r="G217" s="6" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="H217" s="7">
         <v>44575</v>
@@ -16400,7 +16400,7 @@
       <c r="E218" s="5"/>
       <c r="F218" s="5"/>
       <c r="G218" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H218" s="7">
         <v>44663</v>
@@ -16474,7 +16474,7 @@
       <c r="E219" s="5"/>
       <c r="F219" s="5"/>
       <c r="G219" s="6" t="s">
-        <v>257</v>
+        <v>307</v>
       </c>
       <c r="H219" s="7">
         <v>44575</v>
@@ -16497,7 +16497,7 @@
       </c>
       <c r="M219" s="13" t="str">
         <f t="shared" si="37"/>
-        <v>"typhoon": "&lt;a href='https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard'&gt;https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard&lt;/a&gt; This dataset has been generated by combining PSGC and 4Ps data from DSWD"</v>
+        <v>"typhoon": "&lt;a href='https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard'&gt;https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard&lt;/a&gt; This dataset has been generated by combining PSGC and 4Ps data from DSWD."</v>
       </c>
       <c r="N219" s="26" t="str">
         <f t="shared" si="38"/>
@@ -16521,7 +16521,7 @@
       </c>
       <c r="S219" s="13" t="str">
         <f t="shared" si="43"/>
-        <v>"typhoon": "&lt;a href='https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard'&gt;https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard&lt;/a&gt; This dataset has been generated by combining PSGC and 4Ps data from DSWD"}},</v>
+        <v>"typhoon": "&lt;a href='https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard'&gt;https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard&lt;/a&gt; This dataset has been generated by combining PSGC and 4Ps data from DSWD."}},</v>
       </c>
     </row>
     <row r="220" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
@@ -16540,7 +16540,7 @@
       <c r="E220" s="5"/>
       <c r="F220" s="5"/>
       <c r="G220" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H220" s="7">
         <v>44575</v>
@@ -16930,7 +16930,7 @@
         <v>42</v>
       </c>
       <c r="C226" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D226" s="9" t="s">
         <v>203</v>
@@ -17268,11 +17268,11 @@
         <v>207</v>
       </c>
       <c r="E231" s="21" t="s">
-        <v>262</v>
+        <v>304</v>
       </c>
       <c r="F231" s="5"/>
       <c r="G231" s="6" t="s">
-        <v>287</v>
+        <v>305</v>
       </c>
       <c r="H231" s="19"/>
       <c r="I231" s="14" t="str">
@@ -17293,7 +17293,7 @@
       </c>
       <c r="M231" s="13" t="str">
         <f t="shared" si="37"/>
-        <v>"typhoon": "&lt;p&gt;Forecasted maximum windspeed exposure for each municipalities during the duration of the typhoon event. The source for this forecast data is ECMWF&lt;/p&gt;"</v>
+        <v>"typhoon": "&lt;p&gt;Forecasted maximum windspeed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;"</v>
       </c>
       <c r="N231" s="26" t="str">
         <f t="shared" si="38"/>
@@ -17317,7 +17317,7 @@
       </c>
       <c r="S231" s="13" t="str">
         <f t="shared" si="43"/>
-        <v>"windspeed": {"PHL": {"typhoon": "&lt;p&gt;Forecasted maximum windspeed exposure for each municipalities during the duration of the typhoon event. The source for this forecast data is ECMWF&lt;/p&gt;"}}}}</v>
+        <v>"windspeed": {"PHL": {"typhoon": "&lt;p&gt;Forecasted maximum windspeed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;"}}}}</v>
       </c>
     </row>
     <row r="232" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
@@ -29142,7 +29142,7 @@
         <v>}</v>
       </c>
       <c r="S450" s="13" t="str">
-        <f t="shared" ref="S450:S513" si="87">IF(A450="","",I450&amp;J450&amp;K450&amp;L450&amp;M450&amp;N450&amp;O450&amp;P450&amp;Q450&amp;R450)</f>
+        <f t="shared" ref="S450:S474" si="87">IF(A450="","",I450&amp;J450&amp;K450&amp;L450&amp;M450&amp;N450&amp;O450&amp;P450&amp;Q450&amp;R450)</f>
         <v/>
       </c>
     </row>
@@ -30443,7 +30443,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="VWqU3s0gG2M6+xoETIfHT95lJ0b5gJBaJLS9wt8xVo4ImHte5m5yTUePgkRZstS0HP3ie+k7nPHkcVnr/x5J+A==" saltValue="OE/rskeuU1tKgkO4FmfsXg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="rgnrj6LcHuhNFoCcjmT76K/yaeDqKtixUXjRHLWK1XGhqhjn79XocptlDV/kT16thN8Uk/9RI4XP3V/11yl1Kw==" saltValue="7RGBMHQaOE7ORvXi8UkBdA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="I1:S1048576" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>

</xml_diff>

<commit_message>
fix: correct info popups AB#15512
</commit_message>
<xml_diff>
--- a/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
+++ b/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\510\IBF-system\interfaces\IBF-dashboard\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E21AB5-7276-4AA2-953A-02741FF80BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B414E9E0-0210-4329-8FA0-0148C6463E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14100" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
@@ -1232,9 +1232,9 @@
 &lt;br&gt;
 &lt;p&gt;&lt;strong&gt;Legend:&lt;/strong&gt;&lt;/p&gt;
 &lt;ul&gt;
-&lt;li&gt;full color track points show where the typhoon has already passed&lt;/li&gt;
-&lt;li&gt;the larger track point with the typhoon icon shows the latest location of the typhoon&lt;/li&gt;
-&lt;li&gt;transparent track points show the future predicted path of the typhoon&lt;/li&gt;
+&lt;li&gt;the &lt;strong&gt;larger typhoon icon&lt;/strong&gt; track point shows the &lt;strong&gt;latest location&lt;/strong&gt; of the typhoon&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;full color&lt;/strong&gt; track points show where the typhoon has &lt;strong&gt;already passed&lt;/strong&gt;&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;transparent&lt;/strong&gt; track points show the future &lt;strong&gt;predicted path&lt;/strong&gt; of the typhoon&lt;/li&gt;
 &lt;/ul&gt;</t>
   </si>
 </sst>
@@ -16089,9 +16089,9 @@
 &lt;br&gt;
 &lt;p&gt;&lt;strong&gt;Legend:&lt;/strong&gt;&lt;/p&gt;
 &lt;ul&gt;
-&lt;li&gt;full color track points show where the typhoon has already passed&lt;/li&gt;
-&lt;li&gt;the larger track point with the typhoon icon shows the latest location of the typhoon&lt;/li&gt;
-&lt;li&gt;transparent track points show the future predicted path of the typhoon&lt;/li&gt;
+&lt;li&gt;the &lt;strong&gt;larger typhoon icon&lt;/strong&gt; track point shows the &lt;strong&gt;latest location&lt;/strong&gt; of the typhoon&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;full color&lt;/strong&gt; track points show where the typhoon has &lt;strong&gt;already passed&lt;/strong&gt;&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;transparent&lt;/strong&gt; track points show the future &lt;strong&gt;predicted path&lt;/strong&gt; of the typhoon&lt;/li&gt;
 &lt;/ul&gt;"</v>
       </c>
       <c r="N213" s="26" t="str">
@@ -16120,9 +16120,9 @@
 &lt;br&gt;
 &lt;p&gt;&lt;strong&gt;Legend:&lt;/strong&gt;&lt;/p&gt;
 &lt;ul&gt;
-&lt;li&gt;full color track points show where the typhoon has already passed&lt;/li&gt;
-&lt;li&gt;the larger track point with the typhoon icon shows the latest location of the typhoon&lt;/li&gt;
-&lt;li&gt;transparent track points show the future predicted path of the typhoon&lt;/li&gt;
+&lt;li&gt;the &lt;strong&gt;larger typhoon icon&lt;/strong&gt; track point shows the &lt;strong&gt;latest location&lt;/strong&gt; of the typhoon&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;full color&lt;/strong&gt; track points show where the typhoon has &lt;strong&gt;already passed&lt;/strong&gt;&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;transparent&lt;/strong&gt; track points show the future &lt;strong&gt;predicted path&lt;/strong&gt; of the typhoon&lt;/li&gt;
 &lt;/ul&gt;"}},</v>
       </c>
     </row>
@@ -30481,7 +30481,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="uJyv/qsmS5oTxf41bMl51keLcXbrrzJlVVh5ag7iPdyzm7np7ABe50PjFj0/2UtiWQIhTRmbYUwzbbz/+RhK9g==" saltValue="XQ243qIEMYFrnluYGUTrhA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="P7djcxzfvLGilkH1df/PaYCQ44MOA2sgzdJtaOXcGFOusCSLtkT8PftyAmo85Bnvsloc5y9RjWDBdkGb5zp3mg==" saltValue="YCgTMbMMd0bZuT/30m9h/Q==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="I1:S1048576" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>

</xml_diff>

<commit_message>
fix: copu text to aggregates AB#15514
</commit_message>
<xml_diff>
--- a/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
+++ b/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\510\IBF-system\interfaces\IBF-dashboard\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B414E9E0-0210-4329-8FA0-0148C6463E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77250350-A7B8-430F-9706-840DDA24CEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14100" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="310">
   <si>
     <t>section</t>
   </si>
@@ -1757,8 +1757,8 @@
   <dimension ref="A1:S474"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G213" sqref="G213"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1814,7 +1814,7 @@
       <c r="R1" s="13"/>
       <c r="S1" s="13"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>91</v>
       </c>
@@ -1827,9 +1827,15 @@
       <c r="D2" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
+      <c r="E2" s="21" t="s">
+        <v>306</v>
+      </c>
+      <c r="F2" s="23">
+        <v>44838</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>307</v>
+      </c>
       <c r="H2" s="19"/>
       <c r="I2" s="14" t="str">
         <f t="shared" ref="I2:I65" si="0">IF(A1="section","{","")</f>
@@ -1849,7 +1855,7 @@
       </c>
       <c r="M2" s="13" t="str">
         <f t="shared" ref="M2:M65" si="4">""""&amp;D2&amp;""": """&amp;SUBSTITUTE(G2,"""","'")&amp;""""</f>
-        <v>"typhoon": ""</v>
+        <v>"typhoon": "&lt;p&gt;The number of people affected is calculated based on the predicted number of completely damaged houses, which is derived from the typhoon impact predicting model. To derive a methodology to estimate the number of affected people from a predicted number of completely damaged houses, we performed a log fit between the number of completely damaged houses and the number of affected people for past typhoon events using data derived from DROMIC reports. To estimate potential number of affected population this formula is applied to the predicted number of damaged houses. &lt;p&gt; "</v>
       </c>
       <c r="N2" s="26" t="str">
         <f t="shared" ref="N2:N65" si="5">IF(AND(B3=B2,C3=C2),",","}")</f>
@@ -1873,7 +1879,7 @@
       </c>
       <c r="S2" s="13" t="str">
         <f t="shared" ref="S2:S65" si="10">IF(A2="","",I2&amp;J2&amp;K2&amp;L2&amp;M2&amp;N2&amp;O2&amp;P2&amp;Q2&amp;R2)</f>
-        <v>{"aggregates-section": {"affected_population": {"PHL": {"typhoon": ""}},</v>
+        <v>{"aggregates-section": {"affected_population": {"PHL": {"typhoon": "&lt;p&gt;The number of people affected is calculated based on the predicted number of completely damaged houses, which is derived from the typhoon impact predicting model. To derive a methodology to estimate the number of affected people from a predicted number of completely damaged houses, we performed a log fit between the number of completely damaged houses and the number of affected people for past typhoon events using data derived from DROMIC reports. To estimate potential number of affected population this formula is applied to the predicted number of damaged houses. &lt;p&gt; "}},</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="228" x14ac:dyDescent="0.45">
@@ -30481,7 +30487,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="P7djcxzfvLGilkH1df/PaYCQ44MOA2sgzdJtaOXcGFOusCSLtkT8PftyAmo85Bnvsloc5y9RjWDBdkGb5zp3mg==" saltValue="YCgTMbMMd0bZuT/30m9h/Q==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="dAiW8IJjtv14CqV3+wczJnYL6o9r4sG6Z1DyAUSTZYDGjD5KpWo5/dIefGcQl8IOXKAnKavmPfRS1F81Rf9JRg==" saltValue="JMSO4GVJbCV5gShGBthRPQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="I1:S1048576" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>

</xml_diff>

<commit_message>
feat: update wind speed copy AB#15536
</commit_message>
<xml_diff>
--- a/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
+++ b/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\510\IBF-system\interfaces\IBF-dashboard\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77250350-A7B8-430F-9706-840DDA24CEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1D1AE6-B3B2-4F84-B62F-F30E2E7F7ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14100" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17745" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1206,12 +1206,6 @@
     <t>&lt;p&gt;The predicted impact (72 hours before landfall) is more than 10% of houses being totally damaged at municipal level, in at least 3 municipalities. The source for predicted impact is 510 typhoon impact prediction model.&lt;br&gt;&lt;br&gt;Only municipalities that are included in the EAP can reach a triggered state. For other municipalities all data - such as predicted impact - is visible in the map, but they will never turn in to a triggered state.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>Forecasted maximum windspeed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Forecasted maximum windspeed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;a href='https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard'&gt;https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard&lt;/a&gt; This dataset has been generated by combining PSGC and 4Ps data from DSWD.</t>
   </si>
   <si>
@@ -1236,6 +1230,12 @@
 &lt;li&gt;&lt;strong&gt;full color&lt;/strong&gt; track points show where the typhoon has &lt;strong&gt;already passed&lt;/strong&gt;&lt;/li&gt;
 &lt;li&gt;&lt;strong&gt;transparent&lt;/strong&gt; track points show the future &lt;strong&gt;predicted path&lt;/strong&gt; of the typhoon&lt;/li&gt;
 &lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Forecasted maximum wind speed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Forecasted maximum wind speed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -1757,8 +1757,8 @@
   <dimension ref="A1:S474"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pane ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E219" sqref="E219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1828,13 +1828,13 @@
         <v>207</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F2" s="23">
         <v>44838</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="14" t="str">
@@ -4380,13 +4380,13 @@
         <v>207</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F40" s="23">
         <v>44838</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H40" s="19"/>
       <c r="I40" s="14" t="str">
@@ -16062,13 +16062,13 @@
         <v>207</v>
       </c>
       <c r="E213" s="27" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F213" s="23">
         <v>44841</v>
       </c>
       <c r="G213" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H213" s="7">
         <v>44841</v>
@@ -16518,7 +16518,7 @@
       <c r="E219" s="5"/>
       <c r="F219" s="5"/>
       <c r="G219" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H219" s="7">
         <v>44575</v>
@@ -17312,11 +17312,11 @@
         <v>207</v>
       </c>
       <c r="E231" s="21" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="F231" s="5"/>
       <c r="G231" s="6" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="H231" s="19"/>
       <c r="I231" s="14" t="str">
@@ -17337,7 +17337,7 @@
       </c>
       <c r="M231" s="13" t="str">
         <f t="shared" si="37"/>
-        <v>"typhoon": "&lt;p&gt;Forecasted maximum windspeed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;"</v>
+        <v>"typhoon": "&lt;p&gt;Forecasted maximum wind speed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;"</v>
       </c>
       <c r="N231" s="26" t="str">
         <f t="shared" si="38"/>
@@ -17361,7 +17361,7 @@
       </c>
       <c r="S231" s="13" t="str">
         <f t="shared" si="43"/>
-        <v>"windspeed": {"PHL": {"typhoon": "&lt;p&gt;Forecasted maximum windspeed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;"}}}}</v>
+        <v>"windspeed": {"PHL": {"typhoon": "&lt;p&gt;Forecasted maximum wind speed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;"}}}}</v>
       </c>
     </row>
     <row r="232" spans="1:19" x14ac:dyDescent="0.45">
@@ -30487,7 +30487,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="dAiW8IJjtv14CqV3+wczJnYL6o9r4sG6Z1DyAUSTZYDGjD5KpWo5/dIefGcQl8IOXKAnKavmPfRS1F81Rf9JRg==" saltValue="JMSO4GVJbCV5gShGBthRPQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="TlEUqOuudNb1cjjnEImQdh418KDcJMoYrklwtxSqMDQaNC9zxTdJS+MW9G7DKtXI2YiLYJxOrad2Hp/XXWImSw==" saltValue="cvFhEdg66A1FziwKYFsCvQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="I1:S1048576" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>

</xml_diff>

<commit_message>
feat: update info popup AB#15536
</commit_message>
<xml_diff>
--- a/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
+++ b/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\510\IBF-system\interfaces\IBF-dashboard\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1D1AE6-B3B2-4F84-B62F-F30E2E7F7ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E47E094-84C4-4ABD-91DE-4572E10B2DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17745" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
+    <workbookView xWindow="-28920" yWindow="-32520" windowWidth="29040" windowHeight="15990" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2587" uniqueCount="311">
   <si>
     <t>section</t>
   </si>
@@ -1232,10 +1232,13 @@
 &lt;/ul&gt;</t>
   </si>
   <si>
-    <t>Forecasted maximum wind speed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.</t>
+    <t>&lt;p&gt;Forecasted maximum wind speed exposure in kilometer per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Forecasted maximum wind speed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;</t>
+    <t>Forecasted 3-second gust maximum wind speed in kilometers per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Forecasted 3-second gust maximum wind speed in kilometers per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -1757,8 +1760,8 @@
   <dimension ref="A1:S474"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E219" sqref="E219"/>
+      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G231" sqref="G231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17312,11 +17315,11 @@
         <v>207</v>
       </c>
       <c r="E231" s="21" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F231" s="5"/>
       <c r="G231" s="6" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H231" s="19"/>
       <c r="I231" s="14" t="str">
@@ -17337,7 +17340,7 @@
       </c>
       <c r="M231" s="13" t="str">
         <f t="shared" si="37"/>
-        <v>"typhoon": "&lt;p&gt;Forecasted maximum wind speed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;"</v>
+        <v>"typhoon": "&lt;p&gt;Forecasted 3-second gust maximum wind speed in kilometers per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;"</v>
       </c>
       <c r="N231" s="26" t="str">
         <f t="shared" si="38"/>
@@ -17361,7 +17364,7 @@
       </c>
       <c r="S231" s="13" t="str">
         <f t="shared" si="43"/>
-        <v>"windspeed": {"PHL": {"typhoon": "&lt;p&gt;Forecasted maximum wind speed exposure in kilomter per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;"}}}}</v>
+        <v>"windspeed": {"PHL": {"typhoon": "&lt;p&gt;Forecasted 3-second gust maximum wind speed in kilometers per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;"}}}}</v>
       </c>
     </row>
     <row r="232" spans="1:19" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
fix: update track info popup AB#15832
</commit_message>
<xml_diff>
--- a/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
+++ b/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\IBF-system\interfaces\IBF-dashboard\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A74DA3-9C28-4B84-984C-1BA9492C8AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E168FBF-1F1C-49AD-84A9-A47D505B0039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15195" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
+    <workbookView xWindow="13830" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1215,27 +1215,27 @@
     <t xml:space="preserve">&lt;p&gt;The number of people affected is calculated based on the predicted number of completely damaged houses, which is derived from the typhoon impact predicting model. To derive a methodology to estimate the number of affected people from a predicted number of completely damaged houses, we performed a log fit between the number of completely damaged houses and the number of affected people for past typhoon events using data derived from DROMIC reports. To estimate potential number of affected population this formula is applied to the predicted number of damaged houses. &lt;p&gt; </t>
   </si>
   <si>
+    <t>Forecasted 3-second gust maximum wind speed in kilometers per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Forecasted 1 minute average maximum wind speed in kilometers per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>Forecasted track of the Typhoon event. The source for this forecast data is ECMWF.
-Legend:
-- full color track points show where the typhoon has already passed
-- the larger track point with the typhoon icon shows the latest location of the typhoon
-- transparent track points show the future predicted path of the typhoon</t>
+Point tracker legend:
+- Circle with typhoon icon - shows the latest location of the typhoon.
+- Full color circle - Shows where the typhoon has already passed.
+- Transparent dashed circle - Shows the future predicted path of the typhoon.</t>
   </si>
   <si>
     <t>&lt;p&gt;Forecasted track of the Typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;
 &lt;br&gt;
-&lt;p&gt;&lt;strong&gt;Legend:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Trackpoint legend:&lt;/strong&gt;&lt;/p&gt;
 &lt;ul&gt;
-&lt;li&gt;the &lt;strong&gt;larger typhoon icon&lt;/strong&gt; track point shows the &lt;strong&gt;latest location&lt;/strong&gt; of the typhoon&lt;/li&gt;
-&lt;li&gt;&lt;strong&gt;full color&lt;/strong&gt; track points show where the typhoon has &lt;strong&gt;already passed&lt;/strong&gt;&lt;/li&gt;
-&lt;li&gt;&lt;strong&gt;transparent&lt;/strong&gt; track points show the future &lt;strong&gt;predicted path&lt;/strong&gt; of the typhoon&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Circle with typhoon icon&lt;/strong&gt; shows the latest location of the typhoon&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Full color circle&lt;/strong&gt; shows where the typhoon has already passed&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Transparent dashed circle&lt;/strong&gt; shows the future predicted path of the typhoon&lt;/li&gt;
 &lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>Forecasted 3-second gust maximum wind speed in kilometers per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Forecasted 1 minute average maximum wind speed in kilometers per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -1757,8 +1757,8 @@
   <dimension ref="A1:S474"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G231" sqref="G231"/>
+      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F213" sqref="F213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -16048,7 +16048,7 @@
         <v>"malaria": "Predicted travel time (minutes) to nearest city &lt;a href='https://malariaatlas.org/research-project/accessibility-to-healthcare/'&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="213" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="9" t="s">
         <v>118</v>
       </c>
@@ -16062,13 +16062,13 @@
         <v>207</v>
       </c>
       <c r="E213" s="27" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="F213" s="23">
         <v>44841</v>
       </c>
       <c r="G213" s="6" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H213" s="7">
         <v>44841</v>
@@ -16093,11 +16093,11 @@
         <f t="shared" si="37"/>
         <v>"typhoon": "&lt;p&gt;Forecasted track of the Typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;
 &lt;br&gt;
-&lt;p&gt;&lt;strong&gt;Legend:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Trackpoint legend:&lt;/strong&gt;&lt;/p&gt;
 &lt;ul&gt;
-&lt;li&gt;the &lt;strong&gt;larger typhoon icon&lt;/strong&gt; track point shows the &lt;strong&gt;latest location&lt;/strong&gt; of the typhoon&lt;/li&gt;
-&lt;li&gt;&lt;strong&gt;full color&lt;/strong&gt; track points show where the typhoon has &lt;strong&gt;already passed&lt;/strong&gt;&lt;/li&gt;
-&lt;li&gt;&lt;strong&gt;transparent&lt;/strong&gt; track points show the future &lt;strong&gt;predicted path&lt;/strong&gt; of the typhoon&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Circle with typhoon icon&lt;/strong&gt; shows the latest location of the typhoon&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Full color circle&lt;/strong&gt; shows where the typhoon has already passed&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Transparent dashed circle&lt;/strong&gt; shows the future predicted path of the typhoon&lt;/li&gt;
 &lt;/ul&gt;"</v>
       </c>
       <c r="N213" s="26" t="str">
@@ -16124,11 +16124,11 @@
         <f t="shared" si="43"/>
         <v>"typhoon_track": {"PHL": {"typhoon": "&lt;p&gt;Forecasted track of the Typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;
 &lt;br&gt;
-&lt;p&gt;&lt;strong&gt;Legend:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Trackpoint legend:&lt;/strong&gt;&lt;/p&gt;
 &lt;ul&gt;
-&lt;li&gt;the &lt;strong&gt;larger typhoon icon&lt;/strong&gt; track point shows the &lt;strong&gt;latest location&lt;/strong&gt; of the typhoon&lt;/li&gt;
-&lt;li&gt;&lt;strong&gt;full color&lt;/strong&gt; track points show where the typhoon has &lt;strong&gt;already passed&lt;/strong&gt;&lt;/li&gt;
-&lt;li&gt;&lt;strong&gt;transparent&lt;/strong&gt; track points show the future &lt;strong&gt;predicted path&lt;/strong&gt; of the typhoon&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Circle with typhoon icon&lt;/strong&gt; shows the latest location of the typhoon&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Full color circle&lt;/strong&gt; shows where the typhoon has already passed&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Transparent dashed circle&lt;/strong&gt; shows the future predicted path of the typhoon&lt;/li&gt;
 &lt;/ul&gt;"}},</v>
       </c>
     </row>
@@ -17312,11 +17312,11 @@
         <v>207</v>
       </c>
       <c r="E231" s="21" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F231" s="5"/>
       <c r="G231" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H231" s="19"/>
       <c r="I231" s="14" t="str">
@@ -30487,7 +30487,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="yt4kRCuY1xkV42/sZ+yEgl2+uuHzpzCYSY7VDTXx1J87tOeJDJOr0Ygf+PbNJeydbamNLprtz8SX3lNl/drctw==" saltValue="v7mn/wmwn87E8eOuohwa9g==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="IbuVl4rPIN7HlHuYJct35uLN8bMIsNT609mjl91+BzkxXUBe/+MVRGbr+2BS39v1jQiccvKwhXkmCx0n8x1dbQ==" saltValue="JRBRoDublWUHZJIj7FN3VA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="I1:S1048576" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>

</xml_diff>

<commit_message>
fix: change mwi layer u5 to u18 AB#16004
</commit_message>
<xml_diff>
--- a/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
+++ b/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\IBF-system\interfaces\IBF-dashboard\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E168FBF-1F1C-49AD-84A9-A47D505B0039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAA661B-B97F-48A4-850A-33B21AEBFB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13830" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
+    <workbookView xWindow="13770" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="313">
   <si>
     <t>section</t>
   </si>
@@ -1237,6 +1237,15 @@
 &lt;li&gt;&lt;strong&gt;Transparent dashed circle&lt;/strong&gt; shows the future predicted path of the typhoon&lt;/li&gt;
 &lt;/ul&gt;</t>
   </si>
+  <si>
+    <t>exposed_pop_u18</t>
+  </si>
+  <si>
+    <t>Exposed population under 18. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022.</t>
+  </si>
+  <si>
+    <t>Exposed population over 65. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022.</t>
+  </si>
 </sst>
 </file>
 
@@ -1757,8 +1766,8 @@
   <dimension ref="A1:S474"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F213" sqref="F213"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1970,7 +1979,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="6" t="s">
-        <v>288</v>
+        <v>312</v>
       </c>
       <c r="H4" s="7">
         <v>44785</v>
@@ -1993,7 +2002,7 @@
       </c>
       <c r="M4" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>"floods": "TBD. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022."</v>
+        <v>"floods": "Exposed population over 65. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022."</v>
       </c>
       <c r="N4" s="26" t="str">
         <f t="shared" si="5"/>
@@ -2017,7 +2026,7 @@
       </c>
       <c r="S4" s="13" t="str">
         <f t="shared" si="10"/>
-        <v>"exposed_pop_65": {"MWI": {"floods": "TBD. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022."}},</v>
+        <v>"exposed_pop_65": {"MWI": {"floods": "Exposed population over 65. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022."}},</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2025,7 +2034,7 @@
         <v>91</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>284</v>
+        <v>310</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>283</v>
@@ -2036,7 +2045,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="6" t="s">
-        <v>288</v>
+        <v>311</v>
       </c>
       <c r="H5" s="7">
         <v>44785</v>
@@ -2051,7 +2060,7 @@
       </c>
       <c r="K5" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>"exposed_pop_u5": {</v>
+        <v>"exposed_pop_u18": {</v>
       </c>
       <c r="L5" s="25" t="str">
         <f t="shared" si="3"/>
@@ -2059,7 +2068,7 @@
       </c>
       <c r="M5" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>"floods": "TBD. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022."</v>
+        <v>"floods": "Exposed population under 18. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022."</v>
       </c>
       <c r="N5" s="26" t="str">
         <f t="shared" si="5"/>
@@ -2083,7 +2092,7 @@
       </c>
       <c r="S5" s="13" t="str">
         <f t="shared" si="10"/>
-        <v>"exposed_pop_u5": {"MWI": {"floods": "TBD. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022."}},</v>
+        <v>"exposed_pop_u18": {"MWI": {"floods": "Exposed population under 18. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022."}},</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="216" x14ac:dyDescent="0.55000000000000004">
@@ -30487,7 +30496,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="IbuVl4rPIN7HlHuYJct35uLN8bMIsNT609mjl91+BzkxXUBe/+MVRGbr+2BS39v1jQiccvKwhXkmCx0n8x1dbQ==" saltValue="JRBRoDublWUHZJIj7FN3VA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="8ZrSTymoAMzn69GGwg+9tYPJH0LR5IMgaOrbNcjw+gpN6Ir6Zn23MEkdlgTafP9txM602gNsr13Mxb9QHdtBGw==" saltValue="0GReQGp3h+HeboN1ph1gyQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="I1:S1048576" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>

</xml_diff>

<commit_message>
fix: adjust trigger statement + alert threshold popup AB#16003
</commit_message>
<xml_diff>
--- a/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
+++ b/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\IBF-system\interfaces\IBF-dashboard\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAA661B-B97F-48A4-850A-33B21AEBFB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AF4E9A-7473-4A00-9BD5-4077D28B90EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13770" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
@@ -1157,13 +1157,6 @@
 Latest updated: August 2022</t>
   </si>
   <si>
-    <t>&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 7-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 7 days. The GLOFAS flood forecast triggers except in the wards where the False Alarm Ratio (FAR) &amp;gt; [value].&lt;/p&gt;
-&lt;p&gt;&lt;br&gt;&lt;/p&gt;
-&lt;p&gt;Source link: &lt;a href="https://www.globalfloods.eu/"&gt;https://www.globalfloods.eu/&lt;/a&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;&lt;br&gt;&lt;/p&gt;
-&lt;p&gt;Latest updated: August 2022&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Number of people exposed is calculated by the population living in the flood extent area within the administrative areas currently triggered. The number of people and the flood extent are derived from the below sources.&lt;/p&gt;
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt;&lt;/p&gt;
 &lt;ul&gt;
@@ -1245,6 +1238,13 @@
   </si>
   <si>
     <t>Exposed population over 65. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 7-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 7 days. The GLOFAS flood forecast triggers except in the Traditional Authorities where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is [value].&lt;/p&gt;
+&lt;p&gt;&lt;br&gt;&lt;/p&gt;
+&lt;p&gt;Source link: &lt;a href="https://www.globalfloods.eu/"&gt;https://www.globalfloods.eu/&lt;/a&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;&lt;br&gt;&lt;/p&gt;
+&lt;p&gt;Latest updated: August 2022&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -1766,8 +1766,8 @@
   <dimension ref="A1:S474"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1828,7 +1828,7 @@
         <v>91</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>18</v>
@@ -1837,13 +1837,13 @@
         <v>207</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F2" s="23">
         <v>44838</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="14" t="str">
@@ -1979,7 +1979,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H4" s="7">
         <v>44785</v>
@@ -2034,7 +2034,7 @@
         <v>91</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>283</v>
@@ -2045,7 +2045,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H5" s="7">
         <v>44785</v>
@@ -2589,7 +2589,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H13" s="7">
         <v>44785</v>
@@ -4380,7 +4380,7 @@
         <v>118</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>18</v>
@@ -4389,13 +4389,13 @@
         <v>207</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F40" s="23">
         <v>44838</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H40" s="19"/>
       <c r="I40" s="14" t="str">
@@ -4869,7 +4869,7 @@
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="6" t="s">
-        <v>293</v>
+        <v>312</v>
       </c>
       <c r="H47" s="7">
         <v>44798</v>
@@ -4892,7 +4892,7 @@
       </c>
       <c r="M47" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>"floods": "&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 7-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 7 days. The GLOFAS flood forecast triggers except in the wards where the False Alarm Ratio (FAR) &amp;gt; [value].&lt;/p&gt;
+        <v>"floods": "&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 7-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 7 days. The GLOFAS flood forecast triggers except in the Traditional Authorities where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is [value].&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
 &lt;p&gt;Source link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;&amp;nbsp;&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
@@ -4920,7 +4920,7 @@
       </c>
       <c r="S47" s="13" t="str">
         <f t="shared" si="10"/>
-        <v>"MWI": {"floods": "&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 7-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 7 days. The GLOFAS flood forecast triggers except in the wards where the False Alarm Ratio (FAR) &amp;gt; [value].&lt;/p&gt;
+        <v>"MWI": {"floods": "&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 7-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 7 days. The GLOFAS flood forecast triggers except in the Traditional Authorities where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is [value].&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
 &lt;p&gt;Source link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;&amp;nbsp;&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
@@ -5073,11 +5073,11 @@
         <v>207</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F50" s="5"/>
       <c r="G50" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H50" s="19"/>
       <c r="I50" s="14" t="str">
@@ -7551,7 +7551,7 @@
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
       <c r="G86" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H86" s="7">
         <v>44798</v>
@@ -11393,7 +11393,7 @@
       <c r="E143" s="5"/>
       <c r="F143" s="5"/>
       <c r="G143" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H143" s="7">
         <v>44798</v>
@@ -12075,7 +12075,7 @@
       <c r="E153" s="5"/>
       <c r="F153" s="5"/>
       <c r="G153" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H153" s="7">
         <v>44798</v>
@@ -14264,7 +14264,7 @@
         <v>118</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C186" s="9" t="s">
         <v>19</v>
@@ -14275,7 +14275,7 @@
       <c r="E186" s="5"/>
       <c r="F186" s="5"/>
       <c r="G186" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H186" s="7">
         <v>44737</v>
@@ -16071,13 +16071,13 @@
         <v>207</v>
       </c>
       <c r="E213" s="27" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F213" s="23">
         <v>44841</v>
       </c>
       <c r="G213" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H213" s="7">
         <v>44841</v>
@@ -16527,7 +16527,7 @@
       <c r="E219" s="5"/>
       <c r="F219" s="5"/>
       <c r="G219" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H219" s="7">
         <v>44575</v>
@@ -17321,11 +17321,11 @@
         <v>207</v>
       </c>
       <c r="E231" s="21" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F231" s="5"/>
       <c r="G231" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H231" s="19"/>
       <c r="I231" s="14" t="str">
@@ -30496,7 +30496,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8ZrSTymoAMzn69GGwg+9tYPJH0LR5IMgaOrbNcjw+gpN6Ir6Zn23MEkdlgTafP9txM602gNsr13Mxb9QHdtBGw==" saltValue="0GReQGp3h+HeboN1ph1gyQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="QaIoN5CQiY8j9jVDiBu0ghj66Fr/wSuefPd43LzH4ih6po52K8m6UJJTFscZ7+ZshOVuzZhPNSvZpfJh2E5EWA==" saltValue="mSKTYDcp8DaPifl/73fNJQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="I1:S1048576" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>

</xml_diff>

<commit_message>
fix: info popups MWI AB#16003
</commit_message>
<xml_diff>
--- a/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
+++ b/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\IBF-system\interfaces\IBF-dashboard\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AF4E9A-7473-4A00-9BD5-4077D28B90EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA602020-E767-4897-9599-5FA989901B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13770" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
+    <workbookView xWindow="15195" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="315">
   <si>
     <t>section</t>
   </si>
@@ -1234,17 +1234,25 @@
     <t>exposed_pop_u18</t>
   </si>
   <si>
-    <t>Exposed population under 18. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022.</t>
-  </si>
-  <si>
-    <t>Exposed population over 65. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022.</t>
-  </si>
-  <si>
     <t>&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 7-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 7 days. The GLOFAS flood forecast triggers except in the Traditional Authorities where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is [value].&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
 &lt;p&gt;Source link: &lt;a href="https://www.globalfloods.eu/"&gt;https://www.globalfloods.eu/&lt;/a&gt;&amp;nbsp;&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
 &lt;p&gt;Latest updated: August 2022&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Number of Exposed Population 65+ is calculated by total target population living in the flood extent area within the administrative areas currently triggered. The target population are those living in the households classified as Poor, Poorer, Poorest and whose household head is older than 65 years old.
+Source target population: Unified Beneficiary Registration (UBR). Department of Economy Planning and Development, Malawi. Collected and processed in 2022.</t>
+  </si>
+  <si>
+    <t>Number of Exposed Population U18 is calculated by total target population living in the flood extent area within the administrative areas currently triggered. The target population are those living in the households classified as Poor, Poorer, Poorest and whose household head is below 18 years old.
+Source target population: Unified Beneficiary Registration (UBR). Department of Economy Planning and Development, Malawi. Collected and processed in 2022.</t>
+  </si>
+  <si>
+    <t>Number of Exposed Population 65+ is calculated by total target population living in the flood extent area within the administrative areas currently triggered. The target population are those living in the households classified as Poor, Poorer, Poorest and whose household head is older than 65 years old.&lt;br&gt;&lt;br&gt;Source target population: Unified Beneficiary Registration (UBR). Department of Economy Planning and Development, Malawi. Collected and processed in 2022.</t>
+  </si>
+  <si>
+    <t>Number of Exposed Population U18 is calculated by total target population living in the flood extent area within the administrative areas currently triggered. The target population are those living in the households classified as Poor, Poorer, Poorest and whose household head is below 18 years old.&lt;br&gt;&lt;br&gt;Source target population: Unified Beneficiary Registration (UBR). Department of Economy Planning and Development, Malawi. Collected and processed in 2022.</t>
   </si>
 </sst>
 </file>
@@ -1766,8 +1774,8 @@
   <dimension ref="A1:S474"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1963,7 +1971,7 @@
 &lt;ul&gt;    &lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021.&lt;/li&gt;    &lt;li&gt;Source assessment:&lt;br&gt;&lt;a data-fr-linked='true' href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;&lt;/li&gt;    &lt;li&gt;Source Livestock unit (LSU) &lt;a href='https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)'&gt;&amp;nbsp;https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="9" t="s">
         <v>91</v>
       </c>
@@ -1976,10 +1984,12 @@
       <c r="D4" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="21" t="s">
+        <v>311</v>
+      </c>
       <c r="F4" s="5"/>
       <c r="G4" s="6" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="H4" s="7">
         <v>44785</v>
@@ -2002,7 +2012,7 @@
       </c>
       <c r="M4" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>"floods": "Exposed population over 65. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022."</v>
+        <v>"floods": "Number of Exposed Population 65+ is calculated by total target population living in the flood extent area within the administrative areas currently triggered. The target population are those living in the households classified as Poor, Poorer, Poorest and whose household head is older than 65 years old.&lt;br&gt;&lt;br&gt;Source target population: Unified Beneficiary Registration (UBR). Department of Economy Planning and Development, Malawi. Collected and processed in 2022."</v>
       </c>
       <c r="N4" s="26" t="str">
         <f t="shared" si="5"/>
@@ -2026,10 +2036,10 @@
       </c>
       <c r="S4" s="13" t="str">
         <f t="shared" si="10"/>
-        <v>"exposed_pop_65": {"MWI": {"floods": "Exposed population over 65. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022."}},</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>"exposed_pop_65": {"MWI": {"floods": "Number of Exposed Population 65+ is calculated by total target population living in the flood extent area within the administrative areas currently triggered. The target population are those living in the households classified as Poor, Poorer, Poorest and whose household head is older than 65 years old.&lt;br&gt;&lt;br&gt;Source target population: Unified Beneficiary Registration (UBR). Department of Economy Planning and Development, Malawi. Collected and processed in 2022."}},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="9" t="s">
         <v>91</v>
       </c>
@@ -2042,10 +2052,12 @@
       <c r="D5" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="21" t="s">
+        <v>312</v>
+      </c>
       <c r="F5" s="5"/>
       <c r="G5" s="6" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="H5" s="7">
         <v>44785</v>
@@ -2068,7 +2080,7 @@
       </c>
       <c r="M5" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>"floods": "Exposed population under 18. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022."</v>
+        <v>"floods": "Number of Exposed Population U18 is calculated by total target population living in the flood extent area within the administrative areas currently triggered. The target population are those living in the households classified as Poor, Poorer, Poorest and whose household head is below 18 years old.&lt;br&gt;&lt;br&gt;Source target population: Unified Beneficiary Registration (UBR). Department of Economy Planning and Development, Malawi. Collected and processed in 2022."</v>
       </c>
       <c r="N5" s="26" t="str">
         <f t="shared" si="5"/>
@@ -2092,7 +2104,7 @@
       </c>
       <c r="S5" s="13" t="str">
         <f t="shared" si="10"/>
-        <v>"exposed_pop_u18": {"MWI": {"floods": "Exposed population under 18. This layer is based on Unified Beneficiary Registration (UBR) data provided by Department of Economy Planning and Development of Malawi. Data collected and processed in 2022."}},</v>
+        <v>"exposed_pop_u18": {"MWI": {"floods": "Number of Exposed Population U18 is calculated by total target population living in the flood extent area within the administrative areas currently triggered. The target population are those living in the households classified as Poor, Poorer, Poorest and whose household head is below 18 years old.&lt;br&gt;&lt;br&gt;Source target population: Unified Beneficiary Registration (UBR). Department of Economy Planning and Development, Malawi. Collected and processed in 2022."}},</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="216" x14ac:dyDescent="0.55000000000000004">
@@ -4869,7 +4881,7 @@
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="H47" s="7">
         <v>44798</v>
@@ -30496,7 +30508,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="QaIoN5CQiY8j9jVDiBu0ghj66Fr/wSuefPd43LzH4ih6po52K8m6UJJTFscZ7+ZshOVuzZhPNSvZpfJh2E5EWA==" saltValue="mSKTYDcp8DaPifl/73fNJQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Rr1klvWwGHyA/xKmRa0RDFBmzyu0ZAhyI8J7CBDMoegI+xOh29M/5Ch2M2Lk+43ctWhS4BtjwGstcoHOBOZ87Q==" saltValue="IC5fsweyHFnaZiNXSpQhLQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="I1:S1048576" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>

</xml_diff>

<commit_message>
fix: change leadtime to 6-day AB#16463
</commit_message>
<xml_diff>
--- a/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
+++ b/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\IBF-system\interfaces\IBF-dashboard\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6695253-6044-46A6-84FA-741F37E24B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B65F7AD-CBD0-4179-88CD-4F91F4B6A685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13770" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
@@ -1119,14 +1119,6 @@
     <t>&lt;p&gt;The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 10-years) based on a global hydrological model.&lt;br&gt;&lt;br&gt;Source link: Flood hazard map of the World - 10-year return period. European Commission, Joint Research Centre (JRC). 2016. &lt;a href="https://data.jrc.ec.europa.eu/dataset/jrc-floods-floodmapgl_rp10y-tif"&gt;Flood hazard map of the World - 10-year return period - European Commission (europa.eu)&lt;/a&gt;.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 7 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The [percentage]% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>The layer shows each administrative area triggered based on two parameters from the 7-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 7 days. The GLOFAS flood forecast triggers except in the wards where the False Alarm Ratio (FAR) &gt; [value].
-Source link: https://www.globalfloods.eu/
-Latest updated: August 2022</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Number of people exposed is calculated by the population living in the flood extent area within the administrative areas currently triggered. The number of people and the flood extent are derived from the below sources.&lt;/p&gt;
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt;&lt;/p&gt;
 &lt;ul&gt;
@@ -1185,13 +1177,6 @@
   </si>
   <si>
     <t>exposed_pop_u18</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 7-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 7 days. The GLOFAS flood forecast triggers except in the Traditional Authorities where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is [value].&lt;/p&gt;
-&lt;p&gt;&lt;br&gt;&lt;/p&gt;
-&lt;p&gt;Source link: &lt;a href="https://www.globalfloods.eu/"&gt;https://www.globalfloods.eu/&lt;/a&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;&lt;br&gt;&lt;/p&gt;
-&lt;p&gt;Latest updated: August 2022&lt;/p&gt;</t>
   </si>
   <si>
     <t>Number of Exposed Population 65+ is calculated by total target population living in the flood extent area within the administrative areas currently triggered. The target population are those living in the households classified as Poor, Poorer, Poorest and whose household head is older than 65 years old.
@@ -1253,6 +1238,21 @@
   </si>
   <si>
     <t>dams</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 6-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 6 days. The GLOFAS flood forecast triggers except in the Traditional Authorities where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is [value].&lt;/p&gt;
+&lt;p&gt;&lt;br&gt;&lt;/p&gt;
+&lt;p&gt;Source link: &lt;a href="https://www.globalfloods.eu/"&gt;https://www.globalfloods.eu/&lt;/a&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;&lt;br&gt;&lt;/p&gt;
+&lt;p&gt;Latest updated: August 2022&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>The layer shows each administrative area triggered based on two parameters from the 6-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 6 days. The GLOFAS flood forecast triggers except in the wards where the False Alarm Ratio (FAR) &gt; [value].
+Source link: https://www.globalfloods.eu/
+Latest updated: August 2022</t>
+  </si>
+  <si>
+    <t>This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 6 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The [percentage]% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -1769,11 +1769,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D31E7F-BFF5-4ADE-901A-4F6BC662C23D}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:S474"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E71" sqref="E71"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G137" sqref="A1:S474"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1829,12 +1830,12 @@
       <c r="R1" s="13"/>
       <c r="S1" s="13"/>
     </row>
-    <row r="2" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:19" ht="129.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="9" t="s">
         <v>90</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>18</v>
@@ -1843,13 +1844,13 @@
         <v>206</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F2" s="23">
         <v>44838</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="14" t="str">
@@ -1897,7 +1898,7 @@
         <v>{"aggregates-section": {"affected_population": {"PHL": {"typhoon": "&lt;p&gt;The number of people affected is calculated based on the predicted number of completely damaged houses, which is derived from the typhoon impact predicting model. To derive a methodology to estimate the number of affected people from a predicted number of completely damaged houses, we performed a log fit between the number of completely damaged houses and the number of affected people for past typhoon events using data derived from DROMIC reports. To estimate potential number of affected population this formula is applied to the predicted number of damaged houses. &lt;p&gt; "}},</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
         <v>90</v>
       </c>
@@ -1983,11 +1984,11 @@
         <v>202</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="6" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H4" s="7">
         <v>44785</v>
@@ -2042,7 +2043,7 @@
         <v>90</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>275</v>
@@ -2051,11 +2052,11 @@
         <v>202</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="6" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H5" s="7">
         <v>44785</v>
@@ -2105,7 +2106,7 @@
         <v>"exposed_pop_u18": {"MWI": {"floods": "Number of Exposed Population U18 is calculated by total target population living in the flood extent area within the administrative areas currently triggered. The target population are those living in the households classified as Poor, Poorer, Poorest and whose household head is below 18 years old.&lt;br&gt;&lt;br&gt;Source target population: Unified Beneficiary Registration (UBR). Department of Economy Planning and Development, Malawi. Collected and processed in 2022."}},</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="216" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:19" ht="216" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="9" t="s">
         <v>90</v>
       </c>
@@ -2171,7 +2172,7 @@
         <v>"female_head_hh": {"UGA": {"floods": "Estimated exposed number of people living in female-headed households living in the flood extent area within the areas currently triggered. This number is calculated by multiplying the overall percentage of households with adult females as decision-maker and main income producer in an area, by the total exposed population in that area.&lt;br /&gt;&lt;br /&gt;Note that the estimate number is not the number of households, but the number of people living in a housholds. In this calculation a household size of 4.7 is used as average estimate.&lt;br /&gt;&lt;br /&gt;. The number of people in female headed households in the flood extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source data:&lt;ul&gt;&lt;li&gt;Female Headed Households: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014.&lt;/li&gt;&lt;li&gt;Total Population: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Flood extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt;&lt;/ul&gt;:"}},</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="9" t="s">
         <v>90</v>
       </c>
@@ -2237,7 +2238,7 @@
         <v>"houses_affected": {"PHL": {"typhoon": "&lt;p&gt;Total Number of completely  damaged houses as predicted by 510 typhoon impact prediction model&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:19" ht="129.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="9" t="s">
         <v>90</v>
       </c>
@@ -2303,7 +2304,7 @@
         <v>"population_affected": {"EGY": {"heavy-rain": "Number of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br/&gt;Explanation Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."},</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="9" t="s">
         <v>90</v>
       </c>
@@ -2369,7 +2370,7 @@
         <v>"ETH": {"drought": "Number of people exposed is calculated by the population living within the districts currently triggered. The number of people per district are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="9" t="s">
         <v>90</v>
       </c>
@@ -2433,7 +2434,7 @@
         <v>"floods": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="9" t="s">
         <v>90</v>
       </c>
@@ -2513,7 +2514,7 @@
 &lt;/ul&gt;",</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="9" t="s">
         <v>90</v>
       </c>
@@ -2599,7 +2600,7 @@
       <c r="E13" s="21"/>
       <c r="F13" s="5"/>
       <c r="G13" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H13" s="7">
         <v>44785</v>
@@ -2655,7 +2656,7 @@
  &lt;li&gt;Source Flood Extent: Flood hazard map of the World - 10-year return period. European Commission, Joint Research Centre (JRC). 2016. &lt;a href='https://data.jrc.ec.europa.eu/dataset/jrc-floods-floodmapgl_rp10y-tif'&gt;Flood hazard map of the World - 10-year return period - European Commission (europa.eu)&lt;/a&gt;.&lt;/li&gt; &lt;/ul&gt; &lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="216" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:19" ht="216" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="9" t="s">
         <v>90</v>
       </c>
@@ -2723,7 +2724,7 @@
 &lt;p&gt;Source Links:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Source (Population Data): High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Source Flood Extent: The flood extent maps are generated by the National Operational Assesment of Hazards(NOAH) project.&lt;a href='https://noah.up.edu.ph/'&gt;https://noah.up.edu.ph/&lt;/a&gt; The 25-year rain return flood hazard maps show low, medium, and high flood hazards represented as yellow, orange, and red respectively. Flood hazards consider take both the height and velocity of the water into consideration and calculates the hazard levels based on the danger they pose to people and structures. Generally, for an average Filipino with a height of 5’ 6”, areas with flood depths from the knee down can be considered to have low hazard levels. Those with flood depths ranging from the knee to neck are considered to have medium hazard levels, and those covered with floods that are higher than the neck have high hazard levels. However, since the flow velocity is also considered, areas that have shallow but fast-flowing flood waters may have a higher hazard level than that denoted by the height of the flood covering it.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:19" ht="129.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="9" t="s">
         <v>90</v>
       </c>
@@ -2731,7 +2732,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>202</v>
@@ -2787,7 +2788,7 @@
         <v>"SSD": {"floods": "&lt;p&gt;Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;/p&gt;&lt;p&gt;Source Links:&lt;/p&gt;&lt;ul&gt;    &lt;li&gt;Source (Population Data): High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;     &lt;li&gt;Source Flood Extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt; &lt;/ul&gt; &lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="9" t="s">
         <v>90</v>
       </c>
@@ -2803,7 +2804,7 @@
       <c r="E16" s="21"/>
       <c r="F16" s="5"/>
       <c r="G16" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="str">
@@ -2851,7 +2852,7 @@
         <v>"UGA": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="9" t="s">
         <v>90</v>
       </c>
@@ -2917,7 +2918,7 @@
         <v>"floods": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="9" t="s">
         <v>90</v>
       </c>
@@ -2981,7 +2982,7 @@
         <v>"ZMB": {"floods": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:19" ht="302.39999999999998" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="9" t="s">
         <v>90</v>
       </c>
@@ -3051,7 +3052,7 @@
         <v>"ZWE": {"drought": "&lt;p&gt;Number of people exposed is calculated by the population living in the droughts alert threshold reached area within the district currently triggered. The number of people and the drought extent is derived from the below sources.&lt;/p&gt; &lt;p&gt;Source links:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Population Data: Worldpop &lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Drought alert threshold reached: ENSO: Seasonal ERSSTv5 (1991-2020 base period) 3-month running average in Ni&amp;ntilde;o 3.4 (5oNorth-5oSouth) (170-120oWest)). &lt;a href='https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt'&gt;https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt&lt;/a&gt; and CHIRPS: Rainfall Estimates from Rain Gauge and Satellite Observations | Climate Hazards Center - UC Santa Barbara (&lt;a href='https://www.chc.ucsb.edu/data/chirps'&gt;https://www.chc.ucsb.edu/data/chirps&lt;/a&gt;)&amp;nbsp;&lt;/li&gt;&lt;li&gt;Crop Yield data: Izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA, &lt;a href='https://doi.org/10.1594/PANGAEA.909132'&gt;https://doi.org/10.1594/PANGAEA.909132&lt;/a&gt;,Supplement to Iizumi, Toshichika; Sakai, T (2020): The global dataset of historical yields for major crops 1981&amp;ndash;2016. Scientific Data, 7(1), &lt;a href='https://doi.org/10.1038/s41597-020-0433-7'&gt;https://doi.org/10.1038/s41597-020-0433-7&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:19" ht="187.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="9" t="s">
         <v>90</v>
       </c>
@@ -3117,7 +3118,7 @@
         <v>"population_over65": {"UGA": {"floods": "Estimate exposed number of people over 65 years of age living in the flood extent area within the areas currently triggered. This number is calculated by multiplying the overall percentage of households with people over 65 years of age, by the total exposed population in that area. The number of people over 65 years of age in the flood extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source data:&lt;ul&gt;&lt;li&gt;Population over 65: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014.&lt;/li&gt;&lt;li&gt;Total Population: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Flood extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt;&lt;/ul&gt;:"}},</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:19" ht="187.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="9" t="s">
         <v>90</v>
       </c>
@@ -3183,7 +3184,7 @@
         <v>"population_u8": {"UGA": {"floods": "Estimate exposed number of people under 8 years of age living in the flood extent area within the areas currently triggered. This number is calculated by multiplying the overall percentage of households with people under 8 years of age, by the total exposed population in that area. The number of people under 8 years of age in the flood extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source data:&lt;ul&gt;&lt;li&gt;Population under 8: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014.&lt;/li&gt;&lt;li&gt;Total Population: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Flood extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt;&lt;/ul&gt;:"}},</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="9" t="s">
         <v>90</v>
       </c>
@@ -3247,7 +3248,7 @@
         <v>"populationTotal": {"EGY": {"heavy-rain": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="9" t="s">
         <v>90</v>
       </c>
@@ -3313,7 +3314,7 @@
         <v>"ETH": {"drought": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="9" t="s">
         <v>90</v>
       </c>
@@ -3377,7 +3378,7 @@
         <v>"floods": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="9" t="s">
         <v>90</v>
       </c>
@@ -3441,7 +3442,7 @@
         <v>"malaria": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="9" t="s">
         <v>90</v>
       </c>
@@ -3511,7 +3512,7 @@
         <v>"KEN": {"drought": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="9" t="s">
         <v>90</v>
       </c>
@@ -3651,7 +3652,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; peanutButter: An R package to produce rapid-response gridded population estimates from building footprints, version 1.0.0 version 1.0.0. Accessed 15-08-2022. WorldPop, University of Southampton. 2021. &amp;nbsp;&lt;a href='https://apps.worldpop.org/peanutButter/'&gt;https://apps.worldpop.org/peanutButter/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="9" t="s">
         <v>90</v>
       </c>
@@ -3719,7 +3720,7 @@
 &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="9" t="s">
         <v>90</v>
       </c>
@@ -3727,7 +3728,7 @@
         <v>11</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>202</v>
@@ -3785,7 +3786,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="9" t="s">
         <v>90</v>
       </c>
@@ -3851,7 +3852,7 @@
         <v>"UGA": {"drought": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="9" t="s">
         <v>90</v>
       </c>
@@ -3917,7 +3918,7 @@
         <v>"floods": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="9" t="s">
         <v>90</v>
       </c>
@@ -3981,7 +3982,7 @@
         <v>"ZMB": {"floods": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="9" t="s">
         <v>90</v>
       </c>
@@ -4051,7 +4052,7 @@
         <v>"ZWE": {"drought": "Population data is aggregated per administrative area, from the following original source: Worldpop data:&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;Estimates of total number of people per grid square broken down by gender and age groupings.&lt;/li&gt;&lt;li&gt;Accessed 07-2020 The mapping approach is Pezzulo, C. et al. Sub-national mapping of population pyramids and dependency ratios in Africa and Asia. Sci. Data 4:170089 doi:10.1038/sdata.2017.89 (2017)&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="9" t="s">
         <v>90</v>
       </c>
@@ -4117,7 +4118,7 @@
         <v>"potential_cases": {"ETH": {"malaria": "Potential number of cases are calculated with the assumtion of a rough proportionality between malaria mosquito enviromental suitability and malaria risk. Then estimating a time lag between optimal malaria mosquito environmental conditions and the peak in number of malaria cases."},</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="9" t="s">
         <v>90</v>
       </c>
@@ -4183,7 +4184,7 @@
         <v>"PHL": {"dengue": "Number of potential dengue cases, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="9" t="s">
         <v>90</v>
       </c>
@@ -4249,7 +4250,7 @@
         <v>"potential_cases_65": {"ETH": {"malaria": "Elderly: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="9" t="s">
         <v>90</v>
       </c>
@@ -4315,7 +4316,7 @@
         <v>"PHL": {"dengue": "Number of potential dengue cases among people above 65 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="9" t="s">
         <v>90</v>
       </c>
@@ -4381,7 +4382,7 @@
         <v>"potential_cases_U5": {"ETH": {"malaria": "Potential cases under 5. Vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="9" t="s">
         <v>90</v>
       </c>
@@ -4447,7 +4448,7 @@
         <v>"potential_cases_U9": {"PHL": {"dengue": "Number of potential dengue cases among children under 9 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="9" t="s">
         <v>90</v>
       </c>
@@ -4517,12 +4518,12 @@
         <v>"small_ruminants_exposed": {"ZWE": {"drought": "Number of exposed small ruminants (sheep and goats) is calculated by the small ruminants per province within the droughts alert threshold reached area currently triggered. Livestock numbers small ruminants exists of the number of small ruminants multiplied with the Livestock unit (LSU):0.1 to aggregate livestock from various species  (as reference unit 1.0, which is the grazing equivalent of one adult dairy cow producing 3000 kg of milk annually, without additional concentrated foodstuffs). &lt;br /&gt;&lt;br /&gt;Source Links:&lt;ul&gt;&lt;li&gt;Number of small ruminants (sheep and goats) mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021&lt;/li&gt;&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0 '&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0. &lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"}}},</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:19" ht="129.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="9" t="s">
         <v>117</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>18</v>
@@ -4531,13 +4532,13 @@
         <v>206</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F42" s="23">
         <v>44838</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H42" s="19"/>
       <c r="I42" s="14" t="str">
@@ -4585,7 +4586,7 @@
         <v>"layers-section": {"affected_population": {"PHL": {"typhoon": "&lt;p&gt;The number of people affected is calculated based on the predicted number of completely damaged houses, which is derived from the typhoon impact predicting model. To derive a methodology to estimate the number of affected people from a predicted number of completely damaged houses, we performed a log fit between the number of completely damaged houses and the number of affected people for past typhoon events using data derived from DROMIC reports. To estimate potential number of affected population this formula is applied to the predicted number of damaged houses. &lt;p&gt; "}},</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="9" t="s">
         <v>117</v>
       </c>
@@ -4601,7 +4602,7 @@
       <c r="E43" s="21"/>
       <c r="F43" s="5"/>
       <c r="G43" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H43" s="19"/>
       <c r="I43" s="14" t="str">
@@ -4649,7 +4650,7 @@
         <v>"alert_threshold": {"EGY": {"heavy-rain": "Not currently available"},</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="9" t="s">
         <v>117</v>
       </c>
@@ -4665,7 +4666,7 @@
       <c r="E44" s="21"/>
       <c r="F44" s="5"/>
       <c r="G44" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H44" s="7">
         <v>44737</v>
@@ -4715,7 +4716,7 @@
         <v>"ETH": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="9" t="s">
         <v>117</v>
       </c>
@@ -4731,7 +4732,7 @@
       <c r="E45" s="21"/>
       <c r="F45" s="5"/>
       <c r="G45" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H45" s="19"/>
       <c r="I45" s="14" t="str">
@@ -4779,7 +4780,7 @@
         <v>"floods": "Not currently available",</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="9" t="s">
         <v>117</v>
       </c>
@@ -4845,7 +4846,7 @@
         <v>"malaria": "An alert is released when two conditions are simultaneously the relative number of malaria cases is anomalous accordance to WHO guidelines, by comparing it to its monthly averages, the second condition is that the absolute number of malaria cases is high and thus likely to require humanitarian intervention."},</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:19" ht="201.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="9" t="s">
         <v>117</v>
       </c>
@@ -4921,7 +4922,7 @@
 &lt;p&gt;For further information please refer to the EAP&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="9" t="s">
         <v>117</v>
       </c>
@@ -5011,11 +5012,11 @@
         <v>202</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>282</v>
+        <v>310</v>
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="6" t="s">
-        <v>298</v>
+        <v>309</v>
       </c>
       <c r="H49" s="7">
         <v>44798</v>
@@ -5038,7 +5039,7 @@
       </c>
       <c r="M49" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>"floods": "&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 7-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 7 days. The GLOFAS flood forecast triggers except in the Traditional Authorities where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is [value].&lt;/p&gt;
+        <v>"floods": "&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 6-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 6 days. The GLOFAS flood forecast triggers except in the Traditional Authorities where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is [value].&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
 &lt;p&gt;Source link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;&amp;nbsp;&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
@@ -5066,14 +5067,14 @@
       </c>
       <c r="S49" s="13" t="str">
         <f t="shared" si="10"/>
-        <v>"MWI": {"floods": "&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 7-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 7 days. The GLOFAS flood forecast triggers except in the Traditional Authorities where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is [value].&lt;/p&gt;
+        <v>"MWI": {"floods": "&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 6-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 6 days. The GLOFAS flood forecast triggers except in the Traditional Authorities where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is [value].&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
 &lt;p&gt;Source link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;&amp;nbsp;&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
 &lt;p&gt;Latest updated: August 2022&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:19" ht="129.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="9" t="s">
         <v>117</v>
       </c>
@@ -5139,7 +5140,7 @@
         <v>"PHL": {"dengue": "Administrative divisions that reached alert threshold, in terms of number of potential cases. &lt;br /&gt;&lt;br /&gt; See definition at: &lt;a href='https://rodekruis.sharepoint.com/sites/510-CRAVK-510/Gedeelde%20%20documenten/Forms/AllItems.aspx?id=%2Fsites%2F510%2DCRAVK%2D510%2FGedeelde%20%20documenten%2F%5BRD%5D%20Epidemics%20Priority%20Index%2FIBF%2Ddengue%2Fdocuments%2FIBF%5Fdengue%5Ftechnical%5Fnote%2Epdf&amp;parent=%2Fsites%2F510%2DCRAVK%2D510%2FGedeelde%20%20documenten%2F%5BRD%5D%20Epidemics%20Priority%20Index%2FIBF%2Ddengue%2Fdocuments&amp;p=true&amp;originalPath=aHR0cHM6Ly9yb2Rla3J1aXMuc2hhcmVwb2ludC5jb20vc2l0ZXMvNTEwLUNSQVZLLTUxMC9fbGF5b3V0cy8xNS9ndWVzdGFjY2Vzcy5hc3B4P2RvY2lkPTBmOTI0OWIzNWRhNGQ0YzBhOTg1YjMzMzkzZmMzODhkZiZhdXRoa2V5PUFRU0xubmFmR0YtTTJ0MUNHSWcwaGRBJmV4cGlyYXRpb249MjAyMi0wNi0xNFQyMiUzYTAwJTNhMDAuMDAwWiZydGltZT1TS016R0dzeDJVZw'&gt; link to technical documentation&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="9" t="s">
         <v>117</v>
       </c>
@@ -5205,7 +5206,7 @@
         <v>"floods": "&lt;p&gt;The layer shows each county triggered based on two parameters from the 3-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least 50% probability of occurrence of a 5 year return period flood within the next 7 days. The GLOFAS flood forecast triggers except in the  manucipalities where the False Alarm Ratio (RAR) &amp;gt;0.5&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Source link&lt;/strong&gt;: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Latest updated:&amp;nbsp;&lt;/strong&gt;September 2021&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="9" t="s">
         <v>117</v>
       </c>
@@ -5219,11 +5220,11 @@
         <v>206</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H52" s="19"/>
       <c r="I52" s="14" t="str">
@@ -5271,7 +5272,7 @@
         <v>"typhoon": "&lt;p&gt;The predicted impact (72 hours before landfall) is more than 10% of houses being totally damaged at municipal level, in at least 3 municipalities. The source for predicted impact is 510 typhoon impact prediction model.&lt;br&gt;&lt;br&gt;Only municipalities that are included in the EAP can reach a triggered state. For other municipalities all data - such as predicted impact - is visible in the map, but they will never turn in to a triggered state.&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="9" t="s">
         <v>117</v>
       </c>
@@ -5279,7 +5280,7 @@
         <v>88</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>202</v>
@@ -5287,7 +5288,7 @@
       <c r="E53" s="21"/>
       <c r="F53" s="5"/>
       <c r="G53" s="6" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="H53" s="19"/>
       <c r="I53" s="14" t="str">
@@ -5339,7 +5340,7 @@
 &lt;p&gt;&lt;strong&gt;Latest updated:&amp;nbsp;&lt;/strong&gt;September 2021&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="9" t="s">
         <v>117</v>
       </c>
@@ -5355,7 +5356,7 @@
       <c r="E54" s="21"/>
       <c r="F54" s="5"/>
       <c r="G54" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H54" s="19"/>
       <c r="I54" s="14" t="str">
@@ -5403,7 +5404,7 @@
         <v>"UGA": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="9" t="s">
         <v>117</v>
       </c>
@@ -5419,7 +5420,7 @@
       <c r="E55" s="21"/>
       <c r="F55" s="5"/>
       <c r="G55" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H55" s="19"/>
       <c r="I55" s="14" t="str">
@@ -5467,7 +5468,7 @@
         <v>"floods": "Not currently available"},</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="9" t="s">
         <v>117</v>
       </c>
@@ -5483,7 +5484,7 @@
       <c r="E56" s="21"/>
       <c r="F56" s="5"/>
       <c r="G56" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H56" s="19"/>
       <c r="I56" s="14" t="str">
@@ -5531,7 +5532,7 @@
         <v>"ZMB": {"floods": "Not currently available"},</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:19" ht="409.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="9" t="s">
         <v>117</v>
       </c>
@@ -5601,7 +5602,7 @@
         <v>"ZWE": {"drought": "&lt;p&gt;The layer shows each province in the country with a drought risk at the end of the growing season (April), and as such determine which provinces are triggered when at least one of their districts is expected to face a +/- 6 year return period drought.&lt;/p&gt; &lt;p&gt;The drought model is to assess a drought prediction skill of the 3-month running average Ni&amp;ntilde;o 3.4 values and initiates a drought risk when there is a potential negative crop yield anomaly predicted. The model is developed based on the XGBoost algorithm tested and trained with historical ENSO: Seasonal ERSSTv5 and CHIRPS Rainfall data in relation to historical negative crop yield anomalies in April, which is used as drought impact proxy. Loss of crops, livestock loss, and child malnutrition and stunting are indicated by the ZRCS DRM working group and representatives from IFRC, PNS, and Red Cross Climate Centre (RCCC) &amp;nbsp;as targeted drought impact&lt;/p&gt;&lt;p&gt;Source links:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;ENSO: Seasonal ERSSTv5 (1991-2020 base period) 3-month running average in Ni&amp;ntilde;o 3.4 (5oNorth-5oSouth) (170-120oWest)) &lt;a href='https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt'&gt;https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt&lt;/a&gt;&lt;/li&gt;&lt;li&gt;CHIRPS: Rainfall Estimates from Rain Gauge and Satellite Observations | Climate Hazards Center - UC Santa Barbara (&lt;a href='https://www.chc.ucsb.edu/data/chirps'&gt;https://www.chc.ucsb.edu/data/chirps&lt;/a&gt;)&amp;nbsp;&lt;/li&gt;     &lt;li&gt;Crop Yield data: Izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA, &lt;a href='https://doi.org/10.1594/PANGAEA.909132'&gt;https://doi.org/10.1594/PANGAEA.909132&lt;/a&gt;,Supplement to Iizumi, Toshichika; Sakai, T (2020): The global dataset of historical yields for major crops 1981&amp;ndash;2016. Scientific Data, 7(1), &lt;a href='https://doi.org/10.1038/s41597-020-0433-7'&gt;https://doi.org/10.1038/s41597-020-0433-7&lt;/a&gt;&lt;/li&gt; &lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="9" t="s">
         <v>117</v>
       </c>
@@ -5617,7 +5618,7 @@
       <c r="E58" s="21"/>
       <c r="F58" s="5"/>
       <c r="G58" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H58" s="19"/>
       <c r="I58" s="14" t="str">
@@ -5665,7 +5666,7 @@
         <v>"cattle": {"UGA": {"drought": "Not currently available"},</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:19" ht="201.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="9" t="s">
         <v>117</v>
       </c>
@@ -5735,7 +5736,7 @@
         <v>"ZWE": {"drought": "&lt;p&gt;Livestock numbers cattle exists of the number of cattle multiplied with the Livestock unit (LSU): 1.0 &amp;nbsp;as reference unit to aggregate livestock from various species, which is the grazing equivalent of one adult dairy cow producing 3000 kg of milk annually, without additional concentrated foodstuffs.&lt;/p&gt; &lt;p&gt;Source Links :&lt;/p&gt; &lt;ul&gt;     &lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021.&lt;/li&gt;     &lt;li&gt;Source assessment:&lt;br&gt;&lt;a data-fr-linked='true' href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;&lt;/li&gt;     &lt;li&gt;Source Livestock unit (LSU) &lt;a href='https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)'&gt;&amp;nbsp;https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)&lt;/a&gt;&lt;/li&gt; &lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="9" t="s">
         <v>117</v>
       </c>
@@ -5751,7 +5752,7 @@
       <c r="E60" s="21"/>
       <c r="F60" s="5"/>
       <c r="G60" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H60" s="19"/>
       <c r="I60" s="14" t="str">
@@ -5799,7 +5800,7 @@
         <v>"cattle_exposed": {"UGA": {"drought": "Not currently available"},</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="9" t="s">
         <v>117</v>
       </c>
@@ -5869,7 +5870,7 @@
         <v>"ZWE": {"drought": "&lt;p&gt;Number of exposed cattle is calculated by the cattle per province within the droughts alert threshold reached area currently triggered. Livestock numbers cattle exists of the number of cattle multiplied with the Livestock unit (LSU): 1.0 as reference unit, which is the grazing equivalent of one adult dairy cow producing 3000 kg of milk annually, without additional concentrated foodstuffs.&amp;nbsp;&lt;/p&gt;&lt;p&gt;Source Links :&lt;/p&gt; &lt;ul&gt;     &lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021.&lt;/li&gt;     &lt;li&gt;Source assessment:&lt;br&gt;&lt;a data-fr-linked='true' href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;&lt;/li&gt;     &lt;li&gt;Source Livestock unit (LSU) &lt;a href='https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)'&gt;&amp;nbsp;https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)&lt;/a&gt;&lt;/li&gt; &lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:19" ht="144" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="9" t="s">
         <v>117</v>
       </c>
@@ -5933,7 +5934,7 @@
         <v>"covid_risk": {"UGA": {"floods": "The COVID-19 Risk Index is a composite index for the context of exposure, vulnerability to COVID and the capacity to anticipate, cope with and recover from the impacts of COVID-19 (a higher percentage indicates a higher risk to COVID-19). The National Society  selected the following criteria below:&lt;br /&gt;&lt;br /&gt;Exposure&lt;ul&gt;&lt;li&gt;population / km2&lt;/li&gt;&lt;/ul&gt;Vulnerability&lt;ul&gt;&lt;li&gt;% population 65+&lt;/li&gt;&lt;li&gt;% poverty incidence&lt;/li&gt;&lt;/ul&gt;Lack of Coping Capacity&lt;ul&gt;&lt;li&gt;% with no toilet facility&lt;/li&gt;&lt;li&gt;% access to safe drinking water&lt;/li&gt;&lt;li&gt;% illiterate&lt;/li&gt;&lt;li&gt;% with mobile access&lt;/li&gt;&lt;li&gt;% with internet access&lt;/li&gt;&lt;li&gt;% received remittances&lt;/li&gt;&lt;li&gt;HIV: incidence per 100&lt;/li&gt;&lt;li&gt;MALARIA: Plasmodium Falciparum incidence per 1000&lt;/li&gt;&lt;li&gt;% households which consume less than two meals per day&lt;/li&gt;&lt;li&gt;# healh facilities per person&lt;/li&gt;&lt;li&gt;% with a health facility within 5 km&lt;/li&gt;&lt;/ul&gt;&lt;br/&gt;Source link: &lt;a href='https://nlrc.maps.arcgis.com/apps/opsdashboard/index.html#/9ca9f0f452b04046b8594a74c31f0c3b'&gt;https://nlrc.maps.arcgis.com/apps/opsdashboard/index.html#/9ca9f0f452b04046b8594a74c31f0c3b&lt;/a&gt;."}},</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="9" t="s">
         <v>117</v>
       </c>
@@ -5999,7 +6000,7 @@
         <v>"cropland": {"ETH": {"drought": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010",</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="9" t="s">
         <v>117</v>
       </c>
@@ -6063,7 +6064,7 @@
         <v>"floods": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="9" t="s">
         <v>117</v>
       </c>
@@ -6151,7 +6152,7 @@
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="9" t="s">
         <v>117</v>
       </c>
@@ -6239,7 +6240,7 @@
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="9" t="s">
         <v>117</v>
       </c>
@@ -6255,7 +6256,7 @@
       <c r="E67" s="21"/>
       <c r="F67" s="5"/>
       <c r="G67" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H67" s="19"/>
       <c r="I67" s="14" t="str">
@@ -6303,7 +6304,7 @@
         <v>"UGA": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="9" t="s">
         <v>117</v>
       </c>
@@ -6369,7 +6370,7 @@
         <v>"floods": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="9" t="s">
         <v>117</v>
       </c>
@@ -6433,7 +6434,7 @@
         <v>"ZMB": {"floods": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:19" ht="187.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="9" t="s">
         <v>117</v>
       </c>
@@ -6503,12 +6504,12 @@
         <v>"ZWE": {"drought": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link Zimbabwe: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"}},</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="9" t="s">
         <v>117</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C71" s="9" t="s">
         <v>9</v>
@@ -6573,7 +6574,7 @@
         <v>"dams": {"ZWE": {"drought": "This layer represents a selection of dams, and their associated reservoirs in Zimbabwe. The selection is made, based on the  Zimbabwe National Water Authority (ZINWA).&lt;br /&gt;&lt;br /&gt;Source Link Zimbabwe:&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.zinwa.co.zw/dam-levels/'&gt;https://www.zinwa.co.zw/dam-levels/&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="9" t="s">
         <v>117</v>
       </c>
@@ -6639,7 +6640,7 @@
         <v>"dengue_cases_average": {"PHL": {"dengue": "Number of dengue cases per administrative division per year. &lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://doh.gov.ph/statistics'&gt;https://doh.gov.ph/statistics/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="9" t="s">
         <v>117</v>
       </c>
@@ -6705,7 +6706,7 @@
         <v>"dengue_incidence_average": {"PHL": {"dengue": "Number of dengue cases per 10.000.000 people per administrative division per year. &lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://doh.gov.ph/statistics'&gt;https://doh.gov.ph/statistics/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="388.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:19" ht="388.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="9" t="s">
         <v>117</v>
       </c>
@@ -6795,7 +6796,7 @@
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:19" ht="187.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="9" t="s">
         <v>117</v>
       </c>
@@ -6883,7 +6884,7 @@
 &lt;br&gt;For further information please refer to the EAP"},</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="9" t="s">
         <v>117</v>
       </c>
@@ -6899,7 +6900,7 @@
       <c r="E76" s="21"/>
       <c r="F76" s="5"/>
       <c r="G76" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H76" s="19"/>
       <c r="I76" s="14" t="str">
@@ -6947,7 +6948,7 @@
         <v>"UGA": {"drought": "Not currently available"},</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:19" ht="244.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="9" t="s">
         <v>117</v>
       </c>
@@ -7017,15 +7018,15 @@
         <v>"ZWE": {"drought": "The drought vulnerability index is a composite index for the context of exposure to drought and the capacity to anticipate, cope with and recover from the impacts of droughts. The ZRCS selected nine main criteria:&lt;ul&gt;&lt;li&gt;14% Labor constrained households: 7 %unemployment rate 15+  and 7% economically non-active&lt;/li&gt;&lt;li&gt;15% Child, women and elderly headed households: 5% Female headed HH , 5% Head of Household (19-), 5% Head of Household (65+)&lt;/li&gt;&lt;li&gt;14% People with disabilities&lt;/li&gt;&lt;li&gt;15 % Pregnant and breast-feeding women, and children under five years: 5% pregnant women, 5% breast-feeding women, 5% children under five years&lt;/li&gt;&lt;li&gt;14 % Severe acute malnutrition&lt;/li&gt;&lt;li&gt;7% employment agriculture&lt;/li&gt;&lt;li&gt;7% cattle per km2&lt;/li&gt;&lt;li&gt;7% HIV prevalence&lt;/li&gt;&lt;li&gt;7% HIV ART Coverage&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="9" t="s">
         <v>117</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>202</v>
@@ -7033,7 +7034,7 @@
       <c r="E78" s="21"/>
       <c r="F78" s="5"/>
       <c r="G78" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H78" s="19"/>
       <c r="I78" s="14" t="str">
@@ -7095,11 +7096,11 @@
         <v>202</v>
       </c>
       <c r="E79" s="21" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F79" s="5"/>
       <c r="G79" s="6" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H79" s="7">
         <v>44785</v>
@@ -7154,7 +7155,7 @@
         <v>117</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C80" s="9" t="s">
         <v>275</v>
@@ -7163,11 +7164,11 @@
         <v>202</v>
       </c>
       <c r="E80" s="21" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F80" s="5"/>
       <c r="G80" s="6" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H80" s="19"/>
       <c r="I80" s="14" t="str">
@@ -7215,7 +7216,7 @@
         <v>"exposed_pop_u18": {"MWI": {"floods": "Number of Exposed Population U18 is calculated by total target population living in the flood extent area within the administrative areas currently triggered. The target population are those living in the households classified as Poor, Poorer, Poorest and whose household head is below 18 years old.&lt;br&gt;&lt;br&gt;Source target population: Unified Beneficiary Registration (UBR). Department of Economy Planning and Development, Malawi. Collected and processed in 2022."}},</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="9" t="s">
         <v>117</v>
       </c>
@@ -7281,7 +7282,7 @@
         <v>"female_head_hh": {"UGA": {"floods": "Percentage of people living in female headed households.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."}},</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="57.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:19" ht="57.7" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="9" t="s">
         <v>117</v>
       </c>
@@ -7345,7 +7346,7 @@
         <v>"flood_extent": {"ETH": {"floods": "The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="73.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:19" ht="73.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="9" t="s">
         <v>117</v>
       </c>
@@ -7483,7 +7484,7 @@
         <v>"MWI": {"floods": "&lt;p&gt;The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 10-years) based on a global hydrological model.&lt;br&gt;&lt;br&gt;Source link: Flood hazard map of the World - 10-year return period. European Commission, Joint Research Centre (JRC). 2016. &lt;a href='https://data.jrc.ec.europa.eu/dataset/jrc-floods-floodmapgl_rp10y-tif'&gt;Flood hazard map of the World - 10-year return period - European Commission (europa.eu)&lt;/a&gt;.&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="9" t="s">
         <v>117</v>
       </c>
@@ -7559,7 +7560,7 @@
 covering it. "},</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="9" t="s">
         <v>117</v>
       </c>
@@ -7567,7 +7568,7 @@
         <v>44</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D86" s="9" t="s">
         <v>202</v>
@@ -7623,7 +7624,7 @@
         <v>"SSD": {"floods": "The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="9" t="s">
         <v>117</v>
       </c>
@@ -7689,7 +7690,7 @@
         <v>"UGA": {"floods": "The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="9" t="s">
         <v>117</v>
       </c>
@@ -7753,7 +7754,7 @@
         <v>"ZMB": {"floods": "The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."}},</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:19" ht="201.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="9" t="s">
         <v>117</v>
       </c>
@@ -7819,7 +7820,7 @@
         <v>"flood_susceptibility": {"EGY": {"heavy-rain": "Flood susceptibility identifies the most vulnerable areas based on physical characteristics that determine the propensity for flooding” (Vojtek and Vojtekova, 2019). The mapping of flood susceptible areas involves the analysis of multiple criteria for different characteristics of the region that collectively contribute to the likelihood of floods.&lt;br/&gt;&lt;br/&gt;Nine influencing parameters based on a variety of satellite imagery and spatial datasets are the input factors of the model, such as topographical (Elevation model, Slope), physical (Land cover, Hydrological soil group) and hydrological properties (Height Above Nearest Drainage, Distance from Nearest Drainage, Topographic Wetness Index Slope, Rain intensity, Rain duration). Set of weights based on expert knowledge (The Analytical Hierarchical Process) from REACH (2019) was adapted in this analysis.&lt;br/&gt;&lt;br/&gt;&lt;strong&gt;LEGEND:&lt;/strong&gt; There are 4 classes of flood susceptibility. The higher the flood susceptibility, the darker blue the color.&lt;br/&gt;&lt;br/&gt;SOURCES:&lt;ul&gt;&lt;li&gt;REACH. Yemen Flood Susceptibility. 2019. &lt;a href='https://reliefweb.int/sites/reliefweb.int/files/resources/REACH_YEM_MethodologyNote_HVA_FloodSusceptibility_01APR2020_EN_V2.pdf'&gt;https://reliefweb.int/sites/reliefweb.int/files/resources/REACH_YEM_MethodologyNote_HVA_FloodSusceptibility_01APR2020_EN_V2.pdf&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Vojtek, M.; Vojteková, J. Flood Susceptibility Mapping on a National Scale in Slovakia Using the Analytical Hierarchy Process. Water 2019, 11, 364. &lt;a href='https://doi.org/10.3390/w11020364'&gt;https://doi.org/10.3390/w11020364&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="216" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:19" ht="216" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="9" t="s">
         <v>117</v>
       </c>
@@ -7905,7 +7906,7 @@
       <c r="E91" s="21"/>
       <c r="F91" s="5"/>
       <c r="G91" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H91" s="7">
         <v>44798</v>
@@ -7955,7 +7956,7 @@
         <v>"MWI": {"floods": "The flood vulnerability index is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts of floods. The vulnerability index is selected with the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Flood physical exposure. &lt;/li&gt;&lt;li&gt; 20% Poverty: Poverty incidence &lt;/li&gt;&lt;li&gt;20% Gender: Female headed household &lt;/li&gt;&lt;li&gt;20% Age: Population below 5 years &lt;/li&gt;&lt;li&gt;20 % Disability: People with disability&lt;/li&gt;&lt;/ul&gt;."},</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="9" t="s">
         <v>117</v>
       </c>
@@ -7971,7 +7972,7 @@
       <c r="E92" s="21"/>
       <c r="F92" s="5"/>
       <c r="G92" s="6" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H92" s="7">
         <v>44575</v>
@@ -8021,7 +8022,7 @@
         <v>"UGA": {"floods": "The disaster vulnerability index is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts of floods. The National Society and Technical Working group selected the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Poverty: Poverty incidence&lt;/li&gt;&lt;li&gt;20% Gender: Female headed household&lt;/li&gt;&lt;li&gt;10% Age: Population below 8-years&lt;/li&gt;&lt;li&gt;10% Age: population 65+,&lt;/li&gt;&lt;li&gt;10 % type of construction: permanent wall type&lt;/li&gt;&lt;li&gt;10 %type of construction: permanent roof type&lt;/li&gt;&lt;li&gt;20% Refugees legal status #of displaced person&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;For further information please refer to the EAP. For source links, see each individual layer."}},</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="9" t="s">
         <v>117</v>
       </c>
@@ -8085,7 +8086,7 @@
         <v>"glofas_stations": {"ETH": {"floods": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 5 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60/70/80% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="288" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:19" ht="288" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="9" t="s">
         <v>117</v>
       </c>
@@ -8171,7 +8172,7 @@
       <c r="E95" s="21"/>
       <c r="F95" s="5"/>
       <c r="G95" s="6" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
       <c r="H95" s="7">
         <v>44798</v>
@@ -8194,7 +8195,7 @@
       </c>
       <c r="M95" s="13" t="str">
         <f t="shared" si="15"/>
-        <v>"floods": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 7 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The [percentage]% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"</v>
+        <v>"floods": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 6 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The [percentage]% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"</v>
       </c>
       <c r="N95" s="26" t="str">
         <f t="shared" si="16"/>
@@ -8218,10 +8219,10 @@
       </c>
       <c r="S95" s="13" t="str">
         <f t="shared" si="21"/>
-        <v>"MWI": {"floods": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 7 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The [percentage]% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
-      </c>
-    </row>
-    <row r="96" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+        <v>"MWI": {"floods": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 6 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The [percentage]% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="9" t="s">
         <v>117</v>
       </c>
@@ -8285,7 +8286,7 @@
         <v>"PHL": {"floods": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 3 days ahead in this layer) for the large river basins. The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60/70/80% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="9" t="s">
         <v>117</v>
       </c>
@@ -8293,7 +8294,7 @@
         <v>32</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D97" s="9" t="s">
         <v>202</v>
@@ -8349,7 +8350,7 @@
         <v>"SSD": {"floods": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 3 days ahead in this layer) for the large river basins. The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60/70/80% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="9" t="s">
         <v>117</v>
       </c>
@@ -8415,7 +8416,7 @@
         <v>"UGA": {"floods": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 5 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60/70/80% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="9" t="s">
         <v>117</v>
       </c>
@@ -8479,7 +8480,7 @@
         <v>"ZMB": {"floods": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 5 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60/70/80% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="9" t="s">
         <v>117</v>
       </c>
@@ -8545,7 +8546,7 @@
         <v>"grassland": {"ETH": {"drought": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010",</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="9" t="s">
         <v>117</v>
       </c>
@@ -8609,7 +8610,7 @@
         <v>"floods": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:19" ht="187.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="9" t="s">
         <v>117</v>
       </c>
@@ -8693,7 +8694,7 @@
 &lt;p&gt;&lt;strong&gt;Latest updated: &lt;/strong&gt;2010&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="9" t="s">
         <v>117</v>
       </c>
@@ -8761,7 +8762,7 @@
         <v>"floods": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="9" t="s">
         <v>117</v>
       </c>
@@ -8777,7 +8778,7 @@
       <c r="E104" s="21"/>
       <c r="F104" s="5"/>
       <c r="G104" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H104" s="19"/>
       <c r="I104" s="14" t="str">
@@ -8825,7 +8826,7 @@
         <v>"UGA": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="9" t="s">
         <v>117</v>
       </c>
@@ -8891,7 +8892,7 @@
         <v>"floods": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="9" t="s">
         <v>117</v>
       </c>
@@ -8955,7 +8956,7 @@
         <v>"ZMB": {"floods": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="9" t="s">
         <v>117</v>
       </c>
@@ -9025,7 +9026,7 @@
         <v>"ZWE": {"drought": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"}},</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="9" t="s">
         <v>117</v>
       </c>
@@ -9091,7 +9092,7 @@
         <v>"health_sites": {"ETH": {"drought": "Health facilities by type and location. Health facility types &lt;strong&gt;hospital&lt;/strong&gt; and &lt;strong&gt;clinic&lt;/strong&gt; are shown with different markers. Other types are omitted and rare in the data.&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;a/&gt;",</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="9" t="s">
         <v>117</v>
       </c>
@@ -9155,7 +9156,7 @@
         <v>"floods": "Health facilities by type and location. Health facility types &lt;strong&gt;hospital&lt;/strong&gt; and &lt;strong&gt;clinic&lt;/strong&gt; are shown with different markers. Other types are omitted and rare in the data.&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;a/&gt;",</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="9" t="s">
         <v>117</v>
       </c>
@@ -9219,7 +9220,7 @@
         <v>"malaria": "Health facilities by type and location. Health facility types &lt;strong&gt;hospital&lt;/strong&gt; and &lt;strong&gt;clinic&lt;/strong&gt; are shown with different markers. Other types are omitted and rare in the data.&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;a/&gt;"},</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="9" t="s">
         <v>117</v>
       </c>
@@ -9291,7 +9292,7 @@
 &lt;p&gt;&lt;strong&gt;Source link&lt;/strong&gt;: &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="9" t="s">
         <v>117</v>
       </c>
@@ -9357,7 +9358,7 @@
         <v>"PHL": {"dengue": "Health facilities by type and location. Health facility types &lt;strong&gt;hospital&lt;/strong&gt; and &lt;strong&gt;clinic&lt;/strong&gt; are shown with different markers. Other types are omitted and rare in the data.&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;a/&gt;",</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="9" t="s">
         <v>117</v>
       </c>
@@ -9431,7 +9432,7 @@
 &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="9" t="s">
         <v>117</v>
       </c>
@@ -9505,7 +9506,7 @@
 &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="9" t="s">
         <v>117</v>
       </c>
@@ -9573,7 +9574,7 @@
         <v>"Hotspot_General": {"ETH": {"drought": "Area of Concern or Hotspot is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on food, livelihood and nutrition insecurity and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response (related to water, human health, education, seed, livestock health and feed)",</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="9" t="s">
         <v>117</v>
       </c>
@@ -9639,7 +9640,7 @@
         <v>"floods": "Area of Concern or Hotspot is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on food, livelihood and nutrition insecurity and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response (related to water, human health, education, seed, livestock health and feed)",</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="9" t="s">
         <v>117</v>
       </c>
@@ -9707,7 +9708,7 @@
         <v>"malaria": "Area of Concern or Hotspot is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on food, livelihood and nutrition insecurity and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response (related to water, human health, education, seed, livestock health and feed)"}},</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="9" t="s">
         <v>117</v>
       </c>
@@ -9775,7 +9776,7 @@
         <v>"Hotspot_Health": {"ETH": {"malaria": "Area of Concern or Hotspot for health is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on health and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response"}},</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="9" t="s">
         <v>117</v>
       </c>
@@ -9841,7 +9842,7 @@
         <v>"Hotspot_Nutrition": {"ETH": {"drought": "Area of Concern or Hotspot for nutrition is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on nutrition insecurity and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response"}},</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="9" t="s">
         <v>117</v>
       </c>
@@ -9909,7 +9910,7 @@
         <v>"Hotspot_Water": {"ETH": {"drought": "Area of Concern or Hotspot for Water is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on WASH and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response",</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="9" t="s">
         <v>117</v>
       </c>
@@ -9975,7 +9976,7 @@
         <v>"floods": "Area of Concern or Hotspot for Water is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on WASH and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response",</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="9" t="s">
         <v>117</v>
       </c>
@@ -10043,7 +10044,7 @@
         <v>"malaria": "Area of Concern or Hotspot for Water is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on WASH and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response"}},</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="9" t="s">
         <v>117</v>
       </c>
@@ -10109,7 +10110,7 @@
         <v>"houses_affected": {"PHL": {"typhoon": "&lt;p&gt;Total Number of completely  damaged houses as predicted by 510 typhoon impact prediction model&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="9" t="s">
         <v>117</v>
       </c>
@@ -10125,7 +10126,7 @@
       <c r="E124" s="21"/>
       <c r="F124" s="5"/>
       <c r="G124" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H124" s="19"/>
       <c r="I124" s="14" t="str">
@@ -10173,7 +10174,7 @@
         <v>"IPC_forecast_long": {"ETH": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="9" t="s">
         <v>117</v>
       </c>
@@ -10239,7 +10240,7 @@
         <v>"malaria": "IPC long forecast: Most likely food security outcomes -  the medium-term projection &lt;a href='https://fews.net/IPC'&gt;https://fews.net/IPC&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="9" t="s">
         <v>117</v>
       </c>
@@ -10255,7 +10256,7 @@
       <c r="E126" s="21"/>
       <c r="F126" s="5"/>
       <c r="G126" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H126" s="19"/>
       <c r="I126" s="14" t="str">
@@ -10303,7 +10304,7 @@
         <v>"UGA": {"drought": "Not currently available"}},</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="9" t="s">
         <v>117</v>
       </c>
@@ -10369,7 +10370,7 @@
         <v>"IPC_forecast_short": {"ETH": {"floods": "IPC short forecast: Most likely food security outcomes - the near-term projection  &lt;a href='https://fews.net/IPC'&gt;https://fews.net/IPC&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:19" ht="201.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="9" t="s">
         <v>117</v>
       </c>
@@ -10445,7 +10446,7 @@
 &lt;p&gt;Latest updated: every month&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="9" t="s">
         <v>117</v>
       </c>
@@ -10511,7 +10512,7 @@
         <v>"malaria_risk": {"ETH": {"malaria": "Malaria risk:Spatial limits of Plasmodium vivax malaria transmission (0-none 2- high)  &lt;a href='https://malariaatlas.org/'&gt;https://malariaatlas.org/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="9" t="s">
         <v>117</v>
       </c>
@@ -10577,7 +10578,7 @@
         <v>"malaria_suitable_temperature": {"ETH": {"malaria": "Malaria suitability:Temperature suitability index for Plasmodium vivax transmission, 2010 &lt;a href='https://malariaatlas.org/research-project/accessibility-to-healthcare/'&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="9" t="s">
         <v>117</v>
       </c>
@@ -10643,7 +10644,7 @@
         <v>"motorized_travel_time_to_health": {"ETH": {"malaria": "Access to Health with vehicle: Estimated travel time (minutes) to the nearest healthcare facility, with motorized vehicle &lt;a href='https://malariaatlas.org/research-project/accessibility-to-healthcare/'&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="9" t="s">
         <v>117</v>
       </c>
@@ -10707,7 +10708,7 @@
         <v>"population": {"EGY": {"heavy-rain": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="9" t="s">
         <v>117</v>
       </c>
@@ -10773,7 +10774,7 @@
         <v>"ETH": {"drought": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="9" t="s">
         <v>117</v>
       </c>
@@ -10837,7 +10838,7 @@
         <v>"floods": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="9" t="s">
         <v>117</v>
       </c>
@@ -10909,7 +10910,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="9" t="s">
         <v>117</v>
       </c>
@@ -11049,7 +11050,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; peanutButter: An R package to produce rapid-response gridded population estimates from building footprints, version 1.0.0 version 1.0.0. Accessed 15-08-2022. WorldPop, University of Southampton. 2021. &amp;nbsp;&lt;a href='https://apps.worldpop.org/peanutButter/'&gt;https://apps.worldpop.org/peanutButter/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="9" t="s">
         <v>117</v>
       </c>
@@ -11117,7 +11118,7 @@
 &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="9" t="s">
         <v>117</v>
       </c>
@@ -11125,7 +11126,7 @@
         <v>66</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D139" s="9" t="s">
         <v>202</v>
@@ -11181,7 +11182,7 @@
         <v>"SSD": {"floods": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="9" t="s">
         <v>117</v>
       </c>
@@ -11249,7 +11250,7 @@
 &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="9" t="s">
         <v>117</v>
       </c>
@@ -11315,7 +11316,7 @@
         <v>"floods": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="9" t="s">
         <v>117</v>
       </c>
@@ -11379,7 +11380,7 @@
         <v>"ZMB": {"floods": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="9" t="s">
         <v>117</v>
       </c>
@@ -11449,7 +11450,7 @@
         <v>"ZWE": {"drought": "&lt;p&gt;The population data comes from the following source: Worldpop data:&amp;nbsp;&lt;a href='https://www.worldpop.org/geodata/'&gt;https://www.worldpop.org/geodata/&lt;/a&gt;&lt;/p&gt; &lt;p&gt;Accessed 07-2020 The mapping approach is Pezzulo, C., Hornby, G., Sorichetta, A. et al. Sub-national mapping of population pyramids and dependency ratios in Africa and Asia. Sci Data 4, 170089 (2017). &lt;a href='https://doi.org/10.1038/sdata.2017.89'&gt;https://doi.org/10.1038/sdata.2017.89&lt;/a&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:19" ht="129.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="9" t="s">
         <v>117</v>
       </c>
@@ -11515,7 +11516,7 @@
         <v>"population_affected": {"EGY": {"heavy-rain": "Number of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."},</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="9" t="s">
         <v>117</v>
       </c>
@@ -11581,7 +11582,7 @@
         <v>"ETH": {"drought": "Number of people exposed is calculated by the population living within the districts currently triggered. The number of people data is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="9" t="s">
         <v>117</v>
       </c>
@@ -11645,7 +11646,7 @@
         <v>"floods": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="9" t="s">
         <v>117</v>
       </c>
@@ -11725,7 +11726,7 @@
 &lt;/ul&gt;",</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="9" t="s">
         <v>117</v>
       </c>
@@ -11823,7 +11824,7 @@
       <c r="E149" s="21"/>
       <c r="F149" s="5"/>
       <c r="G149" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H149" s="7">
         <v>44798</v>
@@ -11885,7 +11886,7 @@
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="216" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:19" ht="216" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="9" t="s">
         <v>117</v>
       </c>
@@ -11951,7 +11952,7 @@
         <v>"PHL": {"floods": "&lt;p&gt;Number of people exposed is calculated by the population living in the flood extent area within the manucipality currently triggered. The number of people and the flood extent are derived from the below sources.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Source (Population Data): High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Source Flood Extent: The flood extent maps are generated by the National Operational Assesment of Hazards(NOAH) project.&lt;a href='https://noah.up.edu.ph/'&gt;https://noah.up.edu.ph/&lt;/a&gt; The 25-year rain return flood hazard maps show low, medium, and high flood hazards represented as yellow, orange, and red respectively. Flood hazards consider take both the height and velocity of the water into consideration and calculates the hazard levels based on the danger they pose to people and structures. Generally, for an average Filipino with a height of 5’ 6”, areas with flood depths from the knee down can be considered to have low hazard levels. Those with flood depths ranging from the knee to neck are considered to have medium hazard levels, and those covered with floods that are higher than the neck have high hazard levels. However, since the flow velocity is also considered, areas that have shallow but fast-flowing flood waters may have a higher hazard level than that denoted by the height of the flood covering it.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="9" t="s">
         <v>117</v>
       </c>
@@ -11959,7 +11960,7 @@
         <v>6</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D151" s="9" t="s">
         <v>202</v>
@@ -12025,7 +12026,7 @@
 &lt;/ul&gt;"},</v>
       </c>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="9" t="s">
         <v>117</v>
       </c>
@@ -12041,7 +12042,7 @@
       <c r="E152" s="21"/>
       <c r="F152" s="5"/>
       <c r="G152" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H152" s="19"/>
       <c r="I152" s="14" t="str">
@@ -12089,7 +12090,7 @@
         <v>"UGA": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="9" t="s">
         <v>117</v>
       </c>
@@ -12155,7 +12156,7 @@
         <v>"floods": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="154" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="9" t="s">
         <v>117</v>
       </c>
@@ -12219,7 +12220,7 @@
         <v>"ZMB": {"floods": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="155" spans="1:19" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:19" ht="302.39999999999998" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="9" t="s">
         <v>117</v>
       </c>
@@ -12289,7 +12290,7 @@
         <v>"ZWE": {"drought": "&lt;p&gt;Number of people exposed is calculated by the population living in the droughts alert threshold reached area within the district currently triggered. The number of people and the drought extent is derived from the below sources.&lt;/p&gt; &lt;p&gt;Source links:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Population Data: Worldpop &lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Drought alert threshold reached: ENSO: Seasonal ERSSTv5 (1991-2020 base period) 3-month running average in Ni&amp;ntilde;o 3.4 (5oNorth-5oSouth) (170-120oWest)). &lt;a href='https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt'&gt;https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt&lt;/a&gt; and CHIRPS: Rainfall Estimates from Rain Gauge and Satellite Observations | Climate Hazards Center - UC Santa Barbara (&lt;a href='https://www.chc.ucsb.edu/data/chirps'&gt;https://www.chc.ucsb.edu/data/chirps&lt;/a&gt;)&amp;nbsp;&lt;/li&gt;&lt;li&gt;Crop Yield data: Izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA, &lt;a href='https://doi.org/10.1594/PANGAEA.909132'&gt;https://doi.org/10.1594/PANGAEA.909132&lt;/a&gt;,Supplement to Iizumi, Toshichika; Sakai, T (2020): The global dataset of historical yields for major crops 1981&amp;ndash;2016. Scientific Data, 7(1), &lt;a href='https://doi.org/10.1038/s41597-020-0433-7'&gt;https://doi.org/10.1038/s41597-020-0433-7&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="156" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:19" ht="129.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="9" t="s">
         <v>117</v>
       </c>
@@ -12355,7 +12356,7 @@
         <v>"population_affected_percentage": {"EGY": {"heavy-rain": "Percentage of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."},</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="9" t="s">
         <v>117</v>
       </c>
@@ -12421,7 +12422,7 @@
         <v>"ETH": {"drought": "Percentage of people exposed is calculated by the population living in within the districts currently triggered. The number of people was derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="9" t="s">
         <v>117</v>
       </c>
@@ -12485,7 +12486,7 @@
         <v>"floods": "Percentage of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="159" spans="1:19" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:19" ht="244.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="9" t="s">
         <v>117</v>
       </c>
@@ -12581,7 +12582,7 @@
       <c r="E160" s="21"/>
       <c r="F160" s="5"/>
       <c r="G160" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H160" s="7">
         <v>44798</v>
@@ -12641,7 +12642,7 @@
 &lt;/ul&gt;"},</v>
       </c>
     </row>
-    <row r="161" spans="1:19" ht="216" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:19" ht="216" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="9" t="s">
         <v>117</v>
       </c>
@@ -12709,7 +12710,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Source (Population Data): High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Source Flood Extent: The flood extent maps are generated by the National Operational Assesment of Hazards(NOAH) project.&lt;a href='https://noah.up.edu.ph/'&gt;https://noah.up.edu.ph/&lt;/a&gt; The 25-year rain return flood hazard maps show low, medium, and high flood hazards represented as yellow, orange, and red respectively. Flood hazards consider take both the height and velocity of the water into consideration and calculates the hazard levels based on the danger they pose to people and structures. Generally, for an average Filipino with a height of 5’ 6”, areas with flood depths from the knee down can be considered to have low hazard levels. Those with flood depths ranging from the knee to neck are considered to have medium hazard levels, and those covered with floods that are higher than the neck have high hazard levels. However, since the flow velocity is also considered, areas that have shallow but fast-flowing flood waters may have a higher hazard level than that denoted by the height of the flood covering it.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:19" ht="172.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="9" t="s">
         <v>117</v>
       </c>
@@ -12717,7 +12718,7 @@
         <v>10</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D162" s="9" t="s">
         <v>202</v>
@@ -12783,7 +12784,7 @@
 &lt;/ul&gt;"},</v>
       </c>
     </row>
-    <row r="163" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="9" t="s">
         <v>117</v>
       </c>
@@ -12849,7 +12850,7 @@
         <v>"UGA": {"floods": "Percentage of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="9" t="s">
         <v>117</v>
       </c>
@@ -12913,7 +12914,7 @@
         <v>"ZMB": {"floods": "Percentage of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."}},</v>
       </c>
     </row>
-    <row r="165" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="9" t="s">
         <v>117</v>
       </c>
@@ -12979,7 +12980,7 @@
         <v>"population_over65": {"PHL": {"dengue": "Percentage of people over 65 years of age. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="9" t="s">
         <v>117</v>
       </c>
@@ -13045,7 +13046,7 @@
         <v>"UGA": {"floods": "Percentage of people over 65 years old.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."}},</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="9" t="s">
         <v>117</v>
       </c>
@@ -13111,7 +13112,7 @@
         <v>"population_u5": {"ETH": {"drought": "Under age: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="9" t="s">
         <v>117</v>
       </c>
@@ -13177,7 +13178,7 @@
         <v>"floods": "Under age: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="169" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="9" t="s">
         <v>117</v>
       </c>
@@ -13241,7 +13242,7 @@
         <v>"malaria": "Under age: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="9" t="s">
         <v>117</v>
       </c>
@@ -13307,7 +13308,7 @@
         <v>"population_u8": {"UGA": {"floods": "Percentage of people under 8 years old.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."}},</v>
       </c>
     </row>
-    <row r="171" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="9" t="s">
         <v>117</v>
       </c>
@@ -13373,7 +13374,7 @@
         <v>"population_u9": {"PHL": {"dengue": "Percentage of people under 9 years of age. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="172" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="9" t="s">
         <v>117</v>
       </c>
@@ -13437,7 +13438,7 @@
         <v>"populationTotal": {"EGY": {"heavy-rain": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="173" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="9" t="s">
         <v>117</v>
       </c>
@@ -13503,7 +13504,7 @@
         <v>"ETH": {"drought": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="174" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="9" t="s">
         <v>117</v>
       </c>
@@ -13567,7 +13568,7 @@
         <v>"floods": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="175" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="9" t="s">
         <v>117</v>
       </c>
@@ -13631,7 +13632,7 @@
         <v>"malaria": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="176" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="9" t="s">
         <v>117</v>
       </c>
@@ -13703,7 +13704,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="177" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="9" t="s">
         <v>117</v>
       </c>
@@ -13843,7 +13844,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; peanutButter: An R package to produce rapid-response gridded population estimates from building footprints, version 1.0.0 version 1.0.0. Accessed 15-08-2022. WorldPop, University of Southampton. 2021. &amp;nbsp;&lt;a href='https://apps.worldpop.org/peanutButter/'&gt;https://apps.worldpop.org/peanutButter/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="179" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="9" t="s">
         <v>117</v>
       </c>
@@ -13911,7 +13912,7 @@
 &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="180" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="9" t="s">
         <v>117</v>
       </c>
@@ -13919,7 +13920,7 @@
         <v>11</v>
       </c>
       <c r="C180" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D180" s="9" t="s">
         <v>202</v>
@@ -13977,7 +13978,7 @@
 &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="9" t="s">
         <v>117</v>
       </c>
@@ -14045,7 +14046,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="182" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="9" t="s">
         <v>117</v>
       </c>
@@ -14111,7 +14112,7 @@
         <v>"floods": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="183" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="9" t="s">
         <v>117</v>
       </c>
@@ -14175,7 +14176,7 @@
         <v>"ZMB": {"floods": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="184" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="9" t="s">
         <v>117</v>
       </c>
@@ -14245,7 +14246,7 @@
         <v>"ZWE": {"drought": "Population data is aggregated per administrative area, from the following original source: Worldpop data:&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;Estimates of total number of people per grid square broken down by gender and age groupings.&lt;/li&gt;&lt;li&gt;Accessed 07-2020 The mapping approach is Pezzulo, C. et al. Sub-national mapping of population pyramids and dependency ratios in Africa and Asia. Sci. Data 4:170089 doi:10.1038/sdata.2017.89 (2017)&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="185" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="9" t="s">
         <v>117</v>
       </c>
@@ -14311,7 +14312,7 @@
         <v>"potential_cases": {"ETH": {"malaria": "Potential number of cases are calculated with the assumtion of a rough proportionality between malaria mosquito enviromental suitability and malaria risk. Then estimating a time lag between optimal malaria mosquito environmental conditions and the peak in number of malaria cases."},</v>
       </c>
     </row>
-    <row r="186" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="9" t="s">
         <v>117</v>
       </c>
@@ -14377,7 +14378,7 @@
         <v>"PHL": {"dengue": "Number of potential dengue cases, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="187" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="9" t="s">
         <v>117</v>
       </c>
@@ -14443,7 +14444,7 @@
         <v>"potential_cases_65": {"ETH": {"malaria": "Elderly: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="188" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="9" t="s">
         <v>117</v>
       </c>
@@ -14509,7 +14510,7 @@
         <v>"PHL": {"dengue": "Number of potential dengue cases among people above 65 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="189" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="9" t="s">
         <v>117</v>
       </c>
@@ -14575,7 +14576,7 @@
         <v>"potential_cases_U5": {"ETH": {"malaria": "Potential cases under 5. Vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="190" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="9" t="s">
         <v>117</v>
       </c>
@@ -14641,7 +14642,7 @@
         <v>"potential_cases_U9": {"PHL": {"dengue": "Number of potential dengue cases among children under 9 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="191" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="9" t="s">
         <v>117</v>
       </c>
@@ -14707,7 +14708,7 @@
         <v>"poverty_incidence": {"UGA": {"floods": "Poverty Incidence is defined by the Multidiemensional Poverty Index and a $2 a day threshold. The layer gives an estimate of people living in poverty.&lt;br /&gt;&lt;br /&gt;Source: Tatem AJ, Gething PW, Bhatt S, Weiss D and Pezzulo C (2013) Pilot high resolution poverty maps, University of Southampton/Oxford. DOI: 10.5258/SOTON/WP00285. Year: 2010"}},</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="9" t="s">
         <v>117</v>
       </c>
@@ -14773,7 +14774,7 @@
         <v>"prob_within_50km": {"PHL": {"typhoon": "&lt;p&gt;Probability for a Municipality being with in 50km of the forecasted typhoon track. Source for Typhoon forecast is ECMWF&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="193" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="9" t="s">
         <v>117</v>
       </c>
@@ -14839,7 +14840,7 @@
         <v>"rainfall": {"PHL": {"typhoon": "&lt;p&gt;24 Hour Precipitation Total extracted from forecast issued by The Weather Prediction Center (WPC) of National Atmospheric Administration, NOAA.&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="194" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="9" t="s">
         <v>117</v>
       </c>
@@ -14905,12 +14906,12 @@
         <v>"rainfall_extent": {"EGY": {"heavy-rain": "Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."}},</v>
       </c>
     </row>
-    <row r="195" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="9" t="s">
         <v>117</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C195" s="9" t="s">
         <v>19</v>
@@ -14921,7 +14922,7 @@
       <c r="E195" s="21"/>
       <c r="F195" s="5"/>
       <c r="G195" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H195" s="7">
         <v>44737</v>
@@ -14971,7 +14972,7 @@
         <v>"rainfall_forecast": {"ETH": {"drought": "The rainfall map layer indicates the seasonal forecasting rainfall data for the floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;For the legend see &lt;a href='https://www.icpac.net/seasonal-forecast/'&gt;https://www.icpac.net/seasonal-forecast/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."}},</v>
       </c>
     </row>
-    <row r="196" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="9" t="s">
         <v>117</v>
       </c>
@@ -15035,7 +15036,7 @@
         <v>"red_crescent_branches": {"EGY": {"heavy-rain": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Egyptian Red Crescent Society (ERCS). Year: 2020."}},</v>
       </c>
     </row>
-    <row r="197" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="9" t="s">
         <v>117</v>
       </c>
@@ -15101,7 +15102,7 @@
         <v>"red_cross_branches": {"EGY": {"heavy-rain": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Egyptian Red Crescent Society (ERCS). Year: 2020."},</v>
       </c>
     </row>
-    <row r="198" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="9" t="s">
         <v>117</v>
       </c>
@@ -15167,7 +15168,7 @@
         <v>"ETH": {"drought": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Ethiopia Red Cross Society (ERCS). Year: 2020.",</v>
       </c>
     </row>
-    <row r="199" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="9" t="s">
         <v>117</v>
       </c>
@@ -15233,7 +15234,7 @@
         <v>"floods": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Ethiopia Red Cross Society (ERCS). Year: 2020.",</v>
       </c>
     </row>
-    <row r="200" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="9" t="s">
         <v>117</v>
       </c>
@@ -15297,7 +15298,7 @@
         <v>"malaria": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Ethiopia Red Cross Society (ERCS). Year: 2020."},</v>
       </c>
     </row>
-    <row r="201" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="9" t="s">
         <v>117</v>
       </c>
@@ -15371,7 +15372,7 @@
 &lt;p&gt;&lt;strong&gt;Latest updated:&lt;/strong&gt; 2020.&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="202" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="9" t="s">
         <v>117</v>
       </c>
@@ -15509,7 +15510,7 @@
         <v>"MWI": {"floods": "Data not available yet"},</v>
       </c>
     </row>
-    <row r="204" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="9" t="s">
         <v>117</v>
       </c>
@@ -15575,7 +15576,7 @@
         <v>"PHL": {"dengue": "Data not available yet",</v>
       </c>
     </row>
-    <row r="205" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="9" t="s">
         <v>117</v>
       </c>
@@ -15641,7 +15642,7 @@
         <v>"floods": "Data not available yet"},</v>
       </c>
     </row>
-    <row r="206" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="9" t="s">
         <v>117</v>
       </c>
@@ -15649,7 +15650,7 @@
         <v>34</v>
       </c>
       <c r="C206" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D206" s="9" t="s">
         <v>202</v>
@@ -15705,7 +15706,7 @@
         <v>"SSD": {"floods": "Data not available yet"},</v>
       </c>
     </row>
-    <row r="207" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="9" t="s">
         <v>117</v>
       </c>
@@ -15771,7 +15772,7 @@
         <v>"UGA": {"drought": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Uganda Red Cross Society (URCS). Year: 2020.",</v>
       </c>
     </row>
-    <row r="208" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="9" t="s">
         <v>117</v>
       </c>
@@ -15837,7 +15838,7 @@
         <v>"floods": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Uganda Red Cross Society (URCS). Year: 2020."},</v>
       </c>
     </row>
-    <row r="209" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="9" t="s">
         <v>117</v>
       </c>
@@ -15903,7 +15904,7 @@
         <v>"ZMB": {"floods": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Zambia Red Cross Society (ZRCS). Year: 2020."},</v>
       </c>
     </row>
-    <row r="210" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="9" t="s">
         <v>117</v>
       </c>
@@ -15973,7 +15974,7 @@
         <v>"ZWE": {"drought": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link Zimbabwe: ZRCS last updated July 2021 at provincial level."}},</v>
       </c>
     </row>
-    <row r="211" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="9" t="s">
         <v>117</v>
       </c>
@@ -16045,7 +16046,7 @@
 &lt;a href='https://prism.philrice.gov.ph/dataproducts/'&gt;https://prism.philrice.gov.ph/dataproducts/&lt;/a&gt; This data is based on the Philippine Rice Information System (PRISM) project which primarily aims to establish a nationwide information system on rice that provide information on rice areas and yield at a particular location and time, and information on factors that are affecting the yield. "}},</v>
       </c>
     </row>
-    <row r="212" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="9" t="s">
         <v>117</v>
       </c>
@@ -16061,7 +16062,7 @@
       <c r="E212" s="21"/>
       <c r="F212" s="5"/>
       <c r="G212" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H212" s="7">
         <v>44575</v>
@@ -16111,7 +16112,7 @@
         <v>"roof_type": {"UGA": {"floods": "Not currently available"}},</v>
       </c>
     </row>
-    <row r="213" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="9" t="s">
         <v>117</v>
       </c>
@@ -16127,7 +16128,7 @@
       <c r="E213" s="21"/>
       <c r="F213" s="5"/>
       <c r="G213" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H213" s="19"/>
       <c r="I213" s="14" t="str">
@@ -16175,7 +16176,7 @@
         <v>"small_ruminants": {"UGA": {"drought": "Not currently available"},</v>
       </c>
     </row>
-    <row r="214" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:19" ht="187.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="9" t="s">
         <v>117</v>
       </c>
@@ -16195,7 +16196,7 @@
         <v>44614</v>
       </c>
       <c r="G214" s="6" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="H214" s="7">
         <v>44575</v>
@@ -16255,7 +16256,7 @@
 &lt;a href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;."}},</v>
       </c>
     </row>
-    <row r="215" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="9" t="s">
         <v>117</v>
       </c>
@@ -16271,7 +16272,7 @@
       <c r="E215" s="21"/>
       <c r="F215" s="5"/>
       <c r="G215" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H215" s="19"/>
       <c r="I215" s="14" t="str">
@@ -16319,7 +16320,7 @@
         <v>"small_ruminants_exposed": {"UGA": {"drought": "Not currently available"},</v>
       </c>
     </row>
-    <row r="216" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="9" t="s">
         <v>117</v>
       </c>
@@ -16339,7 +16340,7 @@
         <v>44614</v>
       </c>
       <c r="G216" s="6" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="H216" s="7">
         <v>44575</v>
@@ -16399,7 +16400,7 @@
 &lt;a href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;."}},</v>
       </c>
     </row>
-    <row r="217" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="9" t="s">
         <v>117</v>
       </c>
@@ -16465,7 +16466,7 @@
         <v>"total_houses": {"PHL": {"typhoon": "&lt;p&gt;Total Number of Housing units in each Municipality&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="218" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="9" t="s">
         <v>117</v>
       </c>
@@ -16531,7 +16532,7 @@
         <v>"total_idps": {"ETH": {"drought": "Total Internally Displaced People (IDPs) DTM Ethiopia National Displacement Report 7_2022",</v>
       </c>
     </row>
-    <row r="219" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="9" t="s">
         <v>117</v>
       </c>
@@ -16597,7 +16598,7 @@
         <v>"floods": "Total Internally Displaced People (IDPs) DTM Ethiopia National Displacement Report 7_2022",</v>
       </c>
     </row>
-    <row r="220" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="9" t="s">
         <v>117</v>
       </c>
@@ -16661,7 +16662,7 @@
         <v>"malaria": "Total Internally Displaced People (IDPs) DTM Ethiopia National Displacement Report 7_2022"}},</v>
       </c>
     </row>
-    <row r="221" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="9" t="s">
         <v>117</v>
       </c>
@@ -16727,7 +16728,7 @@
         <v>"travel_time_cities": {"ETH": {"floods": "Predicted travel time (minutes) to nearest city &lt;a href='https://malariaatlas.org/research-project/accessibility-to-healthcare/'&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="222" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="9" t="s">
         <v>117</v>
       </c>
@@ -16791,7 +16792,7 @@
         <v>"malaria": "Predicted travel time (minutes) to nearest city &lt;a href='https://malariaatlas.org/research-project/accessibility-to-healthcare/'&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="223" spans="1:19" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:19" ht="144" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="9" t="s">
         <v>117</v>
       </c>
@@ -16805,13 +16806,13 @@
         <v>206</v>
       </c>
       <c r="E223" s="21" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F223" s="23">
         <v>44879</v>
       </c>
       <c r="G223" s="6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H223" s="7">
         <v>44879</v>
@@ -16877,7 +16878,7 @@
 &lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="224" spans="1:19" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:19" ht="316.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" s="9" t="s">
         <v>117</v>
       </c>
@@ -16967,7 +16968,7 @@
 &lt;p&gt;&lt;strong&gt;Latest updated:&lt;/strong&gt; month, year&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="225" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="9" t="s">
         <v>117</v>
       </c>
@@ -16983,7 +16984,7 @@
       <c r="E225" s="21"/>
       <c r="F225" s="5"/>
       <c r="G225" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H225" s="19"/>
       <c r="I225" s="14" t="str">
@@ -17031,7 +17032,7 @@
         <v>"UGA": {"drought": "Not currently available"}},</v>
       </c>
     </row>
-    <row r="226" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="9" t="s">
         <v>117</v>
       </c>
@@ -17105,7 +17106,7 @@
 Ongoing (updated regularly)",</v>
       </c>
     </row>
-    <row r="227" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" s="9" t="s">
         <v>117</v>
       </c>
@@ -17175,7 +17176,7 @@
 DSWD, NATIONAL HOUSEHOLD TARGETING OFFICE&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="228" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="9" t="s">
         <v>117</v>
       </c>
@@ -17249,7 +17250,7 @@
 Ongoing (updated regularly)",</v>
       </c>
     </row>
-    <row r="229" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" s="9" t="s">
         <v>117</v>
       </c>
@@ -17265,7 +17266,7 @@
       <c r="E229" s="21"/>
       <c r="F229" s="5"/>
       <c r="G229" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H229" s="7">
         <v>44575</v>
@@ -17315,7 +17316,7 @@
         <v>"typhoon": "&lt;a href='https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard'&gt;https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard&lt;/a&gt; This dataset has been generated by combining PSGC and 4Ps data from DSWD."}},</v>
       </c>
     </row>
-    <row r="230" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" s="9" t="s">
         <v>117</v>
       </c>
@@ -17381,7 +17382,7 @@
         <v>"walking_travel_time_to_health": {"ETH": {"malaria": "Ongoing (updated regularly)"}},</v>
       </c>
     </row>
-    <row r="231" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="9" t="s">
         <v>117</v>
       </c>
@@ -17447,7 +17448,7 @@
         <v>"wall_type": {"UGA": {"floods": "Percentage of households with permanent wall materials; percentage of buildings with (partly) concrete or brick walls.&lt;br /&gt;&lt;br /&gt;Source link: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."}},</v>
       </c>
     </row>
-    <row r="232" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" s="9" t="s">
         <v>117</v>
       </c>
@@ -17463,7 +17464,7 @@
       <c r="E232" s="21"/>
       <c r="F232" s="5"/>
       <c r="G232" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H232" s="19"/>
       <c r="I232" s="14" t="str">
@@ -17511,7 +17512,7 @@
         <v>"waterpoints": {"ETH": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="233" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="9" t="s">
         <v>117</v>
       </c>
@@ -17575,7 +17576,7 @@
         <v>"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="234" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="9" t="s">
         <v>117</v>
       </c>
@@ -17645,7 +17646,7 @@
         <v>"KEN": {"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="235" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" s="9" t="s">
         <v>117</v>
       </c>
@@ -17781,7 +17782,7 @@
         <v>"MWI": {"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="237" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="9" t="s">
         <v>117</v>
       </c>
@@ -17847,7 +17848,7 @@
         <v>"UGA": {"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="238" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="9" t="s">
         <v>117</v>
       </c>
@@ -17913,7 +17914,7 @@
         <v>"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="239" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="9" t="s">
         <v>117</v>
       </c>
@@ -17977,7 +17978,7 @@
         <v>"ZMB": {"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="240" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="9" t="s">
         <v>117</v>
       </c>
@@ -18047,7 +18048,7 @@
         <v>"ZWE": {"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="241" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="9" t="s">
         <v>117</v>
       </c>
@@ -18061,11 +18062,11 @@
         <v>206</v>
       </c>
       <c r="E241" s="21" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F241" s="5"/>
       <c r="G241" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H241" s="19"/>
       <c r="I241" s="14" t="str">
@@ -18113,7 +18114,7 @@
         <v>"windspeed": {"PHL": {"typhoon": "&lt;p&gt;Forecasted 1 minute average maximum wind speed in kilometers per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;"}}}}</v>
       </c>
     </row>
-    <row r="242" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="9"/>
       <c r="B242" s="9"/>
       <c r="C242" s="9"/>
@@ -18167,7 +18168,7 @@
         <v/>
       </c>
     </row>
-    <row r="243" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="9"/>
       <c r="B243" s="9"/>
       <c r="C243" s="9"/>
@@ -18221,7 +18222,7 @@
         <v/>
       </c>
     </row>
-    <row r="244" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="9"/>
       <c r="B244" s="9"/>
       <c r="C244" s="9"/>
@@ -18275,7 +18276,7 @@
         <v/>
       </c>
     </row>
-    <row r="245" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="9"/>
       <c r="B245" s="9"/>
       <c r="C245" s="9"/>
@@ -18329,7 +18330,7 @@
         <v/>
       </c>
     </row>
-    <row r="246" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="9"/>
       <c r="B246" s="9"/>
       <c r="C246" s="9"/>
@@ -18383,7 +18384,7 @@
         <v/>
       </c>
     </row>
-    <row r="247" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="9"/>
       <c r="B247" s="9"/>
       <c r="C247" s="9"/>
@@ -18437,7 +18438,7 @@
         <v/>
       </c>
     </row>
-    <row r="248" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" s="9"/>
       <c r="B248" s="9"/>
       <c r="C248" s="9"/>
@@ -18491,7 +18492,7 @@
         <v/>
       </c>
     </row>
-    <row r="249" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" s="9"/>
       <c r="B249" s="9"/>
       <c r="C249" s="9"/>
@@ -18545,7 +18546,7 @@
         <v/>
       </c>
     </row>
-    <row r="250" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" s="9"/>
       <c r="B250" s="9"/>
       <c r="C250" s="9"/>
@@ -18599,7 +18600,7 @@
         <v/>
       </c>
     </row>
-    <row r="251" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" s="9"/>
       <c r="B251" s="9"/>
       <c r="C251" s="9"/>
@@ -18653,7 +18654,7 @@
         <v/>
       </c>
     </row>
-    <row r="252" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" s="9"/>
       <c r="B252" s="9"/>
       <c r="C252" s="9"/>
@@ -18707,7 +18708,7 @@
         <v/>
       </c>
     </row>
-    <row r="253" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="9"/>
       <c r="B253" s="9"/>
       <c r="C253" s="9"/>
@@ -18761,7 +18762,7 @@
         <v/>
       </c>
     </row>
-    <row r="254" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" s="9"/>
       <c r="B254" s="9"/>
       <c r="C254" s="9"/>
@@ -18815,7 +18816,7 @@
         <v/>
       </c>
     </row>
-    <row r="255" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" s="9"/>
       <c r="B255" s="9"/>
       <c r="C255" s="9"/>
@@ -18869,7 +18870,7 @@
         <v/>
       </c>
     </row>
-    <row r="256" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" s="9"/>
       <c r="B256" s="9"/>
       <c r="C256" s="9"/>
@@ -18923,7 +18924,7 @@
         <v/>
       </c>
     </row>
-    <row r="257" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" s="9"/>
       <c r="B257" s="9"/>
       <c r="C257" s="9"/>
@@ -18977,7 +18978,7 @@
         <v/>
       </c>
     </row>
-    <row r="258" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" s="9"/>
       <c r="B258" s="9"/>
       <c r="C258" s="9"/>
@@ -19031,7 +19032,7 @@
         <v/>
       </c>
     </row>
-    <row r="259" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="9"/>
       <c r="B259" s="9"/>
       <c r="C259" s="9"/>
@@ -19085,7 +19086,7 @@
         <v/>
       </c>
     </row>
-    <row r="260" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" s="9"/>
       <c r="B260" s="9"/>
       <c r="C260" s="9"/>
@@ -19139,7 +19140,7 @@
         <v/>
       </c>
     </row>
-    <row r="261" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="9"/>
       <c r="B261" s="9"/>
       <c r="C261" s="9"/>
@@ -19193,7 +19194,7 @@
         <v/>
       </c>
     </row>
-    <row r="262" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A262" s="9"/>
       <c r="B262" s="9"/>
       <c r="C262" s="9"/>
@@ -19247,7 +19248,7 @@
         <v/>
       </c>
     </row>
-    <row r="263" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" s="9"/>
       <c r="B263" s="9"/>
       <c r="C263" s="9"/>
@@ -19301,7 +19302,7 @@
         <v/>
       </c>
     </row>
-    <row r="264" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" s="9"/>
       <c r="B264" s="9"/>
       <c r="C264" s="9"/>
@@ -19355,7 +19356,7 @@
         <v/>
       </c>
     </row>
-    <row r="265" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" s="9"/>
       <c r="B265" s="9"/>
       <c r="C265" s="9"/>
@@ -19409,7 +19410,7 @@
         <v/>
       </c>
     </row>
-    <row r="266" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" s="9"/>
       <c r="B266" s="9"/>
       <c r="C266" s="9"/>
@@ -19463,7 +19464,7 @@
         <v/>
       </c>
     </row>
-    <row r="267" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" s="9"/>
       <c r="B267" s="9"/>
       <c r="C267" s="9"/>
@@ -19517,7 +19518,7 @@
         <v/>
       </c>
     </row>
-    <row r="268" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" s="9"/>
       <c r="B268" s="9"/>
       <c r="C268" s="9"/>
@@ -19571,7 +19572,7 @@
         <v/>
       </c>
     </row>
-    <row r="269" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" s="9"/>
       <c r="B269" s="9"/>
       <c r="C269" s="9"/>
@@ -19625,7 +19626,7 @@
         <v/>
       </c>
     </row>
-    <row r="270" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" s="9"/>
       <c r="B270" s="9"/>
       <c r="C270" s="9"/>
@@ -19679,7 +19680,7 @@
         <v/>
       </c>
     </row>
-    <row r="271" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" s="9"/>
       <c r="B271" s="9"/>
       <c r="C271" s="9"/>
@@ -19733,7 +19734,7 @@
         <v/>
       </c>
     </row>
-    <row r="272" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" s="9"/>
       <c r="B272" s="9"/>
       <c r="C272" s="9"/>
@@ -19787,7 +19788,7 @@
         <v/>
       </c>
     </row>
-    <row r="273" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A273" s="9"/>
       <c r="B273" s="9"/>
       <c r="C273" s="9"/>
@@ -19841,7 +19842,7 @@
         <v/>
       </c>
     </row>
-    <row r="274" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" s="9"/>
       <c r="B274" s="9"/>
       <c r="C274" s="9"/>
@@ -19895,7 +19896,7 @@
         <v/>
       </c>
     </row>
-    <row r="275" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A275" s="9"/>
       <c r="B275" s="9"/>
       <c r="C275" s="9"/>
@@ -19949,7 +19950,7 @@
         <v/>
       </c>
     </row>
-    <row r="276" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" s="9"/>
       <c r="B276" s="9"/>
       <c r="C276" s="9"/>
@@ -20003,7 +20004,7 @@
         <v/>
       </c>
     </row>
-    <row r="277" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" s="9"/>
       <c r="B277" s="9"/>
       <c r="C277" s="9"/>
@@ -20057,7 +20058,7 @@
         <v/>
       </c>
     </row>
-    <row r="278" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" s="9"/>
       <c r="B278" s="9"/>
       <c r="C278" s="9"/>
@@ -20111,7 +20112,7 @@
         <v/>
       </c>
     </row>
-    <row r="279" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" s="9"/>
       <c r="B279" s="9"/>
       <c r="C279" s="9"/>
@@ -20165,7 +20166,7 @@
         <v/>
       </c>
     </row>
-    <row r="280" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" s="9"/>
       <c r="B280" s="9"/>
       <c r="C280" s="9"/>
@@ -20219,7 +20220,7 @@
         <v/>
       </c>
     </row>
-    <row r="281" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" s="9"/>
       <c r="B281" s="9"/>
       <c r="C281" s="9"/>
@@ -20273,7 +20274,7 @@
         <v/>
       </c>
     </row>
-    <row r="282" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" s="9"/>
       <c r="B282" s="9"/>
       <c r="C282" s="9"/>
@@ -20327,7 +20328,7 @@
         <v/>
       </c>
     </row>
-    <row r="283" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" s="9"/>
       <c r="B283" s="9"/>
       <c r="C283" s="9"/>
@@ -20381,7 +20382,7 @@
         <v/>
       </c>
     </row>
-    <row r="284" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" s="9"/>
       <c r="B284" s="9"/>
       <c r="C284" s="9"/>
@@ -20435,7 +20436,7 @@
         <v/>
       </c>
     </row>
-    <row r="285" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" s="9"/>
       <c r="B285" s="9"/>
       <c r="C285" s="9"/>
@@ -20489,7 +20490,7 @@
         <v/>
       </c>
     </row>
-    <row r="286" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" s="9"/>
       <c r="B286" s="9"/>
       <c r="C286" s="9"/>
@@ -20543,7 +20544,7 @@
         <v/>
       </c>
     </row>
-    <row r="287" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" s="9"/>
       <c r="B287" s="9"/>
       <c r="C287" s="9"/>
@@ -20597,7 +20598,7 @@
         <v/>
       </c>
     </row>
-    <row r="288" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" s="9"/>
       <c r="B288" s="9"/>
       <c r="C288" s="9"/>
@@ -20651,7 +20652,7 @@
         <v/>
       </c>
     </row>
-    <row r="289" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" s="9"/>
       <c r="B289" s="9"/>
       <c r="C289" s="9"/>
@@ -20705,7 +20706,7 @@
         <v/>
       </c>
     </row>
-    <row r="290" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A290" s="9"/>
       <c r="B290" s="9"/>
       <c r="C290" s="9"/>
@@ -20759,7 +20760,7 @@
         <v/>
       </c>
     </row>
-    <row r="291" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" s="9"/>
       <c r="B291" s="9"/>
       <c r="C291" s="9"/>
@@ -20813,7 +20814,7 @@
         <v/>
       </c>
     </row>
-    <row r="292" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" s="9"/>
       <c r="B292" s="9"/>
       <c r="C292" s="9"/>
@@ -20867,7 +20868,7 @@
         <v/>
       </c>
     </row>
-    <row r="293" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="293" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" s="9"/>
       <c r="B293" s="9"/>
       <c r="C293" s="9"/>
@@ -20921,7 +20922,7 @@
         <v/>
       </c>
     </row>
-    <row r="294" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" s="9"/>
       <c r="B294" s="9"/>
       <c r="C294" s="9"/>
@@ -20975,7 +20976,7 @@
         <v/>
       </c>
     </row>
-    <row r="295" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" s="9"/>
       <c r="B295" s="9"/>
       <c r="C295" s="9"/>
@@ -21029,7 +21030,7 @@
         <v/>
       </c>
     </row>
-    <row r="296" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="296" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" s="9"/>
       <c r="B296" s="9"/>
       <c r="C296" s="9"/>
@@ -21083,7 +21084,7 @@
         <v/>
       </c>
     </row>
-    <row r="297" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="297" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" s="9"/>
       <c r="B297" s="9"/>
       <c r="C297" s="9"/>
@@ -21137,7 +21138,7 @@
         <v/>
       </c>
     </row>
-    <row r="298" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="298" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" s="9"/>
       <c r="B298" s="9"/>
       <c r="C298" s="9"/>
@@ -21191,7 +21192,7 @@
         <v/>
       </c>
     </row>
-    <row r="299" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="299" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" s="9"/>
       <c r="B299" s="9"/>
       <c r="C299" s="9"/>
@@ -21245,7 +21246,7 @@
         <v/>
       </c>
     </row>
-    <row r="300" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="300" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" s="9"/>
       <c r="B300" s="9"/>
       <c r="C300" s="9"/>
@@ -21299,7 +21300,7 @@
         <v/>
       </c>
     </row>
-    <row r="301" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" s="9"/>
       <c r="B301" s="9"/>
       <c r="C301" s="9"/>
@@ -21353,7 +21354,7 @@
         <v/>
       </c>
     </row>
-    <row r="302" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" s="9"/>
       <c r="B302" s="9"/>
       <c r="C302" s="9"/>
@@ -21407,7 +21408,7 @@
         <v/>
       </c>
     </row>
-    <row r="303" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" s="9"/>
       <c r="B303" s="9"/>
       <c r="C303" s="9"/>
@@ -21461,7 +21462,7 @@
         <v/>
       </c>
     </row>
-    <row r="304" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" s="9"/>
       <c r="B304" s="9"/>
       <c r="C304" s="9"/>
@@ -21515,7 +21516,7 @@
         <v/>
       </c>
     </row>
-    <row r="305" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" s="9"/>
       <c r="B305" s="9"/>
       <c r="C305" s="9"/>
@@ -21569,7 +21570,7 @@
         <v/>
       </c>
     </row>
-    <row r="306" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" s="9"/>
       <c r="B306" s="9"/>
       <c r="C306" s="9"/>
@@ -21623,7 +21624,7 @@
         <v/>
       </c>
     </row>
-    <row r="307" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" s="9"/>
       <c r="B307" s="9"/>
       <c r="C307" s="9"/>
@@ -21677,7 +21678,7 @@
         <v/>
       </c>
     </row>
-    <row r="308" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" s="9"/>
       <c r="B308" s="9"/>
       <c r="C308" s="9"/>
@@ -21731,7 +21732,7 @@
         <v/>
       </c>
     </row>
-    <row r="309" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A309" s="9"/>
       <c r="B309" s="9"/>
       <c r="C309" s="9"/>
@@ -21785,7 +21786,7 @@
         <v/>
       </c>
     </row>
-    <row r="310" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" s="9"/>
       <c r="B310" s="9"/>
       <c r="C310" s="9"/>
@@ -21839,7 +21840,7 @@
         <v/>
       </c>
     </row>
-    <row r="311" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="311" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A311" s="9"/>
       <c r="B311" s="9"/>
       <c r="C311" s="9"/>
@@ -21893,7 +21894,7 @@
         <v/>
       </c>
     </row>
-    <row r="312" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="312" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A312" s="9"/>
       <c r="B312" s="9"/>
       <c r="C312" s="9"/>
@@ -21947,7 +21948,7 @@
         <v/>
       </c>
     </row>
-    <row r="313" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" s="9"/>
       <c r="B313" s="9"/>
       <c r="C313" s="9"/>
@@ -22001,7 +22002,7 @@
         <v/>
       </c>
     </row>
-    <row r="314" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" s="9"/>
       <c r="B314" s="9"/>
       <c r="C314" s="9"/>
@@ -22055,7 +22056,7 @@
         <v/>
       </c>
     </row>
-    <row r="315" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="315" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A315" s="9"/>
       <c r="B315" s="9"/>
       <c r="C315" s="9"/>
@@ -22109,7 +22110,7 @@
         <v/>
       </c>
     </row>
-    <row r="316" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="316" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A316" s="9"/>
       <c r="B316" s="9"/>
       <c r="C316" s="9"/>
@@ -22163,7 +22164,7 @@
         <v/>
       </c>
     </row>
-    <row r="317" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="317" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A317" s="9"/>
       <c r="B317" s="9"/>
       <c r="C317" s="9"/>
@@ -22217,7 +22218,7 @@
         <v/>
       </c>
     </row>
-    <row r="318" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="318" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A318" s="9"/>
       <c r="B318" s="9"/>
       <c r="C318" s="9"/>
@@ -22271,7 +22272,7 @@
         <v/>
       </c>
     </row>
-    <row r="319" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" s="9"/>
       <c r="B319" s="9"/>
       <c r="C319" s="9"/>
@@ -22325,7 +22326,7 @@
         <v/>
       </c>
     </row>
-    <row r="320" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="320" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" s="9"/>
       <c r="B320" s="9"/>
       <c r="C320" s="9"/>
@@ -22379,7 +22380,7 @@
         <v/>
       </c>
     </row>
-    <row r="321" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="321" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A321" s="9"/>
       <c r="B321" s="9"/>
       <c r="C321" s="9"/>
@@ -22433,7 +22434,7 @@
         <v/>
       </c>
     </row>
-    <row r="322" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="322" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A322" s="9"/>
       <c r="B322" s="9"/>
       <c r="C322" s="9"/>
@@ -22487,7 +22488,7 @@
         <v/>
       </c>
     </row>
-    <row r="323" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="323" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" s="9"/>
       <c r="B323" s="9"/>
       <c r="C323" s="9"/>
@@ -22541,7 +22542,7 @@
         <v/>
       </c>
     </row>
-    <row r="324" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="324" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" s="9"/>
       <c r="B324" s="9"/>
       <c r="C324" s="9"/>
@@ -22595,7 +22596,7 @@
         <v/>
       </c>
     </row>
-    <row r="325" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="325" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" s="9"/>
       <c r="B325" s="9"/>
       <c r="C325" s="9"/>
@@ -22649,7 +22650,7 @@
         <v/>
       </c>
     </row>
-    <row r="326" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="326" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A326" s="9"/>
       <c r="B326" s="9"/>
       <c r="C326" s="9"/>
@@ -22703,7 +22704,7 @@
         <v/>
       </c>
     </row>
-    <row r="327" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="327" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A327" s="9"/>
       <c r="B327" s="9"/>
       <c r="C327" s="9"/>
@@ -22757,7 +22758,7 @@
         <v/>
       </c>
     </row>
-    <row r="328" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="328" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" s="9"/>
       <c r="B328" s="9"/>
       <c r="C328" s="9"/>
@@ -22811,7 +22812,7 @@
         <v/>
       </c>
     </row>
-    <row r="329" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="329" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" s="9"/>
       <c r="B329" s="9"/>
       <c r="C329" s="9"/>
@@ -22865,7 +22866,7 @@
         <v/>
       </c>
     </row>
-    <row r="330" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="330" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" s="9"/>
       <c r="B330" s="9"/>
       <c r="C330" s="9"/>
@@ -22919,7 +22920,7 @@
         <v/>
       </c>
     </row>
-    <row r="331" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="331" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" s="9"/>
       <c r="B331" s="9"/>
       <c r="C331" s="9"/>
@@ -22973,7 +22974,7 @@
         <v/>
       </c>
     </row>
-    <row r="332" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="332" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" s="9"/>
       <c r="B332" s="9"/>
       <c r="C332" s="9"/>
@@ -23027,7 +23028,7 @@
         <v/>
       </c>
     </row>
-    <row r="333" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="333" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" s="9"/>
       <c r="B333" s="9"/>
       <c r="C333" s="9"/>
@@ -23081,7 +23082,7 @@
         <v/>
       </c>
     </row>
-    <row r="334" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="334" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A334" s="9"/>
       <c r="B334" s="9"/>
       <c r="C334" s="9"/>
@@ -23135,7 +23136,7 @@
         <v/>
       </c>
     </row>
-    <row r="335" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="335" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A335" s="9"/>
       <c r="B335" s="9"/>
       <c r="C335" s="9"/>
@@ -23189,7 +23190,7 @@
         <v/>
       </c>
     </row>
-    <row r="336" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="336" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" s="9"/>
       <c r="B336" s="9"/>
       <c r="C336" s="9"/>
@@ -23243,7 +23244,7 @@
         <v/>
       </c>
     </row>
-    <row r="337" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="337" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A337" s="9"/>
       <c r="B337" s="9"/>
       <c r="C337" s="9"/>
@@ -23297,7 +23298,7 @@
         <v/>
       </c>
     </row>
-    <row r="338" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="338" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A338" s="9"/>
       <c r="B338" s="9"/>
       <c r="C338" s="9"/>
@@ -23351,7 +23352,7 @@
         <v/>
       </c>
     </row>
-    <row r="339" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="339" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A339" s="9"/>
       <c r="B339" s="9"/>
       <c r="C339" s="9"/>
@@ -23405,7 +23406,7 @@
         <v/>
       </c>
     </row>
-    <row r="340" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="340" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" s="9"/>
       <c r="B340" s="9"/>
       <c r="C340" s="9"/>
@@ -23459,7 +23460,7 @@
         <v/>
       </c>
     </row>
-    <row r="341" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="341" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A341" s="9"/>
       <c r="B341" s="9"/>
       <c r="C341" s="9"/>
@@ -23513,7 +23514,7 @@
         <v/>
       </c>
     </row>
-    <row r="342" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="342" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" s="9"/>
       <c r="B342" s="9"/>
       <c r="C342" s="9"/>
@@ -23567,7 +23568,7 @@
         <v/>
       </c>
     </row>
-    <row r="343" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="343" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A343" s="9"/>
       <c r="B343" s="9"/>
       <c r="C343" s="9"/>
@@ -23621,7 +23622,7 @@
         <v/>
       </c>
     </row>
-    <row r="344" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="344" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A344" s="9"/>
       <c r="B344" s="9"/>
       <c r="C344" s="9"/>
@@ -23675,7 +23676,7 @@
         <v/>
       </c>
     </row>
-    <row r="345" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="345" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A345" s="9"/>
       <c r="B345" s="9"/>
       <c r="C345" s="9"/>
@@ -23729,7 +23730,7 @@
         <v/>
       </c>
     </row>
-    <row r="346" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="346" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A346" s="9"/>
       <c r="B346" s="9"/>
       <c r="C346" s="9"/>
@@ -23783,7 +23784,7 @@
         <v/>
       </c>
     </row>
-    <row r="347" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="347" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A347" s="9"/>
       <c r="B347" s="9"/>
       <c r="C347" s="9"/>
@@ -23837,7 +23838,7 @@
         <v/>
       </c>
     </row>
-    <row r="348" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="348" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A348" s="9"/>
       <c r="B348" s="9"/>
       <c r="C348" s="9"/>
@@ -23891,7 +23892,7 @@
         <v/>
       </c>
     </row>
-    <row r="349" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="349" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A349" s="9"/>
       <c r="B349" s="9"/>
       <c r="C349" s="9"/>
@@ -23945,7 +23946,7 @@
         <v/>
       </c>
     </row>
-    <row r="350" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="350" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A350" s="9"/>
       <c r="B350" s="9"/>
       <c r="C350" s="9"/>
@@ -23999,7 +24000,7 @@
         <v/>
       </c>
     </row>
-    <row r="351" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="351" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A351" s="9"/>
       <c r="B351" s="9"/>
       <c r="C351" s="9"/>
@@ -24053,7 +24054,7 @@
         <v/>
       </c>
     </row>
-    <row r="352" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="352" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A352" s="9"/>
       <c r="B352" s="9"/>
       <c r="C352" s="9"/>
@@ -24107,7 +24108,7 @@
         <v/>
       </c>
     </row>
-    <row r="353" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="353" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A353" s="9"/>
       <c r="B353" s="9"/>
       <c r="C353" s="9"/>
@@ -24161,7 +24162,7 @@
         <v/>
       </c>
     </row>
-    <row r="354" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="354" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A354" s="9"/>
       <c r="B354" s="9"/>
       <c r="C354" s="9"/>
@@ -24215,7 +24216,7 @@
         <v/>
       </c>
     </row>
-    <row r="355" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="355" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A355" s="9"/>
       <c r="B355" s="9"/>
       <c r="C355" s="9"/>
@@ -24269,7 +24270,7 @@
         <v/>
       </c>
     </row>
-    <row r="356" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="356" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A356" s="9"/>
       <c r="B356" s="9"/>
       <c r="C356" s="9"/>
@@ -24323,7 +24324,7 @@
         <v/>
       </c>
     </row>
-    <row r="357" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="357" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A357" s="9"/>
       <c r="B357" s="9"/>
       <c r="C357" s="9"/>
@@ -24377,7 +24378,7 @@
         <v/>
       </c>
     </row>
-    <row r="358" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="358" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A358" s="9"/>
       <c r="B358" s="9"/>
       <c r="C358" s="9"/>
@@ -24431,7 +24432,7 @@
         <v/>
       </c>
     </row>
-    <row r="359" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="359" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A359" s="9"/>
       <c r="B359" s="9"/>
       <c r="C359" s="9"/>
@@ -24485,7 +24486,7 @@
         <v/>
       </c>
     </row>
-    <row r="360" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="360" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A360" s="9"/>
       <c r="B360" s="9"/>
       <c r="C360" s="9"/>
@@ -24539,7 +24540,7 @@
         <v/>
       </c>
     </row>
-    <row r="361" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="361" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A361" s="9"/>
       <c r="B361" s="9"/>
       <c r="C361" s="9"/>
@@ -24593,7 +24594,7 @@
         <v/>
       </c>
     </row>
-    <row r="362" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="362" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A362" s="9"/>
       <c r="B362" s="9"/>
       <c r="C362" s="9"/>
@@ -24647,7 +24648,7 @@
         <v/>
       </c>
     </row>
-    <row r="363" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="363" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A363" s="9"/>
       <c r="B363" s="9"/>
       <c r="C363" s="9"/>
@@ -24701,7 +24702,7 @@
         <v/>
       </c>
     </row>
-    <row r="364" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="364" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A364" s="9"/>
       <c r="B364" s="9"/>
       <c r="C364" s="9"/>
@@ -24755,7 +24756,7 @@
         <v/>
       </c>
     </row>
-    <row r="365" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="365" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A365" s="9"/>
       <c r="B365" s="9"/>
       <c r="C365" s="9"/>
@@ -24809,7 +24810,7 @@
         <v/>
       </c>
     </row>
-    <row r="366" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="366" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A366" s="9"/>
       <c r="B366" s="9"/>
       <c r="C366" s="9"/>
@@ -24863,7 +24864,7 @@
         <v/>
       </c>
     </row>
-    <row r="367" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="367" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A367" s="9"/>
       <c r="B367" s="9"/>
       <c r="C367" s="9"/>
@@ -24917,7 +24918,7 @@
         <v/>
       </c>
     </row>
-    <row r="368" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="368" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A368" s="9"/>
       <c r="B368" s="9"/>
       <c r="C368" s="9"/>
@@ -24971,7 +24972,7 @@
         <v/>
       </c>
     </row>
-    <row r="369" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="369" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A369" s="9"/>
       <c r="B369" s="9"/>
       <c r="C369" s="9"/>
@@ -25025,7 +25026,7 @@
         <v/>
       </c>
     </row>
-    <row r="370" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="370" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A370" s="9"/>
       <c r="B370" s="9"/>
       <c r="C370" s="9"/>
@@ -25079,7 +25080,7 @@
         <v/>
       </c>
     </row>
-    <row r="371" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="371" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A371" s="9"/>
       <c r="B371" s="9"/>
       <c r="C371" s="9"/>
@@ -25133,7 +25134,7 @@
         <v/>
       </c>
     </row>
-    <row r="372" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="372" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A372" s="9"/>
       <c r="B372" s="9"/>
       <c r="C372" s="9"/>
@@ -25187,7 +25188,7 @@
         <v/>
       </c>
     </row>
-    <row r="373" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="373" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A373" s="9"/>
       <c r="B373" s="9"/>
       <c r="C373" s="9"/>
@@ -25241,7 +25242,7 @@
         <v/>
       </c>
     </row>
-    <row r="374" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="374" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A374" s="9"/>
       <c r="B374" s="9"/>
       <c r="C374" s="9"/>
@@ -25295,7 +25296,7 @@
         <v/>
       </c>
     </row>
-    <row r="375" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="375" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A375" s="9"/>
       <c r="B375" s="9"/>
       <c r="C375" s="9"/>
@@ -25349,7 +25350,7 @@
         <v/>
       </c>
     </row>
-    <row r="376" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="376" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A376" s="9"/>
       <c r="B376" s="9"/>
       <c r="C376" s="9"/>
@@ -25403,7 +25404,7 @@
         <v/>
       </c>
     </row>
-    <row r="377" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="377" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A377" s="9"/>
       <c r="B377" s="9"/>
       <c r="C377" s="9"/>
@@ -25457,7 +25458,7 @@
         <v/>
       </c>
     </row>
-    <row r="378" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="378" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A378" s="9"/>
       <c r="B378" s="9"/>
       <c r="C378" s="9"/>
@@ -25511,7 +25512,7 @@
         <v/>
       </c>
     </row>
-    <row r="379" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="379" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A379" s="9"/>
       <c r="B379" s="9"/>
       <c r="C379" s="9"/>
@@ -25565,7 +25566,7 @@
         <v/>
       </c>
     </row>
-    <row r="380" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="380" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A380" s="9"/>
       <c r="B380" s="9"/>
       <c r="C380" s="9"/>
@@ -25619,7 +25620,7 @@
         <v/>
       </c>
     </row>
-    <row r="381" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="381" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A381" s="9"/>
       <c r="B381" s="9"/>
       <c r="C381" s="9"/>
@@ -25673,7 +25674,7 @@
         <v/>
       </c>
     </row>
-    <row r="382" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="382" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A382" s="9"/>
       <c r="B382" s="9"/>
       <c r="C382" s="9"/>
@@ -25727,7 +25728,7 @@
         <v/>
       </c>
     </row>
-    <row r="383" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="383" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A383" s="9"/>
       <c r="B383" s="9"/>
       <c r="C383" s="9"/>
@@ -25781,7 +25782,7 @@
         <v/>
       </c>
     </row>
-    <row r="384" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="384" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A384" s="9"/>
       <c r="B384" s="9"/>
       <c r="C384" s="9"/>
@@ -25835,7 +25836,7 @@
         <v/>
       </c>
     </row>
-    <row r="385" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="385" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A385" s="9"/>
       <c r="B385" s="9"/>
       <c r="C385" s="9"/>
@@ -25889,7 +25890,7 @@
         <v/>
       </c>
     </row>
-    <row r="386" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="386" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A386" s="9"/>
       <c r="B386" s="9"/>
       <c r="C386" s="9"/>
@@ -25943,7 +25944,7 @@
         <v/>
       </c>
     </row>
-    <row r="387" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="387" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A387" s="9"/>
       <c r="B387" s="9"/>
       <c r="C387" s="9"/>
@@ -25997,7 +25998,7 @@
         <v/>
       </c>
     </row>
-    <row r="388" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="388" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A388" s="9"/>
       <c r="B388" s="9"/>
       <c r="C388" s="9"/>
@@ -26051,7 +26052,7 @@
         <v/>
       </c>
     </row>
-    <row r="389" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="389" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A389" s="9"/>
       <c r="B389" s="9"/>
       <c r="C389" s="9"/>
@@ -26105,7 +26106,7 @@
         <v/>
       </c>
     </row>
-    <row r="390" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="390" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A390" s="9"/>
       <c r="B390" s="9"/>
       <c r="C390" s="9"/>
@@ -26159,7 +26160,7 @@
         <v/>
       </c>
     </row>
-    <row r="391" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="391" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A391" s="9"/>
       <c r="B391" s="9"/>
       <c r="C391" s="9"/>
@@ -26213,7 +26214,7 @@
         <v/>
       </c>
     </row>
-    <row r="392" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="392" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A392" s="9"/>
       <c r="B392" s="9"/>
       <c r="C392" s="9"/>
@@ -26267,7 +26268,7 @@
         <v/>
       </c>
     </row>
-    <row r="393" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="393" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A393" s="9"/>
       <c r="B393" s="9"/>
       <c r="C393" s="9"/>
@@ -26321,7 +26322,7 @@
         <v/>
       </c>
     </row>
-    <row r="394" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="394" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A394" s="9"/>
       <c r="B394" s="9"/>
       <c r="C394" s="9"/>
@@ -26375,7 +26376,7 @@
         <v/>
       </c>
     </row>
-    <row r="395" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="395" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A395" s="9"/>
       <c r="B395" s="9"/>
       <c r="C395" s="9"/>
@@ -26429,7 +26430,7 @@
         <v/>
       </c>
     </row>
-    <row r="396" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="396" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A396" s="9"/>
       <c r="B396" s="9"/>
       <c r="C396" s="9"/>
@@ -26483,7 +26484,7 @@
         <v/>
       </c>
     </row>
-    <row r="397" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="397" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A397" s="9"/>
       <c r="B397" s="9"/>
       <c r="C397" s="9"/>
@@ -26537,7 +26538,7 @@
         <v/>
       </c>
     </row>
-    <row r="398" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="398" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A398" s="9"/>
       <c r="B398" s="9"/>
       <c r="C398" s="9"/>
@@ -26591,7 +26592,7 @@
         <v/>
       </c>
     </row>
-    <row r="399" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="399" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A399" s="9"/>
       <c r="B399" s="9"/>
       <c r="C399" s="9"/>
@@ -26645,7 +26646,7 @@
         <v/>
       </c>
     </row>
-    <row r="400" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="400" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A400" s="9"/>
       <c r="B400" s="9"/>
       <c r="C400" s="9"/>
@@ -26699,7 +26700,7 @@
         <v/>
       </c>
     </row>
-    <row r="401" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="401" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A401" s="9"/>
       <c r="B401" s="9"/>
       <c r="C401" s="9"/>
@@ -26753,7 +26754,7 @@
         <v/>
       </c>
     </row>
-    <row r="402" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="402" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A402" s="9"/>
       <c r="B402" s="9"/>
       <c r="C402" s="9"/>
@@ -26807,7 +26808,7 @@
         <v/>
       </c>
     </row>
-    <row r="403" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="403" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A403" s="9"/>
       <c r="B403" s="9"/>
       <c r="C403" s="9"/>
@@ -26861,7 +26862,7 @@
         <v/>
       </c>
     </row>
-    <row r="404" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="404" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A404" s="9"/>
       <c r="B404" s="9"/>
       <c r="C404" s="9"/>
@@ -26915,7 +26916,7 @@
         <v/>
       </c>
     </row>
-    <row r="405" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="405" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A405" s="9"/>
       <c r="B405" s="9"/>
       <c r="C405" s="9"/>
@@ -26969,7 +26970,7 @@
         <v/>
       </c>
     </row>
-    <row r="406" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="406" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A406" s="9"/>
       <c r="B406" s="9"/>
       <c r="C406" s="9"/>
@@ -27023,7 +27024,7 @@
         <v/>
       </c>
     </row>
-    <row r="407" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="407" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A407" s="9"/>
       <c r="B407" s="9"/>
       <c r="C407" s="9"/>
@@ -27077,7 +27078,7 @@
         <v/>
       </c>
     </row>
-    <row r="408" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="408" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A408" s="9"/>
       <c r="B408" s="9"/>
       <c r="C408" s="9"/>
@@ -27131,7 +27132,7 @@
         <v/>
       </c>
     </row>
-    <row r="409" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="409" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A409" s="9"/>
       <c r="B409" s="9"/>
       <c r="C409" s="9"/>
@@ -27185,7 +27186,7 @@
         <v/>
       </c>
     </row>
-    <row r="410" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="410" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A410" s="9"/>
       <c r="B410" s="9"/>
       <c r="C410" s="9"/>
@@ -27239,7 +27240,7 @@
         <v/>
       </c>
     </row>
-    <row r="411" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="411" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A411" s="9"/>
       <c r="B411" s="9"/>
       <c r="C411" s="9"/>
@@ -27293,7 +27294,7 @@
         <v/>
       </c>
     </row>
-    <row r="412" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="412" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A412" s="9"/>
       <c r="B412" s="9"/>
       <c r="C412" s="9"/>
@@ -27347,7 +27348,7 @@
         <v/>
       </c>
     </row>
-    <row r="413" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="413" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A413" s="9"/>
       <c r="B413" s="9"/>
       <c r="C413" s="9"/>
@@ -27401,7 +27402,7 @@
         <v/>
       </c>
     </row>
-    <row r="414" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="414" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A414" s="9"/>
       <c r="B414" s="9"/>
       <c r="C414" s="9"/>
@@ -27455,7 +27456,7 @@
         <v/>
       </c>
     </row>
-    <row r="415" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="415" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A415" s="9"/>
       <c r="B415" s="9"/>
       <c r="C415" s="9"/>
@@ -27509,7 +27510,7 @@
         <v/>
       </c>
     </row>
-    <row r="416" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="416" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A416" s="9"/>
       <c r="B416" s="9"/>
       <c r="C416" s="9"/>
@@ -27563,7 +27564,7 @@
         <v/>
       </c>
     </row>
-    <row r="417" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="417" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A417" s="9"/>
       <c r="B417" s="9"/>
       <c r="C417" s="9"/>
@@ -27617,7 +27618,7 @@
         <v/>
       </c>
     </row>
-    <row r="418" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="418" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A418" s="9"/>
       <c r="B418" s="9"/>
       <c r="C418" s="9"/>
@@ -27671,7 +27672,7 @@
         <v/>
       </c>
     </row>
-    <row r="419" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="419" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A419" s="9"/>
       <c r="B419" s="9"/>
       <c r="C419" s="9"/>
@@ -27725,7 +27726,7 @@
         <v/>
       </c>
     </row>
-    <row r="420" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="420" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A420" s="9"/>
       <c r="B420" s="9"/>
       <c r="C420" s="9"/>
@@ -27779,7 +27780,7 @@
         <v/>
       </c>
     </row>
-    <row r="421" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="421" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A421" s="9"/>
       <c r="B421" s="9"/>
       <c r="C421" s="9"/>
@@ -27833,7 +27834,7 @@
         <v/>
       </c>
     </row>
-    <row r="422" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="422" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A422" s="9"/>
       <c r="B422" s="9"/>
       <c r="C422" s="9"/>
@@ -27887,7 +27888,7 @@
         <v/>
       </c>
     </row>
-    <row r="423" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="423" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A423" s="9"/>
       <c r="B423" s="9"/>
       <c r="C423" s="9"/>
@@ -27941,7 +27942,7 @@
         <v/>
       </c>
     </row>
-    <row r="424" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="424" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A424" s="9"/>
       <c r="B424" s="9"/>
       <c r="C424" s="9"/>
@@ -27995,7 +27996,7 @@
         <v/>
       </c>
     </row>
-    <row r="425" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="425" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A425" s="9"/>
       <c r="B425" s="9"/>
       <c r="C425" s="9"/>
@@ -28049,7 +28050,7 @@
         <v/>
       </c>
     </row>
-    <row r="426" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="426" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A426" s="9"/>
       <c r="B426" s="9"/>
       <c r="C426" s="9"/>
@@ -28103,7 +28104,7 @@
         <v/>
       </c>
     </row>
-    <row r="427" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="427" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A427" s="9"/>
       <c r="B427" s="9"/>
       <c r="C427" s="9"/>
@@ -28157,7 +28158,7 @@
         <v/>
       </c>
     </row>
-    <row r="428" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="428" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A428" s="9"/>
       <c r="B428" s="9"/>
       <c r="C428" s="9"/>
@@ -28211,7 +28212,7 @@
         <v/>
       </c>
     </row>
-    <row r="429" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="429" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A429" s="9"/>
       <c r="B429" s="9"/>
       <c r="C429" s="9"/>
@@ -28265,7 +28266,7 @@
         <v/>
       </c>
     </row>
-    <row r="430" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="430" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A430" s="9"/>
       <c r="B430" s="9"/>
       <c r="C430" s="9"/>
@@ -28319,7 +28320,7 @@
         <v/>
       </c>
     </row>
-    <row r="431" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="431" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A431" s="9"/>
       <c r="B431" s="9"/>
       <c r="C431" s="9"/>
@@ -28373,7 +28374,7 @@
         <v/>
       </c>
     </row>
-    <row r="432" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="432" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A432" s="9"/>
       <c r="B432" s="9"/>
       <c r="C432" s="9"/>
@@ -28427,7 +28428,7 @@
         <v/>
       </c>
     </row>
-    <row r="433" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="433" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A433" s="9"/>
       <c r="B433" s="9"/>
       <c r="C433" s="9"/>
@@ -28481,7 +28482,7 @@
         <v/>
       </c>
     </row>
-    <row r="434" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="434" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A434" s="9"/>
       <c r="B434" s="9"/>
       <c r="C434" s="9"/>
@@ -28535,7 +28536,7 @@
         <v/>
       </c>
     </row>
-    <row r="435" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="435" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A435" s="9"/>
       <c r="B435" s="9"/>
       <c r="C435" s="9"/>
@@ -28589,7 +28590,7 @@
         <v/>
       </c>
     </row>
-    <row r="436" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="436" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A436" s="9"/>
       <c r="B436" s="9"/>
       <c r="C436" s="9"/>
@@ -28643,7 +28644,7 @@
         <v/>
       </c>
     </row>
-    <row r="437" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="437" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A437" s="9"/>
       <c r="B437" s="9"/>
       <c r="C437" s="9"/>
@@ -28697,7 +28698,7 @@
         <v/>
       </c>
     </row>
-    <row r="438" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="438" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A438" s="9"/>
       <c r="B438" s="9"/>
       <c r="C438" s="9"/>
@@ -28751,7 +28752,7 @@
         <v/>
       </c>
     </row>
-    <row r="439" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="439" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A439" s="9"/>
       <c r="B439" s="9"/>
       <c r="C439" s="9"/>
@@ -28805,7 +28806,7 @@
         <v/>
       </c>
     </row>
-    <row r="440" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="440" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A440" s="9"/>
       <c r="B440" s="9"/>
       <c r="C440" s="9"/>
@@ -28859,7 +28860,7 @@
         <v/>
       </c>
     </row>
-    <row r="441" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="441" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A441" s="9"/>
       <c r="B441" s="9"/>
       <c r="C441" s="9"/>
@@ -28913,7 +28914,7 @@
         <v/>
       </c>
     </row>
-    <row r="442" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="442" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A442" s="9"/>
       <c r="B442" s="9"/>
       <c r="C442" s="9"/>
@@ -28967,7 +28968,7 @@
         <v/>
       </c>
     </row>
-    <row r="443" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="443" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A443" s="9"/>
       <c r="B443" s="9"/>
       <c r="C443" s="9"/>
@@ -29021,7 +29022,7 @@
         <v/>
       </c>
     </row>
-    <row r="444" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="444" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A444" s="9"/>
       <c r="B444" s="9"/>
       <c r="C444" s="9"/>
@@ -29075,7 +29076,7 @@
         <v/>
       </c>
     </row>
-    <row r="445" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="445" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A445" s="9"/>
       <c r="B445" s="9"/>
       <c r="C445" s="9"/>
@@ -29129,7 +29130,7 @@
         <v/>
       </c>
     </row>
-    <row r="446" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="446" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A446" s="9"/>
       <c r="B446" s="9"/>
       <c r="C446" s="9"/>
@@ -29183,7 +29184,7 @@
         <v/>
       </c>
     </row>
-    <row r="447" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="447" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A447" s="9"/>
       <c r="B447" s="9"/>
       <c r="C447" s="9"/>
@@ -29237,7 +29238,7 @@
         <v/>
       </c>
     </row>
-    <row r="448" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="448" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A448" s="9"/>
       <c r="B448" s="9"/>
       <c r="C448" s="9"/>
@@ -29291,7 +29292,7 @@
         <v/>
       </c>
     </row>
-    <row r="449" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="449" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A449" s="9"/>
       <c r="B449" s="9"/>
       <c r="C449" s="9"/>
@@ -29345,7 +29346,7 @@
         <v/>
       </c>
     </row>
-    <row r="450" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="450" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A450" s="9"/>
       <c r="B450" s="9"/>
       <c r="C450" s="9"/>
@@ -29395,11 +29396,11 @@
         <v>}</v>
       </c>
       <c r="S450" s="13" t="str">
-        <f t="shared" ref="S450:S513" si="87">IF(A450="","",I450&amp;J450&amp;K450&amp;L450&amp;M450&amp;N450&amp;O450&amp;P450&amp;Q450&amp;R450)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="451" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" ref="S450:S474" si="87">IF(A450="","",I450&amp;J450&amp;K450&amp;L450&amp;M450&amp;N450&amp;O450&amp;P450&amp;Q450&amp;R450)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="451" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A451" s="9"/>
       <c r="B451" s="9"/>
       <c r="C451" s="9"/>
@@ -29453,7 +29454,7 @@
         <v/>
       </c>
     </row>
-    <row r="452" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="452" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A452" s="9"/>
       <c r="B452" s="9"/>
       <c r="C452" s="9"/>
@@ -29507,7 +29508,7 @@
         <v/>
       </c>
     </row>
-    <row r="453" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="453" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A453" s="9"/>
       <c r="B453" s="9"/>
       <c r="C453" s="9"/>
@@ -29561,7 +29562,7 @@
         <v/>
       </c>
     </row>
-    <row r="454" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="454" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A454" s="9"/>
       <c r="B454" s="9"/>
       <c r="C454" s="9"/>
@@ -29615,7 +29616,7 @@
         <v/>
       </c>
     </row>
-    <row r="455" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="455" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A455" s="9"/>
       <c r="B455" s="9"/>
       <c r="C455" s="9"/>
@@ -29669,7 +29670,7 @@
         <v/>
       </c>
     </row>
-    <row r="456" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="456" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A456" s="9"/>
       <c r="B456" s="9"/>
       <c r="C456" s="9"/>
@@ -29723,7 +29724,7 @@
         <v/>
       </c>
     </row>
-    <row r="457" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="457" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A457" s="9"/>
       <c r="B457" s="9"/>
       <c r="C457" s="9"/>
@@ -29777,7 +29778,7 @@
         <v/>
       </c>
     </row>
-    <row r="458" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="458" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A458" s="9"/>
       <c r="B458" s="9"/>
       <c r="C458" s="9"/>
@@ -29831,7 +29832,7 @@
         <v/>
       </c>
     </row>
-    <row r="459" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="459" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A459" s="9"/>
       <c r="B459" s="9"/>
       <c r="C459" s="9"/>
@@ -29885,7 +29886,7 @@
         <v/>
       </c>
     </row>
-    <row r="460" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="460" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A460" s="9"/>
       <c r="B460" s="9"/>
       <c r="C460" s="9"/>
@@ -29939,7 +29940,7 @@
         <v/>
       </c>
     </row>
-    <row r="461" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="461" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A461" s="9"/>
       <c r="B461" s="9"/>
       <c r="C461" s="9"/>
@@ -29993,7 +29994,7 @@
         <v/>
       </c>
     </row>
-    <row r="462" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="462" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A462" s="9"/>
       <c r="B462" s="9"/>
       <c r="C462" s="9"/>
@@ -30047,7 +30048,7 @@
         <v/>
       </c>
     </row>
-    <row r="463" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="463" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A463" s="9"/>
       <c r="B463" s="9"/>
       <c r="C463" s="9"/>
@@ -30101,7 +30102,7 @@
         <v/>
       </c>
     </row>
-    <row r="464" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="464" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A464" s="9"/>
       <c r="B464" s="9"/>
       <c r="C464" s="9"/>
@@ -30155,7 +30156,7 @@
         <v/>
       </c>
     </row>
-    <row r="465" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="465" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A465" s="9"/>
       <c r="B465" s="9"/>
       <c r="C465" s="9"/>
@@ -30209,7 +30210,7 @@
         <v/>
       </c>
     </row>
-    <row r="466" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="466" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A466" s="9"/>
       <c r="B466" s="9"/>
       <c r="C466" s="9"/>
@@ -30263,7 +30264,7 @@
         <v/>
       </c>
     </row>
-    <row r="467" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="467" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A467" s="9"/>
       <c r="B467" s="9"/>
       <c r="C467" s="9"/>
@@ -30317,7 +30318,7 @@
         <v/>
       </c>
     </row>
-    <row r="468" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="468" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A468" s="9"/>
       <c r="B468" s="9"/>
       <c r="C468" s="9"/>
@@ -30371,7 +30372,7 @@
         <v/>
       </c>
     </row>
-    <row r="469" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="469" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A469" s="9"/>
       <c r="B469" s="9"/>
       <c r="C469" s="9"/>
@@ -30425,7 +30426,7 @@
         <v/>
       </c>
     </row>
-    <row r="470" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="470" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A470" s="9"/>
       <c r="B470" s="9"/>
       <c r="C470" s="9"/>
@@ -30479,7 +30480,7 @@
         <v/>
       </c>
     </row>
-    <row r="471" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="471" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A471" s="9"/>
       <c r="B471" s="9"/>
       <c r="C471" s="9"/>
@@ -30533,7 +30534,7 @@
         <v/>
       </c>
     </row>
-    <row r="472" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="472" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A472" s="9"/>
       <c r="B472" s="9"/>
       <c r="C472" s="9"/>
@@ -30587,7 +30588,7 @@
         <v/>
       </c>
     </row>
-    <row r="473" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="473" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A473" s="9"/>
       <c r="B473" s="9"/>
       <c r="C473" s="9"/>
@@ -30641,7 +30642,7 @@
         <v/>
       </c>
     </row>
-    <row r="474" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="474" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A474" s="9"/>
       <c r="B474" s="9"/>
       <c r="C474" s="9"/>
@@ -30696,12 +30697,17 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="2U6kYg2wyLQnrjZDj1L6HsXSQEK1E+XoQ4i9mzhNu3zShnN+s8sM0GoLIJVD26j8zbJ5uUPROI/45ibohTx2Fw==" saltValue="rYVYkJRN1YklUuwAr+3s0Q==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="4qIM/uYZBbuB2flOCssCipXRrNt8BOgLeV2LioGRgy9IcsU4aNGHcB1aoeFWDzAyXFDfpsBVROP8ajfWLaUZtg==" saltValue="7RQ6t7ZWLRBrA6W5Ixk/Aw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="I1:S1048576" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>
   </protectedRanges>
   <autoFilter ref="A1:S474" xr:uid="{E7D31E7F-BFF5-4ADE-901A-4F6BC662C23D}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="MWI"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S474">
       <sortCondition ref="A1:A474"/>
     </sortState>

</xml_diff>

<commit_message>
fix: update MWI alert popup + trigger statement AB#16464
</commit_message>
<xml_diff>
--- a/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
+++ b/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\IBF-system\interfaces\IBF-dashboard\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B65F7AD-CBD0-4179-88CD-4F91F4B6A685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF28E02-1168-4748-93AF-1D31D9867D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13770" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
@@ -1240,19 +1240,19 @@
     <t>dams</t>
   </si>
   <si>
-    <t>&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 6-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 6 days. The GLOFAS flood forecast triggers except in the Traditional Authorities where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is [value].&lt;/p&gt;
+    <t>This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 6 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The [percentage]% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>The layer shows each administrative area triggered based on two parameters from the 6-days GloFAS forecast on a daily basis at 10:35 CET: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least 60% probability of occurrence of a 5 year return period flood within the next 6 days. The GloFAS flood forecast triggers except in the Traditional Areas where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is 0.5.
+Source link: https://www.globalfloods.eu/
+Latest updated: August 2022</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 6-days GloFAS forecast on a daily basis at 10:35 CET: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least 60% probability of occurrence of a 5 year return period flood within the next 6 days. The GloFAS flood forecast triggers except in the Traditional Areas where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is 0.5.&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
 &lt;p&gt;Source link: &lt;a href="https://www.globalfloods.eu/"&gt;https://www.globalfloods.eu/&lt;/a&gt;&amp;nbsp;&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
 &lt;p&gt;Latest updated: August 2022&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>The layer shows each administrative area triggered based on two parameters from the 6-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 6 days. The GLOFAS flood forecast triggers except in the wards where the False Alarm Ratio (FAR) &gt; [value].
-Source link: https://www.globalfloods.eu/
-Latest updated: August 2022</t>
-  </si>
-  <si>
-    <t>This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 6 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The [percentage]% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -1769,12 +1769,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D31E7F-BFF5-4ADE-901A-4F6BC662C23D}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:S474"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G137" sqref="A1:S474"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1830,7 +1829,7 @@
       <c r="R1" s="13"/>
       <c r="S1" s="13"/>
     </row>
-    <row r="2" spans="1:19" ht="129.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="9" t="s">
         <v>90</v>
       </c>
@@ -1898,7 +1897,7 @@
         <v>{"aggregates-section": {"affected_population": {"PHL": {"typhoon": "&lt;p&gt;The number of people affected is calculated based on the predicted number of completely damaged houses, which is derived from the typhoon impact predicting model. To derive a methodology to estimate the number of affected people from a predicted number of completely damaged houses, we performed a log fit between the number of completely damaged houses and the number of affected people for past typhoon events using data derived from DROMIC reports. To estimate potential number of affected population this formula is applied to the predicted number of damaged houses. &lt;p&gt; "}},</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
         <v>90</v>
       </c>
@@ -2106,7 +2105,7 @@
         <v>"exposed_pop_u18": {"MWI": {"floods": "Number of Exposed Population U18 is calculated by total target population living in the flood extent area within the administrative areas currently triggered. The target population are those living in the households classified as Poor, Poorer, Poorest and whose household head is below 18 years old.&lt;br&gt;&lt;br&gt;Source target population: Unified Beneficiary Registration (UBR). Department of Economy Planning and Development, Malawi. Collected and processed in 2022."}},</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="216" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:19" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="9" t="s">
         <v>90</v>
       </c>
@@ -2172,7 +2171,7 @@
         <v>"female_head_hh": {"UGA": {"floods": "Estimated exposed number of people living in female-headed households living in the flood extent area within the areas currently triggered. This number is calculated by multiplying the overall percentage of households with adult females as decision-maker and main income producer in an area, by the total exposed population in that area.&lt;br /&gt;&lt;br /&gt;Note that the estimate number is not the number of households, but the number of people living in a housholds. In this calculation a household size of 4.7 is used as average estimate.&lt;br /&gt;&lt;br /&gt;. The number of people in female headed households in the flood extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source data:&lt;ul&gt;&lt;li&gt;Female Headed Households: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014.&lt;/li&gt;&lt;li&gt;Total Population: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Flood extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt;&lt;/ul&gt;:"}},</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="9" t="s">
         <v>90</v>
       </c>
@@ -2238,7 +2237,7 @@
         <v>"houses_affected": {"PHL": {"typhoon": "&lt;p&gt;Total Number of completely  damaged houses as predicted by 510 typhoon impact prediction model&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="129.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="9" t="s">
         <v>90</v>
       </c>
@@ -2304,7 +2303,7 @@
         <v>"population_affected": {"EGY": {"heavy-rain": "Number of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br/&gt;Explanation Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."},</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="9" t="s">
         <v>90</v>
       </c>
@@ -2370,7 +2369,7 @@
         <v>"ETH": {"drought": "Number of people exposed is calculated by the population living within the districts currently triggered. The number of people per district are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="9" t="s">
         <v>90</v>
       </c>
@@ -2434,7 +2433,7 @@
         <v>"floods": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="9" t="s">
         <v>90</v>
       </c>
@@ -2514,7 +2513,7 @@
 &lt;/ul&gt;",</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="9" t="s">
         <v>90</v>
       </c>
@@ -2656,7 +2655,7 @@
  &lt;li&gt;Source Flood Extent: Flood hazard map of the World - 10-year return period. European Commission, Joint Research Centre (JRC). 2016. &lt;a href='https://data.jrc.ec.europa.eu/dataset/jrc-floods-floodmapgl_rp10y-tif'&gt;Flood hazard map of the World - 10-year return period - European Commission (europa.eu)&lt;/a&gt;.&lt;/li&gt; &lt;/ul&gt; &lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="216" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:19" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="9" t="s">
         <v>90</v>
       </c>
@@ -2724,7 +2723,7 @@
 &lt;p&gt;Source Links:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Source (Population Data): High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Source Flood Extent: The flood extent maps are generated by the National Operational Assesment of Hazards(NOAH) project.&lt;a href='https://noah.up.edu.ph/'&gt;https://noah.up.edu.ph/&lt;/a&gt; The 25-year rain return flood hazard maps show low, medium, and high flood hazards represented as yellow, orange, and red respectively. Flood hazards consider take both the height and velocity of the water into consideration and calculates the hazard levels based on the danger they pose to people and structures. Generally, for an average Filipino with a height of 5’ 6”, areas with flood depths from the knee down can be considered to have low hazard levels. Those with flood depths ranging from the knee to neck are considered to have medium hazard levels, and those covered with floods that are higher than the neck have high hazard levels. However, since the flow velocity is also considered, areas that have shallow but fast-flowing flood waters may have a higher hazard level than that denoted by the height of the flood covering it.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="129.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="9" t="s">
         <v>90</v>
       </c>
@@ -2788,7 +2787,7 @@
         <v>"SSD": {"floods": "&lt;p&gt;Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;/p&gt;&lt;p&gt;Source Links:&lt;/p&gt;&lt;ul&gt;    &lt;li&gt;Source (Population Data): High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;     &lt;li&gt;Source Flood Extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt; &lt;/ul&gt; &lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="9" t="s">
         <v>90</v>
       </c>
@@ -2852,7 +2851,7 @@
         <v>"UGA": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="9" t="s">
         <v>90</v>
       </c>
@@ -2918,7 +2917,7 @@
         <v>"floods": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="9" t="s">
         <v>90</v>
       </c>
@@ -2982,7 +2981,7 @@
         <v>"ZMB": {"floods": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="302.39999999999998" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:19" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="9" t="s">
         <v>90</v>
       </c>
@@ -3052,7 +3051,7 @@
         <v>"ZWE": {"drought": "&lt;p&gt;Number of people exposed is calculated by the population living in the droughts alert threshold reached area within the district currently triggered. The number of people and the drought extent is derived from the below sources.&lt;/p&gt; &lt;p&gt;Source links:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Population Data: Worldpop &lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Drought alert threshold reached: ENSO: Seasonal ERSSTv5 (1991-2020 base period) 3-month running average in Ni&amp;ntilde;o 3.4 (5oNorth-5oSouth) (170-120oWest)). &lt;a href='https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt'&gt;https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt&lt;/a&gt; and CHIRPS: Rainfall Estimates from Rain Gauge and Satellite Observations | Climate Hazards Center - UC Santa Barbara (&lt;a href='https://www.chc.ucsb.edu/data/chirps'&gt;https://www.chc.ucsb.edu/data/chirps&lt;/a&gt;)&amp;nbsp;&lt;/li&gt;&lt;li&gt;Crop Yield data: Izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA, &lt;a href='https://doi.org/10.1594/PANGAEA.909132'&gt;https://doi.org/10.1594/PANGAEA.909132&lt;/a&gt;,Supplement to Iizumi, Toshichika; Sakai, T (2020): The global dataset of historical yields for major crops 1981&amp;ndash;2016. Scientific Data, 7(1), &lt;a href='https://doi.org/10.1038/s41597-020-0433-7'&gt;https://doi.org/10.1038/s41597-020-0433-7&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="187.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="9" t="s">
         <v>90</v>
       </c>
@@ -3118,7 +3117,7 @@
         <v>"population_over65": {"UGA": {"floods": "Estimate exposed number of people over 65 years of age living in the flood extent area within the areas currently triggered. This number is calculated by multiplying the overall percentage of households with people over 65 years of age, by the total exposed population in that area. The number of people over 65 years of age in the flood extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source data:&lt;ul&gt;&lt;li&gt;Population over 65: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014.&lt;/li&gt;&lt;li&gt;Total Population: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Flood extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt;&lt;/ul&gt;:"}},</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="187.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="9" t="s">
         <v>90</v>
       </c>
@@ -3184,7 +3183,7 @@
         <v>"population_u8": {"UGA": {"floods": "Estimate exposed number of people under 8 years of age living in the flood extent area within the areas currently triggered. This number is calculated by multiplying the overall percentage of households with people under 8 years of age, by the total exposed population in that area. The number of people under 8 years of age in the flood extent is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source data:&lt;ul&gt;&lt;li&gt;Population under 8: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014.&lt;/li&gt;&lt;li&gt;Total Population: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Flood extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt;&lt;/ul&gt;:"}},</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="9" t="s">
         <v>90</v>
       </c>
@@ -3248,7 +3247,7 @@
         <v>"populationTotal": {"EGY": {"heavy-rain": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="9" t="s">
         <v>90</v>
       </c>
@@ -3314,7 +3313,7 @@
         <v>"ETH": {"drought": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="9" t="s">
         <v>90</v>
       </c>
@@ -3378,7 +3377,7 @@
         <v>"floods": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="9" t="s">
         <v>90</v>
       </c>
@@ -3442,7 +3441,7 @@
         <v>"malaria": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="9" t="s">
         <v>90</v>
       </c>
@@ -3512,7 +3511,7 @@
         <v>"KEN": {"drought": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="9" t="s">
         <v>90</v>
       </c>
@@ -3652,7 +3651,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; peanutButter: An R package to produce rapid-response gridded population estimates from building footprints, version 1.0.0 version 1.0.0. Accessed 15-08-2022. WorldPop, University of Southampton. 2021. &amp;nbsp;&lt;a href='https://apps.worldpop.org/peanutButter/'&gt;https://apps.worldpop.org/peanutButter/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="9" t="s">
         <v>90</v>
       </c>
@@ -3720,7 +3719,7 @@
 &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="9" t="s">
         <v>90</v>
       </c>
@@ -3786,7 +3785,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="9" t="s">
         <v>90</v>
       </c>
@@ -3852,7 +3851,7 @@
         <v>"UGA": {"drought": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="9" t="s">
         <v>90</v>
       </c>
@@ -3918,7 +3917,7 @@
         <v>"floods": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="9" t="s">
         <v>90</v>
       </c>
@@ -3982,7 +3981,7 @@
         <v>"ZMB": {"floods": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="9" t="s">
         <v>90</v>
       </c>
@@ -4052,7 +4051,7 @@
         <v>"ZWE": {"drought": "Population data is aggregated per administrative area, from the following original source: Worldpop data:&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;Estimates of total number of people per grid square broken down by gender and age groupings.&lt;/li&gt;&lt;li&gt;Accessed 07-2020 The mapping approach is Pezzulo, C. et al. Sub-national mapping of population pyramids and dependency ratios in Africa and Asia. Sci. Data 4:170089 doi:10.1038/sdata.2017.89 (2017)&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="9" t="s">
         <v>90</v>
       </c>
@@ -4118,7 +4117,7 @@
         <v>"potential_cases": {"ETH": {"malaria": "Potential number of cases are calculated with the assumtion of a rough proportionality between malaria mosquito enviromental suitability and malaria risk. Then estimating a time lag between optimal malaria mosquito environmental conditions and the peak in number of malaria cases."},</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="9" t="s">
         <v>90</v>
       </c>
@@ -4184,7 +4183,7 @@
         <v>"PHL": {"dengue": "Number of potential dengue cases, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="9" t="s">
         <v>90</v>
       </c>
@@ -4250,7 +4249,7 @@
         <v>"potential_cases_65": {"ETH": {"malaria": "Elderly: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="9" t="s">
         <v>90</v>
       </c>
@@ -4316,7 +4315,7 @@
         <v>"PHL": {"dengue": "Number of potential dengue cases among people above 65 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="9" t="s">
         <v>90</v>
       </c>
@@ -4382,7 +4381,7 @@
         <v>"potential_cases_U5": {"ETH": {"malaria": "Potential cases under 5. Vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="9" t="s">
         <v>90</v>
       </c>
@@ -4448,7 +4447,7 @@
         <v>"potential_cases_U9": {"PHL": {"dengue": "Number of potential dengue cases among children under 9 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="9" t="s">
         <v>90</v>
       </c>
@@ -4518,7 +4517,7 @@
         <v>"small_ruminants_exposed": {"ZWE": {"drought": "Number of exposed small ruminants (sheep and goats) is calculated by the small ruminants per province within the droughts alert threshold reached area currently triggered. Livestock numbers small ruminants exists of the number of small ruminants multiplied with the Livestock unit (LSU):0.1 to aggregate livestock from various species  (as reference unit 1.0, which is the grazing equivalent of one adult dairy cow producing 3000 kg of milk annually, without additional concentrated foodstuffs). &lt;br /&gt;&lt;br /&gt;Source Links:&lt;ul&gt;&lt;li&gt;Number of small ruminants (sheep and goats) mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021&lt;/li&gt;&lt;li&gt;Source assessment:&lt;br /&gt;&lt;a href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0 '&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0. &lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"}}},</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="129.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="9" t="s">
         <v>117</v>
       </c>
@@ -4586,7 +4585,7 @@
         <v>"layers-section": {"affected_population": {"PHL": {"typhoon": "&lt;p&gt;The number of people affected is calculated based on the predicted number of completely damaged houses, which is derived from the typhoon impact predicting model. To derive a methodology to estimate the number of affected people from a predicted number of completely damaged houses, we performed a log fit between the number of completely damaged houses and the number of affected people for past typhoon events using data derived from DROMIC reports. To estimate potential number of affected population this formula is applied to the predicted number of damaged houses. &lt;p&gt; "}},</v>
       </c>
     </row>
-    <row r="43" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="9" t="s">
         <v>117</v>
       </c>
@@ -4650,7 +4649,7 @@
         <v>"alert_threshold": {"EGY": {"heavy-rain": "Not currently available"},</v>
       </c>
     </row>
-    <row r="44" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="9" t="s">
         <v>117</v>
       </c>
@@ -4716,7 +4715,7 @@
         <v>"ETH": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="45" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="9" t="s">
         <v>117</v>
       </c>
@@ -4780,7 +4779,7 @@
         <v>"floods": "Not currently available",</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="9" t="s">
         <v>117</v>
       </c>
@@ -4846,7 +4845,7 @@
         <v>"malaria": "An alert is released when two conditions are simultaneously the relative number of malaria cases is anomalous accordance to WHO guidelines, by comparing it to its monthly averages, the second condition is that the absolute number of malaria cases is high and thus likely to require humanitarian intervention."},</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="201.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:19" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="9" t="s">
         <v>117</v>
       </c>
@@ -4922,7 +4921,7 @@
 &lt;p&gt;For further information please refer to the EAP&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="9" t="s">
         <v>117</v>
       </c>
@@ -4998,7 +4997,7 @@
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:19" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="9" t="s">
         <v>117</v>
       </c>
@@ -5016,7 +5015,7 @@
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="6" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="H49" s="7">
         <v>44798</v>
@@ -5039,7 +5038,7 @@
       </c>
       <c r="M49" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>"floods": "&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 6-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 6 days. The GLOFAS flood forecast triggers except in the Traditional Authorities where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is [value].&lt;/p&gt;
+        <v>"floods": "&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 6-days GloFAS forecast on a daily basis at 10:35 CET: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least 60% probability of occurrence of a 5 year return period flood within the next 6 days. The GloFAS flood forecast triggers except in the Traditional Areas where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is 0.5.&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
 &lt;p&gt;Source link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;&amp;nbsp;&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
@@ -5067,14 +5066,14 @@
       </c>
       <c r="S49" s="13" t="str">
         <f t="shared" si="10"/>
-        <v>"MWI": {"floods": "&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 6-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least [percentage]% probability of occurrence of a [number of] year return period flood within the next 6 days. The GLOFAS flood forecast triggers except in the Traditional Authorities where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is [value].&lt;/p&gt;
+        <v>"MWI": {"floods": "&lt;p&gt;The layer shows each administrative area triggered based on two parameters from the 6-days GloFAS forecast on a daily basis at 10:35 CET: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least 60% probability of occurrence of a 5 year return period flood within the next 6 days. The GloFAS flood forecast triggers except in the Traditional Areas where the False Alarm Ratio (FAR) exceeds the predetermined maximum value which is 0.5.&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
 &lt;p&gt;Source link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;&amp;nbsp;&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
 &lt;p&gt;Latest updated: August 2022&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="129.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="9" t="s">
         <v>117</v>
       </c>
@@ -5140,7 +5139,7 @@
         <v>"PHL": {"dengue": "Administrative divisions that reached alert threshold, in terms of number of potential cases. &lt;br /&gt;&lt;br /&gt; See definition at: &lt;a href='https://rodekruis.sharepoint.com/sites/510-CRAVK-510/Gedeelde%20%20documenten/Forms/AllItems.aspx?id=%2Fsites%2F510%2DCRAVK%2D510%2FGedeelde%20%20documenten%2F%5BRD%5D%20Epidemics%20Priority%20Index%2FIBF%2Ddengue%2Fdocuments%2FIBF%5Fdengue%5Ftechnical%5Fnote%2Epdf&amp;parent=%2Fsites%2F510%2DCRAVK%2D510%2FGedeelde%20%20documenten%2F%5BRD%5D%20Epidemics%20Priority%20Index%2FIBF%2Ddengue%2Fdocuments&amp;p=true&amp;originalPath=aHR0cHM6Ly9yb2Rla3J1aXMuc2hhcmVwb2ludC5jb20vc2l0ZXMvNTEwLUNSQVZLLTUxMC9fbGF5b3V0cy8xNS9ndWVzdGFjY2Vzcy5hc3B4P2RvY2lkPTBmOTI0OWIzNWRhNGQ0YzBhOTg1YjMzMzkzZmMzODhkZiZhdXRoa2V5PUFRU0xubmFmR0YtTTJ0MUNHSWcwaGRBJmV4cGlyYXRpb249MjAyMi0wNi0xNFQyMiUzYTAwJTNhMDAuMDAwWiZydGltZT1TS016R0dzeDJVZw'&gt; link to technical documentation&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="9" t="s">
         <v>117</v>
       </c>
@@ -5206,7 +5205,7 @@
         <v>"floods": "&lt;p&gt;The layer shows each county triggered based on two parameters from the 3-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least 50% probability of occurrence of a 5 year return period flood within the next 7 days. The GLOFAS flood forecast triggers except in the  manucipalities where the False Alarm Ratio (RAR) &amp;gt;0.5&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Source link&lt;/strong&gt;: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Latest updated:&amp;nbsp;&lt;/strong&gt;September 2021&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="9" t="s">
         <v>117</v>
       </c>
@@ -5272,7 +5271,7 @@
         <v>"typhoon": "&lt;p&gt;The predicted impact (72 hours before landfall) is more than 10% of houses being totally damaged at municipal level, in at least 3 municipalities. The source for predicted impact is 510 typhoon impact prediction model.&lt;br&gt;&lt;br&gt;Only municipalities that are included in the EAP can reach a triggered state. For other municipalities all data - such as predicted impact - is visible in the map, but they will never turn in to a triggered state.&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="9" t="s">
         <v>117</v>
       </c>
@@ -5340,7 +5339,7 @@
 &lt;p&gt;&lt;strong&gt;Latest updated:&amp;nbsp;&lt;/strong&gt;September 2021&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="54" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="9" t="s">
         <v>117</v>
       </c>
@@ -5404,7 +5403,7 @@
         <v>"UGA": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="55" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="9" t="s">
         <v>117</v>
       </c>
@@ -5468,7 +5467,7 @@
         <v>"floods": "Not currently available"},</v>
       </c>
     </row>
-    <row r="56" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="9" t="s">
         <v>117</v>
       </c>
@@ -5532,7 +5531,7 @@
         <v>"ZMB": {"floods": "Not currently available"},</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="409.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:19" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="9" t="s">
         <v>117</v>
       </c>
@@ -5602,7 +5601,7 @@
         <v>"ZWE": {"drought": "&lt;p&gt;The layer shows each province in the country with a drought risk at the end of the growing season (April), and as such determine which provinces are triggered when at least one of their districts is expected to face a +/- 6 year return period drought.&lt;/p&gt; &lt;p&gt;The drought model is to assess a drought prediction skill of the 3-month running average Ni&amp;ntilde;o 3.4 values and initiates a drought risk when there is a potential negative crop yield anomaly predicted. The model is developed based on the XGBoost algorithm tested and trained with historical ENSO: Seasonal ERSSTv5 and CHIRPS Rainfall data in relation to historical negative crop yield anomalies in April, which is used as drought impact proxy. Loss of crops, livestock loss, and child malnutrition and stunting are indicated by the ZRCS DRM working group and representatives from IFRC, PNS, and Red Cross Climate Centre (RCCC) &amp;nbsp;as targeted drought impact&lt;/p&gt;&lt;p&gt;Source links:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;ENSO: Seasonal ERSSTv5 (1991-2020 base period) 3-month running average in Ni&amp;ntilde;o 3.4 (5oNorth-5oSouth) (170-120oWest)) &lt;a href='https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt'&gt;https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt&lt;/a&gt;&lt;/li&gt;&lt;li&gt;CHIRPS: Rainfall Estimates from Rain Gauge and Satellite Observations | Climate Hazards Center - UC Santa Barbara (&lt;a href='https://www.chc.ucsb.edu/data/chirps'&gt;https://www.chc.ucsb.edu/data/chirps&lt;/a&gt;)&amp;nbsp;&lt;/li&gt;     &lt;li&gt;Crop Yield data: Izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA, &lt;a href='https://doi.org/10.1594/PANGAEA.909132'&gt;https://doi.org/10.1594/PANGAEA.909132&lt;/a&gt;,Supplement to Iizumi, Toshichika; Sakai, T (2020): The global dataset of historical yields for major crops 1981&amp;ndash;2016. Scientific Data, 7(1), &lt;a href='https://doi.org/10.1038/s41597-020-0433-7'&gt;https://doi.org/10.1038/s41597-020-0433-7&lt;/a&gt;&lt;/li&gt; &lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="58" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="9" t="s">
         <v>117</v>
       </c>
@@ -5666,7 +5665,7 @@
         <v>"cattle": {"UGA": {"drought": "Not currently available"},</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="201.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:19" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="9" t="s">
         <v>117</v>
       </c>
@@ -5736,7 +5735,7 @@
         <v>"ZWE": {"drought": "&lt;p&gt;Livestock numbers cattle exists of the number of cattle multiplied with the Livestock unit (LSU): 1.0 &amp;nbsp;as reference unit to aggregate livestock from various species, which is the grazing equivalent of one adult dairy cow producing 3000 kg of milk annually, without additional concentrated foodstuffs.&lt;/p&gt; &lt;p&gt;Source Links :&lt;/p&gt; &lt;ul&gt;     &lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021.&lt;/li&gt;     &lt;li&gt;Source assessment:&lt;br&gt;&lt;a data-fr-linked='true' href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;&lt;/li&gt;     &lt;li&gt;Source Livestock unit (LSU) &lt;a href='https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)'&gt;&amp;nbsp;https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)&lt;/a&gt;&lt;/li&gt; &lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="60" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="9" t="s">
         <v>117</v>
       </c>
@@ -5800,7 +5799,7 @@
         <v>"cattle_exposed": {"UGA": {"drought": "Not currently available"},</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="9" t="s">
         <v>117</v>
       </c>
@@ -5870,7 +5869,7 @@
         <v>"ZWE": {"drought": "&lt;p&gt;Number of exposed cattle is calculated by the cattle per province within the droughts alert threshold reached area currently triggered. Livestock numbers cattle exists of the number of cattle multiplied with the Livestock unit (LSU): 1.0 as reference unit, which is the grazing equivalent of one adult dairy cow producing 3000 kg of milk annually, without additional concentrated foodstuffs.&amp;nbsp;&lt;/p&gt;&lt;p&gt;Source Links :&lt;/p&gt; &lt;ul&gt;     &lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021.&lt;/li&gt;     &lt;li&gt;Source assessment:&lt;br&gt;&lt;a data-fr-linked='true' href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;&lt;/li&gt;     &lt;li&gt;Source Livestock unit (LSU) &lt;a href='https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)'&gt;&amp;nbsp;https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)&lt;/a&gt;&lt;/li&gt; &lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="144" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:19" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="9" t="s">
         <v>117</v>
       </c>
@@ -5934,7 +5933,7 @@
         <v>"covid_risk": {"UGA": {"floods": "The COVID-19 Risk Index is a composite index for the context of exposure, vulnerability to COVID and the capacity to anticipate, cope with and recover from the impacts of COVID-19 (a higher percentage indicates a higher risk to COVID-19). The National Society  selected the following criteria below:&lt;br /&gt;&lt;br /&gt;Exposure&lt;ul&gt;&lt;li&gt;population / km2&lt;/li&gt;&lt;/ul&gt;Vulnerability&lt;ul&gt;&lt;li&gt;% population 65+&lt;/li&gt;&lt;li&gt;% poverty incidence&lt;/li&gt;&lt;/ul&gt;Lack of Coping Capacity&lt;ul&gt;&lt;li&gt;% with no toilet facility&lt;/li&gt;&lt;li&gt;% access to safe drinking water&lt;/li&gt;&lt;li&gt;% illiterate&lt;/li&gt;&lt;li&gt;% with mobile access&lt;/li&gt;&lt;li&gt;% with internet access&lt;/li&gt;&lt;li&gt;% received remittances&lt;/li&gt;&lt;li&gt;HIV: incidence per 100&lt;/li&gt;&lt;li&gt;MALARIA: Plasmodium Falciparum incidence per 1000&lt;/li&gt;&lt;li&gt;% households which consume less than two meals per day&lt;/li&gt;&lt;li&gt;# healh facilities per person&lt;/li&gt;&lt;li&gt;% with a health facility within 5 km&lt;/li&gt;&lt;/ul&gt;&lt;br/&gt;Source link: &lt;a href='https://nlrc.maps.arcgis.com/apps/opsdashboard/index.html#/9ca9f0f452b04046b8594a74c31f0c3b'&gt;https://nlrc.maps.arcgis.com/apps/opsdashboard/index.html#/9ca9f0f452b04046b8594a74c31f0c3b&lt;/a&gt;."}},</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="9" t="s">
         <v>117</v>
       </c>
@@ -6000,7 +5999,7 @@
         <v>"cropland": {"ETH": {"drought": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010",</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="9" t="s">
         <v>117</v>
       </c>
@@ -6064,7 +6063,7 @@
         <v>"floods": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="9" t="s">
         <v>117</v>
       </c>
@@ -6152,7 +6151,7 @@
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="9" t="s">
         <v>117</v>
       </c>
@@ -6240,7 +6239,7 @@
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="67" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="9" t="s">
         <v>117</v>
       </c>
@@ -6304,7 +6303,7 @@
         <v>"UGA": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="9" t="s">
         <v>117</v>
       </c>
@@ -6370,7 +6369,7 @@
         <v>"floods": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="9" t="s">
         <v>117</v>
       </c>
@@ -6434,7 +6433,7 @@
         <v>"ZMB": {"floods": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="187.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="9" t="s">
         <v>117</v>
       </c>
@@ -6504,7 +6503,7 @@
         <v>"ZWE": {"drought": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link Zimbabwe: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"}},</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="9" t="s">
         <v>117</v>
       </c>
@@ -6574,7 +6573,7 @@
         <v>"dams": {"ZWE": {"drought": "This layer represents a selection of dams, and their associated reservoirs in Zimbabwe. The selection is made, based on the  Zimbabwe National Water Authority (ZINWA).&lt;br /&gt;&lt;br /&gt;Source Link Zimbabwe:&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.zinwa.co.zw/dam-levels/'&gt;https://www.zinwa.co.zw/dam-levels/&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="9" t="s">
         <v>117</v>
       </c>
@@ -6640,7 +6639,7 @@
         <v>"dengue_cases_average": {"PHL": {"dengue": "Number of dengue cases per administrative division per year. &lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://doh.gov.ph/statistics'&gt;https://doh.gov.ph/statistics/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="9" t="s">
         <v>117</v>
       </c>
@@ -6706,7 +6705,7 @@
         <v>"dengue_incidence_average": {"PHL": {"dengue": "Number of dengue cases per 10.000.000 people per administrative division per year. &lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://doh.gov.ph/statistics'&gt;https://doh.gov.ph/statistics/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="388.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:19" ht="388.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="9" t="s">
         <v>117</v>
       </c>
@@ -6796,7 +6795,7 @@
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="187.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="9" t="s">
         <v>117</v>
       </c>
@@ -6884,7 +6883,7 @@
 &lt;br&gt;For further information please refer to the EAP"},</v>
       </c>
     </row>
-    <row r="76" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="9" t="s">
         <v>117</v>
       </c>
@@ -6948,7 +6947,7 @@
         <v>"UGA": {"drought": "Not currently available"},</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="244.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:19" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="9" t="s">
         <v>117</v>
       </c>
@@ -7018,7 +7017,7 @@
         <v>"ZWE": {"drought": "The drought vulnerability index is a composite index for the context of exposure to drought and the capacity to anticipate, cope with and recover from the impacts of droughts. The ZRCS selected nine main criteria:&lt;ul&gt;&lt;li&gt;14% Labor constrained households: 7 %unemployment rate 15+  and 7% economically non-active&lt;/li&gt;&lt;li&gt;15% Child, women and elderly headed households: 5% Female headed HH , 5% Head of Household (19-), 5% Head of Household (65+)&lt;/li&gt;&lt;li&gt;14% People with disabilities&lt;/li&gt;&lt;li&gt;15 % Pregnant and breast-feeding women, and children under five years: 5% pregnant women, 5% breast-feeding women, 5% children under five years&lt;/li&gt;&lt;li&gt;14 % Severe acute malnutrition&lt;/li&gt;&lt;li&gt;7% employment agriculture&lt;/li&gt;&lt;li&gt;7% cattle per km2&lt;/li&gt;&lt;li&gt;7% HIV prevalence&lt;/li&gt;&lt;li&gt;7% HIV ART Coverage&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="78" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="9" t="s">
         <v>117</v>
       </c>
@@ -7216,7 +7215,7 @@
         <v>"exposed_pop_u18": {"MWI": {"floods": "Number of Exposed Population U18 is calculated by total target population living in the flood extent area within the administrative areas currently triggered. The target population are those living in the households classified as Poor, Poorer, Poorest and whose household head is below 18 years old.&lt;br&gt;&lt;br&gt;Source target population: Unified Beneficiary Registration (UBR). Department of Economy Planning and Development, Malawi. Collected and processed in 2022."}},</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="9" t="s">
         <v>117</v>
       </c>
@@ -7282,7 +7281,7 @@
         <v>"female_head_hh": {"UGA": {"floods": "Percentage of people living in female headed households.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."}},</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="57.7" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:19" ht="57.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="9" t="s">
         <v>117</v>
       </c>
@@ -7346,7 +7345,7 @@
         <v>"flood_extent": {"ETH": {"floods": "The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="73.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:19" ht="73.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="9" t="s">
         <v>117</v>
       </c>
@@ -7484,7 +7483,7 @@
         <v>"MWI": {"floods": "&lt;p&gt;The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 10-years) based on a global hydrological model.&lt;br&gt;&lt;br&gt;Source link: Flood hazard map of the World - 10-year return period. European Commission, Joint Research Centre (JRC). 2016. &lt;a href='https://data.jrc.ec.europa.eu/dataset/jrc-floods-floodmapgl_rp10y-tif'&gt;Flood hazard map of the World - 10-year return period - European Commission (europa.eu)&lt;/a&gt;.&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="9" t="s">
         <v>117</v>
       </c>
@@ -7560,7 +7559,7 @@
 covering it. "},</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="9" t="s">
         <v>117</v>
       </c>
@@ -7624,7 +7623,7 @@
         <v>"SSD": {"floods": "The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="9" t="s">
         <v>117</v>
       </c>
@@ -7690,7 +7689,7 @@
         <v>"UGA": {"floods": "The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="9" t="s">
         <v>117</v>
       </c>
@@ -7754,7 +7753,7 @@
         <v>"ZMB": {"floods": "The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."}},</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="201.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:19" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="9" t="s">
         <v>117</v>
       </c>
@@ -7820,7 +7819,7 @@
         <v>"flood_susceptibility": {"EGY": {"heavy-rain": "Flood susceptibility identifies the most vulnerable areas based on physical characteristics that determine the propensity for flooding” (Vojtek and Vojtekova, 2019). The mapping of flood susceptible areas involves the analysis of multiple criteria for different characteristics of the region that collectively contribute to the likelihood of floods.&lt;br/&gt;&lt;br/&gt;Nine influencing parameters based on a variety of satellite imagery and spatial datasets are the input factors of the model, such as topographical (Elevation model, Slope), physical (Land cover, Hydrological soil group) and hydrological properties (Height Above Nearest Drainage, Distance from Nearest Drainage, Topographic Wetness Index Slope, Rain intensity, Rain duration). Set of weights based on expert knowledge (The Analytical Hierarchical Process) from REACH (2019) was adapted in this analysis.&lt;br/&gt;&lt;br/&gt;&lt;strong&gt;LEGEND:&lt;/strong&gt; There are 4 classes of flood susceptibility. The higher the flood susceptibility, the darker blue the color.&lt;br/&gt;&lt;br/&gt;SOURCES:&lt;ul&gt;&lt;li&gt;REACH. Yemen Flood Susceptibility. 2019. &lt;a href='https://reliefweb.int/sites/reliefweb.int/files/resources/REACH_YEM_MethodologyNote_HVA_FloodSusceptibility_01APR2020_EN_V2.pdf'&gt;https://reliefweb.int/sites/reliefweb.int/files/resources/REACH_YEM_MethodologyNote_HVA_FloodSusceptibility_01APR2020_EN_V2.pdf&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Vojtek, M.; Vojteková, J. Flood Susceptibility Mapping on a National Scale in Slovakia Using the Analytical Hierarchy Process. Water 2019, 11, 364. &lt;a href='https://doi.org/10.3390/w11020364'&gt;https://doi.org/10.3390/w11020364&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="216" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:19" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="9" t="s">
         <v>117</v>
       </c>
@@ -7956,7 +7955,7 @@
         <v>"MWI": {"floods": "The flood vulnerability index is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts of floods. The vulnerability index is selected with the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Flood physical exposure. &lt;/li&gt;&lt;li&gt; 20% Poverty: Poverty incidence &lt;/li&gt;&lt;li&gt;20% Gender: Female headed household &lt;/li&gt;&lt;li&gt;20% Age: Population below 5 years &lt;/li&gt;&lt;li&gt;20 % Disability: People with disability&lt;/li&gt;&lt;/ul&gt;."},</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="9" t="s">
         <v>117</v>
       </c>
@@ -8022,7 +8021,7 @@
         <v>"UGA": {"floods": "The disaster vulnerability index is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts of floods. The National Society and Technical Working group selected the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Poverty: Poverty incidence&lt;/li&gt;&lt;li&gt;20% Gender: Female headed household&lt;/li&gt;&lt;li&gt;10% Age: Population below 8-years&lt;/li&gt;&lt;li&gt;10% Age: population 65+,&lt;/li&gt;&lt;li&gt;10 % type of construction: permanent wall type&lt;/li&gt;&lt;li&gt;10 %type of construction: permanent roof type&lt;/li&gt;&lt;li&gt;20% Refugees legal status #of displaced person&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;For further information please refer to the EAP. For source links, see each individual layer."}},</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="9" t="s">
         <v>117</v>
       </c>
@@ -8086,7 +8085,7 @@
         <v>"glofas_stations": {"ETH": {"floods": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 5 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60/70/80% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="288" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:19" ht="288" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="9" t="s">
         <v>117</v>
       </c>
@@ -8172,7 +8171,7 @@
       <c r="E95" s="21"/>
       <c r="F95" s="5"/>
       <c r="G95" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H95" s="7">
         <v>44798</v>
@@ -8222,7 +8221,7 @@
         <v>"MWI": {"floods": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 6 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The [percentage]% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="9" t="s">
         <v>117</v>
       </c>
@@ -8286,7 +8285,7 @@
         <v>"PHL": {"floods": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 3 days ahead in this layer) for the large river basins. The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60/70/80% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="9" t="s">
         <v>117</v>
       </c>
@@ -8350,7 +8349,7 @@
         <v>"SSD": {"floods": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 3 days ahead in this layer) for the large river basins. The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60/70/80% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="9" t="s">
         <v>117</v>
       </c>
@@ -8416,7 +8415,7 @@
         <v>"UGA": {"floods": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 5 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60/70/80% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="9" t="s">
         <v>117</v>
       </c>
@@ -8480,7 +8479,7 @@
         <v>"ZMB": {"floods": "This layer provides the location where the Global Flood Awareness System (GLoFAS) forecast is used for the trigger. This forecast is often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 5 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60/70/80% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="9" t="s">
         <v>117</v>
       </c>
@@ -8546,7 +8545,7 @@
         <v>"grassland": {"ETH": {"drought": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010",</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="9" t="s">
         <v>117</v>
       </c>
@@ -8610,7 +8609,7 @@
         <v>"floods": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="187.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="9" t="s">
         <v>117</v>
       </c>
@@ -8694,7 +8693,7 @@
 &lt;p&gt;&lt;strong&gt;Latest updated: &lt;/strong&gt;2010&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="9" t="s">
         <v>117</v>
       </c>
@@ -8762,7 +8761,7 @@
         <v>"floods": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="104" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="9" t="s">
         <v>117</v>
       </c>
@@ -8826,7 +8825,7 @@
         <v>"UGA": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="9" t="s">
         <v>117</v>
       </c>
@@ -8892,7 +8891,7 @@
         <v>"floods": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="9" t="s">
         <v>117</v>
       </c>
@@ -8956,7 +8955,7 @@
         <v>"ZMB": {"floods": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="9" t="s">
         <v>117</v>
       </c>
@@ -9026,7 +9025,7 @@
         <v>"ZWE": {"drought": "The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Source Link: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"}},</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="9" t="s">
         <v>117</v>
       </c>
@@ -9092,7 +9091,7 @@
         <v>"health_sites": {"ETH": {"drought": "Health facilities by type and location. Health facility types &lt;strong&gt;hospital&lt;/strong&gt; and &lt;strong&gt;clinic&lt;/strong&gt; are shown with different markers. Other types are omitted and rare in the data.&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;a/&gt;",</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="9" t="s">
         <v>117</v>
       </c>
@@ -9156,7 +9155,7 @@
         <v>"floods": "Health facilities by type and location. Health facility types &lt;strong&gt;hospital&lt;/strong&gt; and &lt;strong&gt;clinic&lt;/strong&gt; are shown with different markers. Other types are omitted and rare in the data.&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;a/&gt;",</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="9" t="s">
         <v>117</v>
       </c>
@@ -9220,7 +9219,7 @@
         <v>"malaria": "Health facilities by type and location. Health facility types &lt;strong&gt;hospital&lt;/strong&gt; and &lt;strong&gt;clinic&lt;/strong&gt; are shown with different markers. Other types are omitted and rare in the data.&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;a/&gt;"},</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="9" t="s">
         <v>117</v>
       </c>
@@ -9292,7 +9291,7 @@
 &lt;p&gt;&lt;strong&gt;Source link&lt;/strong&gt;: &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="9" t="s">
         <v>117</v>
       </c>
@@ -9358,7 +9357,7 @@
         <v>"PHL": {"dengue": "Health facilities by type and location. Health facility types &lt;strong&gt;hospital&lt;/strong&gt; and &lt;strong&gt;clinic&lt;/strong&gt; are shown with different markers. Other types are omitted and rare in the data.&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;a/&gt;",</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="9" t="s">
         <v>117</v>
       </c>
@@ -9432,7 +9431,7 @@
 &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="9" t="s">
         <v>117</v>
       </c>
@@ -9506,7 +9505,7 @@
 &lt;a href='https://healthsites.io/'&gt;https://healthsites.io/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="9" t="s">
         <v>117</v>
       </c>
@@ -9574,7 +9573,7 @@
         <v>"Hotspot_General": {"ETH": {"drought": "Area of Concern or Hotspot is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on food, livelihood and nutrition insecurity and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response (related to water, human health, education, seed, livestock health and feed)",</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="9" t="s">
         <v>117</v>
       </c>
@@ -9640,7 +9639,7 @@
         <v>"floods": "Area of Concern or Hotspot is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on food, livelihood and nutrition insecurity and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response (related to water, human health, education, seed, livestock health and feed)",</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="9" t="s">
         <v>117</v>
       </c>
@@ -9708,7 +9707,7 @@
         <v>"malaria": "Area of Concern or Hotspot is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on food, livelihood and nutrition insecurity and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response (related to water, human health, education, seed, livestock health and feed)"}},</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="9" t="s">
         <v>117</v>
       </c>
@@ -9776,7 +9775,7 @@
         <v>"Hotspot_Health": {"ETH": {"malaria": "Area of Concern or Hotspot for health is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on health and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response"}},</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="9" t="s">
         <v>117</v>
       </c>
@@ -9842,7 +9841,7 @@
         <v>"Hotspot_Nutrition": {"ETH": {"drought": "Area of Concern or Hotspot for nutrition is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on nutrition insecurity and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response"}},</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="9" t="s">
         <v>117</v>
       </c>
@@ -9910,7 +9909,7 @@
         <v>"Hotspot_Water": {"ETH": {"drought": "Area of Concern or Hotspot for Water is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on WASH and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response",</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="9" t="s">
         <v>117</v>
       </c>
@@ -9976,7 +9975,7 @@
         <v>"floods": "Area of Concern or Hotspot for Water is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on WASH and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response",</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="9" t="s">
         <v>117</v>
       </c>
@@ -10044,7 +10043,7 @@
         <v>"malaria": "Area of Concern or Hotspot for Water is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on WASH and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response"}},</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="9" t="s">
         <v>117</v>
       </c>
@@ -10110,7 +10109,7 @@
         <v>"houses_affected": {"PHL": {"typhoon": "&lt;p&gt;Total Number of completely  damaged houses as predicted by 510 typhoon impact prediction model&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="124" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="9" t="s">
         <v>117</v>
       </c>
@@ -10174,7 +10173,7 @@
         <v>"IPC_forecast_long": {"ETH": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="9" t="s">
         <v>117</v>
       </c>
@@ -10240,7 +10239,7 @@
         <v>"malaria": "IPC long forecast: Most likely food security outcomes -  the medium-term projection &lt;a href='https://fews.net/IPC'&gt;https://fews.net/IPC&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="126" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="9" t="s">
         <v>117</v>
       </c>
@@ -10304,7 +10303,7 @@
         <v>"UGA": {"drought": "Not currently available"}},</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="9" t="s">
         <v>117</v>
       </c>
@@ -10370,7 +10369,7 @@
         <v>"IPC_forecast_short": {"ETH": {"floods": "IPC short forecast: Most likely food security outcomes - the near-term projection  &lt;a href='https://fews.net/IPC'&gt;https://fews.net/IPC&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="201.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:19" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="9" t="s">
         <v>117</v>
       </c>
@@ -10446,7 +10445,7 @@
 &lt;p&gt;Latest updated: every month&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="9" t="s">
         <v>117</v>
       </c>
@@ -10512,7 +10511,7 @@
         <v>"malaria_risk": {"ETH": {"malaria": "Malaria risk:Spatial limits of Plasmodium vivax malaria transmission (0-none 2- high)  &lt;a href='https://malariaatlas.org/'&gt;https://malariaatlas.org/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="9" t="s">
         <v>117</v>
       </c>
@@ -10578,7 +10577,7 @@
         <v>"malaria_suitable_temperature": {"ETH": {"malaria": "Malaria suitability:Temperature suitability index for Plasmodium vivax transmission, 2010 &lt;a href='https://malariaatlas.org/research-project/accessibility-to-healthcare/'&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="9" t="s">
         <v>117</v>
       </c>
@@ -10644,7 +10643,7 @@
         <v>"motorized_travel_time_to_health": {"ETH": {"malaria": "Access to Health with vehicle: Estimated travel time (minutes) to the nearest healthcare facility, with motorized vehicle &lt;a href='https://malariaatlas.org/research-project/accessibility-to-healthcare/'&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="9" t="s">
         <v>117</v>
       </c>
@@ -10708,7 +10707,7 @@
         <v>"population": {"EGY": {"heavy-rain": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="9" t="s">
         <v>117</v>
       </c>
@@ -10774,7 +10773,7 @@
         <v>"ETH": {"drought": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="9" t="s">
         <v>117</v>
       </c>
@@ -10838,7 +10837,7 @@
         <v>"floods": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="9" t="s">
         <v>117</v>
       </c>
@@ -10910,7 +10909,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="9" t="s">
         <v>117</v>
       </c>
@@ -11050,7 +11049,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; peanutButter: An R package to produce rapid-response gridded population estimates from building footprints, version 1.0.0 version 1.0.0. Accessed 15-08-2022. WorldPop, University of Southampton. 2021. &amp;nbsp;&lt;a href='https://apps.worldpop.org/peanutButter/'&gt;https://apps.worldpop.org/peanutButter/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="9" t="s">
         <v>117</v>
       </c>
@@ -11118,7 +11117,7 @@
 &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="9" t="s">
         <v>117</v>
       </c>
@@ -11182,7 +11181,7 @@
         <v>"SSD": {"floods": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="9" t="s">
         <v>117</v>
       </c>
@@ -11250,7 +11249,7 @@
 &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="9" t="s">
         <v>117</v>
       </c>
@@ -11316,7 +11315,7 @@
         <v>"floods": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="9" t="s">
         <v>117</v>
       </c>
@@ -11380,7 +11379,7 @@
         <v>"ZMB": {"floods": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="9" t="s">
         <v>117</v>
       </c>
@@ -11450,7 +11449,7 @@
         <v>"ZWE": {"drought": "&lt;p&gt;The population data comes from the following source: Worldpop data:&amp;nbsp;&lt;a href='https://www.worldpop.org/geodata/'&gt;https://www.worldpop.org/geodata/&lt;/a&gt;&lt;/p&gt; &lt;p&gt;Accessed 07-2020 The mapping approach is Pezzulo, C., Hornby, G., Sorichetta, A. et al. Sub-national mapping of population pyramids and dependency ratios in Africa and Asia. Sci Data 4, 170089 (2017). &lt;a href='https://doi.org/10.1038/sdata.2017.89'&gt;https://doi.org/10.1038/sdata.2017.89&lt;/a&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="129.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="9" t="s">
         <v>117</v>
       </c>
@@ -11516,7 +11515,7 @@
         <v>"population_affected": {"EGY": {"heavy-rain": "Number of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."},</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="9" t="s">
         <v>117</v>
       </c>
@@ -11582,7 +11581,7 @@
         <v>"ETH": {"drought": "Number of people exposed is calculated by the population living within the districts currently triggered. The number of people data is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="9" t="s">
         <v>117</v>
       </c>
@@ -11646,7 +11645,7 @@
         <v>"floods": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="9" t="s">
         <v>117</v>
       </c>
@@ -11726,7 +11725,7 @@
 &lt;/ul&gt;",</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="9" t="s">
         <v>117</v>
       </c>
@@ -11886,7 +11885,7 @@
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="216" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:19" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="9" t="s">
         <v>117</v>
       </c>
@@ -11952,7 +11951,7 @@
         <v>"PHL": {"floods": "&lt;p&gt;Number of people exposed is calculated by the population living in the flood extent area within the manucipality currently triggered. The number of people and the flood extent are derived from the below sources.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Source (Population Data): High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Source Flood Extent: The flood extent maps are generated by the National Operational Assesment of Hazards(NOAH) project.&lt;a href='https://noah.up.edu.ph/'&gt;https://noah.up.edu.ph/&lt;/a&gt; The 25-year rain return flood hazard maps show low, medium, and high flood hazards represented as yellow, orange, and red respectively. Flood hazards consider take both the height and velocity of the water into consideration and calculates the hazard levels based on the danger they pose to people and structures. Generally, for an average Filipino with a height of 5’ 6”, areas with flood depths from the knee down can be considered to have low hazard levels. Those with flood depths ranging from the knee to neck are considered to have medium hazard levels, and those covered with floods that are higher than the neck have high hazard levels. However, since the flow velocity is also considered, areas that have shallow but fast-flowing flood waters may have a higher hazard level than that denoted by the height of the flood covering it.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="158.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="9" t="s">
         <v>117</v>
       </c>
@@ -12026,7 +12025,7 @@
 &lt;/ul&gt;"},</v>
       </c>
     </row>
-    <row r="152" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="9" t="s">
         <v>117</v>
       </c>
@@ -12090,7 +12089,7 @@
         <v>"UGA": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="9" t="s">
         <v>117</v>
       </c>
@@ -12156,7 +12155,7 @@
         <v>"floods": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="154" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="9" t="s">
         <v>117</v>
       </c>
@@ -12220,7 +12219,7 @@
         <v>"ZMB": {"floods": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="155" spans="1:19" ht="302.39999999999998" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:19" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="9" t="s">
         <v>117</v>
       </c>
@@ -12290,7 +12289,7 @@
         <v>"ZWE": {"drought": "&lt;p&gt;Number of people exposed is calculated by the population living in the droughts alert threshold reached area within the district currently triggered. The number of people and the drought extent is derived from the below sources.&lt;/p&gt; &lt;p&gt;Source links:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Population Data: Worldpop &lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Drought alert threshold reached: ENSO: Seasonal ERSSTv5 (1991-2020 base period) 3-month running average in Ni&amp;ntilde;o 3.4 (5oNorth-5oSouth) (170-120oWest)). &lt;a href='https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt'&gt;https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt&lt;/a&gt; and CHIRPS: Rainfall Estimates from Rain Gauge and Satellite Observations | Climate Hazards Center - UC Santa Barbara (&lt;a href='https://www.chc.ucsb.edu/data/chirps'&gt;https://www.chc.ucsb.edu/data/chirps&lt;/a&gt;)&amp;nbsp;&lt;/li&gt;&lt;li&gt;Crop Yield data: Izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA, &lt;a href='https://doi.org/10.1594/PANGAEA.909132'&gt;https://doi.org/10.1594/PANGAEA.909132&lt;/a&gt;,Supplement to Iizumi, Toshichika; Sakai, T (2020): The global dataset of historical yields for major crops 1981&amp;ndash;2016. Scientific Data, 7(1), &lt;a href='https://doi.org/10.1038/s41597-020-0433-7'&gt;https://doi.org/10.1038/s41597-020-0433-7&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="156" spans="1:19" ht="129.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="9" t="s">
         <v>117</v>
       </c>
@@ -12356,7 +12355,7 @@
         <v>"population_affected_percentage": {"EGY": {"heavy-rain": "Percentage of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."},</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="9" t="s">
         <v>117</v>
       </c>
@@ -12422,7 +12421,7 @@
         <v>"ETH": {"drought": "Percentage of people exposed is calculated by the population living in within the districts currently triggered. The number of people was derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="9" t="s">
         <v>117</v>
       </c>
@@ -12486,7 +12485,7 @@
         <v>"floods": "Percentage of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="159" spans="1:19" ht="244.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:19" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="9" t="s">
         <v>117</v>
       </c>
@@ -12642,7 +12641,7 @@
 &lt;/ul&gt;"},</v>
       </c>
     </row>
-    <row r="161" spans="1:19" ht="216" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:19" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="9" t="s">
         <v>117</v>
       </c>
@@ -12710,7 +12709,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Source (Population Data): High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Source Flood Extent: The flood extent maps are generated by the National Operational Assesment of Hazards(NOAH) project.&lt;a href='https://noah.up.edu.ph/'&gt;https://noah.up.edu.ph/&lt;/a&gt; The 25-year rain return flood hazard maps show low, medium, and high flood hazards represented as yellow, orange, and red respectively. Flood hazards consider take both the height and velocity of the water into consideration and calculates the hazard levels based on the danger they pose to people and structures. Generally, for an average Filipino with a height of 5’ 6”, areas with flood depths from the knee down can be considered to have low hazard levels. Those with flood depths ranging from the knee to neck are considered to have medium hazard levels, and those covered with floods that are higher than the neck have high hazard levels. However, since the flow velocity is also considered, areas that have shallow but fast-flowing flood waters may have a higher hazard level than that denoted by the height of the flood covering it.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="172.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:19" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="9" t="s">
         <v>117</v>
       </c>
@@ -12784,7 +12783,7 @@
 &lt;/ul&gt;"},</v>
       </c>
     </row>
-    <row r="163" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="9" t="s">
         <v>117</v>
       </c>
@@ -12850,7 +12849,7 @@
         <v>"UGA": {"floods": "Percentage of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="115.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="9" t="s">
         <v>117</v>
       </c>
@@ -12914,7 +12913,7 @@
         <v>"ZMB": {"floods": "Percentage of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."}},</v>
       </c>
     </row>
-    <row r="165" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="9" t="s">
         <v>117</v>
       </c>
@@ -12980,7 +12979,7 @@
         <v>"population_over65": {"PHL": {"dengue": "Percentage of people over 65 years of age. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="9" t="s">
         <v>117</v>
       </c>
@@ -13046,7 +13045,7 @@
         <v>"UGA": {"floods": "Percentage of people over 65 years old.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."}},</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="9" t="s">
         <v>117</v>
       </c>
@@ -13112,7 +13111,7 @@
         <v>"population_u5": {"ETH": {"drought": "Under age: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="9" t="s">
         <v>117</v>
       </c>
@@ -13178,7 +13177,7 @@
         <v>"floods": "Under age: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="169" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="9" t="s">
         <v>117</v>
       </c>
@@ -13242,7 +13241,7 @@
         <v>"malaria": "Under age: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="9" t="s">
         <v>117</v>
       </c>
@@ -13308,7 +13307,7 @@
         <v>"population_u8": {"UGA": {"floods": "Percentage of people under 8 years old.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."}},</v>
       </c>
     </row>
-    <row r="171" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="9" t="s">
         <v>117</v>
       </c>
@@ -13374,7 +13373,7 @@
         <v>"population_u9": {"PHL": {"dengue": "Percentage of people under 9 years of age. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="172" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="9" t="s">
         <v>117</v>
       </c>
@@ -13438,7 +13437,7 @@
         <v>"populationTotal": {"EGY": {"heavy-rain": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="173" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="9" t="s">
         <v>117</v>
       </c>
@@ -13504,7 +13503,7 @@
         <v>"ETH": {"drought": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="174" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="9" t="s">
         <v>117</v>
       </c>
@@ -13568,7 +13567,7 @@
         <v>"floods": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="175" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="9" t="s">
         <v>117</v>
       </c>
@@ -13632,7 +13631,7 @@
         <v>"malaria": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="176" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="9" t="s">
         <v>117</v>
       </c>
@@ -13704,7 +13703,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="177" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="9" t="s">
         <v>117</v>
       </c>
@@ -13844,7 +13843,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; peanutButter: An R package to produce rapid-response gridded population estimates from building footprints, version 1.0.0 version 1.0.0. Accessed 15-08-2022. WorldPop, University of Southampton. 2021. &amp;nbsp;&lt;a href='https://apps.worldpop.org/peanutButter/'&gt;https://apps.worldpop.org/peanutButter/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="179" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="9" t="s">
         <v>117</v>
       </c>
@@ -13912,7 +13911,7 @@
 &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="180" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="9" t="s">
         <v>117</v>
       </c>
@@ -13978,7 +13977,7 @@
 &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="9" t="s">
         <v>117</v>
       </c>
@@ -14046,7 +14045,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="182" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="9" t="s">
         <v>117</v>
       </c>
@@ -14112,7 +14111,7 @@
         <v>"floods": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="183" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="9" t="s">
         <v>117</v>
       </c>
@@ -14176,7 +14175,7 @@
         <v>"ZMB": {"floods": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="184" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="9" t="s">
         <v>117</v>
       </c>
@@ -14246,7 +14245,7 @@
         <v>"ZWE": {"drought": "Population data is aggregated per administrative area, from the following original source: Worldpop data:&lt;ul&gt;&lt;li&gt;&lt;a href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;Estimates of total number of people per grid square broken down by gender and age groupings.&lt;/li&gt;&lt;li&gt;Accessed 07-2020 The mapping approach is Pezzulo, C. et al. Sub-national mapping of population pyramids and dependency ratios in Africa and Asia. Sci. Data 4:170089 doi:10.1038/sdata.2017.89 (2017)&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="185" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="9" t="s">
         <v>117</v>
       </c>
@@ -14312,7 +14311,7 @@
         <v>"potential_cases": {"ETH": {"malaria": "Potential number of cases are calculated with the assumtion of a rough proportionality between malaria mosquito enviromental suitability and malaria risk. Then estimating a time lag between optimal malaria mosquito environmental conditions and the peak in number of malaria cases."},</v>
       </c>
     </row>
-    <row r="186" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="9" t="s">
         <v>117</v>
       </c>
@@ -14378,7 +14377,7 @@
         <v>"PHL": {"dengue": "Number of potential dengue cases, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="187" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="9" t="s">
         <v>117</v>
       </c>
@@ -14444,7 +14443,7 @@
         <v>"potential_cases_65": {"ETH": {"malaria": "Elderly: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="188" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="9" t="s">
         <v>117</v>
       </c>
@@ -14510,7 +14509,7 @@
         <v>"PHL": {"dengue": "Number of potential dengue cases among people above 65 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="189" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="9" t="s">
         <v>117</v>
       </c>
@@ -14576,7 +14575,7 @@
         <v>"potential_cases_U5": {"ETH": {"malaria": "Potential cases under 5. Vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="190" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="9" t="s">
         <v>117</v>
       </c>
@@ -14642,7 +14641,7 @@
         <v>"potential_cases_U9": {"PHL": {"dengue": "Number of potential dengue cases among children under 9 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="191" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="9" t="s">
         <v>117</v>
       </c>
@@ -14708,7 +14707,7 @@
         <v>"poverty_incidence": {"UGA": {"floods": "Poverty Incidence is defined by the Multidiemensional Poverty Index and a $2 a day threshold. The layer gives an estimate of people living in poverty.&lt;br /&gt;&lt;br /&gt;Source: Tatem AJ, Gething PW, Bhatt S, Weiss D and Pezzulo C (2013) Pilot high resolution poverty maps, University of Southampton/Oxford. DOI: 10.5258/SOTON/WP00285. Year: 2010"}},</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="9" t="s">
         <v>117</v>
       </c>
@@ -14774,7 +14773,7 @@
         <v>"prob_within_50km": {"PHL": {"typhoon": "&lt;p&gt;Probability for a Municipality being with in 50km of the forecasted typhoon track. Source for Typhoon forecast is ECMWF&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="193" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="9" t="s">
         <v>117</v>
       </c>
@@ -14840,7 +14839,7 @@
         <v>"rainfall": {"PHL": {"typhoon": "&lt;p&gt;24 Hour Precipitation Total extracted from forecast issued by The Weather Prediction Center (WPC) of National Atmospheric Administration, NOAA.&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="194" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="9" t="s">
         <v>117</v>
       </c>
@@ -14906,7 +14905,7 @@
         <v>"rainfall_extent": {"EGY": {"heavy-rain": "Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."}},</v>
       </c>
     </row>
-    <row r="195" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="9" t="s">
         <v>117</v>
       </c>
@@ -14972,7 +14971,7 @@
         <v>"rainfall_forecast": {"ETH": {"drought": "The rainfall map layer indicates the seasonal forecasting rainfall data for the floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;For the legend see &lt;a href='https://www.icpac.net/seasonal-forecast/'&gt;https://www.icpac.net/seasonal-forecast/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."}},</v>
       </c>
     </row>
-    <row r="196" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="9" t="s">
         <v>117</v>
       </c>
@@ -15036,7 +15035,7 @@
         <v>"red_crescent_branches": {"EGY": {"heavy-rain": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Egyptian Red Crescent Society (ERCS). Year: 2020."}},</v>
       </c>
     </row>
-    <row r="197" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="9" t="s">
         <v>117</v>
       </c>
@@ -15102,7 +15101,7 @@
         <v>"red_cross_branches": {"EGY": {"heavy-rain": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Egyptian Red Crescent Society (ERCS). Year: 2020."},</v>
       </c>
     </row>
-    <row r="198" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="9" t="s">
         <v>117</v>
       </c>
@@ -15168,7 +15167,7 @@
         <v>"ETH": {"drought": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Ethiopia Red Cross Society (ERCS). Year: 2020.",</v>
       </c>
     </row>
-    <row r="199" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="9" t="s">
         <v>117</v>
       </c>
@@ -15234,7 +15233,7 @@
         <v>"floods": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Ethiopia Red Cross Society (ERCS). Year: 2020.",</v>
       </c>
     </row>
-    <row r="200" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="9" t="s">
         <v>117</v>
       </c>
@@ -15298,7 +15297,7 @@
         <v>"malaria": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Ethiopia Red Cross Society (ERCS). Year: 2020."},</v>
       </c>
     </row>
-    <row r="201" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="9" t="s">
         <v>117</v>
       </c>
@@ -15372,7 +15371,7 @@
 &lt;p&gt;&lt;strong&gt;Latest updated:&lt;/strong&gt; 2020.&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="202" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="9" t="s">
         <v>117</v>
       </c>
@@ -15510,7 +15509,7 @@
         <v>"MWI": {"floods": "Data not available yet"},</v>
       </c>
     </row>
-    <row r="204" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="9" t="s">
         <v>117</v>
       </c>
@@ -15576,7 +15575,7 @@
         <v>"PHL": {"dengue": "Data not available yet",</v>
       </c>
     </row>
-    <row r="205" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="9" t="s">
         <v>117</v>
       </c>
@@ -15642,7 +15641,7 @@
         <v>"floods": "Data not available yet"},</v>
       </c>
     </row>
-    <row r="206" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="9" t="s">
         <v>117</v>
       </c>
@@ -15706,7 +15705,7 @@
         <v>"SSD": {"floods": "Data not available yet"},</v>
       </c>
     </row>
-    <row r="207" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="9" t="s">
         <v>117</v>
       </c>
@@ -15772,7 +15771,7 @@
         <v>"UGA": {"drought": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Uganda Red Cross Society (URCS). Year: 2020.",</v>
       </c>
     </row>
-    <row r="208" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="9" t="s">
         <v>117</v>
       </c>
@@ -15838,7 +15837,7 @@
         <v>"floods": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Uganda Red Cross Society (URCS). Year: 2020."},</v>
       </c>
     </row>
-    <row r="209" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="9" t="s">
         <v>117</v>
       </c>
@@ -15904,7 +15903,7 @@
         <v>"ZMB": {"floods": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Zambia Red Cross Society (ZRCS). Year: 2020."},</v>
       </c>
     </row>
-    <row r="210" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="9" t="s">
         <v>117</v>
       </c>
@@ -15974,7 +15973,7 @@
         <v>"ZWE": {"drought": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link Zimbabwe: ZRCS last updated July 2021 at provincial level."}},</v>
       </c>
     </row>
-    <row r="211" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="9" t="s">
         <v>117</v>
       </c>
@@ -16046,7 +16045,7 @@
 &lt;a href='https://prism.philrice.gov.ph/dataproducts/'&gt;https://prism.philrice.gov.ph/dataproducts/&lt;/a&gt; This data is based on the Philippine Rice Information System (PRISM) project which primarily aims to establish a nationwide information system on rice that provide information on rice areas and yield at a particular location and time, and information on factors that are affecting the yield. "}},</v>
       </c>
     </row>
-    <row r="212" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="9" t="s">
         <v>117</v>
       </c>
@@ -16112,7 +16111,7 @@
         <v>"roof_type": {"UGA": {"floods": "Not currently available"}},</v>
       </c>
     </row>
-    <row r="213" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="9" t="s">
         <v>117</v>
       </c>
@@ -16176,7 +16175,7 @@
         <v>"small_ruminants": {"UGA": {"drought": "Not currently available"},</v>
       </c>
     </row>
-    <row r="214" spans="1:19" ht="187.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="9" t="s">
         <v>117</v>
       </c>
@@ -16256,7 +16255,7 @@
 &lt;a href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;."}},</v>
       </c>
     </row>
-    <row r="215" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="9" t="s">
         <v>117</v>
       </c>
@@ -16320,7 +16319,7 @@
         <v>"small_ruminants_exposed": {"UGA": {"drought": "Not currently available"},</v>
       </c>
     </row>
-    <row r="216" spans="1:19" ht="230.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="9" t="s">
         <v>117</v>
       </c>
@@ -16400,7 +16399,7 @@
 &lt;a href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;."}},</v>
       </c>
     </row>
-    <row r="217" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="9" t="s">
         <v>117</v>
       </c>
@@ -16466,7 +16465,7 @@
         <v>"total_houses": {"PHL": {"typhoon": "&lt;p&gt;Total Number of Housing units in each Municipality&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="218" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="9" t="s">
         <v>117</v>
       </c>
@@ -16532,7 +16531,7 @@
         <v>"total_idps": {"ETH": {"drought": "Total Internally Displaced People (IDPs) DTM Ethiopia National Displacement Report 7_2022",</v>
       </c>
     </row>
-    <row r="219" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="9" t="s">
         <v>117</v>
       </c>
@@ -16598,7 +16597,7 @@
         <v>"floods": "Total Internally Displaced People (IDPs) DTM Ethiopia National Displacement Report 7_2022",</v>
       </c>
     </row>
-    <row r="220" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="9" t="s">
         <v>117</v>
       </c>
@@ -16662,7 +16661,7 @@
         <v>"malaria": "Total Internally Displaced People (IDPs) DTM Ethiopia National Displacement Report 7_2022"}},</v>
       </c>
     </row>
-    <row r="221" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="9" t="s">
         <v>117</v>
       </c>
@@ -16728,7 +16727,7 @@
         <v>"travel_time_cities": {"ETH": {"floods": "Predicted travel time (minutes) to nearest city &lt;a href='https://malariaatlas.org/research-project/accessibility-to-healthcare/'&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="222" spans="1:19" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="9" t="s">
         <v>117</v>
       </c>
@@ -16792,7 +16791,7 @@
         <v>"malaria": "Predicted travel time (minutes) to nearest city &lt;a href='https://malariaatlas.org/research-project/accessibility-to-healthcare/'&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="223" spans="1:19" ht="144" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:19" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="9" t="s">
         <v>117</v>
       </c>
@@ -16878,7 +16877,7 @@
 &lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="224" spans="1:19" ht="316.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:19" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" s="9" t="s">
         <v>117</v>
       </c>
@@ -16968,7 +16967,7 @@
 &lt;p&gt;&lt;strong&gt;Latest updated:&lt;/strong&gt; month, year&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="225" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="9" t="s">
         <v>117</v>
       </c>
@@ -17032,7 +17031,7 @@
         <v>"UGA": {"drought": "Not currently available"}},</v>
       </c>
     </row>
-    <row r="226" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="9" t="s">
         <v>117</v>
       </c>
@@ -17106,7 +17105,7 @@
 Ongoing (updated regularly)",</v>
       </c>
     </row>
-    <row r="227" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" s="9" t="s">
         <v>117</v>
       </c>
@@ -17176,7 +17175,7 @@
 DSWD, NATIONAL HOUSEHOLD TARGETING OFFICE&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="228" spans="1:19" ht="100.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="9" t="s">
         <v>117</v>
       </c>
@@ -17250,7 +17249,7 @@
 Ongoing (updated regularly)",</v>
       </c>
     </row>
-    <row r="229" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" s="9" t="s">
         <v>117</v>
       </c>
@@ -17316,7 +17315,7 @@
         <v>"typhoon": "&lt;a href='https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard'&gt;https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard&lt;/a&gt; This dataset has been generated by combining PSGC and 4Ps data from DSWD."}},</v>
       </c>
     </row>
-    <row r="230" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" s="9" t="s">
         <v>117</v>
       </c>
@@ -17382,7 +17381,7 @@
         <v>"walking_travel_time_to_health": {"ETH": {"malaria": "Ongoing (updated regularly)"}},</v>
       </c>
     </row>
-    <row r="231" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="9" t="s">
         <v>117</v>
       </c>
@@ -17448,7 +17447,7 @@
         <v>"wall_type": {"UGA": {"floods": "Percentage of households with permanent wall materials; percentage of buildings with (partly) concrete or brick walls.&lt;br /&gt;&lt;br /&gt;Source link: &lt;a href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."}},</v>
       </c>
     </row>
-    <row r="232" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" s="9" t="s">
         <v>117</v>
       </c>
@@ -17512,7 +17511,7 @@
         <v>"waterpoints": {"ETH": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="233" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="9" t="s">
         <v>117</v>
       </c>
@@ -17576,7 +17575,7 @@
         <v>"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="234" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="9" t="s">
         <v>117</v>
       </c>
@@ -17646,7 +17645,7 @@
         <v>"KEN": {"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="235" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" s="9" t="s">
         <v>117</v>
       </c>
@@ -17782,7 +17781,7 @@
         <v>"MWI": {"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="237" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="9" t="s">
         <v>117</v>
       </c>
@@ -17848,7 +17847,7 @@
         <v>"UGA": {"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="238" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="9" t="s">
         <v>117</v>
       </c>
@@ -17914,7 +17913,7 @@
         <v>"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="239" spans="1:19" ht="57.6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="9" t="s">
         <v>117</v>
       </c>
@@ -17978,7 +17977,7 @@
         <v>"ZMB": {"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="240" spans="1:19" ht="86.4" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="9" t="s">
         <v>117</v>
       </c>
@@ -18048,7 +18047,7 @@
         <v>"ZWE": {"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="241" spans="1:19" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="9" t="s">
         <v>117</v>
       </c>
@@ -18114,7 +18113,7 @@
         <v>"windspeed": {"PHL": {"typhoon": "&lt;p&gt;Forecasted 1 minute average maximum wind speed in kilometers per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;"}}}}</v>
       </c>
     </row>
-    <row r="242" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="9"/>
       <c r="B242" s="9"/>
       <c r="C242" s="9"/>
@@ -18168,7 +18167,7 @@
         <v/>
       </c>
     </row>
-    <row r="243" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="9"/>
       <c r="B243" s="9"/>
       <c r="C243" s="9"/>
@@ -18222,7 +18221,7 @@
         <v/>
       </c>
     </row>
-    <row r="244" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="9"/>
       <c r="B244" s="9"/>
       <c r="C244" s="9"/>
@@ -18276,7 +18275,7 @@
         <v/>
       </c>
     </row>
-    <row r="245" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="9"/>
       <c r="B245" s="9"/>
       <c r="C245" s="9"/>
@@ -18330,7 +18329,7 @@
         <v/>
       </c>
     </row>
-    <row r="246" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="9"/>
       <c r="B246" s="9"/>
       <c r="C246" s="9"/>
@@ -18384,7 +18383,7 @@
         <v/>
       </c>
     </row>
-    <row r="247" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="9"/>
       <c r="B247" s="9"/>
       <c r="C247" s="9"/>
@@ -18438,7 +18437,7 @@
         <v/>
       </c>
     </row>
-    <row r="248" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" s="9"/>
       <c r="B248" s="9"/>
       <c r="C248" s="9"/>
@@ -18492,7 +18491,7 @@
         <v/>
       </c>
     </row>
-    <row r="249" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" s="9"/>
       <c r="B249" s="9"/>
       <c r="C249" s="9"/>
@@ -18546,7 +18545,7 @@
         <v/>
       </c>
     </row>
-    <row r="250" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" s="9"/>
       <c r="B250" s="9"/>
       <c r="C250" s="9"/>
@@ -18600,7 +18599,7 @@
         <v/>
       </c>
     </row>
-    <row r="251" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" s="9"/>
       <c r="B251" s="9"/>
       <c r="C251" s="9"/>
@@ -18654,7 +18653,7 @@
         <v/>
       </c>
     </row>
-    <row r="252" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" s="9"/>
       <c r="B252" s="9"/>
       <c r="C252" s="9"/>
@@ -18708,7 +18707,7 @@
         <v/>
       </c>
     </row>
-    <row r="253" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="9"/>
       <c r="B253" s="9"/>
       <c r="C253" s="9"/>
@@ -18762,7 +18761,7 @@
         <v/>
       </c>
     </row>
-    <row r="254" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" s="9"/>
       <c r="B254" s="9"/>
       <c r="C254" s="9"/>
@@ -18816,7 +18815,7 @@
         <v/>
       </c>
     </row>
-    <row r="255" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" s="9"/>
       <c r="B255" s="9"/>
       <c r="C255" s="9"/>
@@ -18870,7 +18869,7 @@
         <v/>
       </c>
     </row>
-    <row r="256" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" s="9"/>
       <c r="B256" s="9"/>
       <c r="C256" s="9"/>
@@ -18924,7 +18923,7 @@
         <v/>
       </c>
     </row>
-    <row r="257" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" s="9"/>
       <c r="B257" s="9"/>
       <c r="C257" s="9"/>
@@ -18978,7 +18977,7 @@
         <v/>
       </c>
     </row>
-    <row r="258" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" s="9"/>
       <c r="B258" s="9"/>
       <c r="C258" s="9"/>
@@ -19032,7 +19031,7 @@
         <v/>
       </c>
     </row>
-    <row r="259" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="9"/>
       <c r="B259" s="9"/>
       <c r="C259" s="9"/>
@@ -19086,7 +19085,7 @@
         <v/>
       </c>
     </row>
-    <row r="260" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" s="9"/>
       <c r="B260" s="9"/>
       <c r="C260" s="9"/>
@@ -19140,7 +19139,7 @@
         <v/>
       </c>
     </row>
-    <row r="261" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="9"/>
       <c r="B261" s="9"/>
       <c r="C261" s="9"/>
@@ -19194,7 +19193,7 @@
         <v/>
       </c>
     </row>
-    <row r="262" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A262" s="9"/>
       <c r="B262" s="9"/>
       <c r="C262" s="9"/>
@@ -19248,7 +19247,7 @@
         <v/>
       </c>
     </row>
-    <row r="263" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" s="9"/>
       <c r="B263" s="9"/>
       <c r="C263" s="9"/>
@@ -19302,7 +19301,7 @@
         <v/>
       </c>
     </row>
-    <row r="264" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" s="9"/>
       <c r="B264" s="9"/>
       <c r="C264" s="9"/>
@@ -19356,7 +19355,7 @@
         <v/>
       </c>
     </row>
-    <row r="265" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" s="9"/>
       <c r="B265" s="9"/>
       <c r="C265" s="9"/>
@@ -19410,7 +19409,7 @@
         <v/>
       </c>
     </row>
-    <row r="266" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" s="9"/>
       <c r="B266" s="9"/>
       <c r="C266" s="9"/>
@@ -19464,7 +19463,7 @@
         <v/>
       </c>
     </row>
-    <row r="267" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" s="9"/>
       <c r="B267" s="9"/>
       <c r="C267" s="9"/>
@@ -19518,7 +19517,7 @@
         <v/>
       </c>
     </row>
-    <row r="268" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" s="9"/>
       <c r="B268" s="9"/>
       <c r="C268" s="9"/>
@@ -19572,7 +19571,7 @@
         <v/>
       </c>
     </row>
-    <row r="269" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" s="9"/>
       <c r="B269" s="9"/>
       <c r="C269" s="9"/>
@@ -19626,7 +19625,7 @@
         <v/>
       </c>
     </row>
-    <row r="270" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" s="9"/>
       <c r="B270" s="9"/>
       <c r="C270" s="9"/>
@@ -19680,7 +19679,7 @@
         <v/>
       </c>
     </row>
-    <row r="271" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" s="9"/>
       <c r="B271" s="9"/>
       <c r="C271" s="9"/>
@@ -19734,7 +19733,7 @@
         <v/>
       </c>
     </row>
-    <row r="272" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" s="9"/>
       <c r="B272" s="9"/>
       <c r="C272" s="9"/>
@@ -19788,7 +19787,7 @@
         <v/>
       </c>
     </row>
-    <row r="273" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A273" s="9"/>
       <c r="B273" s="9"/>
       <c r="C273" s="9"/>
@@ -19842,7 +19841,7 @@
         <v/>
       </c>
     </row>
-    <row r="274" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" s="9"/>
       <c r="B274" s="9"/>
       <c r="C274" s="9"/>
@@ -19896,7 +19895,7 @@
         <v/>
       </c>
     </row>
-    <row r="275" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A275" s="9"/>
       <c r="B275" s="9"/>
       <c r="C275" s="9"/>
@@ -19950,7 +19949,7 @@
         <v/>
       </c>
     </row>
-    <row r="276" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" s="9"/>
       <c r="B276" s="9"/>
       <c r="C276" s="9"/>
@@ -20004,7 +20003,7 @@
         <v/>
       </c>
     </row>
-    <row r="277" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" s="9"/>
       <c r="B277" s="9"/>
       <c r="C277" s="9"/>
@@ -20058,7 +20057,7 @@
         <v/>
       </c>
     </row>
-    <row r="278" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" s="9"/>
       <c r="B278" s="9"/>
       <c r="C278" s="9"/>
@@ -20112,7 +20111,7 @@
         <v/>
       </c>
     </row>
-    <row r="279" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" s="9"/>
       <c r="B279" s="9"/>
       <c r="C279" s="9"/>
@@ -20166,7 +20165,7 @@
         <v/>
       </c>
     </row>
-    <row r="280" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" s="9"/>
       <c r="B280" s="9"/>
       <c r="C280" s="9"/>
@@ -20220,7 +20219,7 @@
         <v/>
       </c>
     </row>
-    <row r="281" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" s="9"/>
       <c r="B281" s="9"/>
       <c r="C281" s="9"/>
@@ -20274,7 +20273,7 @@
         <v/>
       </c>
     </row>
-    <row r="282" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" s="9"/>
       <c r="B282" s="9"/>
       <c r="C282" s="9"/>
@@ -20328,7 +20327,7 @@
         <v/>
       </c>
     </row>
-    <row r="283" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" s="9"/>
       <c r="B283" s="9"/>
       <c r="C283" s="9"/>
@@ -20382,7 +20381,7 @@
         <v/>
       </c>
     </row>
-    <row r="284" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" s="9"/>
       <c r="B284" s="9"/>
       <c r="C284" s="9"/>
@@ -20436,7 +20435,7 @@
         <v/>
       </c>
     </row>
-    <row r="285" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" s="9"/>
       <c r="B285" s="9"/>
       <c r="C285" s="9"/>
@@ -20490,7 +20489,7 @@
         <v/>
       </c>
     </row>
-    <row r="286" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" s="9"/>
       <c r="B286" s="9"/>
       <c r="C286" s="9"/>
@@ -20544,7 +20543,7 @@
         <v/>
       </c>
     </row>
-    <row r="287" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" s="9"/>
       <c r="B287" s="9"/>
       <c r="C287" s="9"/>
@@ -20598,7 +20597,7 @@
         <v/>
       </c>
     </row>
-    <row r="288" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" s="9"/>
       <c r="B288" s="9"/>
       <c r="C288" s="9"/>
@@ -20652,7 +20651,7 @@
         <v/>
       </c>
     </row>
-    <row r="289" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" s="9"/>
       <c r="B289" s="9"/>
       <c r="C289" s="9"/>
@@ -20706,7 +20705,7 @@
         <v/>
       </c>
     </row>
-    <row r="290" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A290" s="9"/>
       <c r="B290" s="9"/>
       <c r="C290" s="9"/>
@@ -20760,7 +20759,7 @@
         <v/>
       </c>
     </row>
-    <row r="291" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" s="9"/>
       <c r="B291" s="9"/>
       <c r="C291" s="9"/>
@@ -20814,7 +20813,7 @@
         <v/>
       </c>
     </row>
-    <row r="292" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" s="9"/>
       <c r="B292" s="9"/>
       <c r="C292" s="9"/>
@@ -20868,7 +20867,7 @@
         <v/>
       </c>
     </row>
-    <row r="293" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="293" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" s="9"/>
       <c r="B293" s="9"/>
       <c r="C293" s="9"/>
@@ -20922,7 +20921,7 @@
         <v/>
       </c>
     </row>
-    <row r="294" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" s="9"/>
       <c r="B294" s="9"/>
       <c r="C294" s="9"/>
@@ -20976,7 +20975,7 @@
         <v/>
       </c>
     </row>
-    <row r="295" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" s="9"/>
       <c r="B295" s="9"/>
       <c r="C295" s="9"/>
@@ -21030,7 +21029,7 @@
         <v/>
       </c>
     </row>
-    <row r="296" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="296" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" s="9"/>
       <c r="B296" s="9"/>
       <c r="C296" s="9"/>
@@ -21084,7 +21083,7 @@
         <v/>
       </c>
     </row>
-    <row r="297" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="297" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" s="9"/>
       <c r="B297" s="9"/>
       <c r="C297" s="9"/>
@@ -21138,7 +21137,7 @@
         <v/>
       </c>
     </row>
-    <row r="298" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="298" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" s="9"/>
       <c r="B298" s="9"/>
       <c r="C298" s="9"/>
@@ -21192,7 +21191,7 @@
         <v/>
       </c>
     </row>
-    <row r="299" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="299" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" s="9"/>
       <c r="B299" s="9"/>
       <c r="C299" s="9"/>
@@ -21246,7 +21245,7 @@
         <v/>
       </c>
     </row>
-    <row r="300" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="300" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" s="9"/>
       <c r="B300" s="9"/>
       <c r="C300" s="9"/>
@@ -21300,7 +21299,7 @@
         <v/>
       </c>
     </row>
-    <row r="301" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" s="9"/>
       <c r="B301" s="9"/>
       <c r="C301" s="9"/>
@@ -21354,7 +21353,7 @@
         <v/>
       </c>
     </row>
-    <row r="302" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" s="9"/>
       <c r="B302" s="9"/>
       <c r="C302" s="9"/>
@@ -21408,7 +21407,7 @@
         <v/>
       </c>
     </row>
-    <row r="303" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" s="9"/>
       <c r="B303" s="9"/>
       <c r="C303" s="9"/>
@@ -21462,7 +21461,7 @@
         <v/>
       </c>
     </row>
-    <row r="304" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" s="9"/>
       <c r="B304" s="9"/>
       <c r="C304" s="9"/>
@@ -21516,7 +21515,7 @@
         <v/>
       </c>
     </row>
-    <row r="305" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" s="9"/>
       <c r="B305" s="9"/>
       <c r="C305" s="9"/>
@@ -21570,7 +21569,7 @@
         <v/>
       </c>
     </row>
-    <row r="306" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" s="9"/>
       <c r="B306" s="9"/>
       <c r="C306" s="9"/>
@@ -21624,7 +21623,7 @@
         <v/>
       </c>
     </row>
-    <row r="307" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" s="9"/>
       <c r="B307" s="9"/>
       <c r="C307" s="9"/>
@@ -21678,7 +21677,7 @@
         <v/>
       </c>
     </row>
-    <row r="308" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" s="9"/>
       <c r="B308" s="9"/>
       <c r="C308" s="9"/>
@@ -21732,7 +21731,7 @@
         <v/>
       </c>
     </row>
-    <row r="309" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A309" s="9"/>
       <c r="B309" s="9"/>
       <c r="C309" s="9"/>
@@ -21786,7 +21785,7 @@
         <v/>
       </c>
     </row>
-    <row r="310" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" s="9"/>
       <c r="B310" s="9"/>
       <c r="C310" s="9"/>
@@ -21840,7 +21839,7 @@
         <v/>
       </c>
     </row>
-    <row r="311" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="311" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A311" s="9"/>
       <c r="B311" s="9"/>
       <c r="C311" s="9"/>
@@ -21894,7 +21893,7 @@
         <v/>
       </c>
     </row>
-    <row r="312" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="312" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A312" s="9"/>
       <c r="B312" s="9"/>
       <c r="C312" s="9"/>
@@ -21948,7 +21947,7 @@
         <v/>
       </c>
     </row>
-    <row r="313" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" s="9"/>
       <c r="B313" s="9"/>
       <c r="C313" s="9"/>
@@ -22002,7 +22001,7 @@
         <v/>
       </c>
     </row>
-    <row r="314" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" s="9"/>
       <c r="B314" s="9"/>
       <c r="C314" s="9"/>
@@ -22056,7 +22055,7 @@
         <v/>
       </c>
     </row>
-    <row r="315" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="315" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A315" s="9"/>
       <c r="B315" s="9"/>
       <c r="C315" s="9"/>
@@ -22110,7 +22109,7 @@
         <v/>
       </c>
     </row>
-    <row r="316" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="316" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A316" s="9"/>
       <c r="B316" s="9"/>
       <c r="C316" s="9"/>
@@ -22164,7 +22163,7 @@
         <v/>
       </c>
     </row>
-    <row r="317" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="317" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A317" s="9"/>
       <c r="B317" s="9"/>
       <c r="C317" s="9"/>
@@ -22218,7 +22217,7 @@
         <v/>
       </c>
     </row>
-    <row r="318" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="318" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A318" s="9"/>
       <c r="B318" s="9"/>
       <c r="C318" s="9"/>
@@ -22272,7 +22271,7 @@
         <v/>
       </c>
     </row>
-    <row r="319" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" s="9"/>
       <c r="B319" s="9"/>
       <c r="C319" s="9"/>
@@ -22326,7 +22325,7 @@
         <v/>
       </c>
     </row>
-    <row r="320" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="320" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" s="9"/>
       <c r="B320" s="9"/>
       <c r="C320" s="9"/>
@@ -22380,7 +22379,7 @@
         <v/>
       </c>
     </row>
-    <row r="321" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="321" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A321" s="9"/>
       <c r="B321" s="9"/>
       <c r="C321" s="9"/>
@@ -22434,7 +22433,7 @@
         <v/>
       </c>
     </row>
-    <row r="322" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="322" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A322" s="9"/>
       <c r="B322" s="9"/>
       <c r="C322" s="9"/>
@@ -22488,7 +22487,7 @@
         <v/>
       </c>
     </row>
-    <row r="323" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="323" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" s="9"/>
       <c r="B323" s="9"/>
       <c r="C323" s="9"/>
@@ -22542,7 +22541,7 @@
         <v/>
       </c>
     </row>
-    <row r="324" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="324" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" s="9"/>
       <c r="B324" s="9"/>
       <c r="C324" s="9"/>
@@ -22596,7 +22595,7 @@
         <v/>
       </c>
     </row>
-    <row r="325" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="325" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" s="9"/>
       <c r="B325" s="9"/>
       <c r="C325" s="9"/>
@@ -22650,7 +22649,7 @@
         <v/>
       </c>
     </row>
-    <row r="326" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="326" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A326" s="9"/>
       <c r="B326" s="9"/>
       <c r="C326" s="9"/>
@@ -22704,7 +22703,7 @@
         <v/>
       </c>
     </row>
-    <row r="327" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="327" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A327" s="9"/>
       <c r="B327" s="9"/>
       <c r="C327" s="9"/>
@@ -22758,7 +22757,7 @@
         <v/>
       </c>
     </row>
-    <row r="328" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="328" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" s="9"/>
       <c r="B328" s="9"/>
       <c r="C328" s="9"/>
@@ -22812,7 +22811,7 @@
         <v/>
       </c>
     </row>
-    <row r="329" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="329" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" s="9"/>
       <c r="B329" s="9"/>
       <c r="C329" s="9"/>
@@ -22866,7 +22865,7 @@
         <v/>
       </c>
     </row>
-    <row r="330" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="330" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" s="9"/>
       <c r="B330" s="9"/>
       <c r="C330" s="9"/>
@@ -22920,7 +22919,7 @@
         <v/>
       </c>
     </row>
-    <row r="331" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="331" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" s="9"/>
       <c r="B331" s="9"/>
       <c r="C331" s="9"/>
@@ -22974,7 +22973,7 @@
         <v/>
       </c>
     </row>
-    <row r="332" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="332" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" s="9"/>
       <c r="B332" s="9"/>
       <c r="C332" s="9"/>
@@ -23028,7 +23027,7 @@
         <v/>
       </c>
     </row>
-    <row r="333" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="333" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" s="9"/>
       <c r="B333" s="9"/>
       <c r="C333" s="9"/>
@@ -23082,7 +23081,7 @@
         <v/>
       </c>
     </row>
-    <row r="334" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="334" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A334" s="9"/>
       <c r="B334" s="9"/>
       <c r="C334" s="9"/>
@@ -23136,7 +23135,7 @@
         <v/>
       </c>
     </row>
-    <row r="335" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="335" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A335" s="9"/>
       <c r="B335" s="9"/>
       <c r="C335" s="9"/>
@@ -23190,7 +23189,7 @@
         <v/>
       </c>
     </row>
-    <row r="336" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="336" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" s="9"/>
       <c r="B336" s="9"/>
       <c r="C336" s="9"/>
@@ -23244,7 +23243,7 @@
         <v/>
       </c>
     </row>
-    <row r="337" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="337" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A337" s="9"/>
       <c r="B337" s="9"/>
       <c r="C337" s="9"/>
@@ -23298,7 +23297,7 @@
         <v/>
       </c>
     </row>
-    <row r="338" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="338" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A338" s="9"/>
       <c r="B338" s="9"/>
       <c r="C338" s="9"/>
@@ -23352,7 +23351,7 @@
         <v/>
       </c>
     </row>
-    <row r="339" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="339" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A339" s="9"/>
       <c r="B339" s="9"/>
       <c r="C339" s="9"/>
@@ -23406,7 +23405,7 @@
         <v/>
       </c>
     </row>
-    <row r="340" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="340" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" s="9"/>
       <c r="B340" s="9"/>
       <c r="C340" s="9"/>
@@ -23460,7 +23459,7 @@
         <v/>
       </c>
     </row>
-    <row r="341" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="341" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A341" s="9"/>
       <c r="B341" s="9"/>
       <c r="C341" s="9"/>
@@ -23514,7 +23513,7 @@
         <v/>
       </c>
     </row>
-    <row r="342" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="342" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" s="9"/>
       <c r="B342" s="9"/>
       <c r="C342" s="9"/>
@@ -23568,7 +23567,7 @@
         <v/>
       </c>
     </row>
-    <row r="343" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="343" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A343" s="9"/>
       <c r="B343" s="9"/>
       <c r="C343" s="9"/>
@@ -23622,7 +23621,7 @@
         <v/>
       </c>
     </row>
-    <row r="344" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="344" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A344" s="9"/>
       <c r="B344" s="9"/>
       <c r="C344" s="9"/>
@@ -23676,7 +23675,7 @@
         <v/>
       </c>
     </row>
-    <row r="345" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="345" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A345" s="9"/>
       <c r="B345" s="9"/>
       <c r="C345" s="9"/>
@@ -23730,7 +23729,7 @@
         <v/>
       </c>
     </row>
-    <row r="346" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="346" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A346" s="9"/>
       <c r="B346" s="9"/>
       <c r="C346" s="9"/>
@@ -23784,7 +23783,7 @@
         <v/>
       </c>
     </row>
-    <row r="347" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="347" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A347" s="9"/>
       <c r="B347" s="9"/>
       <c r="C347" s="9"/>
@@ -23838,7 +23837,7 @@
         <v/>
       </c>
     </row>
-    <row r="348" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="348" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A348" s="9"/>
       <c r="B348" s="9"/>
       <c r="C348" s="9"/>
@@ -23892,7 +23891,7 @@
         <v/>
       </c>
     </row>
-    <row r="349" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="349" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A349" s="9"/>
       <c r="B349" s="9"/>
       <c r="C349" s="9"/>
@@ -23946,7 +23945,7 @@
         <v/>
       </c>
     </row>
-    <row r="350" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="350" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A350" s="9"/>
       <c r="B350" s="9"/>
       <c r="C350" s="9"/>
@@ -24000,7 +23999,7 @@
         <v/>
       </c>
     </row>
-    <row r="351" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="351" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A351" s="9"/>
       <c r="B351" s="9"/>
       <c r="C351" s="9"/>
@@ -24054,7 +24053,7 @@
         <v/>
       </c>
     </row>
-    <row r="352" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="352" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A352" s="9"/>
       <c r="B352" s="9"/>
       <c r="C352" s="9"/>
@@ -24108,7 +24107,7 @@
         <v/>
       </c>
     </row>
-    <row r="353" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="353" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A353" s="9"/>
       <c r="B353" s="9"/>
       <c r="C353" s="9"/>
@@ -24162,7 +24161,7 @@
         <v/>
       </c>
     </row>
-    <row r="354" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="354" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A354" s="9"/>
       <c r="B354" s="9"/>
       <c r="C354" s="9"/>
@@ -24216,7 +24215,7 @@
         <v/>
       </c>
     </row>
-    <row r="355" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="355" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A355" s="9"/>
       <c r="B355" s="9"/>
       <c r="C355" s="9"/>
@@ -24270,7 +24269,7 @@
         <v/>
       </c>
     </row>
-    <row r="356" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="356" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A356" s="9"/>
       <c r="B356" s="9"/>
       <c r="C356" s="9"/>
@@ -24324,7 +24323,7 @@
         <v/>
       </c>
     </row>
-    <row r="357" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="357" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A357" s="9"/>
       <c r="B357" s="9"/>
       <c r="C357" s="9"/>
@@ -24378,7 +24377,7 @@
         <v/>
       </c>
     </row>
-    <row r="358" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="358" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A358" s="9"/>
       <c r="B358" s="9"/>
       <c r="C358" s="9"/>
@@ -24432,7 +24431,7 @@
         <v/>
       </c>
     </row>
-    <row r="359" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="359" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A359" s="9"/>
       <c r="B359" s="9"/>
       <c r="C359" s="9"/>
@@ -24486,7 +24485,7 @@
         <v/>
       </c>
     </row>
-    <row r="360" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="360" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A360" s="9"/>
       <c r="B360" s="9"/>
       <c r="C360" s="9"/>
@@ -24540,7 +24539,7 @@
         <v/>
       </c>
     </row>
-    <row r="361" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="361" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A361" s="9"/>
       <c r="B361" s="9"/>
       <c r="C361" s="9"/>
@@ -24594,7 +24593,7 @@
         <v/>
       </c>
     </row>
-    <row r="362" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="362" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A362" s="9"/>
       <c r="B362" s="9"/>
       <c r="C362" s="9"/>
@@ -24648,7 +24647,7 @@
         <v/>
       </c>
     </row>
-    <row r="363" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="363" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A363" s="9"/>
       <c r="B363" s="9"/>
       <c r="C363" s="9"/>
@@ -24702,7 +24701,7 @@
         <v/>
       </c>
     </row>
-    <row r="364" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="364" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A364" s="9"/>
       <c r="B364" s="9"/>
       <c r="C364" s="9"/>
@@ -24756,7 +24755,7 @@
         <v/>
       </c>
     </row>
-    <row r="365" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="365" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A365" s="9"/>
       <c r="B365" s="9"/>
       <c r="C365" s="9"/>
@@ -24810,7 +24809,7 @@
         <v/>
       </c>
     </row>
-    <row r="366" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="366" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A366" s="9"/>
       <c r="B366" s="9"/>
       <c r="C366" s="9"/>
@@ -24864,7 +24863,7 @@
         <v/>
       </c>
     </row>
-    <row r="367" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="367" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A367" s="9"/>
       <c r="B367" s="9"/>
       <c r="C367" s="9"/>
@@ -24918,7 +24917,7 @@
         <v/>
       </c>
     </row>
-    <row r="368" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="368" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A368" s="9"/>
       <c r="B368" s="9"/>
       <c r="C368" s="9"/>
@@ -24972,7 +24971,7 @@
         <v/>
       </c>
     </row>
-    <row r="369" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="369" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A369" s="9"/>
       <c r="B369" s="9"/>
       <c r="C369" s="9"/>
@@ -25026,7 +25025,7 @@
         <v/>
       </c>
     </row>
-    <row r="370" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="370" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A370" s="9"/>
       <c r="B370" s="9"/>
       <c r="C370" s="9"/>
@@ -25080,7 +25079,7 @@
         <v/>
       </c>
     </row>
-    <row r="371" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="371" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A371" s="9"/>
       <c r="B371" s="9"/>
       <c r="C371" s="9"/>
@@ -25134,7 +25133,7 @@
         <v/>
       </c>
     </row>
-    <row r="372" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="372" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A372" s="9"/>
       <c r="B372" s="9"/>
       <c r="C372" s="9"/>
@@ -25188,7 +25187,7 @@
         <v/>
       </c>
     </row>
-    <row r="373" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="373" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A373" s="9"/>
       <c r="B373" s="9"/>
       <c r="C373" s="9"/>
@@ -25242,7 +25241,7 @@
         <v/>
       </c>
     </row>
-    <row r="374" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="374" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A374" s="9"/>
       <c r="B374" s="9"/>
       <c r="C374" s="9"/>
@@ -25296,7 +25295,7 @@
         <v/>
       </c>
     </row>
-    <row r="375" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="375" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A375" s="9"/>
       <c r="B375" s="9"/>
       <c r="C375" s="9"/>
@@ -25350,7 +25349,7 @@
         <v/>
       </c>
     </row>
-    <row r="376" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="376" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A376" s="9"/>
       <c r="B376" s="9"/>
       <c r="C376" s="9"/>
@@ -25404,7 +25403,7 @@
         <v/>
       </c>
     </row>
-    <row r="377" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="377" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A377" s="9"/>
       <c r="B377" s="9"/>
       <c r="C377" s="9"/>
@@ -25458,7 +25457,7 @@
         <v/>
       </c>
     </row>
-    <row r="378" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="378" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A378" s="9"/>
       <c r="B378" s="9"/>
       <c r="C378" s="9"/>
@@ -25512,7 +25511,7 @@
         <v/>
       </c>
     </row>
-    <row r="379" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="379" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A379" s="9"/>
       <c r="B379" s="9"/>
       <c r="C379" s="9"/>
@@ -25566,7 +25565,7 @@
         <v/>
       </c>
     </row>
-    <row r="380" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="380" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A380" s="9"/>
       <c r="B380" s="9"/>
       <c r="C380" s="9"/>
@@ -25620,7 +25619,7 @@
         <v/>
       </c>
     </row>
-    <row r="381" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="381" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A381" s="9"/>
       <c r="B381" s="9"/>
       <c r="C381" s="9"/>
@@ -25674,7 +25673,7 @@
         <v/>
       </c>
     </row>
-    <row r="382" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="382" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A382" s="9"/>
       <c r="B382" s="9"/>
       <c r="C382" s="9"/>
@@ -25728,7 +25727,7 @@
         <v/>
       </c>
     </row>
-    <row r="383" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="383" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A383" s="9"/>
       <c r="B383" s="9"/>
       <c r="C383" s="9"/>
@@ -25782,7 +25781,7 @@
         <v/>
       </c>
     </row>
-    <row r="384" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="384" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A384" s="9"/>
       <c r="B384" s="9"/>
       <c r="C384" s="9"/>
@@ -25836,7 +25835,7 @@
         <v/>
       </c>
     </row>
-    <row r="385" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="385" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A385" s="9"/>
       <c r="B385" s="9"/>
       <c r="C385" s="9"/>
@@ -25890,7 +25889,7 @@
         <v/>
       </c>
     </row>
-    <row r="386" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="386" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A386" s="9"/>
       <c r="B386" s="9"/>
       <c r="C386" s="9"/>
@@ -25944,7 +25943,7 @@
         <v/>
       </c>
     </row>
-    <row r="387" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="387" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A387" s="9"/>
       <c r="B387" s="9"/>
       <c r="C387" s="9"/>
@@ -25998,7 +25997,7 @@
         <v/>
       </c>
     </row>
-    <row r="388" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="388" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A388" s="9"/>
       <c r="B388" s="9"/>
       <c r="C388" s="9"/>
@@ -26052,7 +26051,7 @@
         <v/>
       </c>
     </row>
-    <row r="389" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="389" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A389" s="9"/>
       <c r="B389" s="9"/>
       <c r="C389" s="9"/>
@@ -26106,7 +26105,7 @@
         <v/>
       </c>
     </row>
-    <row r="390" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="390" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A390" s="9"/>
       <c r="B390" s="9"/>
       <c r="C390" s="9"/>
@@ -26160,7 +26159,7 @@
         <v/>
       </c>
     </row>
-    <row r="391" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="391" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A391" s="9"/>
       <c r="B391" s="9"/>
       <c r="C391" s="9"/>
@@ -26214,7 +26213,7 @@
         <v/>
       </c>
     </row>
-    <row r="392" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="392" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A392" s="9"/>
       <c r="B392" s="9"/>
       <c r="C392" s="9"/>
@@ -26268,7 +26267,7 @@
         <v/>
       </c>
     </row>
-    <row r="393" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="393" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A393" s="9"/>
       <c r="B393" s="9"/>
       <c r="C393" s="9"/>
@@ -26322,7 +26321,7 @@
         <v/>
       </c>
     </row>
-    <row r="394" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="394" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A394" s="9"/>
       <c r="B394" s="9"/>
       <c r="C394" s="9"/>
@@ -26376,7 +26375,7 @@
         <v/>
       </c>
     </row>
-    <row r="395" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="395" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A395" s="9"/>
       <c r="B395" s="9"/>
       <c r="C395" s="9"/>
@@ -26430,7 +26429,7 @@
         <v/>
       </c>
     </row>
-    <row r="396" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="396" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A396" s="9"/>
       <c r="B396" s="9"/>
       <c r="C396" s="9"/>
@@ -26484,7 +26483,7 @@
         <v/>
       </c>
     </row>
-    <row r="397" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="397" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A397" s="9"/>
       <c r="B397" s="9"/>
       <c r="C397" s="9"/>
@@ -26538,7 +26537,7 @@
         <v/>
       </c>
     </row>
-    <row r="398" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="398" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A398" s="9"/>
       <c r="B398" s="9"/>
       <c r="C398" s="9"/>
@@ -26592,7 +26591,7 @@
         <v/>
       </c>
     </row>
-    <row r="399" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="399" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A399" s="9"/>
       <c r="B399" s="9"/>
       <c r="C399" s="9"/>
@@ -26646,7 +26645,7 @@
         <v/>
       </c>
     </row>
-    <row r="400" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="400" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A400" s="9"/>
       <c r="B400" s="9"/>
       <c r="C400" s="9"/>
@@ -26700,7 +26699,7 @@
         <v/>
       </c>
     </row>
-    <row r="401" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="401" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A401" s="9"/>
       <c r="B401" s="9"/>
       <c r="C401" s="9"/>
@@ -26754,7 +26753,7 @@
         <v/>
       </c>
     </row>
-    <row r="402" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="402" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A402" s="9"/>
       <c r="B402" s="9"/>
       <c r="C402" s="9"/>
@@ -26808,7 +26807,7 @@
         <v/>
       </c>
     </row>
-    <row r="403" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="403" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A403" s="9"/>
       <c r="B403" s="9"/>
       <c r="C403" s="9"/>
@@ -26862,7 +26861,7 @@
         <v/>
       </c>
     </row>
-    <row r="404" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="404" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A404" s="9"/>
       <c r="B404" s="9"/>
       <c r="C404" s="9"/>
@@ -26916,7 +26915,7 @@
         <v/>
       </c>
     </row>
-    <row r="405" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="405" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A405" s="9"/>
       <c r="B405" s="9"/>
       <c r="C405" s="9"/>
@@ -26970,7 +26969,7 @@
         <v/>
       </c>
     </row>
-    <row r="406" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="406" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A406" s="9"/>
       <c r="B406" s="9"/>
       <c r="C406" s="9"/>
@@ -27024,7 +27023,7 @@
         <v/>
       </c>
     </row>
-    <row r="407" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="407" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A407" s="9"/>
       <c r="B407" s="9"/>
       <c r="C407" s="9"/>
@@ -27078,7 +27077,7 @@
         <v/>
       </c>
     </row>
-    <row r="408" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="408" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A408" s="9"/>
       <c r="B408" s="9"/>
       <c r="C408" s="9"/>
@@ -27132,7 +27131,7 @@
         <v/>
       </c>
     </row>
-    <row r="409" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="409" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A409" s="9"/>
       <c r="B409" s="9"/>
       <c r="C409" s="9"/>
@@ -27186,7 +27185,7 @@
         <v/>
       </c>
     </row>
-    <row r="410" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="410" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A410" s="9"/>
       <c r="B410" s="9"/>
       <c r="C410" s="9"/>
@@ -27240,7 +27239,7 @@
         <v/>
       </c>
     </row>
-    <row r="411" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="411" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A411" s="9"/>
       <c r="B411" s="9"/>
       <c r="C411" s="9"/>
@@ -27294,7 +27293,7 @@
         <v/>
       </c>
     </row>
-    <row r="412" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="412" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A412" s="9"/>
       <c r="B412" s="9"/>
       <c r="C412" s="9"/>
@@ -27348,7 +27347,7 @@
         <v/>
       </c>
     </row>
-    <row r="413" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="413" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A413" s="9"/>
       <c r="B413" s="9"/>
       <c r="C413" s="9"/>
@@ -27402,7 +27401,7 @@
         <v/>
       </c>
     </row>
-    <row r="414" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="414" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A414" s="9"/>
       <c r="B414" s="9"/>
       <c r="C414" s="9"/>
@@ -27456,7 +27455,7 @@
         <v/>
       </c>
     </row>
-    <row r="415" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="415" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A415" s="9"/>
       <c r="B415" s="9"/>
       <c r="C415" s="9"/>
@@ -27510,7 +27509,7 @@
         <v/>
       </c>
     </row>
-    <row r="416" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="416" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A416" s="9"/>
       <c r="B416" s="9"/>
       <c r="C416" s="9"/>
@@ -27564,7 +27563,7 @@
         <v/>
       </c>
     </row>
-    <row r="417" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="417" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A417" s="9"/>
       <c r="B417" s="9"/>
       <c r="C417" s="9"/>
@@ -27618,7 +27617,7 @@
         <v/>
       </c>
     </row>
-    <row r="418" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="418" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A418" s="9"/>
       <c r="B418" s="9"/>
       <c r="C418" s="9"/>
@@ -27672,7 +27671,7 @@
         <v/>
       </c>
     </row>
-    <row r="419" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="419" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A419" s="9"/>
       <c r="B419" s="9"/>
       <c r="C419" s="9"/>
@@ -27726,7 +27725,7 @@
         <v/>
       </c>
     </row>
-    <row r="420" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="420" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A420" s="9"/>
       <c r="B420" s="9"/>
       <c r="C420" s="9"/>
@@ -27780,7 +27779,7 @@
         <v/>
       </c>
     </row>
-    <row r="421" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="421" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A421" s="9"/>
       <c r="B421" s="9"/>
       <c r="C421" s="9"/>
@@ -27834,7 +27833,7 @@
         <v/>
       </c>
     </row>
-    <row r="422" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="422" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A422" s="9"/>
       <c r="B422" s="9"/>
       <c r="C422" s="9"/>
@@ -27888,7 +27887,7 @@
         <v/>
       </c>
     </row>
-    <row r="423" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="423" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A423" s="9"/>
       <c r="B423" s="9"/>
       <c r="C423" s="9"/>
@@ -27942,7 +27941,7 @@
         <v/>
       </c>
     </row>
-    <row r="424" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="424" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A424" s="9"/>
       <c r="B424" s="9"/>
       <c r="C424" s="9"/>
@@ -27996,7 +27995,7 @@
         <v/>
       </c>
     </row>
-    <row r="425" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="425" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A425" s="9"/>
       <c r="B425" s="9"/>
       <c r="C425" s="9"/>
@@ -28050,7 +28049,7 @@
         <v/>
       </c>
     </row>
-    <row r="426" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="426" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A426" s="9"/>
       <c r="B426" s="9"/>
       <c r="C426" s="9"/>
@@ -28104,7 +28103,7 @@
         <v/>
       </c>
     </row>
-    <row r="427" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="427" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A427" s="9"/>
       <c r="B427" s="9"/>
       <c r="C427" s="9"/>
@@ -28158,7 +28157,7 @@
         <v/>
       </c>
     </row>
-    <row r="428" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="428" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A428" s="9"/>
       <c r="B428" s="9"/>
       <c r="C428" s="9"/>
@@ -28212,7 +28211,7 @@
         <v/>
       </c>
     </row>
-    <row r="429" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="429" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A429" s="9"/>
       <c r="B429" s="9"/>
       <c r="C429" s="9"/>
@@ -28266,7 +28265,7 @@
         <v/>
       </c>
     </row>
-    <row r="430" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="430" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A430" s="9"/>
       <c r="B430" s="9"/>
       <c r="C430" s="9"/>
@@ -28320,7 +28319,7 @@
         <v/>
       </c>
     </row>
-    <row r="431" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="431" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A431" s="9"/>
       <c r="B431" s="9"/>
       <c r="C431" s="9"/>
@@ -28374,7 +28373,7 @@
         <v/>
       </c>
     </row>
-    <row r="432" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="432" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A432" s="9"/>
       <c r="B432" s="9"/>
       <c r="C432" s="9"/>
@@ -28428,7 +28427,7 @@
         <v/>
       </c>
     </row>
-    <row r="433" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="433" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A433" s="9"/>
       <c r="B433" s="9"/>
       <c r="C433" s="9"/>
@@ -28482,7 +28481,7 @@
         <v/>
       </c>
     </row>
-    <row r="434" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="434" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A434" s="9"/>
       <c r="B434" s="9"/>
       <c r="C434" s="9"/>
@@ -28536,7 +28535,7 @@
         <v/>
       </c>
     </row>
-    <row r="435" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="435" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A435" s="9"/>
       <c r="B435" s="9"/>
       <c r="C435" s="9"/>
@@ -28590,7 +28589,7 @@
         <v/>
       </c>
     </row>
-    <row r="436" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="436" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A436" s="9"/>
       <c r="B436" s="9"/>
       <c r="C436" s="9"/>
@@ -28644,7 +28643,7 @@
         <v/>
       </c>
     </row>
-    <row r="437" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="437" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A437" s="9"/>
       <c r="B437" s="9"/>
       <c r="C437" s="9"/>
@@ -28698,7 +28697,7 @@
         <v/>
       </c>
     </row>
-    <row r="438" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="438" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A438" s="9"/>
       <c r="B438" s="9"/>
       <c r="C438" s="9"/>
@@ -28752,7 +28751,7 @@
         <v/>
       </c>
     </row>
-    <row r="439" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="439" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A439" s="9"/>
       <c r="B439" s="9"/>
       <c r="C439" s="9"/>
@@ -28806,7 +28805,7 @@
         <v/>
       </c>
     </row>
-    <row r="440" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="440" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A440" s="9"/>
       <c r="B440" s="9"/>
       <c r="C440" s="9"/>
@@ -28860,7 +28859,7 @@
         <v/>
       </c>
     </row>
-    <row r="441" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="441" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A441" s="9"/>
       <c r="B441" s="9"/>
       <c r="C441" s="9"/>
@@ -28914,7 +28913,7 @@
         <v/>
       </c>
     </row>
-    <row r="442" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="442" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A442" s="9"/>
       <c r="B442" s="9"/>
       <c r="C442" s="9"/>
@@ -28968,7 +28967,7 @@
         <v/>
       </c>
     </row>
-    <row r="443" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="443" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A443" s="9"/>
       <c r="B443" s="9"/>
       <c r="C443" s="9"/>
@@ -29022,7 +29021,7 @@
         <v/>
       </c>
     </row>
-    <row r="444" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="444" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A444" s="9"/>
       <c r="B444" s="9"/>
       <c r="C444" s="9"/>
@@ -29076,7 +29075,7 @@
         <v/>
       </c>
     </row>
-    <row r="445" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="445" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A445" s="9"/>
       <c r="B445" s="9"/>
       <c r="C445" s="9"/>
@@ -29130,7 +29129,7 @@
         <v/>
       </c>
     </row>
-    <row r="446" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="446" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A446" s="9"/>
       <c r="B446" s="9"/>
       <c r="C446" s="9"/>
@@ -29184,7 +29183,7 @@
         <v/>
       </c>
     </row>
-    <row r="447" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="447" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A447" s="9"/>
       <c r="B447" s="9"/>
       <c r="C447" s="9"/>
@@ -29238,7 +29237,7 @@
         <v/>
       </c>
     </row>
-    <row r="448" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="448" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A448" s="9"/>
       <c r="B448" s="9"/>
       <c r="C448" s="9"/>
@@ -29292,7 +29291,7 @@
         <v/>
       </c>
     </row>
-    <row r="449" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="449" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A449" s="9"/>
       <c r="B449" s="9"/>
       <c r="C449" s="9"/>
@@ -29346,7 +29345,7 @@
         <v/>
       </c>
     </row>
-    <row r="450" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="450" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A450" s="9"/>
       <c r="B450" s="9"/>
       <c r="C450" s="9"/>
@@ -29400,7 +29399,7 @@
         <v/>
       </c>
     </row>
-    <row r="451" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="451" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A451" s="9"/>
       <c r="B451" s="9"/>
       <c r="C451" s="9"/>
@@ -29454,7 +29453,7 @@
         <v/>
       </c>
     </row>
-    <row r="452" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="452" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A452" s="9"/>
       <c r="B452" s="9"/>
       <c r="C452" s="9"/>
@@ -29508,7 +29507,7 @@
         <v/>
       </c>
     </row>
-    <row r="453" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="453" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A453" s="9"/>
       <c r="B453" s="9"/>
       <c r="C453" s="9"/>
@@ -29562,7 +29561,7 @@
         <v/>
       </c>
     </row>
-    <row r="454" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="454" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A454" s="9"/>
       <c r="B454" s="9"/>
       <c r="C454" s="9"/>
@@ -29616,7 +29615,7 @@
         <v/>
       </c>
     </row>
-    <row r="455" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="455" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A455" s="9"/>
       <c r="B455" s="9"/>
       <c r="C455" s="9"/>
@@ -29670,7 +29669,7 @@
         <v/>
       </c>
     </row>
-    <row r="456" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="456" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A456" s="9"/>
       <c r="B456" s="9"/>
       <c r="C456" s="9"/>
@@ -29724,7 +29723,7 @@
         <v/>
       </c>
     </row>
-    <row r="457" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="457" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A457" s="9"/>
       <c r="B457" s="9"/>
       <c r="C457" s="9"/>
@@ -29778,7 +29777,7 @@
         <v/>
       </c>
     </row>
-    <row r="458" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="458" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A458" s="9"/>
       <c r="B458" s="9"/>
       <c r="C458" s="9"/>
@@ -29832,7 +29831,7 @@
         <v/>
       </c>
     </row>
-    <row r="459" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="459" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A459" s="9"/>
       <c r="B459" s="9"/>
       <c r="C459" s="9"/>
@@ -29886,7 +29885,7 @@
         <v/>
       </c>
     </row>
-    <row r="460" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="460" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A460" s="9"/>
       <c r="B460" s="9"/>
       <c r="C460" s="9"/>
@@ -29940,7 +29939,7 @@
         <v/>
       </c>
     </row>
-    <row r="461" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="461" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A461" s="9"/>
       <c r="B461" s="9"/>
       <c r="C461" s="9"/>
@@ -29994,7 +29993,7 @@
         <v/>
       </c>
     </row>
-    <row r="462" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="462" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A462" s="9"/>
       <c r="B462" s="9"/>
       <c r="C462" s="9"/>
@@ -30048,7 +30047,7 @@
         <v/>
       </c>
     </row>
-    <row r="463" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="463" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A463" s="9"/>
       <c r="B463" s="9"/>
       <c r="C463" s="9"/>
@@ -30102,7 +30101,7 @@
         <v/>
       </c>
     </row>
-    <row r="464" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="464" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A464" s="9"/>
       <c r="B464" s="9"/>
       <c r="C464" s="9"/>
@@ -30156,7 +30155,7 @@
         <v/>
       </c>
     </row>
-    <row r="465" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="465" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A465" s="9"/>
       <c r="B465" s="9"/>
       <c r="C465" s="9"/>
@@ -30210,7 +30209,7 @@
         <v/>
       </c>
     </row>
-    <row r="466" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="466" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A466" s="9"/>
       <c r="B466" s="9"/>
       <c r="C466" s="9"/>
@@ -30264,7 +30263,7 @@
         <v/>
       </c>
     </row>
-    <row r="467" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="467" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A467" s="9"/>
       <c r="B467" s="9"/>
       <c r="C467" s="9"/>
@@ -30318,7 +30317,7 @@
         <v/>
       </c>
     </row>
-    <row r="468" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="468" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A468" s="9"/>
       <c r="B468" s="9"/>
       <c r="C468" s="9"/>
@@ -30372,7 +30371,7 @@
         <v/>
       </c>
     </row>
-    <row r="469" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="469" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A469" s="9"/>
       <c r="B469" s="9"/>
       <c r="C469" s="9"/>
@@ -30426,7 +30425,7 @@
         <v/>
       </c>
     </row>
-    <row r="470" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="470" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A470" s="9"/>
       <c r="B470" s="9"/>
       <c r="C470" s="9"/>
@@ -30480,7 +30479,7 @@
         <v/>
       </c>
     </row>
-    <row r="471" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="471" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A471" s="9"/>
       <c r="B471" s="9"/>
       <c r="C471" s="9"/>
@@ -30534,7 +30533,7 @@
         <v/>
       </c>
     </row>
-    <row r="472" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="472" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A472" s="9"/>
       <c r="B472" s="9"/>
       <c r="C472" s="9"/>
@@ -30588,7 +30587,7 @@
         <v/>
       </c>
     </row>
-    <row r="473" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="473" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A473" s="9"/>
       <c r="B473" s="9"/>
       <c r="C473" s="9"/>
@@ -30642,7 +30641,7 @@
         <v/>
       </c>
     </row>
-    <row r="474" spans="1:19" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="474" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A474" s="9"/>
       <c r="B474" s="9"/>
       <c r="C474" s="9"/>
@@ -30697,17 +30696,12 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="4qIM/uYZBbuB2flOCssCipXRrNt8BOgLeV2LioGRgy9IcsU4aNGHcB1aoeFWDzAyXFDfpsBVROP8ajfWLaUZtg==" saltValue="7RQ6t7ZWLRBrA6W5Ixk/Aw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="5ev8HflTjpHYe0K9YMf9gkXdR+KP1Z+NNp7zICQ4GWwJAO7Hddwb1wB/YqCnDn5FYfiPIgyMxrzIhUQRXVgacw==" saltValue="StUGvRh1xBL/PnQTl7iCLQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="I1:S1048576" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>
   </protectedRanges>
   <autoFilter ref="A1:S474" xr:uid="{E7D31E7F-BFF5-4ADE-901A-4F6BC662C23D}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="MWI"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S474">
       <sortCondition ref="A1:A474"/>
     </sortState>

</xml_diff>

<commit_message>
fix: update track layer popup AB#16444
</commit_message>
<xml_diff>
--- a/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
+++ b/interfaces/IBF-dashboard/src/assets/i18n/layer-popup-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\IBF-system\interfaces\IBF-dashboard\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF28E02-1168-4748-93AF-1D31D9867D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D163E0-B052-4E49-95A6-46823BEF995E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13770" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
+    <workbookView xWindow="16740" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="311">
   <si>
     <t>section</t>
   </si>
@@ -1199,25 +1199,6 @@
     <t>The disaster vulnerability index is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts of floods. The National Society and Technical Working group selected the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Poverty: Poverty incidence&lt;/li&gt;&lt;li&gt;20% Gender: Female headed household&lt;/li&gt;&lt;li&gt;10% Age: Population below 8-years&lt;/li&gt;&lt;li&gt;10% Age: population 65+,&lt;/li&gt;&lt;li&gt;10 % type of construction: permanent wall type&lt;/li&gt;&lt;li&gt;10 %type of construction: permanent roof type&lt;/li&gt;&lt;li&gt;20% Refugees legal status #of displaced person&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;For further information please refer to the EAP. For source links, see each individual layer.</t>
   </si>
   <si>
-    <t>Forecasted track of the Typhoon event. The source for this forecast data is ECMWF.
-Point tracker legend:
-- Circle with typhoon icon - shows the latest location of the typhoon.
-- External circle - shows the point of first landfall.
-- Full color circle - shows where the typhoon has already passed.
-- Transparent dashed circle - Shows the future predicted path of the typhoon.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Forecasted track of the Typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;
-&lt;br&gt;
-&lt;p&gt;&lt;strong&gt;Trackpoint legend:&lt;/strong&gt;&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;&lt;strong&gt;Circle with typhoon icon&lt;/strong&gt; shows the latest location of the typhoon&lt;/li&gt;
-&lt;li&gt;&lt;strong&gt;Circle with additional border&lt;/strong&gt; shows the point of first landfall. The calculated time until landfall is based on this point.&lt;/li&gt;
-&lt;li&gt;&lt;strong&gt;Full color circle&lt;/strong&gt; shows where the typhoon has already passed&lt;/li&gt;
-&lt;li&gt;&lt;strong&gt;Transparent dashed circle&lt;/strong&gt; shows the future predicted path of the typhoon&lt;/li&gt;
-&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>evacuation_centers</t>
   </si>
   <si>
@@ -1253,6 +1234,17 @@
 &lt;p&gt;Source link: &lt;a href="https://www.globalfloods.eu/"&gt;https://www.globalfloods.eu/&lt;/a&gt;&amp;nbsp;&lt;/p&gt;
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;
 &lt;p&gt;Latest updated: August 2022&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Forecasted track of the Typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;
+&lt;br&gt;
+&lt;p&gt;&lt;strong&gt;Trackpoint legend:&lt;/strong&gt;&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;&lt;strong&gt;Circle with typhoon icon&lt;/strong&gt; shows the latest location of the typhoon&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Circle with additional border&lt;/strong&gt; shows the point of first landfall (or - if no landfall - the point closest to land). The calculated lead time of the event is based on this point.&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Full color circle&lt;/strong&gt; shows where the typhoon has already passed&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Transparent dashed circle&lt;/strong&gt; shows the future predicted path of the typhoon&lt;/li&gt;
+&lt;/ul&gt;</t>
   </si>
 </sst>
 </file>
@@ -1772,8 +1764,8 @@
   <dimension ref="A1:S474"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G79" sqref="G79"/>
+      <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G223" sqref="G223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2803,7 +2795,7 @@
       <c r="E16" s="21"/>
       <c r="F16" s="5"/>
       <c r="G16" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="str">
@@ -4601,7 +4593,7 @@
       <c r="E43" s="21"/>
       <c r="F43" s="5"/>
       <c r="G43" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H43" s="19"/>
       <c r="I43" s="14" t="str">
@@ -4665,7 +4657,7 @@
       <c r="E44" s="21"/>
       <c r="F44" s="5"/>
       <c r="G44" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H44" s="7">
         <v>44737</v>
@@ -4731,7 +4723,7 @@
       <c r="E45" s="21"/>
       <c r="F45" s="5"/>
       <c r="G45" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H45" s="19"/>
       <c r="I45" s="14" t="str">
@@ -5011,11 +5003,11 @@
         <v>202</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H49" s="7">
         <v>44798</v>
@@ -5287,7 +5279,7 @@
       <c r="E53" s="21"/>
       <c r="F53" s="5"/>
       <c r="G53" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H53" s="19"/>
       <c r="I53" s="14" t="str">
@@ -5355,7 +5347,7 @@
       <c r="E54" s="21"/>
       <c r="F54" s="5"/>
       <c r="G54" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H54" s="19"/>
       <c r="I54" s="14" t="str">
@@ -5419,7 +5411,7 @@
       <c r="E55" s="21"/>
       <c r="F55" s="5"/>
       <c r="G55" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H55" s="19"/>
       <c r="I55" s="14" t="str">
@@ -5483,7 +5475,7 @@
       <c r="E56" s="21"/>
       <c r="F56" s="5"/>
       <c r="G56" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H56" s="19"/>
       <c r="I56" s="14" t="str">
@@ -5617,7 +5609,7 @@
       <c r="E58" s="21"/>
       <c r="F58" s="5"/>
       <c r="G58" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H58" s="19"/>
       <c r="I58" s="14" t="str">
@@ -5751,7 +5743,7 @@
       <c r="E60" s="21"/>
       <c r="F60" s="5"/>
       <c r="G60" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H60" s="19"/>
       <c r="I60" s="14" t="str">
@@ -6255,7 +6247,7 @@
       <c r="E67" s="21"/>
       <c r="F67" s="5"/>
       <c r="G67" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H67" s="19"/>
       <c r="I67" s="14" t="str">
@@ -6508,7 +6500,7 @@
         <v>117</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C71" s="9" t="s">
         <v>9</v>
@@ -6899,7 +6891,7 @@
       <c r="E76" s="21"/>
       <c r="F76" s="5"/>
       <c r="G76" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H76" s="19"/>
       <c r="I76" s="14" t="str">
@@ -7022,7 +7014,7 @@
         <v>117</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C78" s="9" t="s">
         <v>300</v>
@@ -7033,7 +7025,7 @@
       <c r="E78" s="21"/>
       <c r="F78" s="5"/>
       <c r="G78" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H78" s="19"/>
       <c r="I78" s="14" t="str">
@@ -8171,7 +8163,7 @@
       <c r="E95" s="21"/>
       <c r="F95" s="5"/>
       <c r="G95" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H95" s="7">
         <v>44798</v>
@@ -8777,7 +8769,7 @@
       <c r="E104" s="21"/>
       <c r="F104" s="5"/>
       <c r="G104" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H104" s="19"/>
       <c r="I104" s="14" t="str">
@@ -10125,7 +10117,7 @@
       <c r="E124" s="21"/>
       <c r="F124" s="5"/>
       <c r="G124" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H124" s="19"/>
       <c r="I124" s="14" t="str">
@@ -10255,7 +10247,7 @@
       <c r="E126" s="21"/>
       <c r="F126" s="5"/>
       <c r="G126" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H126" s="19"/>
       <c r="I126" s="14" t="str">
@@ -12041,7 +12033,7 @@
       <c r="E152" s="21"/>
       <c r="F152" s="5"/>
       <c r="G152" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H152" s="19"/>
       <c r="I152" s="14" t="str">
@@ -16061,7 +16053,7 @@
       <c r="E212" s="21"/>
       <c r="F212" s="5"/>
       <c r="G212" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H212" s="7">
         <v>44575</v>
@@ -16127,7 +16119,7 @@
       <c r="E213" s="21"/>
       <c r="F213" s="5"/>
       <c r="G213" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H213" s="19"/>
       <c r="I213" s="14" t="str">
@@ -16195,7 +16187,7 @@
         <v>44614</v>
       </c>
       <c r="G214" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H214" s="7">
         <v>44575</v>
@@ -16271,7 +16263,7 @@
       <c r="E215" s="21"/>
       <c r="F215" s="5"/>
       <c r="G215" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H215" s="19"/>
       <c r="I215" s="14" t="str">
@@ -16339,7 +16331,7 @@
         <v>44614</v>
       </c>
       <c r="G216" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H216" s="7">
         <v>44575</v>
@@ -16804,14 +16796,12 @@
       <c r="D223" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="E223" s="21" t="s">
-        <v>302</v>
-      </c>
+      <c r="E223" s="21"/>
       <c r="F223" s="23">
         <v>44879</v>
       </c>
       <c r="G223" s="6" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="H223" s="7">
         <v>44879</v>
@@ -16839,7 +16829,7 @@
 &lt;p&gt;&lt;strong&gt;Trackpoint legend:&lt;/strong&gt;&lt;/p&gt;
 &lt;ul&gt;
 &lt;li&gt;&lt;strong&gt;Circle with typhoon icon&lt;/strong&gt; shows the latest location of the typhoon&lt;/li&gt;
-&lt;li&gt;&lt;strong&gt;Circle with additional border&lt;/strong&gt; shows the point of first landfall. The calculated time until landfall is based on this point.&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Circle with additional border&lt;/strong&gt; shows the point of first landfall (or - if no landfall - the point closest to land). The calculated lead time of the event is based on this point.&lt;/li&gt;
 &lt;li&gt;&lt;strong&gt;Full color circle&lt;/strong&gt; shows where the typhoon has already passed&lt;/li&gt;
 &lt;li&gt;&lt;strong&gt;Transparent dashed circle&lt;/strong&gt; shows the future predicted path of the typhoon&lt;/li&gt;
 &lt;/ul&gt;"</v>
@@ -16871,7 +16861,7 @@
 &lt;p&gt;&lt;strong&gt;Trackpoint legend:&lt;/strong&gt;&lt;/p&gt;
 &lt;ul&gt;
 &lt;li&gt;&lt;strong&gt;Circle with typhoon icon&lt;/strong&gt; shows the latest location of the typhoon&lt;/li&gt;
-&lt;li&gt;&lt;strong&gt;Circle with additional border&lt;/strong&gt; shows the point of first landfall. The calculated time until landfall is based on this point.&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Circle with additional border&lt;/strong&gt; shows the point of first landfall (or - if no landfall - the point closest to land). The calculated lead time of the event is based on this point.&lt;/li&gt;
 &lt;li&gt;&lt;strong&gt;Full color circle&lt;/strong&gt; shows where the typhoon has already passed&lt;/li&gt;
 &lt;li&gt;&lt;strong&gt;Transparent dashed circle&lt;/strong&gt; shows the future predicted path of the typhoon&lt;/li&gt;
 &lt;/ul&gt;"}},</v>
@@ -16983,7 +16973,7 @@
       <c r="E225" s="21"/>
       <c r="F225" s="5"/>
       <c r="G225" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H225" s="19"/>
       <c r="I225" s="14" t="str">
@@ -17463,7 +17453,7 @@
       <c r="E232" s="21"/>
       <c r="F232" s="5"/>
       <c r="G232" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H232" s="19"/>
       <c r="I232" s="14" t="str">
@@ -30696,7 +30686,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="5ev8HflTjpHYe0K9YMf9gkXdR+KP1Z+NNp7zICQ4GWwJAO7Hddwb1wB/YqCnDn5FYfiPIgyMxrzIhUQRXVgacw==" saltValue="StUGvRh1xBL/PnQTl7iCLQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Khb1uXXb0REakVS8prD52uve3y5Nn+5Nk71I9VqNkdIHcCX6zshXnK6MK6vRQ/+1DFxjNWq59VvR9HS/8NmjYA==" saltValue="dG3x9G3qTjFrqd+tXFkXfw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="I1:S1048576" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>

</xml_diff>